<commit_message>
updated the ind_study_matrix.xlsx file with Mitchell indicators
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\admin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C81AD23-C659-4A22-8D29-FB0FE58E7BC2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECE9624-E8EC-42CF-9B6C-AB0E732167BF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="3" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="study_regions" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="568">
   <si>
     <t>Domain</t>
   </si>
@@ -1377,9 +1377,6 @@
     <t>ind_activity.distance/1000.0 AS walk_12,</t>
   </si>
   <si>
-    <t>Bris,Melb,Perth,Syd</t>
-  </si>
-  <si>
     <t>full_locale</t>
   </si>
   <si>
@@ -1568,6 +1565,225 @@
   <si>
     <t xml:space="preserve">/km&lt;sup&gt;2&lt;/sup&gt;_x000D_
 </t>
+  </si>
+  <si>
+    <t>food_3</t>
+  </si>
+  <si>
+    <t>Within 1600m of a healthy foods</t>
+  </si>
+  <si>
+    <t>% residential dwellings &lt; 1600m of a healthy food</t>
+  </si>
+  <si>
+    <t>ind_healthy1600.ind_healthyfood1600_hard AS food_3_hard,</t>
+  </si>
+  <si>
+    <t>LEFT JOIN ind_healthy1600 ON p.gnaf_pid = ind_healthy1600.gnaf_pid</t>
+  </si>
+  <si>
+    <t>ind_healthy1600.ind_healthyfood1600_soft AS food_3_soft,</t>
+  </si>
+  <si>
+    <t>food_4</t>
+  </si>
+  <si>
+    <t>Within 1600m of an unhealthy foods</t>
+  </si>
+  <si>
+    <t>% residential dwellings &lt; 1600m of an unhealthy food</t>
+  </si>
+  <si>
+    <t>ind_unhealthy1600.ind_unhealthyfood1600_hard AS food_4_hard,</t>
+  </si>
+  <si>
+    <t>LEFT JOIN ind_unhealthy1600 ON p.gnaf_pid = ind_unhealthy1600.gnaf_pid</t>
+  </si>
+  <si>
+    <t>ind_unhealthy1600.ind_unhealthyfood1600_soft AS food_4_soft,</t>
+  </si>
+  <si>
+    <t>food_5</t>
+  </si>
+  <si>
+    <t>Average distance to closest healthy food</t>
+  </si>
+  <si>
+    <t>ind_unhealthy.distance/1000.0 As food_5,</t>
+  </si>
+  <si>
+    <t>LEFT JOIN ind_unhealthy ON p.gnaf_pid = ind_unhealthy.gnaf_pid</t>
+  </si>
+  <si>
+    <t>food_6</t>
+  </si>
+  <si>
+    <t>Average distance to closest unhealthy food</t>
+  </si>
+  <si>
+    <t>ind_healthy.distance/1000.0 As food_6,</t>
+  </si>
+  <si>
+    <t>LEFT JOIN ind_healthy ON p.gnaf_pid = ind_healthy.gnaf_pid</t>
+  </si>
+  <si>
+    <t>food_7</t>
+  </si>
+  <si>
+    <t>Number of healthy foods within 1600m</t>
+  </si>
+  <si>
+    <t>Average number of healthy foods &lt;1600m</t>
+  </si>
+  <si>
+    <t>healthy.count_coalesced AS food_7,</t>
+  </si>
+  <si>
+    <t>LEFT JOIN (SELECT parcel_dwellings.gnaf_pid, COALESCE(od_counts.count,0) AS count_coalesced FROM parcel_dwellings LEFT JOIN od_counts ON parcel_dwellings.gnaf_pid = od_counts.gnaf_pid AND dest = 28) healthy ON p.gnaf_pid = healthy.gnaf_pid</t>
+  </si>
+  <si>
+    <t>food_8</t>
+  </si>
+  <si>
+    <t>Number of unhealthy foods within 1600m</t>
+  </si>
+  <si>
+    <t>Average number of unhealthy foods &lt;1600m</t>
+  </si>
+  <si>
+    <t>unhealthy.count_coalesced AS food_8,</t>
+  </si>
+  <si>
+    <t>LEFT JOIN (SELECT parcel_dwellings.gnaf_pid, COALESCE(od_counts.count,0) AS count_coalesced FROM parcel_dwellings LEFT JOIN od_counts ON parcel_dwellings.gnaf_pid = od_counts.gnaf_pid AND dest = 29) unhealthy ON p.gnaf_pid = unhealthy.gnaf_pid</t>
+  </si>
+  <si>
+    <t>food_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proportion of healthy food outlets to healthy food and unhealthy food outlets combined within 3200 m </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average proportion of healthy food outlets to healthy food and unhealthy food outlets combined within 3200 m </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proportion of of healthy food outlets to healthy food and unhealthy food outlets combined within 3200 m </t>
+  </si>
+  <si>
+    <t>ind_healthy_ratio.healthy_proportion AS food_9,</t>
+  </si>
+  <si>
+    <t>LEFT JOIN ind_healthy_ratio ON p.gnaf_pid = ind_healthy_ratio.gnaf_pid</t>
+  </si>
+  <si>
+    <t>trans_7</t>
+  </si>
+  <si>
+    <t>Average distance to closest train station</t>
+  </si>
+  <si>
+    <t>ind_train.distance/1000.0 As trans_7,</t>
+  </si>
+  <si>
+    <t>LEFT JOIN ind_train ON p.gnaf_pid = ind_train.gnaf_pid</t>
+  </si>
+  <si>
+    <t>alc_3</t>
+  </si>
+  <si>
+    <t>Average distance to closest on-licence alcohol</t>
+  </si>
+  <si>
+    <t>ind_alc_on.distance/1000.0 As alc_3,</t>
+  </si>
+  <si>
+    <t>LEFT JOIN ind_alc_on ON p.gnaf_pid = ind_alc_on.gnaf_pid</t>
+  </si>
+  <si>
+    <t>alc_4</t>
+  </si>
+  <si>
+    <t>Average distance to closest off-licence alcohol</t>
+  </si>
+  <si>
+    <t>ind_alc_off.distance/1000.0 As alc_4,</t>
+  </si>
+  <si>
+    <t>LEFT JOIN ind_alc_off ON p.gnaf_pid = ind_alc_off.gnaf_pid</t>
+  </si>
+  <si>
+    <t>Bris,Melb,Perth,Syd,Mitchell</t>
+  </si>
+  <si>
+    <t>kinder_1</t>
+  </si>
+  <si>
+    <t>Within 1600m of a kinder</t>
+  </si>
+  <si>
+    <t>% residential dwellings &lt; 1600m of a kinder</t>
+  </si>
+  <si>
+    <t>ind_kinder1600.ind_kindergarten1600_hard AS kinder_1_soft,</t>
+  </si>
+  <si>
+    <t>LEFT JOIN ind_kinder1600 ON p.gnaf_pid = ind_kinder1600.gnaf_pid</t>
+  </si>
+  <si>
+    <t>ind_kinder1600.ind_kindergarten1600_hard AS kinder_1_hard,</t>
+  </si>
+  <si>
+    <t>kinder_2</t>
+  </si>
+  <si>
+    <t>Average distance to closest kinder</t>
+  </si>
+  <si>
+    <t>ind_kinder.distance/1000.0 As kinder_2,</t>
+  </si>
+  <si>
+    <t>LEFT JOIN ind_kinder ON p.gnaf_pid = ind_kinder.gnaf_pid</t>
+  </si>
+  <si>
+    <t>gp_1</t>
+  </si>
+  <si>
+    <t>Within 1600m of a gp</t>
+  </si>
+  <si>
+    <t>% residential dwellings &lt; 1600m of a gp</t>
+  </si>
+  <si>
+    <t>ind_gp1600.ind_genprac1600_hard AS gp_1_hard,</t>
+  </si>
+  <si>
+    <t>LEFT JOIN ind_gp1600 ON p.gnaf_pid = ind_gp1600.gnaf_pid</t>
+  </si>
+  <si>
+    <t>ind_gp1600.ind_genprac1600_hard AS gp_1_soft,</t>
+  </si>
+  <si>
+    <t>gp_2</t>
+  </si>
+  <si>
+    <t>Average distance to closest gp</t>
+  </si>
+  <si>
+    <t>ind_gp.distance/1000.0 As gp_2,</t>
+  </si>
+  <si>
+    <t>LEFT JOIN ind_gp ON p.gnaf_pid = ind_gp.gnaf_pid</t>
+  </si>
+  <si>
+    <t>river_1</t>
+  </si>
+  <si>
+    <t>Average distance to closest river</t>
+  </si>
+  <si>
+    <t>ind_gp.distance/1000.0 As river_1,</t>
+  </si>
+  <si>
+    <t>LEFT JOIN ind_river ON p.gnaf_pid = ind_river.gnaf_pid</t>
   </si>
 </sst>
 </file>
@@ -2662,7 +2878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317EB008-F691-4F16-B99A-D5845A82BBBD}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2683,166 +2899,166 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B1" s="34" t="s">
         <v>215</v>
       </c>
       <c r="C1" s="34" t="s">
+        <v>437</v>
+      </c>
+      <c r="D1" s="35" t="s">
         <v>438</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="E1" s="35" t="s">
         <v>439</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="F1" s="34" t="s">
         <v>440</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="G1" s="34" t="s">
         <v>441</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="H1" s="34" t="s">
         <v>442</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
+        <v>443</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>443</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>444</v>
       </c>
-      <c r="B2" s="37" t="s">
-        <v>444</v>
-      </c>
-      <c r="C2" s="37" t="s">
+      <c r="D2" s="38" t="s">
         <v>445</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="E2" s="39" t="s">
         <v>446</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="F2" s="37" t="s">
         <v>447</v>
-      </c>
-      <c r="F2" s="37" t="s">
-        <v>448</v>
       </c>
       <c r="G2" s="37"/>
       <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B3" s="37" t="s">
         <v>55</v>
       </c>
       <c r="C3" s="37" t="s">
+        <v>449</v>
+      </c>
+      <c r="D3" s="38" t="s">
         <v>450</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="E3" s="39" t="s">
+        <v>446</v>
+      </c>
+      <c r="F3" s="37" t="s">
         <v>451</v>
       </c>
-      <c r="E3" s="39" t="s">
-        <v>447</v>
-      </c>
-      <c r="F3" s="37" t="s">
+      <c r="G3" s="39" t="s">
         <v>452</v>
-      </c>
-      <c r="G3" s="39" t="s">
-        <v>453</v>
       </c>
       <c r="H3" s="37"/>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
+        <v>453</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>453</v>
+      </c>
+      <c r="C4" s="37" t="s">
         <v>454</v>
       </c>
-      <c r="B4" s="37" t="s">
-        <v>454</v>
-      </c>
-      <c r="C4" s="37" t="s">
+      <c r="D4" s="38" t="s">
         <v>455</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="E4" s="39" t="s">
+        <v>446</v>
+      </c>
+      <c r="F4" s="37" t="s">
         <v>456</v>
-      </c>
-      <c r="E4" s="39" t="s">
-        <v>447</v>
-      </c>
-      <c r="F4" s="37" t="s">
-        <v>457</v>
       </c>
       <c r="G4" s="37"/>
       <c r="H4" s="37"/>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
+        <v>457</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>457</v>
+      </c>
+      <c r="C5" s="37" t="s">
         <v>458</v>
       </c>
-      <c r="B5" s="37" t="s">
-        <v>458</v>
-      </c>
-      <c r="C5" s="37" t="s">
+      <c r="D5" s="38" t="s">
         <v>459</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="E5" s="39" t="s">
+        <v>446</v>
+      </c>
+      <c r="F5" s="37" t="s">
         <v>460</v>
-      </c>
-      <c r="E5" s="39" t="s">
-        <v>447</v>
-      </c>
-      <c r="F5" s="37" t="s">
-        <v>461</v>
       </c>
       <c r="G5" s="37"/>
       <c r="H5" s="37"/>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
+        <v>461</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>461</v>
+      </c>
+      <c r="C6" s="37" t="s">
         <v>462</v>
       </c>
-      <c r="B6" s="37" t="s">
-        <v>462</v>
-      </c>
-      <c r="C6" s="37" t="s">
+      <c r="D6" s="38" t="s">
         <v>463</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="E6" s="39" t="s">
+        <v>446</v>
+      </c>
+      <c r="F6" s="37" t="s">
         <v>464</v>
-      </c>
-      <c r="E6" s="39" t="s">
-        <v>447</v>
-      </c>
-      <c r="F6" s="37" t="s">
-        <v>465</v>
       </c>
       <c r="G6" s="37"/>
       <c r="H6" s="37"/>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B7" s="37" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="37" t="s">
+        <v>466</v>
+      </c>
+      <c r="D7" s="38" t="s">
         <v>467</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="E7" s="39" t="s">
+        <v>446</v>
+      </c>
+      <c r="F7" s="37" t="s">
         <v>468</v>
       </c>
-      <c r="E7" s="39" t="s">
-        <v>447</v>
-      </c>
-      <c r="F7" s="37" t="s">
+      <c r="G7" s="39" t="s">
         <v>469</v>
       </c>
-      <c r="G7" s="39" t="s">
+      <c r="H7" s="37" t="s">
         <v>470</v>
-      </c>
-      <c r="H7" s="37" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -2853,66 +3069,66 @@
         <v>45</v>
       </c>
       <c r="C8" s="37" t="s">
+        <v>471</v>
+      </c>
+      <c r="D8" s="37" t="s">
         <v>472</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="E8" s="39" t="s">
+        <v>446</v>
+      </c>
+      <c r="F8" s="37" t="s">
         <v>473</v>
       </c>
-      <c r="E8" s="39" t="s">
-        <v>447</v>
-      </c>
-      <c r="F8" s="37" t="s">
+      <c r="G8" s="39" t="s">
         <v>474</v>
-      </c>
-      <c r="G8" s="39" t="s">
-        <v>475</v>
       </c>
       <c r="H8" s="37"/>
     </row>
     <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B9" s="37" t="s">
         <v>62</v>
       </c>
       <c r="C9" s="37" t="s">
+        <v>476</v>
+      </c>
+      <c r="D9" s="38" t="s">
         <v>477</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="E9" s="39" t="s">
+        <v>446</v>
+      </c>
+      <c r="F9" s="37" t="s">
         <v>478</v>
       </c>
-      <c r="E9" s="39" t="s">
-        <v>447</v>
-      </c>
-      <c r="F9" s="37" t="s">
+      <c r="G9" s="39" t="s">
         <v>479</v>
       </c>
-      <c r="G9" s="39" t="s">
-        <v>480</v>
-      </c>
       <c r="H9" s="37" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
+        <v>480</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>480</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>466</v>
+      </c>
+      <c r="D10" s="38" t="s">
         <v>481</v>
       </c>
-      <c r="B10" s="37" t="s">
-        <v>481</v>
-      </c>
-      <c r="C10" s="37" t="s">
-        <v>467</v>
-      </c>
-      <c r="D10" s="38" t="s">
+      <c r="E10" s="39" t="s">
         <v>482</v>
       </c>
-      <c r="E10" s="39" t="s">
-        <v>483</v>
-      </c>
       <c r="F10" s="37" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G10" s="37"/>
       <c r="H10" s="37"/>
@@ -2941,18 +3157,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="43" t="s">
+        <v>487</v>
+      </c>
+      <c r="B1" s="43" t="s">
         <v>488</v>
-      </c>
-      <c r="B1" s="43" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="46" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B2" s="44" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2960,60 +3176,60 @@
         <v>215</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B7" s="44" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B8" s="44" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="48" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B9" s="45" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
   </sheetData>
@@ -5274,10 +5490,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E520E13B-C7CF-4991-8581-C25916074E3A}">
-  <dimension ref="A1:O67"/>
+  <dimension ref="A1:O86"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6008,7 +6224,7 @@
         <v>1</v>
       </c>
       <c r="N18" s="27" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="O18" s="22" t="s">
         <v>327</v>
@@ -6647,50 +6863,44 @@
         <v>327</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="B33" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="C33" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>382</v>
-      </c>
-      <c r="E33" s="31" t="s">
+    <row r="33" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>531</v>
+      </c>
+      <c r="C33" t="s">
+        <v>480</v>
+      </c>
+      <c r="D33" t="s">
+        <v>532</v>
+      </c>
+      <c r="E33" t="s">
         <v>434</v>
       </c>
-      <c r="F33" s="23" t="s">
-        <v>321</v>
-      </c>
-      <c r="G33" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="H33" s="22" t="s">
-        <v>356</v>
-      </c>
-      <c r="I33" s="22" t="s">
-        <v>247</v>
-      </c>
-      <c r="J33" s="22" t="s">
-        <v>270</v>
-      </c>
-      <c r="K33" s="28" t="s">
-        <v>285</v>
-      </c>
-      <c r="L33" s="22">
-        <v>100</v>
-      </c>
-      <c r="M33" s="30">
-        <v>95</v>
-      </c>
-      <c r="N33" s="30" t="s">
-        <v>331</v>
-      </c>
-      <c r="O33" s="22" t="s">
+      <c r="F33" t="s">
+        <v>317</v>
+      </c>
+      <c r="G33" t="s">
+        <v>532</v>
+      </c>
+      <c r="H33" t="s">
+        <v>532</v>
+      </c>
+      <c r="I33" t="s">
+        <v>533</v>
+      </c>
+      <c r="J33" t="s">
+        <v>534</v>
+      </c>
+      <c r="K33" t="s">
+        <v>291</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="N33" t="s">
+        <v>429</v>
+      </c>
+      <c r="O33" t="s">
         <v>327</v>
       </c>
     </row>
@@ -6699,13 +6909,13 @@
         <v>189</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C34" s="23" t="s">
         <v>34</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
       <c r="E34" s="31" t="s">
         <v>434</v>
@@ -6720,7 +6930,7 @@
         <v>356</v>
       </c>
       <c r="I34" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J34" s="22" t="s">
         <v>270</v>
@@ -6743,34 +6953,34 @@
     </row>
     <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>381</v>
+        <v>400</v>
       </c>
       <c r="E35" s="31" t="s">
         <v>434</v>
       </c>
       <c r="F35" s="23" t="s">
-        <v>428</v>
+        <v>321</v>
       </c>
       <c r="G35" s="22" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H35" s="22" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="I35" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J35" s="22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K35" s="28" t="s">
         <v>285</v>
@@ -6779,7 +6989,7 @@
         <v>100</v>
       </c>
       <c r="M35" s="30">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N35" s="30" t="s">
         <v>331</v>
@@ -6793,13 +7003,13 @@
         <v>190</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C36" s="23" t="s">
         <v>45</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>403</v>
+        <v>381</v>
       </c>
       <c r="E36" s="31" t="s">
         <v>434</v>
@@ -6814,7 +7024,7 @@
         <v>349</v>
       </c>
       <c r="I36" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J36" s="22" t="s">
         <v>271</v>
@@ -6837,34 +7047,34 @@
     </row>
     <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C37" s="23" t="s">
         <v>45</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E37" s="31" t="s">
         <v>434</v>
       </c>
       <c r="F37" s="23" t="s">
-        <v>322</v>
+        <v>428</v>
       </c>
       <c r="G37" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H37" s="22" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="I37" s="22" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J37" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K37" s="28" t="s">
         <v>285</v>
@@ -6873,7 +7083,7 @@
         <v>100</v>
       </c>
       <c r="M37" s="30">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="N37" s="30" t="s">
         <v>331</v>
@@ -6887,13 +7097,13 @@
         <v>191</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C38" s="23" t="s">
         <v>45</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E38" s="31" t="s">
         <v>434</v>
@@ -6908,7 +7118,7 @@
         <v>351</v>
       </c>
       <c r="I38" s="22" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J38" s="22" t="s">
         <v>272</v>
@@ -6931,16 +7141,16 @@
     </row>
     <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C39" s="23" t="s">
         <v>45</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E39" s="31" t="s">
         <v>434</v>
@@ -6949,16 +7159,16 @@
         <v>322</v>
       </c>
       <c r="G39" s="22" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H39" s="22" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I39" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J39" s="22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K39" s="28" t="s">
         <v>285</v>
@@ -6981,13 +7191,13 @@
         <v>192</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C40" s="23" t="s">
         <v>45</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E40" s="31" t="s">
         <v>434</v>
@@ -7002,7 +7212,7 @@
         <v>352</v>
       </c>
       <c r="I40" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J40" s="22" t="s">
         <v>273</v>
@@ -7025,16 +7235,16 @@
     </row>
     <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C41" s="23" t="s">
         <v>45</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E41" s="31" t="s">
         <v>434</v>
@@ -7043,16 +7253,16 @@
         <v>322</v>
       </c>
       <c r="G41" s="22" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H41" s="22" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I41" s="22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J41" s="22" t="s">
-        <v>218</v>
+        <v>273</v>
       </c>
       <c r="K41" s="28" t="s">
         <v>285</v>
@@ -7075,13 +7285,13 @@
         <v>193</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C42" s="23" t="s">
         <v>45</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E42" s="31" t="s">
         <v>434</v>
@@ -7096,7 +7306,7 @@
         <v>353</v>
       </c>
       <c r="I42" s="22" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J42" s="22" t="s">
         <v>218</v>
@@ -7119,34 +7329,34 @@
     </row>
     <row r="43" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="E43" s="31" t="s">
         <v>434</v>
       </c>
       <c r="F43" s="23" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G43" s="22" t="s">
-        <v>283</v>
+        <v>114</v>
       </c>
       <c r="H43" s="22" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="I43" s="22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J43" s="22" t="s">
-        <v>274</v>
+        <v>218</v>
       </c>
       <c r="K43" s="28" t="s">
         <v>285</v>
@@ -7155,7 +7365,7 @@
         <v>100</v>
       </c>
       <c r="M43" s="30">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="N43" s="30" t="s">
         <v>331</v>
@@ -7169,13 +7379,13 @@
         <v>194</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C44" s="23" t="s">
         <v>55</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E44" s="31" t="s">
         <v>434</v>
@@ -7190,7 +7400,7 @@
         <v>357</v>
       </c>
       <c r="I44" s="22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J44" s="22" t="s">
         <v>274</v>
@@ -7213,16 +7423,16 @@
     </row>
     <row r="45" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C45" s="23" t="s">
         <v>55</v>
       </c>
       <c r="D45" s="22" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="E45" s="31" t="s">
         <v>434</v>
@@ -7231,16 +7441,16 @@
         <v>323</v>
       </c>
       <c r="G45" s="22" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H45" s="22" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I45" s="22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J45" s="22" t="s">
-        <v>219</v>
+        <v>274</v>
       </c>
       <c r="K45" s="28" t="s">
         <v>285</v>
@@ -7263,13 +7473,13 @@
         <v>195</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C46" s="23" t="s">
         <v>55</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E46" s="31" t="s">
         <v>434</v>
@@ -7284,7 +7494,7 @@
         <v>358</v>
       </c>
       <c r="I46" s="22" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J46" s="22" t="s">
         <v>219</v>
@@ -7307,34 +7517,34 @@
     </row>
     <row r="47" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="E47" s="31" t="s">
         <v>434</v>
       </c>
       <c r="F47" s="23" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G47" s="22" t="s">
-        <v>126</v>
+        <v>284</v>
       </c>
       <c r="H47" s="22" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="I47" s="22" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J47" s="22" t="s">
-        <v>275</v>
+        <v>219</v>
       </c>
       <c r="K47" s="28" t="s">
         <v>285</v>
@@ -7343,7 +7553,7 @@
         <v>100</v>
       </c>
       <c r="M47" s="30">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="N47" s="30" t="s">
         <v>331</v>
@@ -7357,13 +7567,13 @@
         <v>196</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C48" s="23" t="s">
         <v>62</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E48" s="31" t="s">
         <v>434</v>
@@ -7378,7 +7588,7 @@
         <v>354</v>
       </c>
       <c r="I48" s="22" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J48" s="22" t="s">
         <v>275</v>
@@ -7401,16 +7611,16 @@
     </row>
     <row r="49" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C49" s="23" t="s">
         <v>62</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E49" s="31" t="s">
         <v>434</v>
@@ -7419,16 +7629,16 @@
         <v>324</v>
       </c>
       <c r="G49" s="22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H49" s="22" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I49" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J49" s="22" t="s">
-        <v>220</v>
+        <v>275</v>
       </c>
       <c r="K49" s="28" t="s">
         <v>285</v>
@@ -7451,13 +7661,13 @@
         <v>197</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C50" s="23" t="s">
         <v>62</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E50" s="31" t="s">
         <v>434</v>
@@ -7472,7 +7682,7 @@
         <v>355</v>
       </c>
       <c r="I50" s="22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J50" s="22" t="s">
         <v>220</v>
@@ -7495,40 +7705,43 @@
     </row>
     <row r="51" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>280</v>
+        <v>62</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>379</v>
+        <v>419</v>
       </c>
       <c r="E51" s="31" t="s">
         <v>434</v>
       </c>
       <c r="F51" s="23" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="G51" s="22" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H51" s="22" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="I51" s="22" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J51" s="22" t="s">
-        <v>270</v>
-      </c>
-      <c r="K51" s="22" t="s">
-        <v>286</v>
+        <v>220</v>
+      </c>
+      <c r="K51" s="28" t="s">
+        <v>285</v>
       </c>
       <c r="L51" s="22">
         <v>100</v>
+      </c>
+      <c r="M51" s="30">
+        <v>50</v>
       </c>
       <c r="N51" s="30" t="s">
         <v>331</v>
@@ -7542,13 +7755,13 @@
         <v>198</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C52" s="23" t="s">
         <v>280</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>402</v>
+        <v>379</v>
       </c>
       <c r="E52" s="31" t="s">
         <v>434</v>
@@ -7563,7 +7776,7 @@
         <v>359</v>
       </c>
       <c r="I52" s="22" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J52" s="22" t="s">
         <v>270</v>
@@ -7583,16 +7796,16 @@
     </row>
     <row r="53" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C53" s="23" t="s">
         <v>280</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>420</v>
+        <v>402</v>
       </c>
       <c r="E53" s="31" t="s">
         <v>434</v>
@@ -7601,16 +7814,16 @@
         <v>317</v>
       </c>
       <c r="G53" s="22" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H53" s="22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="I53" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J53" s="22" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="K53" s="22" t="s">
         <v>286</v>
@@ -7630,13 +7843,13 @@
         <v>199</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C54" s="23" t="s">
         <v>280</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E54" s="31" t="s">
         <v>434</v>
@@ -7651,7 +7864,7 @@
         <v>360</v>
       </c>
       <c r="I54" s="22" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J54" s="22" t="s">
         <v>276</v>
@@ -7671,14 +7884,16 @@
     </row>
     <row r="55" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="23" t="s">
-        <v>200</v>
-      </c>
-      <c r="B55" s="23"/>
+        <v>199</v>
+      </c>
+      <c r="B55" s="23" t="s">
+        <v>214</v>
+      </c>
       <c r="C55" s="23" t="s">
         <v>280</v>
       </c>
       <c r="D55" s="22" t="s">
-        <v>373</v>
+        <v>421</v>
       </c>
       <c r="E55" s="31" t="s">
         <v>434</v>
@@ -7687,10 +7902,16 @@
         <v>317</v>
       </c>
       <c r="G55" s="22" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H55" s="22" t="s">
-        <v>373</v>
+        <v>360</v>
+      </c>
+      <c r="I55" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="J55" s="22" t="s">
+        <v>276</v>
       </c>
       <c r="K55" s="22" t="s">
         <v>286</v>
@@ -7707,14 +7928,14 @@
     </row>
     <row r="56" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B56" s="23"/>
       <c r="C56" s="23" t="s">
-        <v>211</v>
+        <v>280</v>
       </c>
       <c r="D56" s="22" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E56" s="31" t="s">
         <v>434</v>
@@ -7723,10 +7944,10 @@
         <v>317</v>
       </c>
       <c r="G56" s="22" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H56" s="22" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K56" s="22" t="s">
         <v>286</v>
@@ -7743,14 +7964,14 @@
     </row>
     <row r="57" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B57" s="23"/>
       <c r="C57" s="23" t="s">
         <v>211</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E57" s="31" t="s">
         <v>434</v>
@@ -7759,10 +7980,10 @@
         <v>317</v>
       </c>
       <c r="G57" s="22" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H57" s="22" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="K57" s="22" t="s">
         <v>286</v>
@@ -7779,14 +8000,14 @@
     </row>
     <row r="58" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="23" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B58" s="23"/>
       <c r="C58" s="23" t="s">
         <v>211</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="E58" s="31" t="s">
         <v>434</v>
@@ -7795,10 +8016,10 @@
         <v>317</v>
       </c>
       <c r="G58" s="22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H58" s="22" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="K58" s="22" t="s">
         <v>286</v>
@@ -7815,14 +8036,14 @@
     </row>
     <row r="59" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B59" s="23"/>
       <c r="C59" s="23" t="s">
         <v>211</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E59" s="31" t="s">
         <v>434</v>
@@ -7831,10 +8052,10 @@
         <v>317</v>
       </c>
       <c r="G59" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H59" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K59" s="22" t="s">
         <v>286</v>
@@ -7851,14 +8072,14 @@
     </row>
     <row r="60" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B60" s="23"/>
       <c r="C60" s="23" t="s">
         <v>211</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E60" s="31" t="s">
         <v>434</v>
@@ -7867,10 +8088,10 @@
         <v>317</v>
       </c>
       <c r="G60" s="22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H60" s="22" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="K60" s="22" t="s">
         <v>286</v>
@@ -7887,14 +8108,14 @@
     </row>
     <row r="61" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B61" s="23"/>
       <c r="C61" s="23" t="s">
         <v>211</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E61" s="31" t="s">
         <v>434</v>
@@ -7903,10 +8124,10 @@
         <v>317</v>
       </c>
       <c r="G61" s="22" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H61" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K61" s="22" t="s">
         <v>286</v>
@@ -7923,14 +8144,14 @@
     </row>
     <row r="62" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B62" s="23"/>
       <c r="C62" s="23" t="s">
         <v>211</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E62" s="31" t="s">
         <v>434</v>
@@ -7939,10 +8160,10 @@
         <v>317</v>
       </c>
       <c r="G62" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H62" s="22" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="K62" s="22" t="s">
         <v>286</v>
@@ -7959,14 +8180,14 @@
     </row>
     <row r="63" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B63" s="23"/>
       <c r="C63" s="23" t="s">
         <v>211</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>424</v>
+        <v>370</v>
       </c>
       <c r="E63" s="31" t="s">
         <v>434</v>
@@ -7975,40 +8196,34 @@
         <v>317</v>
       </c>
       <c r="G63" s="22" t="s">
-        <v>302</v>
+        <v>150</v>
       </c>
       <c r="H63" s="22" t="s">
-        <v>365</v>
-      </c>
-      <c r="I63" s="22" t="s">
-        <v>227</v>
-      </c>
-      <c r="J63" s="22" t="s">
-        <v>237</v>
-      </c>
-      <c r="K63" s="28" t="s">
-        <v>288</v>
+        <v>370</v>
+      </c>
+      <c r="K63" s="22" t="s">
+        <v>286</v>
       </c>
       <c r="L63" s="22">
-        <v>1</v>
-      </c>
-      <c r="N63" s="30"/>
+        <v>100</v>
+      </c>
+      <c r="N63" s="30" t="s">
+        <v>331</v>
+      </c>
       <c r="O63" s="22" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="64" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="23" t="s">
-        <v>207</v>
-      </c>
-      <c r="B64" s="23" t="s">
-        <v>210</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="B64" s="23"/>
       <c r="C64" s="23" t="s">
         <v>211</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>380</v>
+        <v>424</v>
       </c>
       <c r="E64" s="31" t="s">
         <v>434</v>
@@ -8017,26 +8232,24 @@
         <v>317</v>
       </c>
       <c r="G64" s="22" t="s">
-        <v>157</v>
+        <v>302</v>
       </c>
       <c r="H64" s="22" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="I64" s="22" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
       <c r="J64" s="22" t="s">
-        <v>238</v>
-      </c>
-      <c r="K64" s="22" t="s">
-        <v>286</v>
+        <v>237</v>
+      </c>
+      <c r="K64" s="28" t="s">
+        <v>288</v>
       </c>
       <c r="L64" s="22">
-        <v>100</v>
-      </c>
-      <c r="N64" s="30" t="s">
-        <v>331</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="N64" s="30"/>
       <c r="O64" s="22" t="s">
         <v>327</v>
       </c>
@@ -8046,13 +8259,13 @@
         <v>207</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C65" s="23" t="s">
         <v>211</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>401</v>
+        <v>380</v>
       </c>
       <c r="E65" s="31" t="s">
         <v>434</v>
@@ -8067,7 +8280,7 @@
         <v>361</v>
       </c>
       <c r="I65" s="22" t="s">
-        <v>269</v>
+        <v>246</v>
       </c>
       <c r="J65" s="22" t="s">
         <v>238</v>
@@ -8087,14 +8300,16 @@
     </row>
     <row r="66" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="23" t="s">
-        <v>208</v>
-      </c>
-      <c r="B66" s="23"/>
+        <v>207</v>
+      </c>
+      <c r="B66" s="23" t="s">
+        <v>214</v>
+      </c>
       <c r="C66" s="23" t="s">
-        <v>436</v>
+        <v>211</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>422</v>
+        <v>401</v>
       </c>
       <c r="E66" s="31" t="s">
         <v>434</v>
@@ -8103,66 +8318,861 @@
         <v>317</v>
       </c>
       <c r="G66" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="H66" s="22" t="s">
+        <v>361</v>
+      </c>
+      <c r="I66" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="J66" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="K66" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="L66" s="22">
+        <v>100</v>
+      </c>
+      <c r="N66" s="30" t="s">
+        <v>331</v>
+      </c>
+      <c r="O66" s="22" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>495</v>
+      </c>
+      <c r="B67" t="s">
+        <v>210</v>
+      </c>
+      <c r="C67" t="s">
+        <v>480</v>
+      </c>
+      <c r="D67" t="s">
+        <v>496</v>
+      </c>
+      <c r="E67" t="s">
+        <v>434</v>
+      </c>
+      <c r="F67" t="s">
+        <v>317</v>
+      </c>
+      <c r="G67" t="s">
+        <v>497</v>
+      </c>
+      <c r="H67" t="s">
+        <v>496</v>
+      </c>
+      <c r="I67" t="s">
+        <v>498</v>
+      </c>
+      <c r="J67" t="s">
+        <v>499</v>
+      </c>
+      <c r="K67" t="s">
+        <v>286</v>
+      </c>
+      <c r="L67">
+        <v>100</v>
+      </c>
+      <c r="N67" t="s">
+        <v>331</v>
+      </c>
+      <c r="O67" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>495</v>
+      </c>
+      <c r="B68" t="s">
+        <v>214</v>
+      </c>
+      <c r="C68" t="s">
+        <v>480</v>
+      </c>
+      <c r="D68" t="s">
+        <v>496</v>
+      </c>
+      <c r="E68" t="s">
+        <v>434</v>
+      </c>
+      <c r="F68" t="s">
+        <v>317</v>
+      </c>
+      <c r="G68" t="s">
+        <v>497</v>
+      </c>
+      <c r="H68" t="s">
+        <v>496</v>
+      </c>
+      <c r="I68" t="s">
+        <v>500</v>
+      </c>
+      <c r="J68" t="s">
+        <v>499</v>
+      </c>
+      <c r="K68" t="s">
+        <v>286</v>
+      </c>
+      <c r="L68">
+        <v>100</v>
+      </c>
+      <c r="N68" t="s">
+        <v>331</v>
+      </c>
+      <c r="O68" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>501</v>
+      </c>
+      <c r="B69" t="s">
+        <v>210</v>
+      </c>
+      <c r="C69" t="s">
+        <v>480</v>
+      </c>
+      <c r="D69" t="s">
+        <v>502</v>
+      </c>
+      <c r="E69" t="s">
+        <v>434</v>
+      </c>
+      <c r="F69" t="s">
+        <v>317</v>
+      </c>
+      <c r="G69" t="s">
+        <v>503</v>
+      </c>
+      <c r="H69" t="s">
+        <v>502</v>
+      </c>
+      <c r="I69" t="s">
+        <v>504</v>
+      </c>
+      <c r="J69" t="s">
+        <v>505</v>
+      </c>
+      <c r="K69" t="s">
+        <v>286</v>
+      </c>
+      <c r="L69">
+        <v>100</v>
+      </c>
+      <c r="N69" t="s">
+        <v>331</v>
+      </c>
+      <c r="O69" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>501</v>
+      </c>
+      <c r="B70" t="s">
+        <v>214</v>
+      </c>
+      <c r="C70" t="s">
+        <v>480</v>
+      </c>
+      <c r="D70" t="s">
+        <v>502</v>
+      </c>
+      <c r="E70" t="s">
+        <v>434</v>
+      </c>
+      <c r="F70" t="s">
+        <v>317</v>
+      </c>
+      <c r="G70" t="s">
+        <v>503</v>
+      </c>
+      <c r="H70" t="s">
+        <v>502</v>
+      </c>
+      <c r="I70" t="s">
+        <v>506</v>
+      </c>
+      <c r="J70" t="s">
+        <v>505</v>
+      </c>
+      <c r="K70" t="s">
+        <v>286</v>
+      </c>
+      <c r="L70">
+        <v>100</v>
+      </c>
+      <c r="N70" t="s">
+        <v>331</v>
+      </c>
+      <c r="O70" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>507</v>
+      </c>
+      <c r="C71" t="s">
+        <v>480</v>
+      </c>
+      <c r="D71" t="s">
+        <v>508</v>
+      </c>
+      <c r="E71" t="s">
+        <v>434</v>
+      </c>
+      <c r="F71" t="s">
+        <v>317</v>
+      </c>
+      <c r="G71" t="s">
+        <v>508</v>
+      </c>
+      <c r="H71" t="s">
+        <v>508</v>
+      </c>
+      <c r="I71" t="s">
+        <v>509</v>
+      </c>
+      <c r="J71" t="s">
+        <v>510</v>
+      </c>
+      <c r="K71" t="s">
+        <v>291</v>
+      </c>
+      <c r="L71">
+        <v>1</v>
+      </c>
+      <c r="N71" t="s">
+        <v>429</v>
+      </c>
+      <c r="O71" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>511</v>
+      </c>
+      <c r="C72" t="s">
+        <v>480</v>
+      </c>
+      <c r="D72" t="s">
+        <v>512</v>
+      </c>
+      <c r="E72" t="s">
+        <v>434</v>
+      </c>
+      <c r="F72" t="s">
+        <v>317</v>
+      </c>
+      <c r="G72" t="s">
+        <v>512</v>
+      </c>
+      <c r="H72" t="s">
+        <v>512</v>
+      </c>
+      <c r="I72" t="s">
+        <v>513</v>
+      </c>
+      <c r="J72" t="s">
+        <v>514</v>
+      </c>
+      <c r="K72" t="s">
+        <v>291</v>
+      </c>
+      <c r="L72">
+        <v>1</v>
+      </c>
+      <c r="N72" t="s">
+        <v>429</v>
+      </c>
+      <c r="O72" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>515</v>
+      </c>
+      <c r="C73" t="s">
+        <v>480</v>
+      </c>
+      <c r="D73" t="s">
+        <v>516</v>
+      </c>
+      <c r="E73" t="s">
+        <v>434</v>
+      </c>
+      <c r="F73" t="s">
+        <v>317</v>
+      </c>
+      <c r="G73" t="s">
+        <v>517</v>
+      </c>
+      <c r="H73" t="s">
+        <v>516</v>
+      </c>
+      <c r="I73" t="s">
+        <v>518</v>
+      </c>
+      <c r="J73" t="s">
+        <v>519</v>
+      </c>
+      <c r="K73" t="s">
+        <v>292</v>
+      </c>
+      <c r="L73">
+        <v>1</v>
+      </c>
+      <c r="O73" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>520</v>
+      </c>
+      <c r="C74" t="s">
+        <v>480</v>
+      </c>
+      <c r="D74" t="s">
+        <v>521</v>
+      </c>
+      <c r="E74" t="s">
+        <v>434</v>
+      </c>
+      <c r="F74" t="s">
+        <v>317</v>
+      </c>
+      <c r="G74" t="s">
+        <v>522</v>
+      </c>
+      <c r="H74" t="s">
+        <v>521</v>
+      </c>
+      <c r="I74" t="s">
+        <v>523</v>
+      </c>
+      <c r="J74" t="s">
+        <v>524</v>
+      </c>
+      <c r="K74" t="s">
+        <v>292</v>
+      </c>
+      <c r="L74">
+        <v>1</v>
+      </c>
+      <c r="O74" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>525</v>
+      </c>
+      <c r="C75" t="s">
+        <v>480</v>
+      </c>
+      <c r="D75" t="s">
+        <v>526</v>
+      </c>
+      <c r="E75" t="s">
+        <v>434</v>
+      </c>
+      <c r="F75" t="s">
+        <v>317</v>
+      </c>
+      <c r="G75" t="s">
+        <v>527</v>
+      </c>
+      <c r="H75" t="s">
+        <v>528</v>
+      </c>
+      <c r="I75" t="s">
+        <v>529</v>
+      </c>
+      <c r="J75" t="s">
+        <v>530</v>
+      </c>
+      <c r="K75" t="s">
+        <v>288</v>
+      </c>
+      <c r="L75">
+        <v>1</v>
+      </c>
+      <c r="O75" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="B76" s="23"/>
+      <c r="C76" s="23" t="s">
+        <v>543</v>
+      </c>
+      <c r="D76" s="22" t="s">
+        <v>422</v>
+      </c>
+      <c r="E76" s="31" t="s">
+        <v>434</v>
+      </c>
+      <c r="F76" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="G76" s="22" t="s">
         <v>303</v>
       </c>
-      <c r="H66" s="22" t="s">
+      <c r="H76" s="22" t="s">
         <v>363</v>
       </c>
-      <c r="I66" s="22" t="s">
+      <c r="I76" s="22" t="s">
         <v>228</v>
       </c>
-      <c r="J66" s="22" t="s">
+      <c r="J76" s="22" t="s">
         <v>239</v>
       </c>
-      <c r="K66" s="28" t="s">
+      <c r="K76" s="28" t="s">
         <v>292</v>
       </c>
-      <c r="L66" s="22">
+      <c r="L76" s="22">
         <v>1</v>
       </c>
-      <c r="N66" s="30"/>
-      <c r="O66" s="22" t="s">
+      <c r="N76" s="30"/>
+      <c r="O76" s="22" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="23" t="s">
+    <row r="77" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="B67" s="23"/>
-      <c r="C67" s="23" t="s">
-        <v>436</v>
-      </c>
-      <c r="D67" s="22" t="s">
+      <c r="B77" s="23"/>
+      <c r="C77" s="23" t="s">
+        <v>543</v>
+      </c>
+      <c r="D77" s="22" t="s">
         <v>423</v>
       </c>
-      <c r="E67" s="31" t="s">
+      <c r="E77" s="31" t="s">
         <v>434</v>
       </c>
-      <c r="F67" s="23" t="s">
+      <c r="F77" s="23" t="s">
         <v>317</v>
       </c>
-      <c r="G67" s="22" t="s">
+      <c r="G77" s="22" t="s">
         <v>304</v>
       </c>
-      <c r="H67" s="22" t="s">
+      <c r="H77" s="22" t="s">
         <v>364</v>
       </c>
-      <c r="I67" s="22" t="s">
+      <c r="I77" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="J67" s="22" t="s">
+      <c r="J77" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="K67" s="28" t="s">
+      <c r="K77" s="28" t="s">
         <v>292</v>
       </c>
-      <c r="L67" s="22">
+      <c r="L77" s="22">
         <v>1</v>
       </c>
-      <c r="N67" s="30"/>
-      <c r="O67" s="22" t="s">
+      <c r="N77" s="30"/>
+      <c r="O77" s="22" t="s">
         <v>328</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>535</v>
+      </c>
+      <c r="C78" t="s">
+        <v>480</v>
+      </c>
+      <c r="D78" t="s">
+        <v>536</v>
+      </c>
+      <c r="E78" t="s">
+        <v>434</v>
+      </c>
+      <c r="F78" t="s">
+        <v>317</v>
+      </c>
+      <c r="G78" t="s">
+        <v>536</v>
+      </c>
+      <c r="H78" t="s">
+        <v>536</v>
+      </c>
+      <c r="I78" t="s">
+        <v>537</v>
+      </c>
+      <c r="J78" t="s">
+        <v>538</v>
+      </c>
+      <c r="K78" t="s">
+        <v>291</v>
+      </c>
+      <c r="L78">
+        <v>1</v>
+      </c>
+      <c r="N78" t="s">
+        <v>429</v>
+      </c>
+      <c r="O78" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>539</v>
+      </c>
+      <c r="C79" t="s">
+        <v>480</v>
+      </c>
+      <c r="D79" t="s">
+        <v>540</v>
+      </c>
+      <c r="E79" t="s">
+        <v>434</v>
+      </c>
+      <c r="F79" t="s">
+        <v>317</v>
+      </c>
+      <c r="G79" t="s">
+        <v>540</v>
+      </c>
+      <c r="H79" t="s">
+        <v>540</v>
+      </c>
+      <c r="I79" t="s">
+        <v>541</v>
+      </c>
+      <c r="J79" t="s">
+        <v>542</v>
+      </c>
+      <c r="K79" t="s">
+        <v>291</v>
+      </c>
+      <c r="L79">
+        <v>1</v>
+      </c>
+      <c r="N79" t="s">
+        <v>429</v>
+      </c>
+      <c r="O79" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>544</v>
+      </c>
+      <c r="B80" t="s">
+        <v>210</v>
+      </c>
+      <c r="C80" t="s">
+        <v>480</v>
+      </c>
+      <c r="D80" t="s">
+        <v>545</v>
+      </c>
+      <c r="E80" t="s">
+        <v>434</v>
+      </c>
+      <c r="F80" t="s">
+        <v>317</v>
+      </c>
+      <c r="G80" t="s">
+        <v>546</v>
+      </c>
+      <c r="H80" t="s">
+        <v>545</v>
+      </c>
+      <c r="I80" t="s">
+        <v>547</v>
+      </c>
+      <c r="J80" t="s">
+        <v>548</v>
+      </c>
+      <c r="K80" t="s">
+        <v>286</v>
+      </c>
+      <c r="L80">
+        <v>100</v>
+      </c>
+      <c r="N80" t="s">
+        <v>331</v>
+      </c>
+      <c r="O80" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>544</v>
+      </c>
+      <c r="B81" t="s">
+        <v>214</v>
+      </c>
+      <c r="C81" t="s">
+        <v>480</v>
+      </c>
+      <c r="D81" t="s">
+        <v>545</v>
+      </c>
+      <c r="E81" t="s">
+        <v>434</v>
+      </c>
+      <c r="F81" t="s">
+        <v>317</v>
+      </c>
+      <c r="G81" t="s">
+        <v>546</v>
+      </c>
+      <c r="H81" t="s">
+        <v>545</v>
+      </c>
+      <c r="I81" t="s">
+        <v>549</v>
+      </c>
+      <c r="J81" t="s">
+        <v>548</v>
+      </c>
+      <c r="K81" t="s">
+        <v>286</v>
+      </c>
+      <c r="L81">
+        <v>100</v>
+      </c>
+      <c r="N81" t="s">
+        <v>331</v>
+      </c>
+      <c r="O81" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>550</v>
+      </c>
+      <c r="C82" t="s">
+        <v>480</v>
+      </c>
+      <c r="D82" t="s">
+        <v>551</v>
+      </c>
+      <c r="E82" t="s">
+        <v>434</v>
+      </c>
+      <c r="F82" t="s">
+        <v>317</v>
+      </c>
+      <c r="G82" t="s">
+        <v>551</v>
+      </c>
+      <c r="H82" t="s">
+        <v>551</v>
+      </c>
+      <c r="I82" t="s">
+        <v>552</v>
+      </c>
+      <c r="J82" t="s">
+        <v>553</v>
+      </c>
+      <c r="K82" t="s">
+        <v>291</v>
+      </c>
+      <c r="L82">
+        <v>1</v>
+      </c>
+      <c r="N82" t="s">
+        <v>429</v>
+      </c>
+      <c r="O82" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>554</v>
+      </c>
+      <c r="B83" t="s">
+        <v>210</v>
+      </c>
+      <c r="C83" t="s">
+        <v>480</v>
+      </c>
+      <c r="D83" t="s">
+        <v>555</v>
+      </c>
+      <c r="E83" t="s">
+        <v>434</v>
+      </c>
+      <c r="F83" t="s">
+        <v>317</v>
+      </c>
+      <c r="G83" t="s">
+        <v>556</v>
+      </c>
+      <c r="H83" t="s">
+        <v>555</v>
+      </c>
+      <c r="I83" t="s">
+        <v>557</v>
+      </c>
+      <c r="J83" t="s">
+        <v>558</v>
+      </c>
+      <c r="K83" t="s">
+        <v>286</v>
+      </c>
+      <c r="L83">
+        <v>100</v>
+      </c>
+      <c r="N83" t="s">
+        <v>331</v>
+      </c>
+      <c r="O83" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>554</v>
+      </c>
+      <c r="B84" t="s">
+        <v>214</v>
+      </c>
+      <c r="C84" t="s">
+        <v>480</v>
+      </c>
+      <c r="D84" t="s">
+        <v>555</v>
+      </c>
+      <c r="E84" t="s">
+        <v>434</v>
+      </c>
+      <c r="F84" t="s">
+        <v>317</v>
+      </c>
+      <c r="G84" t="s">
+        <v>556</v>
+      </c>
+      <c r="H84" t="s">
+        <v>555</v>
+      </c>
+      <c r="I84" t="s">
+        <v>559</v>
+      </c>
+      <c r="J84" t="s">
+        <v>558</v>
+      </c>
+      <c r="K84" t="s">
+        <v>286</v>
+      </c>
+      <c r="L84">
+        <v>100</v>
+      </c>
+      <c r="N84" t="s">
+        <v>331</v>
+      </c>
+      <c r="O84" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>560</v>
+      </c>
+      <c r="C85" t="s">
+        <v>480</v>
+      </c>
+      <c r="D85" t="s">
+        <v>561</v>
+      </c>
+      <c r="E85" t="s">
+        <v>434</v>
+      </c>
+      <c r="F85" t="s">
+        <v>317</v>
+      </c>
+      <c r="G85" t="s">
+        <v>561</v>
+      </c>
+      <c r="H85" t="s">
+        <v>561</v>
+      </c>
+      <c r="I85" t="s">
+        <v>562</v>
+      </c>
+      <c r="J85" t="s">
+        <v>563</v>
+      </c>
+      <c r="K85" t="s">
+        <v>291</v>
+      </c>
+      <c r="L85">
+        <v>1</v>
+      </c>
+      <c r="N85" t="s">
+        <v>429</v>
+      </c>
+      <c r="O85" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>564</v>
+      </c>
+      <c r="C86" t="s">
+        <v>480</v>
+      </c>
+      <c r="D86" t="s">
+        <v>565</v>
+      </c>
+      <c r="E86" t="s">
+        <v>434</v>
+      </c>
+      <c r="F86" t="s">
+        <v>317</v>
+      </c>
+      <c r="G86" t="s">
+        <v>565</v>
+      </c>
+      <c r="H86" t="s">
+        <v>565</v>
+      </c>
+      <c r="I86" t="s">
+        <v>566</v>
+      </c>
+      <c r="J86" t="s">
+        <v>567</v>
+      </c>
+      <c r="K86" t="s">
+        <v>291</v>
+      </c>
+      <c r="L86">
+        <v>1</v>
+      </c>
+      <c r="N86" t="s">
+        <v>429</v>
+      </c>
+      <c r="O86" t="s">
+        <v>327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the ind_study_matrix.xlsx file with other study regions
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECE9624-E8EC-42CF-9B6C-AB0E732167BF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27AE7ED-9AED-41DB-A6F2-ACC9CDC3C023}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="3" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="study_regions" sheetId="3" r:id="rId1"/>
@@ -30,8 +30,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>SimonTest</author>
+  </authors>
+  <commentList>
+    <comment ref="H7" authorId="0" shapeId="0" xr:uid="{BCB0A9BB-665B-4163-8EB8-B409FEA025B1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>SimonTest:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Should this be melb? It says Syd.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="599">
   <si>
     <t>Domain</t>
   </si>
@@ -1785,12 +1819,105 @@
   <si>
     <t>LEFT JOIN ind_river ON p.gnaf_pid = ind_river.gnaf_pid</t>
   </si>
+  <si>
+    <t>Albury – Wodonga</t>
+  </si>
+  <si>
+    <t>Ballarat</t>
+  </si>
+  <si>
+    <t>Bendigo</t>
+  </si>
+  <si>
+    <t>Cairns</t>
+  </si>
+  <si>
+    <t>Geelong</t>
+  </si>
+  <si>
+    <t>Gold Coast – Tweed Heads</t>
+  </si>
+  <si>
+    <t>Launceston</t>
+  </si>
+  <si>
+    <t>Mackay</t>
+  </si>
+  <si>
+    <t>Newcastle – Maitland</t>
+  </si>
+  <si>
+    <t>Sunshine Coast</t>
+  </si>
+  <si>
+    <t>Toowoomba</t>
+  </si>
+  <si>
+    <t>Townsville</t>
+  </si>
+  <si>
+    <t>Wollongong</t>
+  </si>
+  <si>
+    <t>Vic &amp; NSW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"STATE_NAME" = 'Victoria' AND "STATE_NAME" = 'New South Wales'  AND "LGA_NAME_2"  = 'Albury (C)' AND "LGA_NAME_2"  = 'Wodonga (C)' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"STATE_NAME" = 'Victoria' AND "LGA_NAME_2"  = 'Ballarat (C)' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"STATE_NAME" = 'Victoria' AND "LGA_NAME_2"  = Greater Bendigo (C)' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"STATE_NAME" = 'Victoria' AND "LGA_NAME_2"  = 'Greater Geelong (C)' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"STATE_NAME" = 'Queensland' AND "LGA_NAME_2"  = Cairns (R)' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"STATE_NAME" = 'Queensland' AND "LGA_NAME_2"  = Gold Coast (C)' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"STATE_NAME" = 'Tasmania' AND "LGA_NAME_2"  = Launceston (C)' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"STATE_NAME" = 'Queensland' AND "LGA_NAME_2"  = Mackay (R)' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"STATE_NAME" = 'New South Wales' AND "LGA_NAME_2"  = Newcastle (C)' AND "LGA_NAME_2"  = Maitland (C)' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"STATE_NAME" = 'Queensland' AND "LGA_NAME_2"  = Sunshine Coast (R)' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"STATE_NAME" = 'Queensland' AND "LGA_NAME_2"  = Toowoomba (R)' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"STATE_NAME" = 'Queensland' AND "LGA_NAME_2"  = Townsville (C)' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"STATE_NAME" = 'New South Wales' AND "LGA_NAME_2"  = Wollongong (C)' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">address_points/GDA2020_GA_LCC.gdb/gnaf_2018_nsw AND address_points/GDA2020_GA_LCC.gdb/gnaf_2018_vic </t>
+  </si>
+  <si>
+    <t>['',400]</t>
+  </si>
+  <si>
+    <t>Western Sydney</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"STATE_NAME" = 'New South Wales' AND "LGA_NAME_2"  = Blue Mountains (C)' AND "LGA_NAME_2"  = Camden (A)' AND "LGA_NAME_2"  = Campbelltown (C) (NSW)'  AND "LGA_NAME_2"  = Fairfield (C)' AND "LGA_NAME_2"  = Hawkesbury (C)' AND "LGA_NAME_2"  = Liverpool (C)' AND "LGA_NAME_2"  = Penrith (C)' AND "LGA_NAME_2"  = Wollondilly (A)' </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1879,8 +2006,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1896,6 +2036,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2135,7 +2281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2274,6 +2420,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2875,23 +3027,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317EB008-F691-4F16-B99A-D5845A82BBBD}">
-  <dimension ref="A1:H10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317EB008-F691-4F16-B99A-D5845A82BBBD}">
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" style="40" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="41" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="41" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="41" customWidth="1"/>
     <col min="4" max="4" width="91.140625" style="41" customWidth="1"/>
-    <col min="5" max="5" width="75" style="42" customWidth="1"/>
+    <col min="5" max="5" width="86.140625" style="42" customWidth="1"/>
     <col min="6" max="6" width="51.42578125" style="41" customWidth="1"/>
     <col min="7" max="7" width="40.85546875" style="41" customWidth="1"/>
     <col min="8" max="8" width="67.28515625" style="41" customWidth="1"/>
@@ -3013,7 +3165,7 @@
       <c r="G5" s="37"/>
       <c r="H5" s="37"/>
     </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
         <v>461</v>
       </c>
@@ -3111,7 +3263,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
         <v>480</v>
       </c>
@@ -3133,10 +3285,334 @@
       <c r="G10" s="37"/>
       <c r="H10" s="37"/>
     </row>
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="36" t="s">
+        <v>568</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>568</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>581</v>
+      </c>
+      <c r="D11" s="55" t="s">
+        <v>582</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>482</v>
+      </c>
+      <c r="F11" s="56" t="s">
+        <v>595</v>
+      </c>
+      <c r="G11" s="39" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="36" t="s">
+        <v>569</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>569</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>466</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>583</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>482</v>
+      </c>
+      <c r="F12" s="37" t="s">
+        <v>468</v>
+      </c>
+      <c r="G12" s="39" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="36" t="s">
+        <v>570</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>570</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>466</v>
+      </c>
+      <c r="D13" s="54" t="s">
+        <v>584</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>482</v>
+      </c>
+      <c r="F13" s="37" t="s">
+        <v>468</v>
+      </c>
+      <c r="G13" s="39" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="36" t="s">
+        <v>571</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>571</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>449</v>
+      </c>
+      <c r="D14" s="54" t="s">
+        <v>586</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>482</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>451</v>
+      </c>
+      <c r="G14" s="39" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="36" t="s">
+        <v>572</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>572</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>466</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>585</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>482</v>
+      </c>
+      <c r="F15" s="37" t="s">
+        <v>468</v>
+      </c>
+      <c r="G15" s="39" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="36" t="s">
+        <v>573</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>573</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>449</v>
+      </c>
+      <c r="D16" s="54" t="s">
+        <v>587</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>482</v>
+      </c>
+      <c r="F16" s="37" t="s">
+        <v>451</v>
+      </c>
+      <c r="G16" s="39" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="36" t="s">
+        <v>574</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>574</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>462</v>
+      </c>
+      <c r="D17" s="54" t="s">
+        <v>588</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>482</v>
+      </c>
+      <c r="F17" s="37" t="s">
+        <v>464</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="36" t="s">
+        <v>575</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>575</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>449</v>
+      </c>
+      <c r="D18" s="54" t="s">
+        <v>589</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>482</v>
+      </c>
+      <c r="F18" s="37" t="s">
+        <v>451</v>
+      </c>
+      <c r="G18" s="39" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="36" t="s">
+        <v>576</v>
+      </c>
+      <c r="B19" s="37" t="s">
+        <v>576</v>
+      </c>
+      <c r="D19" s="54" t="s">
+        <v>590</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>482</v>
+      </c>
+      <c r="F19" s="37" t="s">
+        <v>478</v>
+      </c>
+      <c r="G19" s="39" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="36" t="s">
+        <v>577</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>577</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>449</v>
+      </c>
+      <c r="D20" s="54" t="s">
+        <v>591</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>482</v>
+      </c>
+      <c r="F20" s="37" t="s">
+        <v>451</v>
+      </c>
+      <c r="G20" s="39" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="36" t="s">
+        <v>578</v>
+      </c>
+      <c r="B21" s="37" t="s">
+        <v>578</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>449</v>
+      </c>
+      <c r="D21" s="54" t="s">
+        <v>592</v>
+      </c>
+      <c r="E21" s="39" t="s">
+        <v>482</v>
+      </c>
+      <c r="F21" s="37" t="s">
+        <v>451</v>
+      </c>
+      <c r="G21" s="39" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="36" t="s">
+        <v>579</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>579</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>449</v>
+      </c>
+      <c r="D22" s="54" t="s">
+        <v>593</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>482</v>
+      </c>
+      <c r="F22" s="37" t="s">
+        <v>451</v>
+      </c>
+      <c r="G22" s="39" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="36" t="s">
+        <v>580</v>
+      </c>
+      <c r="B23" s="37" t="s">
+        <v>580</v>
+      </c>
+      <c r="C23" s="37" t="s">
+        <v>476</v>
+      </c>
+      <c r="D23" s="54" t="s">
+        <v>594</v>
+      </c>
+      <c r="E23" s="39" t="s">
+        <v>482</v>
+      </c>
+      <c r="F23" s="37" t="s">
+        <v>478</v>
+      </c>
+      <c r="G23" s="39" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="36" t="s">
+        <v>597</v>
+      </c>
+      <c r="B24" s="37" t="s">
+        <v>597</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>476</v>
+      </c>
+      <c r="D24" s="57" t="s">
+        <v>598</v>
+      </c>
+      <c r="E24" s="39" t="s">
+        <v>482</v>
+      </c>
+      <c r="F24" s="39" t="s">
+        <v>482</v>
+      </c>
+      <c r="G24" s="39" t="s">
+        <v>479</v>
+      </c>
+      <c r="H24" s="37" t="s">
+        <v>470</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3241,7 +3717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA10FF44-D24D-4AD6-829C-327E640FAE4C}">
   <dimension ref="A1:AD48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B28" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -5492,7 +5968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E520E13B-C7CF-4991-8581-C25916074E3A}">
   <dimension ref="A1:O86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated config file process
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B116793-4B51-4410-9DBF-1D2567E525F9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616FE48D-DA69-4426-91B6-20F39989A70E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" firstSheet="2" activeTab="2" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" firstSheet="2" activeTab="3" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1976" uniqueCount="884">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1984" uniqueCount="887">
   <si>
     <t>Domain</t>
   </si>
@@ -1374,19 +1374,7 @@
     <t>state</t>
   </si>
   <si>
-    <t>region_where_clause_list</t>
-  </si>
-  <si>
-    <t>region_shape_list</t>
-  </si>
-  <si>
-    <t>points_list</t>
-  </si>
-  <si>
     <t>pos_queries</t>
-  </si>
-  <si>
-    <t>pos_inclusion_list</t>
   </si>
   <si>
     <t>Adelaide</t>
@@ -2425,9 +2413,6 @@
     <t>db_user</t>
   </si>
   <si>
-    <t xml:space="preserve">db_pwd </t>
-  </si>
-  <si>
     <t>localhost</t>
   </si>
   <si>
@@ -2621,12 +2606,6 @@
   </si>
   <si>
     <t>gnaf_pid</t>
-  </si>
-  <si>
-    <t>parcel_dwellings</t>
-  </si>
-  <si>
-    <t>units of analysis (but using a historic naming convention)</t>
   </si>
   <si>
     <t>sampling points unique id</t>
@@ -2773,6 +2752,36 @@
   </si>
   <si>
     <t>Does the destination geodatabase contain destinations grouped by dataset? If so, change this to TRUE</t>
+  </si>
+  <si>
+    <t>combined_dest_template</t>
+  </si>
+  <si>
+    <t>A feature we created to use as a template for a combined feature</t>
+  </si>
+  <si>
+    <t>destinations/combined_dest_template/combined_dest_template.shp</t>
+  </si>
+  <si>
+    <t>db_pwd</t>
+  </si>
+  <si>
+    <t>line_buffer</t>
+  </si>
+  <si>
+    <t>sausage buffer network size  -- in units specified above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transformations for network </t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>pos_inclusion</t>
+  </si>
+  <si>
+    <t>testtt</t>
   </si>
 </sst>
 </file>
@@ -3838,12 +3847,12 @@
   <sheetData>
     <row r="1" spans="1:1" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
     </row>
     <row r="2" spans="1:1" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
     </row>
     <row r="3" spans="1:1" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -3851,27 +3860,27 @@
     </row>
     <row r="4" spans="1:1" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
     </row>
     <row r="5" spans="1:1" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
     </row>
     <row r="8" spans="1:1" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
     </row>
   </sheetData>
@@ -3884,8 +3893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{169A8F36-66C8-40F7-A0A8-79F453EFA097}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3898,38 +3907,38 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="C3" s="72" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="D3" s="61" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="53" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="91"/>
       <c r="D4" s="93" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="97"/>
       <c r="B5" s="98"/>
       <c r="C5" s="57" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="D5" s="92"/>
     </row>
@@ -3937,18 +3946,18 @@
       <c r="A6" s="95"/>
       <c r="B6" s="96"/>
       <c r="C6" s="99" t="s">
-        <v>774</v>
+        <v>769</v>
       </c>
       <c r="D6" s="94"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="64" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="B7" s="54"/>
       <c r="C7" s="63"/>
       <c r="D7" s="68" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3957,7 +3966,7 @@
         <v>432</v>
       </c>
       <c r="C8" s="63" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3966,7 +3975,7 @@
         <v>211</v>
       </c>
       <c r="C9" s="63" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3975,70 +3984,70 @@
         <v>433</v>
       </c>
       <c r="C10" s="63" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="35"/>
       <c r="B11" s="55" t="s">
-        <v>435</v>
+        <v>782</v>
       </c>
       <c r="C11" s="63" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="35"/>
       <c r="B12" s="54" t="s">
-        <v>434</v>
+        <v>784</v>
       </c>
       <c r="C12" s="63" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="35"/>
       <c r="B13" s="54" t="s">
-        <v>436</v>
+        <v>783</v>
       </c>
       <c r="C13" s="63" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="35"/>
       <c r="B14" s="54" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C14" s="63" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
       <c r="B15" s="65" t="s">
-        <v>438</v>
+        <v>885</v>
       </c>
       <c r="C15" s="63" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="35"/>
       <c r="B16" s="65" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="C16" s="63" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="35"/>
       <c r="B17" s="65" t="s">
-        <v>862</v>
+        <v>855</v>
       </c>
       <c r="C17" s="63" t="s">
-        <v>863</v>
+        <v>856</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4050,73 +4059,73 @@
       <c r="A19" s="52"/>
       <c r="B19" s="52"/>
       <c r="C19" s="73" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="D19" s="66"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="64" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="B20" s="35"/>
       <c r="C20" s="63"/>
       <c r="D20" s="65" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="65" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="C21" s="63" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="35"/>
       <c r="B22" s="65" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="C22" s="63" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="35"/>
       <c r="B23" s="65" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="C23" s="63" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="35"/>
       <c r="B24" s="65" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="C24" s="63" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="52"/>
       <c r="B25" s="66" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="C25" s="73" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="D25" s="66"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="67" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="B26" s="65"/>
       <c r="C26" s="63"/>
       <c r="D26" s="65" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -4183,10 +4192,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="67" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="D37" s="68" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -4194,7 +4203,7 @@
         <v>209</v>
       </c>
       <c r="C38" s="69" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -4202,7 +4211,7 @@
         <v>208</v>
       </c>
       <c r="C39" s="69" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -4210,7 +4219,7 @@
         <v>211</v>
       </c>
       <c r="C40" s="69" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4218,7 +4227,7 @@
         <v>303</v>
       </c>
       <c r="C41" s="69" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -4226,7 +4235,7 @@
         <v>429</v>
       </c>
       <c r="C42" s="69" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -4234,7 +4243,7 @@
         <v>305</v>
       </c>
       <c r="C43" s="69" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -4242,7 +4251,7 @@
         <v>328</v>
       </c>
       <c r="C44" s="69" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -4250,7 +4259,7 @@
         <v>161</v>
       </c>
       <c r="C45" s="69" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -4258,7 +4267,7 @@
         <v>212</v>
       </c>
       <c r="C46" s="69" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -4266,7 +4275,7 @@
         <v>213</v>
       </c>
       <c r="C47" s="69" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -4274,7 +4283,7 @@
         <v>278</v>
       </c>
       <c r="C48" s="69" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
     </row>
     <row r="49" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -4282,7 +4291,7 @@
         <v>277</v>
       </c>
       <c r="C49" s="69" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
     </row>
     <row r="50" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -4290,7 +4299,7 @@
         <v>283</v>
       </c>
       <c r="C50" s="69" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
@@ -4298,7 +4307,7 @@
         <v>326</v>
       </c>
       <c r="C51" s="69" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
     </row>
     <row r="52" spans="2:3" ht="45" x14ac:dyDescent="0.25">
@@ -4306,7 +4315,7 @@
         <v>321</v>
       </c>
       <c r="C52" s="69" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
     </row>
   </sheetData>
@@ -4316,11 +4325,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3E5F03-EC28-486B-BA51-9D83D1ACCD02}">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A56" sqref="A56"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4333,72 +4342,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="100" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="B1" s="101" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="C1" s="102" t="s">
-        <v>826</v>
+        <v>821</v>
       </c>
       <c r="D1" s="102" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="B2" s="74" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>832</v>
+        <v>827</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="B3" s="74">
         <v>2016</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>832</v>
+        <v>827</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="B4" s="74" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>832</v>
+        <v>827</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="B5" s="74">
         <v>7845</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>832</v>
+        <v>827</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4406,483 +4415,483 @@
         <v>326</v>
       </c>
       <c r="B6" s="74" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>832</v>
+        <v>827</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="B7" s="74" t="s">
+        <v>729</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>827</v>
+      </c>
+      <c r="D7" s="38" t="s">
         <v>733</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>832</v>
-      </c>
-      <c r="D7" s="38" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="B8" s="74">
         <v>10000</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>832</v>
+        <v>827</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="B9" s="74">
         <v>3000</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>832</v>
+        <v>827</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="B10" s="74">
         <v>3000</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>832</v>
+        <v>827</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>741</v>
+      </c>
+      <c r="B11" s="74" t="s">
+        <v>742</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>827</v>
+      </c>
+      <c r="D11" s="38" t="s">
         <v>745</v>
-      </c>
-      <c r="B11" s="74" t="s">
-        <v>746</v>
-      </c>
-      <c r="C11" s="38" t="s">
-        <v>832</v>
-      </c>
-      <c r="D11" s="38" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="B12" s="74" t="s">
-        <v>769</v>
+        <v>764</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>827</v>
+        <v>822</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="B13" s="74">
         <v>5432</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>827</v>
+        <v>822</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>763</v>
+      </c>
+      <c r="B14" s="74" t="s">
+        <v>765</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>822</v>
+      </c>
+      <c r="D14" s="38" t="s">
         <v>767</v>
-      </c>
-      <c r="B14" s="74" t="s">
-        <v>770</v>
-      </c>
-      <c r="C14" s="38" t="s">
-        <v>827</v>
-      </c>
-      <c r="D14" s="38" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>768</v>
+        <v>880</v>
       </c>
       <c r="B15" s="74" t="s">
-        <v>771</v>
+        <v>766</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>827</v>
+        <v>822</v>
       </c>
       <c r="D15" s="38" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>775</v>
+        <v>770</v>
       </c>
       <c r="B16" s="74" t="s">
-        <v>776</v>
+        <v>771</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>827</v>
+        <v>822</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="B17" s="74" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>828</v>
+        <v>823</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="B18" s="74" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>828</v>
+        <v>823</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="B19" s="74" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>829</v>
+        <v>824</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>753</v>
+      </c>
+      <c r="B20" s="74" t="s">
+        <v>755</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="D20" s="38" t="s">
         <v>757</v>
-      </c>
-      <c r="B20" s="74" t="s">
-        <v>759</v>
-      </c>
-      <c r="C20" s="38" t="s">
-        <v>829</v>
-      </c>
-      <c r="D20" s="38" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="B21" s="74" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>829</v>
+        <v>824</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="B22" s="74" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>829</v>
+        <v>824</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>777</v>
+        <v>772</v>
       </c>
       <c r="B23" s="74" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>804</v>
+        <v>799</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
       <c r="B24" s="74" t="s">
-        <v>780</v>
+        <v>775</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>781</v>
+        <v>776</v>
       </c>
       <c r="B25" s="74" t="s">
-        <v>782</v>
+        <v>777</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>802</v>
+        <v>797</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>785</v>
+      </c>
+      <c r="B26" s="74" t="s">
         <v>790</v>
       </c>
-      <c r="B26" s="74" t="s">
-        <v>795</v>
-      </c>
       <c r="C26" s="38" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>803</v>
+        <v>798</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>786</v>
+      </c>
+      <c r="B27" s="74" t="s">
         <v>791</v>
       </c>
-      <c r="B27" s="74" t="s">
-        <v>796</v>
-      </c>
       <c r="C27" s="38" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>799</v>
+        <v>794</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>787</v>
+      </c>
+      <c r="B28" s="74" t="s">
         <v>792</v>
       </c>
-      <c r="B28" s="74" t="s">
-        <v>797</v>
-      </c>
       <c r="C28" s="38" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>800</v>
+        <v>795</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>788</v>
+      </c>
+      <c r="B29" s="74" t="s">
         <v>793</v>
       </c>
-      <c r="B29" s="74" t="s">
-        <v>798</v>
-      </c>
       <c r="C29" s="38" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="D29" s="38" t="s">
-        <v>801</v>
+        <v>796</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
       <c r="B30" s="74" t="s">
-        <v>805</v>
+        <v>800</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>817</v>
+        <v>812</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>809</v>
+        <v>804</v>
       </c>
       <c r="B31" s="74" t="s">
-        <v>806</v>
+        <v>801</v>
       </c>
       <c r="C31" s="38" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>818</v>
+        <v>813</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>810</v>
+        <v>805</v>
       </c>
       <c r="B32" s="74" t="s">
-        <v>807</v>
+        <v>802</v>
       </c>
       <c r="C32" s="38" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>819</v>
+        <v>814</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>811</v>
+        <v>806</v>
       </c>
       <c r="B33" s="74" t="s">
-        <v>808</v>
+        <v>803</v>
       </c>
       <c r="C33" s="38" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>820</v>
+        <v>815</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>812</v>
+        <v>807</v>
       </c>
       <c r="B34" s="74" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="C34" s="38" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>821</v>
+        <v>816</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>813</v>
+        <v>808</v>
       </c>
       <c r="B35" s="74" t="s">
-        <v>815</v>
+        <v>810</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>822</v>
+        <v>817</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>814</v>
+        <v>809</v>
       </c>
       <c r="B36" s="74" t="s">
-        <v>816</v>
+        <v>811</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>824</v>
+        <v>819</v>
       </c>
       <c r="B37" s="74" t="s">
-        <v>833</v>
+        <v>828</v>
       </c>
       <c r="C37" s="38" t="s">
-        <v>831</v>
+        <v>826</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>836</v>
+        <v>829</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>825</v>
+        <v>820</v>
       </c>
       <c r="B38" s="74">
         <v>7844</v>
       </c>
       <c r="C38" s="38" t="s">
-        <v>831</v>
+        <v>826</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>837</v>
+        <v>830</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="B39" s="74" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="C39" s="38" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="D39" s="38" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="B40" s="74" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="C40" s="38" t="s">
-        <v>839</v>
+        <v>832</v>
       </c>
       <c r="D40" s="38" t="s">
         <v>840</v>
@@ -4890,206 +4899,226 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>841</v>
+        <v>835</v>
       </c>
       <c r="B41" s="74" t="s">
-        <v>844</v>
+        <v>838</v>
       </c>
       <c r="C41" s="38" t="s">
-        <v>839</v>
+        <v>832</v>
       </c>
       <c r="D41" s="38" t="s">
-        <v>847</v>
+        <v>767</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>842</v>
+        <v>836</v>
       </c>
       <c r="B42" s="74" t="s">
-        <v>845</v>
+        <v>839</v>
       </c>
       <c r="C42" s="38" t="s">
-        <v>839</v>
+        <v>832</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>841</v>
+      </c>
+      <c r="B43" s="74" t="s">
+        <v>842</v>
+      </c>
+      <c r="C43" s="38" t="s">
+        <v>832</v>
+      </c>
+      <c r="D43" s="38" t="s">
         <v>843</v>
-      </c>
-      <c r="B43" s="74" t="s">
-        <v>846</v>
-      </c>
-      <c r="C43" s="38" t="s">
-        <v>839</v>
-      </c>
-      <c r="D43" s="38" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="B44" s="74" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="C44" s="38" t="s">
-        <v>839</v>
+        <v>824</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>850</v>
+        <v>883</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>851</v>
+        <v>845</v>
       </c>
       <c r="B45" s="74" t="s">
-        <v>853</v>
+        <v>847</v>
       </c>
       <c r="C45" s="38" t="s">
-        <v>829</v>
+        <v>824</v>
+      </c>
+      <c r="D45" s="38" t="s">
+        <v>883</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>852</v>
-      </c>
-      <c r="B46" s="74" t="s">
-        <v>854</v>
+        <v>287</v>
+      </c>
+      <c r="B46" s="74">
+        <v>1600</v>
       </c>
       <c r="C46" s="38" t="s">
-        <v>829</v>
+        <v>849</v>
+      </c>
+      <c r="D46" s="38" t="s">
+        <v>882</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>287</v>
+        <v>848</v>
       </c>
       <c r="B47" s="74">
         <v>500</v>
       </c>
       <c r="C47" s="38" t="s">
-        <v>856</v>
+        <v>849</v>
       </c>
       <c r="D47" s="38" t="s">
-        <v>860</v>
+        <v>853</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>855</v>
+        <v>881</v>
       </c>
       <c r="B48" s="74">
         <v>50</v>
       </c>
       <c r="C48" s="38" t="s">
-        <v>856</v>
+        <v>849</v>
       </c>
       <c r="D48" s="38" t="s">
-        <v>859</v>
+        <v>852</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>857</v>
+        <v>850</v>
       </c>
       <c r="B49" s="74">
         <v>3000</v>
       </c>
       <c r="C49" s="38" t="s">
-        <v>856</v>
+        <v>849</v>
       </c>
       <c r="D49" s="38" t="s">
-        <v>858</v>
+        <v>851</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>861</v>
+        <v>854</v>
       </c>
       <c r="B50" s="74">
         <v>5</v>
       </c>
       <c r="C50" s="38" t="s">
-        <v>864</v>
+        <v>857</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>865</v>
+        <v>858</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>871</v>
+        <v>864</v>
       </c>
       <c r="B51" s="74">
         <v>50</v>
       </c>
       <c r="C51" s="38" t="s">
-        <v>873</v>
+        <v>866</v>
       </c>
       <c r="D51" s="38" t="s">
-        <v>872</v>
+        <v>865</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>874</v>
+        <v>867</v>
       </c>
       <c r="B52" s="74" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="C52" s="38" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="D52" s="38" t="s">
-        <v>875</v>
+        <v>868</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>876</v>
+        <v>869</v>
       </c>
       <c r="B53" s="74" t="s">
-        <v>877</v>
+        <v>870</v>
       </c>
       <c r="C53" s="38" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="D53" s="38" t="s">
-        <v>878</v>
+        <v>871</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>879</v>
+        <v>872</v>
       </c>
       <c r="B54" s="74" t="s">
-        <v>881</v>
+        <v>874</v>
       </c>
       <c r="C54" s="38" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="D54" s="38" t="s">
-        <v>882</v>
+        <v>875</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>880</v>
+        <v>873</v>
       </c>
       <c r="B55" s="74" t="b">
         <v>0</v>
       </c>
       <c r="C55" s="38" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="D55" s="38" t="s">
-        <v>883</v>
+        <v>876</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>877</v>
+      </c>
+      <c r="B56" s="74" t="s">
+        <v>879</v>
+      </c>
+      <c r="C56" s="38" t="s">
+        <v>683</v>
+      </c>
+      <c r="D56" s="38" t="s">
+        <v>878</v>
       </c>
     </row>
   </sheetData>
@@ -5101,11 +5130,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317EB008-F691-4F16-B99A-D5845A82BBBD}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5133,58 +5162,64 @@
         <v>433</v>
       </c>
       <c r="D1" s="76" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="E1" s="77" t="s">
-        <v>789</v>
+        <v>784</v>
       </c>
       <c r="F1" s="77" t="s">
-        <v>787</v>
+        <v>782</v>
       </c>
       <c r="G1" s="76" t="s">
-        <v>788</v>
+        <v>783</v>
       </c>
       <c r="H1" s="76" t="s">
-        <v>866</v>
+        <v>859</v>
       </c>
       <c r="I1" s="76" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="J1" s="76" t="s">
+        <v>885</v>
+      </c>
+      <c r="K1" s="78" t="s">
+        <v>717</v>
+      </c>
+      <c r="L1" s="78" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="79" t="s">
+        <v>778</v>
+      </c>
+      <c r="B2" s="80" t="s">
+        <v>778</v>
+      </c>
+      <c r="C2" s="80" t="s">
+        <v>779</v>
+      </c>
+      <c r="D2" s="80" t="s">
+        <v>780</v>
+      </c>
+      <c r="E2" s="81" t="s">
+        <v>781</v>
+      </c>
+      <c r="F2" s="81" t="s">
         <v>438</v>
       </c>
-      <c r="K1" s="78" t="s">
-        <v>721</v>
-      </c>
-      <c r="L1" s="78" t="s">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="79" t="s">
-        <v>783</v>
-      </c>
-      <c r="B2" s="80" t="s">
-        <v>783</v>
-      </c>
-      <c r="C2" s="80" t="s">
-        <v>784</v>
-      </c>
-      <c r="D2" s="80" t="s">
-        <v>785</v>
-      </c>
-      <c r="E2" s="81" t="s">
-        <v>786</v>
-      </c>
-      <c r="F2" s="81" t="s">
-        <v>442</v>
-      </c>
       <c r="G2" s="80" t="s">
-        <v>443</v>
-      </c>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
+        <v>439</v>
+      </c>
+      <c r="H2" s="80" t="s">
+        <v>884</v>
+      </c>
+      <c r="I2" s="81" t="s">
+        <v>444</v>
+      </c>
+      <c r="J2" s="80" t="s">
+        <v>886</v>
+      </c>
       <c r="K2" s="82"/>
       <c r="L2" s="82">
         <v>0</v>
@@ -5192,25 +5227,25 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="79" t="s">
+        <v>435</v>
+      </c>
+      <c r="B3" s="80" t="s">
+        <v>610</v>
+      </c>
+      <c r="C3" s="80" t="s">
+        <v>436</v>
+      </c>
+      <c r="D3" s="80" t="s">
+        <v>606</v>
+      </c>
+      <c r="E3" s="81" t="s">
+        <v>437</v>
+      </c>
+      <c r="F3" s="81" t="s">
+        <v>438</v>
+      </c>
+      <c r="G3" s="80" t="s">
         <v>439</v>
-      </c>
-      <c r="B3" s="80" t="s">
-        <v>614</v>
-      </c>
-      <c r="C3" s="80" t="s">
-        <v>440</v>
-      </c>
-      <c r="D3" s="80" t="s">
-        <v>610</v>
-      </c>
-      <c r="E3" s="81" t="s">
-        <v>441</v>
-      </c>
-      <c r="F3" s="81" t="s">
-        <v>442</v>
-      </c>
-      <c r="G3" s="80" t="s">
-        <v>443</v>
       </c>
       <c r="H3" s="80"/>
       <c r="I3" s="80"/>
@@ -5222,31 +5257,31 @@
     </row>
     <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="83" t="s">
+        <v>440</v>
+      </c>
+      <c r="B4" s="84" t="s">
+        <v>609</v>
+      </c>
+      <c r="C4" s="84" t="s">
+        <v>441</v>
+      </c>
+      <c r="D4" s="84" t="s">
+        <v>606</v>
+      </c>
+      <c r="E4" s="85" t="s">
+        <v>442</v>
+      </c>
+      <c r="F4" s="85" t="s">
+        <v>438</v>
+      </c>
+      <c r="G4" s="84" t="s">
+        <v>443</v>
+      </c>
+      <c r="H4" s="84" t="s">
+        <v>860</v>
+      </c>
+      <c r="I4" s="85" t="s">
         <v>444</v>
-      </c>
-      <c r="B4" s="84" t="s">
-        <v>613</v>
-      </c>
-      <c r="C4" s="84" t="s">
-        <v>445</v>
-      </c>
-      <c r="D4" s="84" t="s">
-        <v>610</v>
-      </c>
-      <c r="E4" s="85" t="s">
-        <v>446</v>
-      </c>
-      <c r="F4" s="85" t="s">
-        <v>442</v>
-      </c>
-      <c r="G4" s="84" t="s">
-        <v>447</v>
-      </c>
-      <c r="H4" s="84" t="s">
-        <v>867</v>
-      </c>
-      <c r="I4" s="85" t="s">
-        <v>448</v>
       </c>
       <c r="J4" s="84"/>
       <c r="L4" s="82">
@@ -5255,25 +5290,25 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="86" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B5" s="87" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="C5" s="87" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="D5" s="87" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="E5" s="88" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="F5" s="88" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="G5" s="87" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="H5" s="87"/>
       <c r="I5" s="87"/>
@@ -5285,25 +5320,25 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="83" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B6" s="84" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="C6" s="84" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="D6" s="84" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="E6" s="85" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="F6" s="85" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="G6" s="84" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H6" s="84"/>
       <c r="I6" s="84"/>
@@ -5314,25 +5349,25 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="86" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="B7" s="87" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="C7" s="87" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D7" s="87" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="E7" s="88" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="F7" s="88" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="G7" s="87" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="H7" s="87"/>
       <c r="I7" s="87"/>
@@ -5344,34 +5379,34 @@
     </row>
     <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="83" t="s">
+        <v>456</v>
+      </c>
+      <c r="B8" s="84" t="s">
+        <v>614</v>
+      </c>
+      <c r="C8" s="84" t="s">
+        <v>457</v>
+      </c>
+      <c r="D8" s="84" t="s">
+        <v>606</v>
+      </c>
+      <c r="E8" s="85" t="s">
+        <v>458</v>
+      </c>
+      <c r="F8" s="85" t="s">
+        <v>438</v>
+      </c>
+      <c r="G8" s="84" t="s">
+        <v>459</v>
+      </c>
+      <c r="H8" s="84" t="s">
+        <v>861</v>
+      </c>
+      <c r="I8" s="85" t="s">
         <v>460</v>
       </c>
-      <c r="B8" s="84" t="s">
-        <v>618</v>
-      </c>
-      <c r="C8" s="84" t="s">
-        <v>461</v>
-      </c>
-      <c r="D8" s="84" t="s">
-        <v>610</v>
-      </c>
-      <c r="E8" s="85" t="s">
-        <v>462</v>
-      </c>
-      <c r="F8" s="85" t="s">
-        <v>442</v>
-      </c>
-      <c r="G8" s="84" t="s">
-        <v>463</v>
-      </c>
-      <c r="H8" s="84" t="s">
-        <v>868</v>
-      </c>
-      <c r="I8" s="85" t="s">
-        <v>464</v>
-      </c>
       <c r="J8" s="84" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="L8" s="82">
         <v>0</v>
@@ -5382,28 +5417,28 @@
         <v>45</v>
       </c>
       <c r="B9" s="87" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="C9" s="87" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="D9" s="87" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="E9" s="87" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="F9" s="88" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="G9" s="87" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="H9" s="87" t="s">
-        <v>870</v>
+        <v>863</v>
       </c>
       <c r="I9" s="88" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="J9" s="87"/>
       <c r="K9" s="56"/>
@@ -5413,34 +5448,34 @@
     </row>
     <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="83" t="s">
+        <v>466</v>
+      </c>
+      <c r="B10" s="84" t="s">
+        <v>616</v>
+      </c>
+      <c r="C10" s="84" t="s">
+        <v>467</v>
+      </c>
+      <c r="D10" s="84" t="s">
+        <v>606</v>
+      </c>
+      <c r="E10" s="85" t="s">
+        <v>468</v>
+      </c>
+      <c r="F10" s="85" t="s">
+        <v>438</v>
+      </c>
+      <c r="G10" s="84" t="s">
+        <v>469</v>
+      </c>
+      <c r="H10" s="84" t="s">
+        <v>862</v>
+      </c>
+      <c r="I10" s="85" t="s">
         <v>470</v>
       </c>
-      <c r="B10" s="84" t="s">
-        <v>620</v>
-      </c>
-      <c r="C10" s="84" t="s">
-        <v>471</v>
-      </c>
-      <c r="D10" s="84" t="s">
-        <v>610</v>
-      </c>
-      <c r="E10" s="85" t="s">
-        <v>472</v>
-      </c>
-      <c r="F10" s="85" t="s">
-        <v>442</v>
-      </c>
-      <c r="G10" s="84" t="s">
-        <v>473</v>
-      </c>
-      <c r="H10" s="84" t="s">
-        <v>869</v>
-      </c>
-      <c r="I10" s="85" t="s">
-        <v>474</v>
-      </c>
       <c r="J10" s="84" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="L10" s="82">
         <v>0</v>
@@ -5448,25 +5483,25 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="86" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B11" s="87" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="C11" s="87" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D11" s="87" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="E11" s="88" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="F11" s="88" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="G11" s="87" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="H11" s="87"/>
       <c r="I11" s="87"/>
@@ -5478,29 +5513,29 @@
     </row>
     <row r="12" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="83" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="B12" s="84" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="C12" s="84" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="D12" s="84" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="E12" s="89" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="F12" s="85" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="G12" s="90" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="H12" s="90"/>
       <c r="I12" s="85" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="J12" s="84"/>
       <c r="L12" s="82">
@@ -5509,29 +5544,29 @@
     </row>
     <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="86" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="B13" s="87" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="C13" s="87" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D13" s="87" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="E13" s="88" t="s">
+        <v>571</v>
+      </c>
+      <c r="F13" s="88" t="s">
         <v>575</v>
       </c>
-      <c r="F13" s="88" t="s">
-        <v>579</v>
-      </c>
       <c r="G13" s="87" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="H13" s="87"/>
       <c r="I13" s="88" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="J13" s="87"/>
       <c r="K13" s="56"/>
@@ -5541,29 +5576,29 @@
     </row>
     <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="83" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="B14" s="84" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="C14" s="84" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D14" s="84" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="E14" s="84" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="F14" s="85" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="G14" s="84" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="H14" s="84"/>
       <c r="I14" s="85" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="J14" s="84"/>
       <c r="L14" s="82">
@@ -5572,29 +5607,29 @@
     </row>
     <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="86" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="B15" s="87" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="C15" s="87" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D15" s="87" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="E15" s="87" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="F15" s="88" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="G15" s="87" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="H15" s="87"/>
       <c r="I15" s="88" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="J15" s="87"/>
       <c r="K15" s="56"/>
@@ -5604,29 +5639,29 @@
     </row>
     <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="83" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="B16" s="84" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="C16" s="84" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D16" s="84" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="E16" s="85" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="F16" s="85" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="G16" s="84" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="H16" s="84"/>
       <c r="I16" s="85" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="J16" s="84"/>
       <c r="L16" s="82">
@@ -5635,29 +5670,29 @@
     </row>
     <row r="17" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="86" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="B17" s="87" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="C17" s="87" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D17" s="87" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="E17" s="87" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="F17" s="88" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="G17" s="87" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="H17" s="87"/>
       <c r="I17" s="88" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="J17" s="87"/>
       <c r="K17" s="56"/>
@@ -5667,29 +5702,29 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="83" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="B18" s="84" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="C18" s="84" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D18" s="84" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="E18" s="84" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="F18" s="85" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="G18" s="84" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="H18" s="84"/>
       <c r="I18" s="84" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="J18" s="84"/>
       <c r="L18" s="82">
@@ -5698,29 +5733,29 @@
     </row>
     <row r="19" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="86" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="B19" s="87" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="C19" s="87" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D19" s="87" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="E19" s="87" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="F19" s="88" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="G19" s="87" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="H19" s="87"/>
       <c r="I19" s="88" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="J19" s="87"/>
       <c r="K19" s="56"/>
@@ -5730,29 +5765,29 @@
     </row>
     <row r="20" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="83" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="B20" s="84" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C20" s="84" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="D20" s="84" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="E20" s="84" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="F20" s="85" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="G20" s="84" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="H20" s="84"/>
       <c r="I20" s="85" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="J20" s="84"/>
       <c r="L20" s="82">
@@ -5761,29 +5796,29 @@
     </row>
     <row r="21" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="86" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="B21" s="87" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="C21" s="87" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D21" s="87" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="E21" s="87" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="F21" s="88" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="G21" s="87" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="H21" s="87"/>
       <c r="I21" s="88" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="J21" s="87"/>
       <c r="K21" s="56"/>
@@ -5793,29 +5828,29 @@
     </row>
     <row r="22" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="83" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="B22" s="84" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="C22" s="84" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D22" s="84" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="E22" s="84" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="F22" s="85" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="G22" s="84" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="H22" s="84"/>
       <c r="I22" s="85" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="J22" s="84"/>
       <c r="L22" s="82">
@@ -5824,29 +5859,29 @@
     </row>
     <row r="23" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="86" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="B23" s="87" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="C23" s="87" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D23" s="87" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="E23" s="87" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="F23" s="88" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="G23" s="87" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="H23" s="87"/>
       <c r="I23" s="88" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="J23" s="87"/>
       <c r="K23" s="56"/>
@@ -5856,29 +5891,29 @@
     </row>
     <row r="24" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="83" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="B24" s="84" t="s">
+        <v>603</v>
+      </c>
+      <c r="C24" s="84" t="s">
+        <v>467</v>
+      </c>
+      <c r="D24" s="84" t="s">
         <v>607</v>
       </c>
-      <c r="C24" s="84" t="s">
-        <v>471</v>
-      </c>
-      <c r="D24" s="84" t="s">
-        <v>611</v>
-      </c>
       <c r="E24" s="84" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="F24" s="85" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="G24" s="84" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="H24" s="84"/>
       <c r="I24" s="85" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="J24" s="84"/>
       <c r="L24" s="82">
@@ -5887,32 +5922,32 @@
     </row>
     <row r="25" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="86" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="B25" s="87" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C25" s="87" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="D25" s="87" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="E25" s="90" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="F25" s="88" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="G25" s="88" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="H25" s="88"/>
       <c r="I25" s="88" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="J25" s="87" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="K25" s="56"/>
       <c r="L25" s="82">
@@ -5942,19 +5977,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
+        <v>621</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>622</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>624</v>
+      </c>
+      <c r="E1" s="44" t="s">
         <v>625</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>626</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>627</v>
-      </c>
-      <c r="D1" s="44" t="s">
-        <v>628</v>
-      </c>
-      <c r="E1" s="44" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -5962,7 +5997,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="C2" t="s">
         <v>154</v>
@@ -5976,7 +6011,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="C3" t="s">
         <v>154</v>
@@ -5990,7 +6025,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="C4" t="s">
         <v>154</v>
@@ -6004,7 +6039,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="C5" t="s">
         <v>154</v>
@@ -6018,7 +6053,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="C6" t="s">
         <v>154</v>
@@ -6032,7 +6067,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="C7" t="s">
         <v>154</v>
@@ -6046,7 +6081,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="C8" t="s">
         <v>154</v>
@@ -6060,7 +6095,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="C9" t="s">
         <v>154</v>
@@ -6074,10 +6109,10 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="C10" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D10">
         <v>1600</v>
@@ -6088,10 +6123,10 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="C11" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D11">
         <v>1600</v>
@@ -6102,10 +6137,10 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="C12" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D12">
         <v>1600</v>
@@ -6116,7 +6151,7 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="C13" t="s">
         <v>147</v>
@@ -6130,7 +6165,7 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="C14" t="s">
         <v>147</v>
@@ -6147,7 +6182,7 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="C15" t="s">
         <v>79</v>
@@ -6161,7 +6196,7 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="C16" t="s">
         <v>79</v>
@@ -6175,7 +6210,7 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C17" t="s">
         <v>79</v>
@@ -6189,7 +6224,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="C18" t="s">
         <v>79</v>
@@ -6203,7 +6238,7 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="C19" t="s">
         <v>79</v>
@@ -6217,7 +6252,7 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="C20" t="s">
         <v>79</v>
@@ -6231,7 +6266,7 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="C21" t="s">
         <v>79</v>
@@ -6245,7 +6280,7 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="C22" t="s">
         <v>79</v>
@@ -6259,7 +6294,7 @@
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="C23" t="s">
         <v>79</v>
@@ -6273,7 +6308,7 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="C24" t="s">
         <v>79</v>
@@ -6287,7 +6322,7 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="C25" t="s">
         <v>79</v>
@@ -6301,7 +6336,7 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="C26" t="s">
         <v>79</v>
@@ -6315,7 +6350,7 @@
         <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="C27" t="s">
         <v>79</v>
@@ -6329,7 +6364,7 @@
         <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="C28" t="s">
         <v>79</v>
@@ -6343,7 +6378,7 @@
         <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="C29" t="s">
         <v>79</v>
@@ -6357,7 +6392,7 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="C30" t="s">
         <v>79</v>
@@ -6371,7 +6406,7 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="C31" t="s">
         <v>79</v>
@@ -6385,7 +6420,7 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="C32" t="s">
         <v>79</v>
@@ -6399,7 +6434,7 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="C33" t="s">
         <v>79</v>
@@ -6413,7 +6448,7 @@
         <v>14</v>
       </c>
       <c r="B34" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="C34" t="s">
         <v>79</v>
@@ -6427,7 +6462,7 @@
         <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="C35" t="s">
         <v>79</v>
@@ -6441,7 +6476,7 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="C36" t="s">
         <v>79</v>
@@ -6455,7 +6490,7 @@
         <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="C37" t="s">
         <v>79</v>
@@ -6469,7 +6504,7 @@
         <v>100</v>
       </c>
       <c r="B38" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="C38" t="s">
         <v>16</v>
@@ -6483,7 +6518,7 @@
         <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="C39" t="s">
         <v>147</v>
@@ -6497,7 +6532,7 @@
         <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="C40" t="s">
         <v>147</v>
@@ -6511,7 +6546,7 @@
         <v>16</v>
       </c>
       <c r="B41" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="C41" t="s">
         <v>147</v>
@@ -6525,7 +6560,7 @@
         <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="C42" t="s">
         <v>147</v>
@@ -6539,7 +6574,7 @@
         <v>18</v>
       </c>
       <c r="B43" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="C43" t="s">
         <v>147</v>
@@ -6553,7 +6588,7 @@
         <v>19</v>
       </c>
       <c r="B44" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="C44" t="s">
         <v>147</v>
@@ -6567,7 +6602,7 @@
         <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="C45" t="s">
         <v>147</v>
@@ -6581,7 +6616,7 @@
         <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="C46" t="s">
         <v>16</v>
@@ -6595,7 +6630,7 @@
         <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="C47" t="s">
         <v>16</v>
@@ -6609,7 +6644,7 @@
         <v>22</v>
       </c>
       <c r="B48" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="C48" t="s">
         <v>16</v>
@@ -6623,10 +6658,10 @@
         <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="C49" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D49">
         <v>1600</v>
@@ -6637,10 +6672,10 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="C50" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D50">
         <v>1600</v>
@@ -6651,10 +6686,10 @@
         <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="C51" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D51">
         <v>1600</v>
@@ -9598,7 +9633,7 @@
         <v>1</v>
       </c>
       <c r="N18" s="26" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="O18" s="22" t="s">
         <v>323</v>
@@ -10239,13 +10274,13 @@
     </row>
     <row r="33" spans="1:15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="C33" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D33" s="49" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="E33" t="s">
         <v>430</v>
@@ -10254,16 +10289,16 @@
         <v>313</v>
       </c>
       <c r="G33" s="49" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="H33" s="49" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="I33" s="49" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="J33" s="49" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="K33" t="s">
         <v>287</v>
@@ -11718,16 +11753,16 @@
     </row>
     <row r="67" spans="1:15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="B67" t="s">
         <v>206</v>
       </c>
       <c r="C67" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D67" s="49" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="E67" t="s">
         <v>430</v>
@@ -11736,16 +11771,16 @@
         <v>313</v>
       </c>
       <c r="G67" s="49" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="H67" s="49" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="I67" s="49" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="J67" s="49" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="K67" t="s">
         <v>282</v>
@@ -11762,16 +11797,16 @@
     </row>
     <row r="68" spans="1:15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="B68" t="s">
         <v>210</v>
       </c>
       <c r="C68" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D68" s="49" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="E68" t="s">
         <v>430</v>
@@ -11780,16 +11815,16 @@
         <v>313</v>
       </c>
       <c r="G68" s="49" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="H68" s="49" t="s">
+        <v>486</v>
+      </c>
+      <c r="I68" s="49" t="s">
         <v>490</v>
       </c>
-      <c r="I68" s="49" t="s">
-        <v>494</v>
-      </c>
       <c r="J68" s="49" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="K68" t="s">
         <v>282</v>
@@ -11806,16 +11841,16 @@
     </row>
     <row r="69" spans="1:15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="B69" t="s">
         <v>206</v>
       </c>
       <c r="C69" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D69" s="49" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="E69" t="s">
         <v>430</v>
@@ -11824,16 +11859,16 @@
         <v>313</v>
       </c>
       <c r="G69" s="49" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="H69" s="49" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="I69" s="49" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="J69" s="49" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="K69" t="s">
         <v>282</v>
@@ -11850,16 +11885,16 @@
     </row>
     <row r="70" spans="1:15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="B70" t="s">
         <v>210</v>
       </c>
       <c r="C70" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D70" s="49" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="E70" t="s">
         <v>430</v>
@@ -11868,16 +11903,16 @@
         <v>313</v>
       </c>
       <c r="G70" s="49" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="H70" s="49" t="s">
+        <v>492</v>
+      </c>
+      <c r="I70" s="49" t="s">
         <v>496</v>
       </c>
-      <c r="I70" s="49" t="s">
-        <v>500</v>
-      </c>
       <c r="J70" s="49" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="K70" t="s">
         <v>282</v>
@@ -11894,13 +11929,13 @@
     </row>
     <row r="71" spans="1:15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="C71" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D71" s="49" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="E71" t="s">
         <v>430</v>
@@ -11909,16 +11944,16 @@
         <v>313</v>
       </c>
       <c r="G71" s="49" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="H71" s="49" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="I71" s="49" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="J71" s="49" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="K71" t="s">
         <v>287</v>
@@ -11935,13 +11970,13 @@
     </row>
     <row r="72" spans="1:15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="C72" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D72" s="49" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="E72" t="s">
         <v>430</v>
@@ -11950,16 +11985,16 @@
         <v>313</v>
       </c>
       <c r="G72" s="49" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="H72" s="49" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="I72" s="49" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="J72" s="49" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="K72" t="s">
         <v>287</v>
@@ -11976,13 +12011,13 @@
     </row>
     <row r="73" spans="1:15" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="C73" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D73" s="49" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="E73" t="s">
         <v>430</v>
@@ -11991,16 +12026,16 @@
         <v>313</v>
       </c>
       <c r="G73" s="49" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="H73" s="49" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="I73" s="49" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="J73" s="49" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="K73" t="s">
         <v>288</v>
@@ -12014,13 +12049,13 @@
     </row>
     <row r="74" spans="1:15" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="C74" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D74" s="49" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="E74" t="s">
         <v>430</v>
@@ -12029,16 +12064,16 @@
         <v>313</v>
       </c>
       <c r="G74" s="49" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="H74" s="49" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="I74" s="49" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="J74" s="49" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="K74" t="s">
         <v>288</v>
@@ -12052,13 +12087,13 @@
     </row>
     <row r="75" spans="1:15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="C75" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D75" s="49" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="E75" t="s">
         <v>430</v>
@@ -12067,16 +12102,16 @@
         <v>313</v>
       </c>
       <c r="G75" s="49" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="H75" s="49" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="I75" s="49" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="J75" s="49" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="K75" t="s">
         <v>284</v>
@@ -12094,7 +12129,7 @@
       </c>
       <c r="B76" s="23"/>
       <c r="C76" s="23" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="D76" s="48" t="s">
         <v>418</v>
@@ -12134,7 +12169,7 @@
       </c>
       <c r="B77" s="23"/>
       <c r="C77" s="23" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="D77" s="48" t="s">
         <v>419</v>
@@ -12170,13 +12205,13 @@
     </row>
     <row r="78" spans="1:15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="C78" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D78" s="49" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="E78" t="s">
         <v>430</v>
@@ -12185,16 +12220,16 @@
         <v>313</v>
       </c>
       <c r="G78" s="49" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="H78" s="49" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="I78" s="49" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="J78" s="49" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="K78" t="s">
         <v>287</v>
@@ -12211,13 +12246,13 @@
     </row>
     <row r="79" spans="1:15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C79" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D79" s="49" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="E79" t="s">
         <v>430</v>
@@ -12226,16 +12261,16 @@
         <v>313</v>
       </c>
       <c r="G79" s="49" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="H79" s="49" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="I79" s="49" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="J79" s="49" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="K79" t="s">
         <v>287</v>
@@ -12252,16 +12287,16 @@
     </row>
     <row r="80" spans="1:15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B80" t="s">
         <v>206</v>
       </c>
       <c r="C80" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D80" s="49" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="E80" t="s">
         <v>430</v>
@@ -12270,16 +12305,16 @@
         <v>313</v>
       </c>
       <c r="G80" s="49" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="H80" s="49" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="I80" s="49" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="J80" s="49" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="K80" t="s">
         <v>282</v>
@@ -12296,16 +12331,16 @@
     </row>
     <row r="81" spans="1:15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B81" t="s">
         <v>210</v>
       </c>
       <c r="C81" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D81" s="49" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="E81" t="s">
         <v>430</v>
@@ -12314,16 +12349,16 @@
         <v>313</v>
       </c>
       <c r="G81" s="49" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="H81" s="49" t="s">
+        <v>535</v>
+      </c>
+      <c r="I81" s="49" t="s">
         <v>539</v>
       </c>
-      <c r="I81" s="49" t="s">
-        <v>543</v>
-      </c>
       <c r="J81" s="49" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="K81" t="s">
         <v>282</v>
@@ -12340,13 +12375,13 @@
     </row>
     <row r="82" spans="1:15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="C82" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D82" s="49" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="E82" t="s">
         <v>430</v>
@@ -12355,16 +12390,16 @@
         <v>313</v>
       </c>
       <c r="G82" s="49" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="H82" s="49" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="I82" s="49" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="J82" s="49" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="K82" t="s">
         <v>287</v>
@@ -12381,16 +12416,16 @@
     </row>
     <row r="83" spans="1:15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="B83" t="s">
         <v>206</v>
       </c>
       <c r="C83" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D83" s="49" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="E83" t="s">
         <v>430</v>
@@ -12399,16 +12434,16 @@
         <v>313</v>
       </c>
       <c r="G83" s="49" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="H83" s="49" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="I83" s="49" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="J83" s="49" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="K83" t="s">
         <v>282</v>
@@ -12425,16 +12460,16 @@
     </row>
     <row r="84" spans="1:15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="B84" t="s">
         <v>210</v>
       </c>
       <c r="C84" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D84" s="49" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="E84" t="s">
         <v>430</v>
@@ -12443,16 +12478,16 @@
         <v>313</v>
       </c>
       <c r="G84" s="49" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="H84" s="49" t="s">
+        <v>545</v>
+      </c>
+      <c r="I84" s="49" t="s">
         <v>549</v>
       </c>
-      <c r="I84" s="49" t="s">
-        <v>553</v>
-      </c>
       <c r="J84" s="49" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="K84" t="s">
         <v>282</v>
@@ -12469,13 +12504,13 @@
     </row>
     <row r="85" spans="1:15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C85" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D85" s="49" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="E85" t="s">
         <v>430</v>
@@ -12484,16 +12519,16 @@
         <v>313</v>
       </c>
       <c r="G85" s="49" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="H85" s="49" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="I85" s="49" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="J85" s="49" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="K85" t="s">
         <v>287</v>
@@ -12510,13 +12545,13 @@
     </row>
     <row r="86" spans="1:15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="C86" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D86" s="49" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="E86" t="s">
         <v>430</v>
@@ -12525,16 +12560,16 @@
         <v>313</v>
       </c>
       <c r="G86" s="49" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="H86" s="49" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="I86" s="49" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="J86" s="49" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="K86" t="s">
         <v>287</v>

</xml_diff>

<commit_message>
updated some locale names and added in some osm variables to ind matrix
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB88DA8C-015F-47BE-9478-6916951761B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450E707C-DD7C-40CA-86C5-470240EE2A56}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="3" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2006" uniqueCount="899">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2008" uniqueCount="901">
   <si>
     <t>Domain</t>
   </si>
@@ -2797,21 +2797,6 @@
     <t>Directory of the osm2pgsql.exe executable, relative to folderPath; osm2pgsql is used to import open street map data for our study regions to their respective Postgresql postgis databases.</t>
   </si>
   <si>
-    <t>alburyw</t>
-  </si>
-  <si>
-    <t>goldcoast</t>
-  </si>
-  <si>
-    <t>sunshinecoast</t>
-  </si>
-  <si>
-    <t>newcastle</t>
-  </si>
-  <si>
-    <t>westernsyd</t>
-  </si>
-  <si>
     <t>osm</t>
   </si>
   <si>
@@ -2819,6 +2804,27 @@
   </si>
   <si>
     <t>osm_20181001</t>
+  </si>
+  <si>
+    <t>albury_wodonga</t>
+  </si>
+  <si>
+    <t>newcastle_maitland</t>
+  </si>
+  <si>
+    <t>sunshine_coast</t>
+  </si>
+  <si>
+    <t>western_sydney</t>
+  </si>
+  <si>
+    <t>goldcoast_tweedheads</t>
+  </si>
+  <si>
+    <t>D:/ntnl_li_2018_template/data/study_region/bris/bris_gccsa_2016_10000m_20180208.osm</t>
+  </si>
+  <si>
+    <t>osm_20180208</t>
   </si>
 </sst>
 </file>
@@ -5213,10 +5219,10 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5267,10 +5273,10 @@
         <v>874</v>
       </c>
       <c r="K1" s="71" t="s">
-        <v>896</v>
+        <v>891</v>
       </c>
       <c r="L1" s="71" t="s">
-        <v>897</v>
+        <v>892</v>
       </c>
       <c r="M1" s="73" t="s">
         <v>706</v>
@@ -5344,7 +5350,7 @@
       <c r="J3" s="75"/>
       <c r="K3" s="75"/>
       <c r="L3" s="75" t="s">
-        <v>898</v>
+        <v>893</v>
       </c>
       <c r="M3" s="77"/>
       <c r="N3" s="77">
@@ -5380,8 +5386,12 @@
         <v>439</v>
       </c>
       <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="79"/>
+      <c r="K4" s="79" t="s">
+        <v>899</v>
+      </c>
+      <c r="L4" s="79" t="s">
+        <v>900</v>
+      </c>
       <c r="N4" s="77">
         <v>0</v>
       </c>
@@ -5628,7 +5638,7 @@
         <v>552</v>
       </c>
       <c r="B12" s="79" t="s">
-        <v>891</v>
+        <v>894</v>
       </c>
       <c r="C12" s="79" t="s">
         <v>597</v>
@@ -5795,7 +5805,7 @@
         <v>557</v>
       </c>
       <c r="B17" s="82" t="s">
-        <v>892</v>
+        <v>898</v>
       </c>
       <c r="C17" s="82" t="s">
         <v>436</v>
@@ -5896,7 +5906,7 @@
         <v>560</v>
       </c>
       <c r="B20" s="79" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="C20" s="79" t="s">
         <v>462</v>
@@ -5929,7 +5939,7 @@
         <v>561</v>
       </c>
       <c r="B21" s="82" t="s">
-        <v>893</v>
+        <v>896</v>
       </c>
       <c r="C21" s="82" t="s">
         <v>436</v>
@@ -6063,7 +6073,7 @@
         <v>568</v>
       </c>
       <c r="B25" s="82" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
       <c r="C25" s="82" t="s">
         <v>462</v>

</xml_diff>

<commit_message>
tweaked osm source variable name and corrected reference in config file
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450E707C-DD7C-40CA-86C5-470240EE2A56}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26DD91D8-BE1D-4A9C-9493-B6F9E3958293}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="3" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
@@ -2797,9 +2797,6 @@
     <t>Directory of the osm2pgsql.exe executable, relative to folderPath; osm2pgsql is used to import open street map data for our study regions to their respective Postgresql postgis databases.</t>
   </si>
   <si>
-    <t>osm</t>
-  </si>
-  <si>
     <t>osm_prefix</t>
   </si>
   <si>
@@ -2825,6 +2822,9 @@
   </si>
   <si>
     <t>osm_20180208</t>
+  </si>
+  <si>
+    <t>osm_source</t>
   </si>
 </sst>
 </file>
@@ -5222,7 +5222,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5273,10 +5273,10 @@
         <v>874</v>
       </c>
       <c r="K1" s="71" t="s">
+        <v>900</v>
+      </c>
+      <c r="L1" s="71" t="s">
         <v>891</v>
-      </c>
-      <c r="L1" s="71" t="s">
-        <v>892</v>
       </c>
       <c r="M1" s="73" t="s">
         <v>706</v>
@@ -5350,7 +5350,7 @@
       <c r="J3" s="75"/>
       <c r="K3" s="75"/>
       <c r="L3" s="75" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="M3" s="77"/>
       <c r="N3" s="77">
@@ -5387,10 +5387,10 @@
       </c>
       <c r="J4" s="79"/>
       <c r="K4" s="79" t="s">
+        <v>898</v>
+      </c>
+      <c r="L4" s="79" t="s">
         <v>899</v>
-      </c>
-      <c r="L4" s="79" t="s">
-        <v>900</v>
       </c>
       <c r="N4" s="77">
         <v>0</v>
@@ -5638,7 +5638,7 @@
         <v>552</v>
       </c>
       <c r="B12" s="79" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="C12" s="79" t="s">
         <v>597</v>
@@ -5805,7 +5805,7 @@
         <v>557</v>
       </c>
       <c r="B17" s="82" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="C17" s="82" t="s">
         <v>436</v>
@@ -5906,7 +5906,7 @@
         <v>560</v>
       </c>
       <c r="B20" s="79" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="C20" s="79" t="s">
         <v>462</v>
@@ -5939,7 +5939,7 @@
         <v>561</v>
       </c>
       <c r="B21" s="82" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C21" s="82" t="s">
         <v>436</v>
@@ -6073,7 +6073,7 @@
         <v>568</v>
       </c>
       <c r="B25" s="82" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="C25" s="82" t="s">
         <v>462</v>

</xml_diff>

<commit_message>
updates for new approach  --- specifying locale at command line
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{109D9DDD-830A-44F9-B39B-9A3D146DA1E0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06128446-5C14-4565-8E99-CE0EDD9AEF53}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="3" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2032" uniqueCount="901">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2032" uniqueCount="903">
   <si>
     <t>Domain</t>
   </si>
@@ -1786,12 +1786,6 @@
     <t>Wollongong</t>
   </si>
   <si>
-    <t xml:space="preserve">"STATE_NAME" = 'Victoria' AND "LGA_NAME_2"  = 'Ballarat (C)' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"STATE_NAME" = 'Victoria' AND "LGA_NAME_2"  = 'Greater Geelong (C)' </t>
-  </si>
-  <si>
     <t>['',400]</t>
   </si>
   <si>
@@ -1810,40 +1804,7 @@
     <t xml:space="preserve">"STATE_NAME" = 'Australian Capital Territory' AND "GCCSA_NAME"  = 'Australian Capital Territory' </t>
   </si>
   <si>
-    <t>"STATE_NAME" IN ('New South Wales','Victoria' )  AND "LGA_NAME_2"  IN ('Albury (C)', 'Wodonga (C)')</t>
-  </si>
-  <si>
     <t>"STATE_NAME" = 'New South Wales' AND "LGA_NAME_2"  IN ('Blue Mountains (C)','Camden (A)','Campbelltown (C) (NSW)','Fairfield (C)','Hawkesbury (C)','Liverpool (C)','Penrith (C)','Wollondilly (A)' )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"STATE_NAME" = 'Victoria' AND "LGA_NAME_2"  = 'Greater Bendigo (C)' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"STATE_NAME" = 'Queensland' AND "LGA_NAME_2"  = 'Cairns (R)' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"STATE_NAME" = 'Queensland' AND "LGA_NAME_2"  = 'Gold Coast (C)' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"STATE_NAME" = 'Tasmania' AND "LGA_NAME_2"  = 'Launceston (C)' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"STATE_NAME" = 'Queensland' AND "LGA_NAME_2"  = 'Mackay (R)' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"STATE_NAME" = 'Queensland' AND "LGA_NAME_2"  = 'Sunshine Coast (R)' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"STATE_NAME" = 'Queensland' AND "LGA_NAME_2"  = 'Toowoomba (R)' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"STATE_NAME" = 'Queensland' AND "LGA_NAME_2"  = 'Townsville (C)' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"STATE_NAME" = 'New South Wales' AND "LGA_NAME_2"  = 'Wollongong (C)' </t>
-  </si>
-  <si>
-    <t>"STATE_NAME" = 'New South Wales' AND "LGA_NAME_2"  IN ('Newcastle (C)','Maitland (C)')</t>
   </si>
   <si>
     <t>ballarat</t>
@@ -2830,6 +2791,51 @@
   </si>
   <si>
     <t>Distance within which all Areas of Open Space are sought</t>
+  </si>
+  <si>
+    <t>ABS/derived/ASGS_2016_Volume_4_GDA2020/main_SUA_2016_AUST.shp</t>
+  </si>
+  <si>
+    <t>"SUA_NAME_2" = 'Albury - Wodonga'</t>
+  </si>
+  <si>
+    <t>"SUA_NAME_2" = 'Ballarat'</t>
+  </si>
+  <si>
+    <t>"SUA_NAME_2" = 'Bendigo'</t>
+  </si>
+  <si>
+    <t>"SUA_NAME_2" = 'Cairns'</t>
+  </si>
+  <si>
+    <t>"SUA_NAME_2" = 'Geelong'</t>
+  </si>
+  <si>
+    <t>"SUA_NAME_2" = 'Gold Coast - Tweed Heads'</t>
+  </si>
+  <si>
+    <t>"SUA_NAME_2" = 'Launceston'</t>
+  </si>
+  <si>
+    <t>"SUA_NAME_2" = 'Mackay'</t>
+  </si>
+  <si>
+    <t>"SUA_NAME_2" = 'Newcastle - Maitland'</t>
+  </si>
+  <si>
+    <t>"SUA_NAME_2" = 'Sunshine Coast'</t>
+  </si>
+  <si>
+    <t>"SUA_NAME_2" = 'Toowoomba'</t>
+  </si>
+  <si>
+    <t>"SUA_NAME_2" = 'Wollongong'</t>
+  </si>
+  <si>
+    <t>"SUA_NAME_2" = 'Townsville'</t>
+  </si>
+  <si>
+    <t>SUA</t>
   </si>
 </sst>
 </file>
@@ -3915,12 +3921,12 @@
   <sheetData>
     <row r="1" spans="1:1" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>666</v>
+        <v>653</v>
       </c>
     </row>
     <row r="2" spans="1:1" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>667</v>
+        <v>654</v>
       </c>
     </row>
     <row r="3" spans="1:1" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -3928,27 +3934,27 @@
     </row>
     <row r="4" spans="1:1" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>608</v>
+        <v>595</v>
       </c>
     </row>
     <row r="5" spans="1:1" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
-        <v>668</v>
+        <v>655</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>669</v>
+        <v>656</v>
       </c>
     </row>
     <row r="8" spans="1:1" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
-        <v>607</v>
+        <v>594</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>609</v>
+        <v>596</v>
       </c>
     </row>
   </sheetData>
@@ -3975,12 +3981,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>673</v>
+        <v>660</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="B3" s="34" t="s">
         <v>472</v>
@@ -3989,24 +3995,24 @@
         <v>473</v>
       </c>
       <c r="D3" s="56" t="s">
-        <v>680</v>
+        <v>667</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
-        <v>711</v>
+        <v>698</v>
       </c>
       <c r="B4" s="55"/>
       <c r="C4" s="85"/>
       <c r="D4" s="87" t="s">
-        <v>713</v>
+        <v>700</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="91"/>
       <c r="B5" s="92"/>
       <c r="C5" s="52" t="s">
-        <v>712</v>
+        <v>699</v>
       </c>
       <c r="D5" s="86"/>
     </row>
@@ -4014,18 +4020,18 @@
       <c r="A6" s="89"/>
       <c r="B6" s="90"/>
       <c r="C6" s="93" t="s">
-        <v>758</v>
+        <v>745</v>
       </c>
       <c r="D6" s="88"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
-        <v>670</v>
+        <v>657</v>
       </c>
       <c r="B7" s="49"/>
       <c r="C7" s="58"/>
       <c r="D7" s="63" t="s">
-        <v>681</v>
+        <v>668</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -4058,7 +4064,7 @@
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="35"/>
       <c r="B11" s="50" t="s">
-        <v>771</v>
+        <v>758</v>
       </c>
       <c r="C11" s="58" t="s">
         <v>475</v>
@@ -4067,7 +4073,7 @@
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="35"/>
       <c r="B12" s="49" t="s">
-        <v>773</v>
+        <v>760</v>
       </c>
       <c r="C12" s="58" t="s">
         <v>471</v>
@@ -4076,7 +4082,7 @@
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="35"/>
       <c r="B13" s="49" t="s">
-        <v>772</v>
+        <v>759</v>
       </c>
       <c r="C13" s="58" t="s">
         <v>476</v>
@@ -4094,7 +4100,7 @@
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
       <c r="B15" s="60" t="s">
-        <v>874</v>
+        <v>861</v>
       </c>
       <c r="C15" s="58" t="s">
         <v>477</v>
@@ -4103,19 +4109,19 @@
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="35"/>
       <c r="B16" s="60" t="s">
-        <v>706</v>
+        <v>693</v>
       </c>
       <c r="C16" s="58" t="s">
-        <v>707</v>
+        <v>694</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="35"/>
       <c r="B17" s="60" t="s">
-        <v>844</v>
+        <v>831</v>
       </c>
       <c r="C17" s="58" t="s">
-        <v>845</v>
+        <v>832</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4133,67 +4139,67 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="59" t="s">
-        <v>672</v>
+        <v>659</v>
       </c>
       <c r="B20" s="35"/>
       <c r="C20" s="58"/>
       <c r="D20" s="60" t="s">
-        <v>682</v>
+        <v>669</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="60" t="s">
-        <v>610</v>
+        <v>597</v>
       </c>
       <c r="C21" s="58" t="s">
-        <v>674</v>
+        <v>661</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="35"/>
       <c r="B22" s="60" t="s">
-        <v>611</v>
+        <v>598</v>
       </c>
       <c r="C22" s="58" t="s">
-        <v>675</v>
+        <v>662</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="35"/>
       <c r="B23" s="60" t="s">
-        <v>612</v>
+        <v>599</v>
       </c>
       <c r="C23" s="58" t="s">
-        <v>676</v>
+        <v>663</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="35"/>
       <c r="B24" s="60" t="s">
-        <v>613</v>
+        <v>600</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>677</v>
+        <v>664</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="47"/>
       <c r="B25" s="61" t="s">
-        <v>614</v>
+        <v>601</v>
       </c>
       <c r="C25" s="68" t="s">
-        <v>678</v>
+        <v>665</v>
       </c>
       <c r="D25" s="61"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="62" t="s">
-        <v>679</v>
+        <v>666</v>
       </c>
       <c r="B26" s="60"/>
       <c r="C26" s="58"/>
       <c r="D26" s="60" t="s">
-        <v>683</v>
+        <v>670</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -4260,10 +4266,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="62" t="s">
-        <v>684</v>
+        <v>671</v>
       </c>
       <c r="D37" s="63" t="s">
-        <v>686</v>
+        <v>673</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -4271,7 +4277,7 @@
         <v>205</v>
       </c>
       <c r="C38" s="64" t="s">
-        <v>685</v>
+        <v>672</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -4279,7 +4285,7 @@
         <v>204</v>
       </c>
       <c r="C39" s="64" t="s">
-        <v>687</v>
+        <v>674</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -4287,7 +4293,7 @@
         <v>207</v>
       </c>
       <c r="C40" s="64" t="s">
-        <v>688</v>
+        <v>675</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4295,7 +4301,7 @@
         <v>298</v>
       </c>
       <c r="C41" s="64" t="s">
-        <v>689</v>
+        <v>676</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -4303,7 +4309,7 @@
         <v>424</v>
       </c>
       <c r="C42" s="64" t="s">
-        <v>690</v>
+        <v>677</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -4311,7 +4317,7 @@
         <v>300</v>
       </c>
       <c r="C43" s="64" t="s">
-        <v>691</v>
+        <v>678</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -4319,7 +4325,7 @@
         <v>323</v>
       </c>
       <c r="C44" s="64" t="s">
-        <v>692</v>
+        <v>679</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -4327,7 +4333,7 @@
         <v>158</v>
       </c>
       <c r="C45" s="64" t="s">
-        <v>693</v>
+        <v>680</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -4335,7 +4341,7 @@
         <v>208</v>
       </c>
       <c r="C46" s="64" t="s">
-        <v>694</v>
+        <v>681</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -4343,7 +4349,7 @@
         <v>209</v>
       </c>
       <c r="C47" s="64" t="s">
-        <v>695</v>
+        <v>682</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -4351,7 +4357,7 @@
         <v>273</v>
       </c>
       <c r="C48" s="64" t="s">
-        <v>696</v>
+        <v>683</v>
       </c>
     </row>
     <row r="49" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -4359,7 +4365,7 @@
         <v>272</v>
       </c>
       <c r="C49" s="64" t="s">
-        <v>697</v>
+        <v>684</v>
       </c>
     </row>
     <row r="50" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -4367,7 +4373,7 @@
         <v>278</v>
       </c>
       <c r="C50" s="64" t="s">
-        <v>698</v>
+        <v>685</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
@@ -4375,7 +4381,7 @@
         <v>321</v>
       </c>
       <c r="C51" s="64" t="s">
-        <v>699</v>
+        <v>686</v>
       </c>
     </row>
     <row r="52" spans="2:3" ht="45" x14ac:dyDescent="0.25">
@@ -4383,7 +4389,7 @@
         <v>316</v>
       </c>
       <c r="C52" s="64" t="s">
-        <v>700</v>
+        <v>687</v>
       </c>
     </row>
   </sheetData>
@@ -4410,72 +4416,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="94" t="s">
-        <v>701</v>
+        <v>688</v>
       </c>
       <c r="B1" s="95" t="s">
-        <v>702</v>
+        <v>689</v>
       </c>
       <c r="C1" s="101" t="s">
-        <v>810</v>
+        <v>797</v>
       </c>
       <c r="D1" s="101" t="s">
-        <v>710</v>
+        <v>697</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>703</v>
+        <v>690</v>
       </c>
       <c r="B2" s="69" t="s">
-        <v>704</v>
+        <v>691</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>714</v>
+        <v>701</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>705</v>
+        <v>692</v>
       </c>
       <c r="B3" s="69">
         <v>2016</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>719</v>
+        <v>706</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>708</v>
+        <v>695</v>
       </c>
       <c r="B4" s="69" t="s">
-        <v>715</v>
+        <v>702</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>720</v>
+        <v>707</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>709</v>
+        <v>696</v>
       </c>
       <c r="B5" s="69">
         <v>7845</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>721</v>
+        <v>708</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4483,584 +4489,584 @@
         <v>321</v>
       </c>
       <c r="B6" s="69" t="s">
-        <v>716</v>
+        <v>703</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>723</v>
+        <v>710</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>717</v>
+        <v>704</v>
       </c>
       <c r="B7" s="69" t="s">
-        <v>718</v>
+        <v>705</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>722</v>
+        <v>709</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>724</v>
+        <v>711</v>
       </c>
       <c r="B8" s="69">
         <v>10000</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>728</v>
+        <v>715</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>725</v>
+        <v>712</v>
       </c>
       <c r="B9" s="69">
         <v>3000</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>727</v>
+        <v>714</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>726</v>
+        <v>713</v>
       </c>
       <c r="B10" s="69">
         <v>3000</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>729</v>
+        <v>716</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>730</v>
+        <v>717</v>
       </c>
       <c r="B11" s="69" t="s">
-        <v>731</v>
+        <v>718</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>734</v>
+        <v>721</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>750</v>
+        <v>737</v>
       </c>
       <c r="B12" s="69" t="s">
-        <v>753</v>
+        <v>740</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>811</v>
+        <v>798</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>757</v>
+        <v>744</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>751</v>
+        <v>738</v>
       </c>
       <c r="B13" s="69">
         <v>5432</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>811</v>
+        <v>798</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>756</v>
+        <v>743</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>752</v>
+        <v>739</v>
       </c>
       <c r="B14" s="69" t="s">
-        <v>754</v>
+        <v>741</v>
       </c>
       <c r="C14" s="38" t="s">
-        <v>811</v>
+        <v>798</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>756</v>
+        <v>743</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>869</v>
+        <v>856</v>
       </c>
       <c r="B15" s="69" t="s">
-        <v>755</v>
+        <v>742</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>811</v>
+        <v>798</v>
       </c>
       <c r="D15" s="38" t="s">
-        <v>756</v>
+        <v>743</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>759</v>
+        <v>746</v>
       </c>
       <c r="B16" s="69" t="s">
-        <v>760</v>
+        <v>747</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>811</v>
+        <v>798</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>756</v>
+        <v>743</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>885</v>
+        <v>872</v>
       </c>
       <c r="B17" s="69" t="s">
-        <v>889</v>
+        <v>876</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>811</v>
+        <v>798</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>890</v>
+        <v>877</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>886</v>
+        <v>873</v>
       </c>
       <c r="B18" s="69" t="s">
-        <v>887</v>
+        <v>874</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>811</v>
+        <v>798</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>888</v>
+        <v>875</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>735</v>
+        <v>722</v>
       </c>
       <c r="B19" s="69" t="s">
-        <v>732</v>
+        <v>719</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>812</v>
+        <v>799</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>733</v>
+        <v>720</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>736</v>
+        <v>723</v>
       </c>
       <c r="B20" s="69" t="s">
-        <v>737</v>
+        <v>724</v>
       </c>
       <c r="C20" s="38" t="s">
-        <v>812</v>
+        <v>799</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>738</v>
+        <v>725</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>739</v>
+        <v>726</v>
       </c>
       <c r="B21" s="69" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>813</v>
+        <v>800</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>741</v>
+        <v>728</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>742</v>
+        <v>729</v>
       </c>
       <c r="B22" s="69" t="s">
-        <v>744</v>
+        <v>731</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>813</v>
+        <v>800</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>746</v>
+        <v>733</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>743</v>
+        <v>730</v>
       </c>
       <c r="B23" s="69" t="s">
-        <v>745</v>
+        <v>732</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>813</v>
+        <v>800</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>746</v>
+        <v>733</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>747</v>
+        <v>734</v>
       </c>
       <c r="B24" s="69" t="s">
-        <v>749</v>
+        <v>736</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>813</v>
+        <v>800</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>748</v>
+        <v>735</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>761</v>
+        <v>748</v>
       </c>
       <c r="B25" s="69" t="s">
-        <v>762</v>
+        <v>749</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>788</v>
+        <v>775</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>763</v>
+        <v>750</v>
       </c>
       <c r="B26" s="69" t="s">
-        <v>764</v>
+        <v>751</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>765</v>
+        <v>752</v>
       </c>
       <c r="B27" s="69" t="s">
-        <v>766</v>
+        <v>753</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>786</v>
+        <v>773</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>761</v>
+      </c>
+      <c r="B28" s="69" t="s">
+        <v>766</v>
+      </c>
+      <c r="C28" s="38" t="s">
+        <v>801</v>
+      </c>
+      <c r="D28" s="38" t="s">
         <v>774</v>
-      </c>
-      <c r="B28" s="69" t="s">
-        <v>779</v>
-      </c>
-      <c r="C28" s="38" t="s">
-        <v>814</v>
-      </c>
-      <c r="D28" s="38" t="s">
-        <v>787</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>775</v>
+        <v>762</v>
       </c>
       <c r="B29" s="69" t="s">
-        <v>780</v>
+        <v>767</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
       <c r="D29" s="38" t="s">
-        <v>783</v>
+        <v>770</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>776</v>
+        <v>763</v>
       </c>
       <c r="B30" s="69" t="s">
-        <v>781</v>
+        <v>768</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>784</v>
+        <v>771</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>777</v>
+        <v>764</v>
       </c>
       <c r="B31" s="69" t="s">
-        <v>782</v>
+        <v>769</v>
       </c>
       <c r="C31" s="38" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>785</v>
+        <v>772</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>778</v>
+        <v>765</v>
       </c>
       <c r="B32" s="69" t="s">
-        <v>789</v>
+        <v>776</v>
       </c>
       <c r="C32" s="38" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>801</v>
+        <v>788</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>793</v>
+        <v>780</v>
       </c>
       <c r="B33" s="69" t="s">
-        <v>790</v>
+        <v>777</v>
       </c>
       <c r="C33" s="38" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>802</v>
+        <v>789</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>794</v>
+        <v>781</v>
       </c>
       <c r="B34" s="69" t="s">
-        <v>791</v>
+        <v>778</v>
       </c>
       <c r="C34" s="38" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>803</v>
+        <v>790</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>795</v>
+        <v>782</v>
       </c>
       <c r="B35" s="69" t="s">
-        <v>792</v>
+        <v>779</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>804</v>
+        <v>791</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>796</v>
+        <v>783</v>
       </c>
       <c r="B36" s="69" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>805</v>
+        <v>792</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>797</v>
+        <v>784</v>
       </c>
       <c r="B37" s="69" t="s">
-        <v>799</v>
+        <v>786</v>
       </c>
       <c r="C37" s="38" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>806</v>
+        <v>793</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>798</v>
+        <v>785</v>
       </c>
       <c r="B38" s="69" t="s">
-        <v>800</v>
+        <v>787</v>
       </c>
       <c r="C38" s="38" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>807</v>
+        <v>794</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>808</v>
+        <v>795</v>
       </c>
       <c r="B39" s="69" t="s">
-        <v>817</v>
+        <v>804</v>
       </c>
       <c r="C39" s="38" t="s">
-        <v>815</v>
+        <v>802</v>
       </c>
       <c r="D39" s="38" t="s">
-        <v>818</v>
+        <v>805</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>809</v>
+        <v>796</v>
       </c>
       <c r="B40" s="69">
         <v>7844</v>
       </c>
       <c r="C40" s="38" t="s">
-        <v>815</v>
+        <v>802</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>819</v>
+        <v>806</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>820</v>
+        <v>807</v>
       </c>
       <c r="B41" s="69" t="s">
-        <v>821</v>
+        <v>808</v>
       </c>
       <c r="C41" s="38" t="s">
-        <v>821</v>
+        <v>808</v>
       </c>
       <c r="D41" s="38" t="s">
-        <v>822</v>
+        <v>809</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>823</v>
+        <v>810</v>
       </c>
       <c r="B42" s="69" t="s">
-        <v>826</v>
+        <v>813</v>
       </c>
       <c r="C42" s="38" t="s">
-        <v>821</v>
+        <v>808</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>829</v>
+        <v>816</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>824</v>
+        <v>811</v>
       </c>
       <c r="B43" s="69" t="s">
-        <v>827</v>
+        <v>814</v>
       </c>
       <c r="C43" s="38" t="s">
-        <v>821</v>
+        <v>808</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>756</v>
+        <v>743</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>825</v>
+        <v>812</v>
       </c>
       <c r="B44" s="69" t="s">
-        <v>828</v>
+        <v>815</v>
       </c>
       <c r="C44" s="38" t="s">
-        <v>821</v>
+        <v>808</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>756</v>
+        <v>743</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>830</v>
+        <v>817</v>
       </c>
       <c r="B45" s="69" t="s">
-        <v>831</v>
+        <v>818</v>
       </c>
       <c r="C45" s="38" t="s">
-        <v>821</v>
+        <v>808</v>
       </c>
       <c r="D45" s="38" t="s">
-        <v>832</v>
+        <v>819</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>833</v>
+        <v>820</v>
       </c>
       <c r="B46" s="69" t="s">
-        <v>835</v>
+        <v>822</v>
       </c>
       <c r="C46" s="38" t="s">
-        <v>813</v>
+        <v>800</v>
       </c>
       <c r="D46" s="38" t="s">
-        <v>872</v>
+        <v>859</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>834</v>
+        <v>821</v>
       </c>
       <c r="B47" s="69" t="s">
-        <v>836</v>
+        <v>823</v>
       </c>
       <c r="C47" s="38" t="s">
-        <v>813</v>
+        <v>800</v>
       </c>
       <c r="D47" s="38" t="s">
-        <v>872</v>
+        <v>859</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -5071,164 +5077,164 @@
         <v>1600</v>
       </c>
       <c r="C48" s="38" t="s">
-        <v>838</v>
+        <v>825</v>
       </c>
       <c r="D48" s="38" t="s">
-        <v>871</v>
+        <v>858</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>837</v>
+        <v>824</v>
       </c>
       <c r="B49" s="69">
         <v>500</v>
       </c>
       <c r="C49" s="38" t="s">
-        <v>838</v>
+        <v>825</v>
       </c>
       <c r="D49" s="38" t="s">
-        <v>842</v>
+        <v>829</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>870</v>
+        <v>857</v>
       </c>
       <c r="B50" s="69">
         <v>50</v>
       </c>
       <c r="C50" s="38" t="s">
-        <v>838</v>
+        <v>825</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>841</v>
+        <v>828</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>839</v>
+        <v>826</v>
       </c>
       <c r="B51" s="69">
         <v>3000</v>
       </c>
       <c r="C51" s="38" t="s">
-        <v>838</v>
+        <v>825</v>
       </c>
       <c r="D51" s="38" t="s">
-        <v>840</v>
+        <v>827</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>899</v>
+        <v>886</v>
       </c>
       <c r="B52" s="69">
         <v>3200</v>
       </c>
       <c r="C52" s="38" t="s">
-        <v>838</v>
+        <v>825</v>
       </c>
       <c r="D52" s="38" t="s">
-        <v>900</v>
+        <v>887</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>843</v>
+        <v>830</v>
       </c>
       <c r="B53" s="69">
         <v>5</v>
       </c>
       <c r="C53" s="38" t="s">
-        <v>846</v>
+        <v>833</v>
       </c>
       <c r="D53" s="38" t="s">
-        <v>847</v>
+        <v>834</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>853</v>
+        <v>840</v>
       </c>
       <c r="B54" s="69">
         <v>50</v>
       </c>
       <c r="C54" s="38" t="s">
-        <v>855</v>
+        <v>842</v>
       </c>
       <c r="D54" s="38" t="s">
-        <v>854</v>
+        <v>841</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>856</v>
+        <v>843</v>
       </c>
       <c r="B55" s="69" t="s">
-        <v>672</v>
+        <v>659</v>
       </c>
       <c r="C55" s="38" t="s">
-        <v>672</v>
+        <v>659</v>
       </c>
       <c r="D55" s="38" t="s">
-        <v>857</v>
+        <v>844</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>858</v>
+        <v>845</v>
       </c>
       <c r="B56" s="69" t="s">
-        <v>859</v>
+        <v>846</v>
       </c>
       <c r="C56" s="38" t="s">
-        <v>672</v>
+        <v>659</v>
       </c>
       <c r="D56" s="38" t="s">
-        <v>860</v>
+        <v>847</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>861</v>
+        <v>848</v>
       </c>
       <c r="B57" s="69" t="s">
-        <v>863</v>
+        <v>850</v>
       </c>
       <c r="C57" s="38" t="s">
-        <v>672</v>
+        <v>659</v>
       </c>
       <c r="D57" s="38" t="s">
-        <v>864</v>
+        <v>851</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>862</v>
+        <v>849</v>
       </c>
       <c r="B58" s="69" t="b">
         <v>0</v>
       </c>
       <c r="C58" s="38" t="s">
-        <v>672</v>
+        <v>659</v>
       </c>
       <c r="D58" s="38" t="s">
-        <v>865</v>
+        <v>852</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>866</v>
+        <v>853</v>
       </c>
       <c r="B59" s="69" t="s">
-        <v>868</v>
+        <v>855</v>
       </c>
       <c r="C59" s="38" t="s">
-        <v>672</v>
+        <v>659</v>
       </c>
       <c r="D59" s="38" t="s">
-        <v>867</v>
+        <v>854</v>
       </c>
     </row>
   </sheetData>
@@ -5241,10 +5247,10 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5252,8 +5258,8 @@
     <col min="1" max="1" width="24" style="36" customWidth="1"/>
     <col min="2" max="2" width="36.140625" style="32" customWidth="1"/>
     <col min="3" max="4" width="20.140625" style="32" customWidth="1"/>
-    <col min="5" max="5" width="91.140625" style="32" customWidth="1"/>
-    <col min="6" max="6" width="86.140625" style="33" customWidth="1"/>
+    <col min="5" max="5" width="86.140625" style="33" customWidth="1"/>
+    <col min="6" max="6" width="91.140625" style="32" customWidth="1"/>
     <col min="7" max="8" width="51.42578125" style="32" customWidth="1"/>
     <col min="9" max="9" width="40.85546875" style="32" customWidth="1"/>
     <col min="10" max="11" width="67.28515625" style="32" customWidth="1"/>
@@ -5273,76 +5279,76 @@
         <v>428</v>
       </c>
       <c r="D1" s="71" t="s">
-        <v>594</v>
+        <v>581</v>
       </c>
       <c r="E1" s="72" t="s">
-        <v>773</v>
+        <v>758</v>
       </c>
       <c r="F1" s="72" t="s">
-        <v>771</v>
+        <v>760</v>
       </c>
       <c r="G1" s="71" t="s">
-        <v>772</v>
+        <v>759</v>
       </c>
       <c r="H1" s="71" t="s">
-        <v>848</v>
+        <v>835</v>
       </c>
       <c r="I1" s="71" t="s">
         <v>429</v>
       </c>
       <c r="J1" s="71" t="s">
-        <v>874</v>
+        <v>861</v>
       </c>
       <c r="K1" s="71" t="s">
-        <v>898</v>
+        <v>885</v>
       </c>
       <c r="L1" s="71" t="s">
-        <v>891</v>
+        <v>878</v>
       </c>
       <c r="M1" s="73" t="s">
-        <v>706</v>
+        <v>693</v>
       </c>
       <c r="N1" s="73" t="s">
-        <v>844</v>
+        <v>831</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="74" t="s">
-        <v>767</v>
+        <v>754</v>
       </c>
       <c r="B2" s="75" t="s">
-        <v>767</v>
+        <v>754</v>
       </c>
       <c r="C2" s="75" t="s">
-        <v>768</v>
+        <v>755</v>
       </c>
       <c r="D2" s="75" t="s">
-        <v>769</v>
+        <v>756</v>
       </c>
       <c r="E2" s="76" t="s">
-        <v>770</v>
+        <v>433</v>
       </c>
       <c r="F2" s="76" t="s">
-        <v>433</v>
+        <v>757</v>
       </c>
       <c r="G2" s="75" t="s">
         <v>434</v>
       </c>
       <c r="H2" s="75" t="s">
-        <v>873</v>
+        <v>860</v>
       </c>
       <c r="I2" s="76" t="s">
         <v>439</v>
       </c>
       <c r="J2" s="75" t="s">
-        <v>875</v>
+        <v>862</v>
       </c>
       <c r="K2" s="75" t="str">
         <f>"D:/ntnl_li_2018_template/data/study_region/"&amp;B2&amp;"_20181001.osm"</f>
         <v>D:/ntnl_li_2018_template/data/study_region/testing_20181001.osm</v>
       </c>
       <c r="L2" s="75" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="M2" s="77"/>
       <c r="N2" s="77">
@@ -5354,19 +5360,19 @@
         <v>430</v>
       </c>
       <c r="B3" s="75" t="s">
-        <v>599</v>
+        <v>586</v>
       </c>
       <c r="C3" s="75" t="s">
         <v>431</v>
       </c>
       <c r="D3" s="75" t="s">
-        <v>595</v>
+        <v>582</v>
       </c>
       <c r="E3" s="76" t="s">
+        <v>433</v>
+      </c>
+      <c r="F3" s="76" t="s">
         <v>432</v>
-      </c>
-      <c r="F3" s="76" t="s">
-        <v>433</v>
       </c>
       <c r="G3" s="75" t="s">
         <v>434</v>
@@ -5379,7 +5385,7 @@
         <v>D:/ntnl_li_2018_template/data/study_region/adelaide_20181001.osm</v>
       </c>
       <c r="L3" s="75" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="M3" s="77"/>
       <c r="N3" s="77">
@@ -5391,25 +5397,25 @@
         <v>435</v>
       </c>
       <c r="B4" s="79" t="s">
-        <v>598</v>
+        <v>585</v>
       </c>
       <c r="C4" s="79" t="s">
         <v>436</v>
       </c>
       <c r="D4" s="79" t="s">
-        <v>595</v>
+        <v>582</v>
       </c>
       <c r="E4" s="80" t="s">
+        <v>433</v>
+      </c>
+      <c r="F4" s="80" t="s">
         <v>437</v>
-      </c>
-      <c r="F4" s="80" t="s">
-        <v>433</v>
       </c>
       <c r="G4" s="79" t="s">
         <v>438</v>
       </c>
       <c r="H4" s="79" t="s">
-        <v>849</v>
+        <v>836</v>
       </c>
       <c r="I4" s="80" t="s">
         <v>439</v>
@@ -5420,7 +5426,7 @@
         <v>D:/ntnl_li_2018_template/data/study_region/bris_20181001.osm</v>
       </c>
       <c r="L4" s="79" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="N4" s="32">
         <v>0</v>
@@ -5431,19 +5437,19 @@
         <v>440</v>
       </c>
       <c r="B5" s="82" t="s">
-        <v>600</v>
+        <v>587</v>
       </c>
       <c r="C5" s="82" t="s">
         <v>441</v>
       </c>
       <c r="D5" s="82" t="s">
-        <v>595</v>
+        <v>582</v>
       </c>
       <c r="E5" s="83" t="s">
-        <v>572</v>
+        <v>433</v>
       </c>
       <c r="F5" s="83" t="s">
-        <v>433</v>
+        <v>570</v>
       </c>
       <c r="G5" s="82" t="s">
         <v>442</v>
@@ -5456,7 +5462,7 @@
         <v>D:/ntnl_li_2018_template/data/study_region/canberra_20181001.osm</v>
       </c>
       <c r="L5" s="82" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="M5" s="51"/>
       <c r="N5" s="51">
@@ -5468,19 +5474,19 @@
         <v>443</v>
       </c>
       <c r="B6" s="79" t="s">
-        <v>601</v>
+        <v>588</v>
       </c>
       <c r="C6" s="79" t="s">
         <v>444</v>
       </c>
       <c r="D6" s="79" t="s">
-        <v>595</v>
+        <v>582</v>
       </c>
       <c r="E6" s="80" t="s">
+        <v>433</v>
+      </c>
+      <c r="F6" s="80" t="s">
         <v>445</v>
-      </c>
-      <c r="F6" s="80" t="s">
-        <v>433</v>
       </c>
       <c r="G6" s="79" t="s">
         <v>446</v>
@@ -5493,7 +5499,7 @@
         <v>D:/ntnl_li_2018_template/data/study_region/darwin_20181001.osm</v>
       </c>
       <c r="L6" s="79" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="N6" s="32">
         <v>0</v>
@@ -5504,19 +5510,19 @@
         <v>447</v>
       </c>
       <c r="B7" s="82" t="s">
-        <v>602</v>
+        <v>589</v>
       </c>
       <c r="C7" s="82" t="s">
         <v>448</v>
       </c>
       <c r="D7" s="82" t="s">
-        <v>595</v>
+        <v>582</v>
       </c>
       <c r="E7" s="83" t="s">
+        <v>433</v>
+      </c>
+      <c r="F7" s="83" t="s">
         <v>449</v>
-      </c>
-      <c r="F7" s="83" t="s">
-        <v>433</v>
       </c>
       <c r="G7" s="82" t="s">
         <v>450</v>
@@ -5529,7 +5535,7 @@
         <v>D:/ntnl_li_2018_template/data/study_region/hobart_20181001.osm</v>
       </c>
       <c r="L7" s="82" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="M7" s="51"/>
       <c r="N7" s="51">
@@ -5541,38 +5547,38 @@
         <v>451</v>
       </c>
       <c r="B8" s="79" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="C8" s="79" t="s">
         <v>452</v>
       </c>
       <c r="D8" s="79" t="s">
-        <v>595</v>
+        <v>582</v>
       </c>
       <c r="E8" s="80" t="s">
+        <v>433</v>
+      </c>
+      <c r="F8" s="80" t="s">
         <v>453</v>
-      </c>
-      <c r="F8" s="80" t="s">
-        <v>433</v>
       </c>
       <c r="G8" s="79" t="s">
         <v>454</v>
       </c>
       <c r="H8" s="79" t="s">
-        <v>850</v>
+        <v>837</v>
       </c>
       <c r="I8" s="80" t="s">
         <v>455</v>
       </c>
       <c r="J8" s="79" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="K8" s="79" t="str">
         <f t="shared" si="0"/>
         <v>D:/ntnl_li_2018_template/data/study_region/melb_20181001.osm</v>
       </c>
       <c r="L8" s="79" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="N8" s="32">
         <v>0</v>
@@ -5583,25 +5589,25 @@
         <v>44</v>
       </c>
       <c r="B9" s="82" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="C9" s="82" t="s">
         <v>457</v>
       </c>
       <c r="D9" s="82" t="s">
-        <v>595</v>
-      </c>
-      <c r="E9" s="82" t="s">
+        <v>582</v>
+      </c>
+      <c r="E9" s="83" t="s">
+        <v>433</v>
+      </c>
+      <c r="F9" s="82" t="s">
         <v>458</v>
-      </c>
-      <c r="F9" s="83" t="s">
-        <v>433</v>
       </c>
       <c r="G9" s="82" t="s">
         <v>459</v>
       </c>
       <c r="H9" s="82" t="s">
-        <v>852</v>
+        <v>839</v>
       </c>
       <c r="I9" s="83" t="s">
         <v>460</v>
@@ -5612,7 +5618,7 @@
         <v>D:/ntnl_li_2018_template/data/study_region/perth_20181001.osm</v>
       </c>
       <c r="L9" s="82" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="M9" s="51"/>
       <c r="N9" s="51">
@@ -5624,25 +5630,25 @@
         <v>461</v>
       </c>
       <c r="B10" s="79" t="s">
-        <v>605</v>
+        <v>592</v>
       </c>
       <c r="C10" s="79" t="s">
         <v>462</v>
       </c>
       <c r="D10" s="79" t="s">
-        <v>595</v>
+        <v>582</v>
       </c>
       <c r="E10" s="80" t="s">
+        <v>433</v>
+      </c>
+      <c r="F10" s="80" t="s">
         <v>463</v>
-      </c>
-      <c r="F10" s="80" t="s">
-        <v>433</v>
       </c>
       <c r="G10" s="79" t="s">
         <v>464</v>
       </c>
       <c r="H10" s="79" t="s">
-        <v>851</v>
+        <v>838</v>
       </c>
       <c r="I10" s="80" t="s">
         <v>465</v>
@@ -5655,7 +5661,7 @@
         <v>D:/ntnl_li_2018_template/data/study_region/syd_20181001.osm</v>
       </c>
       <c r="L10" s="79" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="N10" s="32">
         <v>0</v>
@@ -5666,19 +5672,19 @@
         <v>466</v>
       </c>
       <c r="B11" s="82" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="C11" s="82" t="s">
         <v>452</v>
       </c>
       <c r="D11" s="82" t="s">
-        <v>596</v>
+        <v>583</v>
       </c>
       <c r="E11" s="83" t="s">
+        <v>567</v>
+      </c>
+      <c r="F11" s="83" t="s">
         <v>467</v>
-      </c>
-      <c r="F11" s="83" t="s">
-        <v>569</v>
       </c>
       <c r="G11" s="82" t="s">
         <v>454</v>
@@ -5691,7 +5697,7 @@
         <v>D:/ntnl_li_2018_template/data/study_region/mitchell_20181001.osm</v>
       </c>
       <c r="L11" s="82" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="M11" s="51"/>
       <c r="N11" s="51">
@@ -5703,22 +5709,22 @@
         <v>552</v>
       </c>
       <c r="B12" s="79" t="s">
-        <v>893</v>
+        <v>880</v>
       </c>
       <c r="C12" s="79" t="s">
-        <v>597</v>
+        <v>584</v>
       </c>
       <c r="D12" s="79" t="s">
-        <v>596</v>
-      </c>
-      <c r="E12" s="103" t="s">
-        <v>573</v>
-      </c>
-      <c r="F12" s="80" t="s">
+        <v>902</v>
+      </c>
+      <c r="E12" s="80" t="s">
+        <v>888</v>
+      </c>
+      <c r="F12" s="103" t="s">
+        <v>889</v>
+      </c>
+      <c r="G12" s="102" t="s">
         <v>569</v>
-      </c>
-      <c r="G12" s="102" t="s">
-        <v>571</v>
       </c>
       <c r="H12" s="84"/>
       <c r="I12" s="80" t="s">
@@ -5730,7 +5736,7 @@
         <v>D:/ntnl_li_2018_template/data/study_region/albury_wodonga_20181001.osm</v>
       </c>
       <c r="L12" s="79" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="N12" s="32">
         <v>0</v>
@@ -5741,19 +5747,19 @@
         <v>553</v>
       </c>
       <c r="B13" s="82" t="s">
-        <v>585</v>
+        <v>572</v>
       </c>
       <c r="C13" s="82" t="s">
         <v>452</v>
       </c>
       <c r="D13" s="82" t="s">
-        <v>596</v>
+        <v>902</v>
       </c>
       <c r="E13" s="83" t="s">
-        <v>565</v>
+        <v>888</v>
       </c>
       <c r="F13" s="83" t="s">
-        <v>569</v>
+        <v>890</v>
       </c>
       <c r="G13" s="82" t="s">
         <v>454</v>
@@ -5768,7 +5774,7 @@
         <v>D:/ntnl_li_2018_template/data/study_region/ballarat_20181001.osm</v>
       </c>
       <c r="L13" s="82" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="M13" s="51"/>
       <c r="N13" s="51">
@@ -5780,19 +5786,19 @@
         <v>554</v>
       </c>
       <c r="B14" s="79" t="s">
-        <v>586</v>
+        <v>573</v>
       </c>
       <c r="C14" s="79" t="s">
         <v>452</v>
       </c>
       <c r="D14" s="79" t="s">
-        <v>596</v>
-      </c>
-      <c r="E14" s="79" t="s">
-        <v>575</v>
-      </c>
-      <c r="F14" s="80" t="s">
-        <v>569</v>
+        <v>902</v>
+      </c>
+      <c r="E14" s="80" t="s">
+        <v>888</v>
+      </c>
+      <c r="F14" s="79" t="s">
+        <v>891</v>
       </c>
       <c r="G14" s="79" t="s">
         <v>454</v>
@@ -5807,7 +5813,7 @@
         <v>D:/ntnl_li_2018_template/data/study_region/bendigo_20181001.osm</v>
       </c>
       <c r="L14" s="79" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="N14" s="32">
         <v>0</v>
@@ -5818,19 +5824,19 @@
         <v>555</v>
       </c>
       <c r="B15" s="82" t="s">
-        <v>587</v>
+        <v>574</v>
       </c>
       <c r="C15" s="82" t="s">
         <v>436</v>
       </c>
       <c r="D15" s="82" t="s">
-        <v>596</v>
-      </c>
-      <c r="E15" s="82" t="s">
-        <v>576</v>
-      </c>
-      <c r="F15" s="83" t="s">
-        <v>569</v>
+        <v>902</v>
+      </c>
+      <c r="E15" s="83" t="s">
+        <v>888</v>
+      </c>
+      <c r="F15" s="82" t="s">
+        <v>892</v>
       </c>
       <c r="G15" s="82" t="s">
         <v>438</v>
@@ -5845,7 +5851,7 @@
         <v>D:/ntnl_li_2018_template/data/study_region/cairns_20181001.osm</v>
       </c>
       <c r="L15" s="82" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="M15" s="51"/>
       <c r="N15" s="51">
@@ -5857,19 +5863,19 @@
         <v>556</v>
       </c>
       <c r="B16" s="79" t="s">
-        <v>588</v>
+        <v>575</v>
       </c>
       <c r="C16" s="79" t="s">
         <v>452</v>
       </c>
       <c r="D16" s="79" t="s">
-        <v>596</v>
+        <v>902</v>
       </c>
       <c r="E16" s="80" t="s">
-        <v>566</v>
+        <v>888</v>
       </c>
       <c r="F16" s="80" t="s">
-        <v>569</v>
+        <v>893</v>
       </c>
       <c r="G16" s="79" t="s">
         <v>454</v>
@@ -5884,7 +5890,7 @@
         <v>D:/ntnl_li_2018_template/data/study_region/geelong_20181001.osm</v>
       </c>
       <c r="L16" s="79" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="N16" s="32">
         <v>0</v>
@@ -5895,19 +5901,19 @@
         <v>557</v>
       </c>
       <c r="B17" s="82" t="s">
-        <v>897</v>
+        <v>884</v>
       </c>
       <c r="C17" s="82" t="s">
         <v>436</v>
       </c>
       <c r="D17" s="82" t="s">
-        <v>596</v>
-      </c>
-      <c r="E17" s="82" t="s">
-        <v>577</v>
-      </c>
-      <c r="F17" s="83" t="s">
-        <v>569</v>
+        <v>902</v>
+      </c>
+      <c r="E17" s="83" t="s">
+        <v>888</v>
+      </c>
+      <c r="F17" s="82" t="s">
+        <v>894</v>
       </c>
       <c r="G17" s="82" t="s">
         <v>438</v>
@@ -5922,7 +5928,7 @@
         <v>D:/ntnl_li_2018_template/data/study_region/goldcoast_tweedheads_20181001.osm</v>
       </c>
       <c r="L17" s="82" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="M17" s="51"/>
       <c r="N17" s="51">
@@ -5934,26 +5940,26 @@
         <v>558</v>
       </c>
       <c r="B18" s="79" t="s">
-        <v>589</v>
+        <v>576</v>
       </c>
       <c r="C18" s="79" t="s">
         <v>448</v>
       </c>
       <c r="D18" s="79" t="s">
-        <v>596</v>
-      </c>
-      <c r="E18" s="79" t="s">
-        <v>578</v>
-      </c>
-      <c r="F18" s="80" t="s">
-        <v>569</v>
+        <v>902</v>
+      </c>
+      <c r="E18" s="80" t="s">
+        <v>888</v>
+      </c>
+      <c r="F18" s="79" t="s">
+        <v>895</v>
       </c>
       <c r="G18" s="79" t="s">
         <v>450</v>
       </c>
       <c r="H18" s="79"/>
       <c r="I18" s="79" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="J18" s="79"/>
       <c r="K18" s="79" t="str">
@@ -5961,7 +5967,7 @@
         <v>D:/ntnl_li_2018_template/data/study_region/launceston_20181001.osm</v>
       </c>
       <c r="L18" s="79" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="N18" s="32">
         <v>0</v>
@@ -5972,19 +5978,19 @@
         <v>559</v>
       </c>
       <c r="B19" s="82" t="s">
-        <v>590</v>
+        <v>577</v>
       </c>
       <c r="C19" s="82" t="s">
         <v>436</v>
       </c>
       <c r="D19" s="82" t="s">
-        <v>596</v>
-      </c>
-      <c r="E19" s="82" t="s">
-        <v>579</v>
-      </c>
-      <c r="F19" s="83" t="s">
-        <v>569</v>
+        <v>902</v>
+      </c>
+      <c r="E19" s="83" t="s">
+        <v>888</v>
+      </c>
+      <c r="F19" s="82" t="s">
+        <v>896</v>
       </c>
       <c r="G19" s="82" t="s">
         <v>438</v>
@@ -5999,7 +6005,7 @@
         <v>D:/ntnl_li_2018_template/data/study_region/mackay_20181001.osm</v>
       </c>
       <c r="L19" s="82" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="M19" s="51"/>
       <c r="N19" s="51">
@@ -6011,19 +6017,19 @@
         <v>560</v>
       </c>
       <c r="B20" s="79" t="s">
-        <v>894</v>
+        <v>881</v>
       </c>
       <c r="C20" s="79" t="s">
         <v>462</v>
       </c>
       <c r="D20" s="79" t="s">
-        <v>596</v>
-      </c>
-      <c r="E20" s="79" t="s">
-        <v>584</v>
-      </c>
-      <c r="F20" s="80" t="s">
-        <v>569</v>
+        <v>902</v>
+      </c>
+      <c r="E20" s="80" t="s">
+        <v>888</v>
+      </c>
+      <c r="F20" s="79" t="s">
+        <v>897</v>
       </c>
       <c r="G20" s="79" t="s">
         <v>464</v>
@@ -6038,7 +6044,7 @@
         <v>D:/ntnl_li_2018_template/data/study_region/newcastle_maitland_20181001.osm</v>
       </c>
       <c r="L20" s="79" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="N20" s="32">
         <v>0</v>
@@ -6049,19 +6055,19 @@
         <v>561</v>
       </c>
       <c r="B21" s="82" t="s">
-        <v>895</v>
+        <v>882</v>
       </c>
       <c r="C21" s="82" t="s">
         <v>436</v>
       </c>
       <c r="D21" s="82" t="s">
-        <v>596</v>
-      </c>
-      <c r="E21" s="82" t="s">
-        <v>580</v>
-      </c>
-      <c r="F21" s="83" t="s">
-        <v>569</v>
+        <v>902</v>
+      </c>
+      <c r="E21" s="83" t="s">
+        <v>888</v>
+      </c>
+      <c r="F21" s="82" t="s">
+        <v>898</v>
       </c>
       <c r="G21" s="82" t="s">
         <v>438</v>
@@ -6076,7 +6082,7 @@
         <v>D:/ntnl_li_2018_template/data/study_region/sunshine_coast_20181001.osm</v>
       </c>
       <c r="L21" s="82" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="M21" s="51"/>
       <c r="N21" s="51">
@@ -6088,19 +6094,19 @@
         <v>562</v>
       </c>
       <c r="B22" s="79" t="s">
-        <v>591</v>
+        <v>578</v>
       </c>
       <c r="C22" s="79" t="s">
         <v>436</v>
       </c>
       <c r="D22" s="79" t="s">
-        <v>596</v>
-      </c>
-      <c r="E22" s="79" t="s">
-        <v>581</v>
-      </c>
-      <c r="F22" s="80" t="s">
-        <v>569</v>
+        <v>902</v>
+      </c>
+      <c r="E22" s="80" t="s">
+        <v>888</v>
+      </c>
+      <c r="F22" s="79" t="s">
+        <v>899</v>
       </c>
       <c r="G22" s="79" t="s">
         <v>438</v>
@@ -6115,7 +6121,7 @@
         <v>D:/ntnl_li_2018_template/data/study_region/toowoomba_20181001.osm</v>
       </c>
       <c r="L22" s="79" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="N22" s="32">
         <v>0</v>
@@ -6126,19 +6132,19 @@
         <v>563</v>
       </c>
       <c r="B23" s="82" t="s">
-        <v>592</v>
+        <v>579</v>
       </c>
       <c r="C23" s="82" t="s">
         <v>436</v>
       </c>
       <c r="D23" s="82" t="s">
-        <v>596</v>
-      </c>
-      <c r="E23" s="82" t="s">
-        <v>582</v>
-      </c>
-      <c r="F23" s="83" t="s">
-        <v>569</v>
+        <v>902</v>
+      </c>
+      <c r="E23" s="83" t="s">
+        <v>888</v>
+      </c>
+      <c r="F23" s="82" t="s">
+        <v>901</v>
       </c>
       <c r="G23" s="82" t="s">
         <v>438</v>
@@ -6153,7 +6159,7 @@
         <v>D:/ntnl_li_2018_template/data/study_region/townsville_20181001.osm</v>
       </c>
       <c r="L23" s="82" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="M23" s="51"/>
       <c r="N23" s="51">
@@ -6165,19 +6171,19 @@
         <v>564</v>
       </c>
       <c r="B24" s="79" t="s">
-        <v>593</v>
+        <v>580</v>
       </c>
       <c r="C24" s="79" t="s">
         <v>462</v>
       </c>
       <c r="D24" s="79" t="s">
-        <v>596</v>
-      </c>
-      <c r="E24" s="79" t="s">
-        <v>583</v>
-      </c>
-      <c r="F24" s="80" t="s">
-        <v>569</v>
+        <v>902</v>
+      </c>
+      <c r="E24" s="80" t="s">
+        <v>888</v>
+      </c>
+      <c r="F24" s="79" t="s">
+        <v>900</v>
       </c>
       <c r="G24" s="79" t="s">
         <v>464</v>
@@ -6192,7 +6198,7 @@
         <v>D:/ntnl_li_2018_template/data/study_region/wollongong_20181001.osm</v>
       </c>
       <c r="L24" s="79" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="N24" s="32">
         <v>0</v>
@@ -6200,25 +6206,25 @@
     </row>
     <row r="25" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="81" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B25" s="82" t="s">
-        <v>896</v>
+        <v>883</v>
       </c>
       <c r="C25" s="82" t="s">
         <v>462</v>
       </c>
       <c r="D25" s="82" t="s">
-        <v>596</v>
-      </c>
-      <c r="E25" s="84" t="s">
-        <v>574</v>
-      </c>
-      <c r="F25" s="83" t="s">
-        <v>569</v>
+        <v>902</v>
+      </c>
+      <c r="E25" s="83" t="s">
+        <v>567</v>
+      </c>
+      <c r="F25" s="84" t="s">
+        <v>571</v>
       </c>
       <c r="G25" s="83" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="H25" s="83"/>
       <c r="I25" s="83" t="s">
@@ -6232,7 +6238,7 @@
         <v>D:/ntnl_li_2018_template/data/study_region/western_sydney_20181001.osm</v>
       </c>
       <c r="L25" s="82" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="M25" s="51"/>
       <c r="N25" s="51">
@@ -6262,19 +6268,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>610</v>
+        <v>597</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>611</v>
+        <v>598</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>612</v>
+        <v>599</v>
       </c>
       <c r="D1" s="39" t="s">
-        <v>613</v>
+        <v>600</v>
       </c>
       <c r="E1" s="39" t="s">
-        <v>614</v>
+        <v>601</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -6282,7 +6288,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>615</v>
+        <v>602</v>
       </c>
       <c r="C2" t="s">
         <v>151</v>
@@ -6296,7 +6302,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>616</v>
+        <v>603</v>
       </c>
       <c r="C3" t="s">
         <v>151</v>
@@ -6310,7 +6316,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>617</v>
+        <v>604</v>
       </c>
       <c r="C4" t="s">
         <v>151</v>
@@ -6324,7 +6330,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>618</v>
+        <v>605</v>
       </c>
       <c r="C5" t="s">
         <v>151</v>
@@ -6338,7 +6344,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>619</v>
+        <v>606</v>
       </c>
       <c r="C6" t="s">
         <v>151</v>
@@ -6352,7 +6358,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>620</v>
+        <v>607</v>
       </c>
       <c r="C7" t="s">
         <v>151</v>
@@ -6366,7 +6372,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>621</v>
+        <v>608</v>
       </c>
       <c r="C8" t="s">
         <v>151</v>
@@ -6380,7 +6386,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>622</v>
+        <v>609</v>
       </c>
       <c r="C9" t="s">
         <v>151</v>
@@ -6394,10 +6400,10 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>623</v>
+        <v>610</v>
       </c>
       <c r="C10" t="s">
-        <v>624</v>
+        <v>611</v>
       </c>
       <c r="D10">
         <v>1600</v>
@@ -6408,10 +6414,10 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>625</v>
+        <v>612</v>
       </c>
       <c r="C11" t="s">
-        <v>624</v>
+        <v>611</v>
       </c>
       <c r="D11">
         <v>1600</v>
@@ -6422,10 +6428,10 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>626</v>
+        <v>613</v>
       </c>
       <c r="C12" t="s">
-        <v>624</v>
+        <v>611</v>
       </c>
       <c r="D12">
         <v>1600</v>
@@ -6436,7 +6442,7 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>627</v>
+        <v>614</v>
       </c>
       <c r="C13" t="s">
         <v>144</v>
@@ -6450,7 +6456,7 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>628</v>
+        <v>615</v>
       </c>
       <c r="C14" t="s">
         <v>144</v>
@@ -6467,7 +6473,7 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>629</v>
+        <v>616</v>
       </c>
       <c r="C15" t="s">
         <v>76</v>
@@ -6481,7 +6487,7 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>630</v>
+        <v>617</v>
       </c>
       <c r="C16" t="s">
         <v>76</v>
@@ -6495,7 +6501,7 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>631</v>
+        <v>618</v>
       </c>
       <c r="C17" t="s">
         <v>76</v>
@@ -6509,7 +6515,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>632</v>
+        <v>619</v>
       </c>
       <c r="C18" t="s">
         <v>76</v>
@@ -6523,7 +6529,7 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>633</v>
+        <v>620</v>
       </c>
       <c r="C19" t="s">
         <v>76</v>
@@ -6537,7 +6543,7 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="C20" t="s">
         <v>76</v>
@@ -6551,7 +6557,7 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>635</v>
+        <v>622</v>
       </c>
       <c r="C21" t="s">
         <v>76</v>
@@ -6565,7 +6571,7 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>636</v>
+        <v>623</v>
       </c>
       <c r="C22" t="s">
         <v>76</v>
@@ -6579,7 +6585,7 @@
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="C23" t="s">
         <v>76</v>
@@ -6593,7 +6599,7 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>638</v>
+        <v>625</v>
       </c>
       <c r="C24" t="s">
         <v>76</v>
@@ -6607,7 +6613,7 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>639</v>
+        <v>626</v>
       </c>
       <c r="C25" t="s">
         <v>76</v>
@@ -6621,7 +6627,7 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>640</v>
+        <v>627</v>
       </c>
       <c r="C26" t="s">
         <v>76</v>
@@ -6635,7 +6641,7 @@
         <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>641</v>
+        <v>628</v>
       </c>
       <c r="C27" t="s">
         <v>76</v>
@@ -6649,7 +6655,7 @@
         <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>642</v>
+        <v>629</v>
       </c>
       <c r="C28" t="s">
         <v>76</v>
@@ -6663,7 +6669,7 @@
         <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>643</v>
+        <v>630</v>
       </c>
       <c r="C29" t="s">
         <v>76</v>
@@ -6677,7 +6683,7 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>644</v>
+        <v>631</v>
       </c>
       <c r="C30" t="s">
         <v>76</v>
@@ -6691,7 +6697,7 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>645</v>
+        <v>632</v>
       </c>
       <c r="C31" t="s">
         <v>76</v>
@@ -6705,7 +6711,7 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>646</v>
+        <v>633</v>
       </c>
       <c r="C32" t="s">
         <v>76</v>
@@ -6719,7 +6725,7 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>647</v>
+        <v>634</v>
       </c>
       <c r="C33" t="s">
         <v>76</v>
@@ -6733,7 +6739,7 @@
         <v>14</v>
       </c>
       <c r="B34" t="s">
-        <v>648</v>
+        <v>635</v>
       </c>
       <c r="C34" t="s">
         <v>76</v>
@@ -6747,7 +6753,7 @@
         <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>649</v>
+        <v>636</v>
       </c>
       <c r="C35" t="s">
         <v>76</v>
@@ -6761,7 +6767,7 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>650</v>
+        <v>637</v>
       </c>
       <c r="C36" t="s">
         <v>76</v>
@@ -6775,7 +6781,7 @@
         <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>651</v>
+        <v>638</v>
       </c>
       <c r="C37" t="s">
         <v>76</v>
@@ -6789,7 +6795,7 @@
         <v>100</v>
       </c>
       <c r="B38" t="s">
-        <v>652</v>
+        <v>639</v>
       </c>
       <c r="C38" t="s">
         <v>16</v>
@@ -6803,7 +6809,7 @@
         <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>653</v>
+        <v>640</v>
       </c>
       <c r="C39" t="s">
         <v>144</v>
@@ -6817,7 +6823,7 @@
         <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>654</v>
+        <v>641</v>
       </c>
       <c r="C40" t="s">
         <v>144</v>
@@ -6831,7 +6837,7 @@
         <v>16</v>
       </c>
       <c r="B41" t="s">
-        <v>655</v>
+        <v>642</v>
       </c>
       <c r="C41" t="s">
         <v>144</v>
@@ -6845,7 +6851,7 @@
         <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>656</v>
+        <v>643</v>
       </c>
       <c r="C42" t="s">
         <v>144</v>
@@ -6859,7 +6865,7 @@
         <v>18</v>
       </c>
       <c r="B43" t="s">
-        <v>657</v>
+        <v>644</v>
       </c>
       <c r="C43" t="s">
         <v>144</v>
@@ -6873,7 +6879,7 @@
         <v>19</v>
       </c>
       <c r="B44" t="s">
-        <v>658</v>
+        <v>645</v>
       </c>
       <c r="C44" t="s">
         <v>144</v>
@@ -6887,7 +6893,7 @@
         <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>659</v>
+        <v>646</v>
       </c>
       <c r="C45" t="s">
         <v>144</v>
@@ -6901,7 +6907,7 @@
         <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>660</v>
+        <v>647</v>
       </c>
       <c r="C46" t="s">
         <v>16</v>
@@ -6915,7 +6921,7 @@
         <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>661</v>
+        <v>648</v>
       </c>
       <c r="C47" t="s">
         <v>16</v>
@@ -6929,7 +6935,7 @@
         <v>22</v>
       </c>
       <c r="B48" t="s">
-        <v>662</v>
+        <v>649</v>
       </c>
       <c r="C48" t="s">
         <v>16</v>
@@ -6943,10 +6949,10 @@
         <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>663</v>
+        <v>650</v>
       </c>
       <c r="C49" t="s">
-        <v>624</v>
+        <v>611</v>
       </c>
       <c r="D49">
         <v>1600</v>
@@ -6957,10 +6963,10 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>664</v>
+        <v>651</v>
       </c>
       <c r="C50" t="s">
-        <v>624</v>
+        <v>611</v>
       </c>
       <c r="D50">
         <v>1600</v>
@@ -6971,10 +6977,10 @@
         <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>665</v>
+        <v>652</v>
       </c>
       <c r="C51" t="s">
-        <v>624</v>
+        <v>611</v>
       </c>
       <c r="D51">
         <v>1600</v>
@@ -9257,7 +9263,7 @@
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="98" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="D2" s="42" t="s">
         <v>416</v>
@@ -9295,7 +9301,7 @@
         <v>203</v>
       </c>
       <c r="C3" s="98" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="D3" s="43" t="s">
         <v>324</v>
@@ -9342,7 +9348,7 @@
         <v>206</v>
       </c>
       <c r="C4" s="98" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="D4" s="43" t="s">
         <v>324</v>
@@ -9387,7 +9393,7 @@
       </c>
       <c r="B5" s="23"/>
       <c r="C5" s="98" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="D5" s="43" t="s">
         <v>325</v>
@@ -9426,7 +9432,7 @@
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="98" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="D6" s="43" t="s">
         <v>326</v>
@@ -9462,7 +9468,7 @@
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="98" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="D7" s="43" t="s">
         <v>327</v>
@@ -9498,7 +9504,7 @@
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="98" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="D8" s="43" t="s">
         <v>328</v>
@@ -9537,7 +9543,7 @@
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="98" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="D9" s="43" t="s">
         <v>369</v>
@@ -9573,7 +9579,7 @@
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="98" t="s">
-        <v>598</v>
+        <v>585</v>
       </c>
       <c r="D10" s="43" t="s">
         <v>385</v>
@@ -9609,7 +9615,7 @@
       </c>
       <c r="B11" s="23"/>
       <c r="C11" s="98" t="s">
-        <v>598</v>
+        <v>585</v>
       </c>
       <c r="D11" s="43" t="s">
         <v>329</v>
@@ -9648,7 +9654,7 @@
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="98" t="s">
-        <v>598</v>
+        <v>585</v>
       </c>
       <c r="D12" s="43" t="s">
         <v>384</v>
@@ -9687,7 +9693,7 @@
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="98" t="s">
-        <v>605</v>
+        <v>592</v>
       </c>
       <c r="D13" s="43" t="s">
         <v>331</v>
@@ -9726,7 +9732,7 @@
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="98" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>421</v>
@@ -9768,7 +9774,7 @@
       </c>
       <c r="B15" s="23"/>
       <c r="C15" s="98" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>422</v>
@@ -9803,7 +9809,7 @@
         <v>203</v>
       </c>
       <c r="C16" s="98" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="D16" s="23" t="s">
         <v>380</v>
@@ -9847,7 +9853,7 @@
         <v>206</v>
       </c>
       <c r="C17" s="98" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="D17" s="23" t="s">
         <v>381</v>
@@ -9888,7 +9894,7 @@
         <v>173</v>
       </c>
       <c r="C18" s="98" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="D18" s="43" t="s">
         <v>382</v>
@@ -9930,7 +9936,7 @@
       </c>
       <c r="B19" s="23"/>
       <c r="C19" s="98" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="D19" s="23" t="s">
         <v>383</v>
@@ -9974,7 +9980,7 @@
         <v>203</v>
       </c>
       <c r="C20" s="98" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="D20" s="23" t="s">
         <v>379</v>
@@ -10018,7 +10024,7 @@
         <v>206</v>
       </c>
       <c r="C21" s="98" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="D21" s="23" t="s">
         <v>386</v>
@@ -10062,7 +10068,7 @@
         <v>203</v>
       </c>
       <c r="C22" s="98" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="D22" s="43" t="s">
         <v>378</v>
@@ -10109,7 +10115,7 @@
         <v>206</v>
       </c>
       <c r="C23" s="98" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="D23" s="43" t="s">
         <v>388</v>
@@ -10156,7 +10162,7 @@
         <v>203</v>
       </c>
       <c r="C24" s="98" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="D24" s="43" t="s">
         <v>377</v>
@@ -10203,7 +10209,7 @@
         <v>206</v>
       </c>
       <c r="C25" s="98" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="D25" s="43" t="s">
         <v>387</v>
@@ -10248,7 +10254,7 @@
       </c>
       <c r="B26" s="23"/>
       <c r="C26" s="98" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="D26" s="43" t="s">
         <v>376</v>
@@ -10289,7 +10295,7 @@
         <v>203</v>
       </c>
       <c r="C27" s="98" t="s">
-        <v>598</v>
+        <v>585</v>
       </c>
       <c r="D27" s="43" t="s">
         <v>375</v>
@@ -10336,7 +10342,7 @@
         <v>206</v>
       </c>
       <c r="C28" s="98" t="s">
-        <v>598</v>
+        <v>585</v>
       </c>
       <c r="D28" s="43" t="s">
         <v>389</v>
@@ -10383,7 +10389,7 @@
         <v>203</v>
       </c>
       <c r="C29" s="98" t="s">
-        <v>605</v>
+        <v>592</v>
       </c>
       <c r="D29" s="43" t="s">
         <v>402</v>
@@ -10430,7 +10436,7 @@
         <v>206</v>
       </c>
       <c r="C30" s="98" t="s">
-        <v>605</v>
+        <v>592</v>
       </c>
       <c r="D30" s="43" t="s">
         <v>401</v>
@@ -10477,7 +10483,7 @@
         <v>203</v>
       </c>
       <c r="C31" s="98" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="D31" s="43" t="s">
         <v>374</v>
@@ -10521,7 +10527,7 @@
         <v>206</v>
       </c>
       <c r="C32" s="98" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="D32" s="43" t="s">
         <v>390</v>
@@ -10562,7 +10568,7 @@
         <v>516</v>
       </c>
       <c r="C33" s="98" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="D33" s="44" t="s">
         <v>517</v>
@@ -10606,7 +10612,7 @@
         <v>203</v>
       </c>
       <c r="C34" s="98" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="D34" s="43" t="s">
         <v>373</v>
@@ -10653,7 +10659,7 @@
         <v>206</v>
       </c>
       <c r="C35" s="98" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="D35" s="43" t="s">
         <v>391</v>
@@ -10700,7 +10706,7 @@
         <v>203</v>
       </c>
       <c r="C36" s="98" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="D36" s="43" t="s">
         <v>372</v>
@@ -10747,7 +10753,7 @@
         <v>206</v>
       </c>
       <c r="C37" s="98" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="D37" s="43" t="s">
         <v>394</v>
@@ -10794,7 +10800,7 @@
         <v>203</v>
       </c>
       <c r="C38" s="98" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="D38" s="43" t="s">
         <v>395</v>
@@ -10841,7 +10847,7 @@
         <v>206</v>
       </c>
       <c r="C39" s="98" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="D39" s="43" t="s">
         <v>396</v>
@@ -10888,7 +10894,7 @@
         <v>203</v>
       </c>
       <c r="C40" s="98" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="D40" s="43" t="s">
         <v>397</v>
@@ -10935,7 +10941,7 @@
         <v>206</v>
       </c>
       <c r="C41" s="98" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="D41" s="43" t="s">
         <v>398</v>
@@ -10982,7 +10988,7 @@
         <v>203</v>
       </c>
       <c r="C42" s="98" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="D42" s="43" t="s">
         <v>399</v>
@@ -11029,7 +11035,7 @@
         <v>206</v>
       </c>
       <c r="C43" s="98" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="D43" s="43" t="s">
         <v>400</v>
@@ -11076,7 +11082,7 @@
         <v>203</v>
       </c>
       <c r="C44" s="98" t="s">
-        <v>598</v>
+        <v>585</v>
       </c>
       <c r="D44" s="43" t="s">
         <v>405</v>
@@ -11123,7 +11129,7 @@
         <v>206</v>
       </c>
       <c r="C45" s="98" t="s">
-        <v>598</v>
+        <v>585</v>
       </c>
       <c r="D45" s="43" t="s">
         <v>406</v>
@@ -11170,7 +11176,7 @@
         <v>203</v>
       </c>
       <c r="C46" s="98" t="s">
-        <v>598</v>
+        <v>585</v>
       </c>
       <c r="D46" s="43" t="s">
         <v>403</v>
@@ -11217,7 +11223,7 @@
         <v>206</v>
       </c>
       <c r="C47" s="98" t="s">
-        <v>598</v>
+        <v>585</v>
       </c>
       <c r="D47" s="43" t="s">
         <v>404</v>
@@ -11264,7 +11270,7 @@
         <v>203</v>
       </c>
       <c r="C48" s="98" t="s">
-        <v>605</v>
+        <v>592</v>
       </c>
       <c r="D48" s="43" t="s">
         <v>407</v>
@@ -11311,7 +11317,7 @@
         <v>206</v>
       </c>
       <c r="C49" s="98" t="s">
-        <v>605</v>
+        <v>592</v>
       </c>
       <c r="D49" s="43" t="s">
         <v>408</v>
@@ -11358,7 +11364,7 @@
         <v>203</v>
       </c>
       <c r="C50" s="98" t="s">
-        <v>605</v>
+        <v>592</v>
       </c>
       <c r="D50" s="43" t="s">
         <v>409</v>
@@ -11405,7 +11411,7 @@
         <v>206</v>
       </c>
       <c r="C51" s="98" t="s">
-        <v>605</v>
+        <v>592</v>
       </c>
       <c r="D51" s="43" t="s">
         <v>410</v>
@@ -11452,7 +11458,7 @@
         <v>203</v>
       </c>
       <c r="C52" s="98" t="s">
-        <v>879</v>
+        <v>866</v>
       </c>
       <c r="D52" s="43" t="s">
         <v>370</v>
@@ -11496,7 +11502,7 @@
         <v>206</v>
       </c>
       <c r="C53" s="98" t="s">
-        <v>879</v>
+        <v>866</v>
       </c>
       <c r="D53" s="43" t="s">
         <v>393</v>
@@ -11540,7 +11546,7 @@
         <v>203</v>
       </c>
       <c r="C54" s="98" t="s">
-        <v>879</v>
+        <v>866</v>
       </c>
       <c r="D54" s="43" t="s">
         <v>411</v>
@@ -11584,7 +11590,7 @@
         <v>206</v>
       </c>
       <c r="C55" s="98" t="s">
-        <v>879</v>
+        <v>866</v>
       </c>
       <c r="D55" s="43" t="s">
         <v>412</v>
@@ -11626,7 +11632,7 @@
       </c>
       <c r="B56" s="23"/>
       <c r="C56" s="98" t="s">
-        <v>879</v>
+        <v>866</v>
       </c>
       <c r="D56" s="43" t="s">
         <v>364</v>
@@ -11662,7 +11668,7 @@
       </c>
       <c r="B57" s="23"/>
       <c r="C57" s="98" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="D57" s="43" t="s">
         <v>365</v>
@@ -11698,7 +11704,7 @@
       </c>
       <c r="B58" s="23"/>
       <c r="C58" s="98" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="D58" s="43" t="s">
         <v>366</v>
@@ -11734,7 +11740,7 @@
       </c>
       <c r="B59" s="23"/>
       <c r="C59" s="98" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="D59" s="43" t="s">
         <v>357</v>
@@ -11770,7 +11776,7 @@
       </c>
       <c r="B60" s="23"/>
       <c r="C60" s="98" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="D60" s="43" t="s">
         <v>358</v>
@@ -11806,7 +11812,7 @@
       </c>
       <c r="B61" s="23"/>
       <c r="C61" s="98" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="D61" s="43" t="s">
         <v>359</v>
@@ -11842,7 +11848,7 @@
       </c>
       <c r="B62" s="23"/>
       <c r="C62" s="98" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="D62" s="43" t="s">
         <v>360</v>
@@ -11878,7 +11884,7 @@
       </c>
       <c r="B63" s="23"/>
       <c r="C63" s="98" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="D63" s="43" t="s">
         <v>361</v>
@@ -11914,7 +11920,7 @@
       </c>
       <c r="B64" s="23"/>
       <c r="C64" s="98" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="D64" s="43" t="s">
         <v>415</v>
@@ -11956,7 +11962,7 @@
         <v>203</v>
       </c>
       <c r="C65" s="98" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="D65" s="43" t="s">
         <v>371</v>
@@ -12000,7 +12006,7 @@
         <v>206</v>
       </c>
       <c r="C66" s="98" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="D66" s="43" t="s">
         <v>392</v>
@@ -12044,7 +12050,7 @@
         <v>203</v>
       </c>
       <c r="C67" s="98" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="D67" s="44" t="s">
         <v>481</v>
@@ -12088,7 +12094,7 @@
         <v>206</v>
       </c>
       <c r="C68" s="98" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="D68" s="44" t="s">
         <v>481</v>
@@ -12132,7 +12138,7 @@
         <v>203</v>
       </c>
       <c r="C69" s="98" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="D69" s="44" t="s">
         <v>487</v>
@@ -12176,7 +12182,7 @@
         <v>206</v>
       </c>
       <c r="C70" s="98" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="D70" s="44" t="s">
         <v>487</v>
@@ -12217,7 +12223,7 @@
         <v>492</v>
       </c>
       <c r="C71" s="98" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="D71" s="44" t="s">
         <v>493</v>
@@ -12258,7 +12264,7 @@
         <v>496</v>
       </c>
       <c r="C72" s="98" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="D72" s="44" t="s">
         <v>497</v>
@@ -12299,7 +12305,7 @@
         <v>500</v>
       </c>
       <c r="C73" s="98" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="D73" s="44" t="s">
         <v>501</v>
@@ -12337,7 +12343,7 @@
         <v>505</v>
       </c>
       <c r="C74" s="98" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="D74" s="44" t="s">
         <v>506</v>
@@ -12375,7 +12381,7 @@
         <v>510</v>
       </c>
       <c r="C75" s="98" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="D75" s="44" t="s">
         <v>511</v>
@@ -12414,7 +12420,7 @@
       </c>
       <c r="B76" s="23"/>
       <c r="C76" s="98" t="s">
-        <v>880</v>
+        <v>867</v>
       </c>
       <c r="D76" s="43" t="s">
         <v>413</v>
@@ -12454,7 +12460,7 @@
       </c>
       <c r="B77" s="23"/>
       <c r="C77" s="98" t="s">
-        <v>880</v>
+        <v>867</v>
       </c>
       <c r="D77" s="43" t="s">
         <v>414</v>
@@ -12493,7 +12499,7 @@
         <v>520</v>
       </c>
       <c r="C78" s="98" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="D78" s="44" t="s">
         <v>521</v>
@@ -12534,7 +12540,7 @@
         <v>524</v>
       </c>
       <c r="C79" s="98" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="D79" s="44" t="s">
         <v>525</v>
@@ -12578,7 +12584,7 @@
         <v>203</v>
       </c>
       <c r="C80" s="98" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="D80" s="44" t="s">
         <v>529</v>
@@ -12622,7 +12628,7 @@
         <v>206</v>
       </c>
       <c r="C81" s="98" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="D81" s="44" t="s">
         <v>529</v>
@@ -12663,7 +12669,7 @@
         <v>534</v>
       </c>
       <c r="C82" s="98" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="D82" s="44" t="s">
         <v>535</v>
@@ -12707,7 +12713,7 @@
         <v>203</v>
       </c>
       <c r="C83" s="98" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="D83" s="44" t="s">
         <v>539</v>
@@ -12751,7 +12757,7 @@
         <v>206</v>
       </c>
       <c r="C84" s="98" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="D84" s="44" t="s">
         <v>539</v>
@@ -12792,7 +12798,7 @@
         <v>544</v>
       </c>
       <c r="C85" s="98" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="D85" s="44" t="s">
         <v>545</v>
@@ -12833,7 +12839,7 @@
         <v>548</v>
       </c>
       <c r="C86" s="98" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="D86" s="44" t="s">
         <v>549</v>
@@ -12871,13 +12877,13 @@
     </row>
     <row r="87" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="22" t="s">
-        <v>881</v>
+        <v>868</v>
       </c>
       <c r="C87" s="99" t="s">
-        <v>882</v>
+        <v>869</v>
       </c>
       <c r="D87" s="42" t="s">
-        <v>883</v>
+        <v>870</v>
       </c>
       <c r="E87" t="s">
         <v>425</v>
@@ -12886,13 +12892,13 @@
         <v>308</v>
       </c>
       <c r="G87" s="42" t="s">
-        <v>883</v>
+        <v>870</v>
       </c>
       <c r="H87" s="42" t="s">
-        <v>883</v>
+        <v>870</v>
       </c>
       <c r="K87" s="96" t="s">
-        <v>884</v>
+        <v>871</v>
       </c>
       <c r="L87" s="22">
         <v>1</v>
@@ -12923,10 +12929,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>876</v>
+        <v>863</v>
       </c>
       <c r="B1" t="s">
-        <v>877</v>
+        <v>864</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some key AOS and config file updates
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06128446-5C14-4565-8E99-CE0EDD9AEF53}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626E492D-01E3-440E-A426-552D2926B684}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="3" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
@@ -5247,10 +5247,10 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomRight" activeCell="K13" sqref="K13:K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5344,8 +5344,8 @@
         <v>862</v>
       </c>
       <c r="K2" s="75" t="str">
-        <f>"D:/ntnl_li_2018_template/data/study_region/"&amp;B2&amp;"_20181001.osm"</f>
-        <v>D:/ntnl_li_2018_template/data/study_region/testing_20181001.osm</v>
+        <f>"D:/ntnl_li_2018_template/data/study_region/"&amp;B2&amp;"/"&amp;B2&amp;"_"&amp;LOWER(D2)&amp;"_2016_10000m_20181001.osm"</f>
+        <v>D:/ntnl_li_2018_template/data/study_region/testing/testing_gccstest_2016_10000m_20181001.osm</v>
       </c>
       <c r="L2" s="75" t="s">
         <v>879</v>
@@ -5381,8 +5381,8 @@
       <c r="I3" s="75"/>
       <c r="J3" s="75"/>
       <c r="K3" s="75" t="str">
-        <f>"D:/ntnl_li_2018_template/data/study_region/"&amp;B3&amp;"_20181001.osm"</f>
-        <v>D:/ntnl_li_2018_template/data/study_region/adelaide_20181001.osm</v>
+        <f t="shared" ref="K3:K11" si="0">"D:/ntnl_li_2018_template/data/study_region/"&amp;B3&amp;"/"&amp;B3&amp;"_"&amp;LOWER(D3)&amp;"_2016_10000m_20181001.osm"</f>
+        <v>D:/ntnl_li_2018_template/data/study_region/adelaide/adelaide_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="L3" s="75" t="s">
         <v>879</v>
@@ -5421,9 +5421,9 @@
         <v>439</v>
       </c>
       <c r="J4" s="79"/>
-      <c r="K4" s="79" t="str">
-        <f t="shared" ref="K4:K25" si="0">"D:/ntnl_li_2018_template/data/study_region/"&amp;B4&amp;"_20181001.osm"</f>
-        <v>D:/ntnl_li_2018_template/data/study_region/bris_20181001.osm</v>
+      <c r="K4" s="75" t="str">
+        <f t="shared" si="0"/>
+        <v>D:/ntnl_li_2018_template/data/study_region/bris/bris_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="L4" s="79" t="s">
         <v>879</v>
@@ -5457,9 +5457,9 @@
       <c r="H5" s="82"/>
       <c r="I5" s="82"/>
       <c r="J5" s="82"/>
-      <c r="K5" s="82" t="str">
+      <c r="K5" s="75" t="str">
         <f t="shared" si="0"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/canberra_20181001.osm</v>
+        <v>D:/ntnl_li_2018_template/data/study_region/canberra/canberra_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="L5" s="82" t="s">
         <v>879</v>
@@ -5494,9 +5494,9 @@
       <c r="H6" s="79"/>
       <c r="I6" s="79"/>
       <c r="J6" s="79"/>
-      <c r="K6" s="79" t="str">
+      <c r="K6" s="75" t="str">
         <f t="shared" si="0"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/darwin_20181001.osm</v>
+        <v>D:/ntnl_li_2018_template/data/study_region/darwin/darwin_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="L6" s="79" t="s">
         <v>879</v>
@@ -5530,9 +5530,9 @@
       <c r="H7" s="82"/>
       <c r="I7" s="82"/>
       <c r="J7" s="82"/>
-      <c r="K7" s="82" t="str">
+      <c r="K7" s="75" t="str">
         <f t="shared" si="0"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/hobart_20181001.osm</v>
+        <v>D:/ntnl_li_2018_template/data/study_region/hobart/hobart_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="L7" s="82" t="s">
         <v>879</v>
@@ -5573,9 +5573,9 @@
       <c r="J8" s="79" t="s">
         <v>568</v>
       </c>
-      <c r="K8" s="79" t="str">
+      <c r="K8" s="75" t="str">
         <f t="shared" si="0"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/melb_20181001.osm</v>
+        <v>D:/ntnl_li_2018_template/data/study_region/melb/melb_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="L8" s="79" t="s">
         <v>879</v>
@@ -5613,9 +5613,9 @@
         <v>460</v>
       </c>
       <c r="J9" s="82"/>
-      <c r="K9" s="82" t="str">
+      <c r="K9" s="75" t="str">
         <f t="shared" si="0"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/perth_20181001.osm</v>
+        <v>D:/ntnl_li_2018_template/data/study_region/perth/perth_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="L9" s="82" t="s">
         <v>879</v>
@@ -5656,9 +5656,9 @@
       <c r="J10" s="79" t="s">
         <v>456</v>
       </c>
-      <c r="K10" s="79" t="str">
+      <c r="K10" s="75" t="str">
         <f t="shared" si="0"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/syd_20181001.osm</v>
+        <v>D:/ntnl_li_2018_template/data/study_region/syd/syd_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="L10" s="79" t="s">
         <v>879</v>
@@ -5692,9 +5692,9 @@
       <c r="H11" s="82"/>
       <c r="I11" s="82"/>
       <c r="J11" s="82"/>
-      <c r="K11" s="82" t="str">
+      <c r="K11" s="75" t="str">
         <f t="shared" si="0"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/mitchell_20181001.osm</v>
+        <v>D:/ntnl_li_2018_template/data/study_region/mitchell/mitchell_lga_2016_10000m_20181001.osm</v>
       </c>
       <c r="L11" s="82" t="s">
         <v>879</v>
@@ -5731,9 +5731,9 @@
         <v>465</v>
       </c>
       <c r="J12" s="79"/>
-      <c r="K12" s="79" t="str">
-        <f t="shared" si="0"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/albury_wodonga_20181001.osm</v>
+      <c r="K12" s="82" t="str">
+        <f>"D:/ntnl_li_2018_template/data/study_region/"&amp;B12&amp;"/"&amp;B12&amp;"_20181001.osm"</f>
+        <v>D:/ntnl_li_2018_template/data/study_region/albury_wodonga/albury_wodonga_20181001.osm</v>
       </c>
       <c r="L12" s="79" t="s">
         <v>879</v>
@@ -5770,8 +5770,8 @@
       </c>
       <c r="J13" s="82"/>
       <c r="K13" s="82" t="str">
-        <f t="shared" si="0"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/ballarat_20181001.osm</v>
+        <f>"D:/ntnl_li_2018_template/data/study_region/"&amp;B13&amp;"/"&amp;B13&amp;"_20181001.osm"</f>
+        <v>D:/ntnl_li_2018_template/data/study_region/ballarat/ballarat_20181001.osm</v>
       </c>
       <c r="L13" s="82" t="s">
         <v>879</v>
@@ -5808,9 +5808,9 @@
         <v>455</v>
       </c>
       <c r="J14" s="79"/>
-      <c r="K14" s="79" t="str">
-        <f t="shared" si="0"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/bendigo_20181001.osm</v>
+      <c r="K14" s="82" t="str">
+        <f t="shared" ref="K14:K25" si="1">"D:/ntnl_li_2018_template/data/study_region/"&amp;B14&amp;"/"&amp;B14&amp;"_20181001.osm"</f>
+        <v>D:/ntnl_li_2018_template/data/study_region/bendigo/bendigo_20181001.osm</v>
       </c>
       <c r="L14" s="79" t="s">
         <v>879</v>
@@ -5847,8 +5847,8 @@
       </c>
       <c r="J15" s="82"/>
       <c r="K15" s="82" t="str">
-        <f t="shared" si="0"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/cairns_20181001.osm</v>
+        <f t="shared" si="1"/>
+        <v>D:/ntnl_li_2018_template/data/study_region/cairns/cairns_20181001.osm</v>
       </c>
       <c r="L15" s="82" t="s">
         <v>879</v>
@@ -5885,9 +5885,9 @@
         <v>455</v>
       </c>
       <c r="J16" s="79"/>
-      <c r="K16" s="79" t="str">
-        <f t="shared" si="0"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/geelong_20181001.osm</v>
+      <c r="K16" s="82" t="str">
+        <f t="shared" si="1"/>
+        <v>D:/ntnl_li_2018_template/data/study_region/geelong/geelong_20181001.osm</v>
       </c>
       <c r="L16" s="79" t="s">
         <v>879</v>
@@ -5924,8 +5924,8 @@
       </c>
       <c r="J17" s="82"/>
       <c r="K17" s="82" t="str">
-        <f t="shared" si="0"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/goldcoast_tweedheads_20181001.osm</v>
+        <f t="shared" si="1"/>
+        <v>D:/ntnl_li_2018_template/data/study_region/goldcoast_tweedheads/goldcoast_tweedheads_20181001.osm</v>
       </c>
       <c r="L17" s="82" t="s">
         <v>879</v>
@@ -5962,9 +5962,9 @@
         <v>565</v>
       </c>
       <c r="J18" s="79"/>
-      <c r="K18" s="79" t="str">
-        <f t="shared" si="0"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/launceston_20181001.osm</v>
+      <c r="K18" s="82" t="str">
+        <f t="shared" si="1"/>
+        <v>D:/ntnl_li_2018_template/data/study_region/launceston/launceston_20181001.osm</v>
       </c>
       <c r="L18" s="79" t="s">
         <v>879</v>
@@ -6001,8 +6001,8 @@
       </c>
       <c r="J19" s="82"/>
       <c r="K19" s="82" t="str">
-        <f t="shared" si="0"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/mackay_20181001.osm</v>
+        <f t="shared" si="1"/>
+        <v>D:/ntnl_li_2018_template/data/study_region/mackay/mackay_20181001.osm</v>
       </c>
       <c r="L19" s="82" t="s">
         <v>879</v>
@@ -6039,9 +6039,9 @@
         <v>465</v>
       </c>
       <c r="J20" s="79"/>
-      <c r="K20" s="79" t="str">
-        <f t="shared" si="0"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/newcastle_maitland_20181001.osm</v>
+      <c r="K20" s="82" t="str">
+        <f t="shared" si="1"/>
+        <v>D:/ntnl_li_2018_template/data/study_region/newcastle_maitland/newcastle_maitland_20181001.osm</v>
       </c>
       <c r="L20" s="79" t="s">
         <v>879</v>
@@ -6078,8 +6078,8 @@
       </c>
       <c r="J21" s="82"/>
       <c r="K21" s="82" t="str">
-        <f t="shared" si="0"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/sunshine_coast_20181001.osm</v>
+        <f t="shared" si="1"/>
+        <v>D:/ntnl_li_2018_template/data/study_region/sunshine_coast/sunshine_coast_20181001.osm</v>
       </c>
       <c r="L21" s="82" t="s">
         <v>879</v>
@@ -6116,9 +6116,9 @@
         <v>439</v>
       </c>
       <c r="J22" s="79"/>
-      <c r="K22" s="79" t="str">
-        <f t="shared" si="0"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/toowoomba_20181001.osm</v>
+      <c r="K22" s="82" t="str">
+        <f t="shared" si="1"/>
+        <v>D:/ntnl_li_2018_template/data/study_region/toowoomba/toowoomba_20181001.osm</v>
       </c>
       <c r="L22" s="79" t="s">
         <v>879</v>
@@ -6155,8 +6155,8 @@
       </c>
       <c r="J23" s="82"/>
       <c r="K23" s="82" t="str">
-        <f t="shared" si="0"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/townsville_20181001.osm</v>
+        <f t="shared" si="1"/>
+        <v>D:/ntnl_li_2018_template/data/study_region/townsville/townsville_20181001.osm</v>
       </c>
       <c r="L23" s="82" t="s">
         <v>879</v>
@@ -6193,9 +6193,9 @@
         <v>465</v>
       </c>
       <c r="J24" s="79"/>
-      <c r="K24" s="79" t="str">
-        <f t="shared" si="0"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/wollongong_20181001.osm</v>
+      <c r="K24" s="82" t="str">
+        <f t="shared" si="1"/>
+        <v>D:/ntnl_li_2018_template/data/study_region/wollongong/wollongong_20181001.osm</v>
       </c>
       <c r="L24" s="79" t="s">
         <v>879</v>
@@ -6234,8 +6234,8 @@
         <v>456</v>
       </c>
       <c r="K25" s="82" t="str">
-        <f t="shared" si="0"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/western_sydney_20181001.osm</v>
+        <f t="shared" si="1"/>
+        <v>D:/ntnl_li_2018_template/data/study_region/western_sydney/western_sydney_20181001.osm</v>
       </c>
       <c r="L25" s="82" t="s">
         <v>879</v>

</xml_diff>

<commit_message>
updated config for correct processing of parcel dwellings
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DDBAA2-254A-4D9B-8532-A2394B6E6051}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97598ED4-D87B-4D05-807E-1E9CCBDCEC7E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="3" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2064" uniqueCount="932">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2064" uniqueCount="934">
   <si>
     <t>Domain</t>
   </si>
@@ -1798,9 +1798,6 @@
     <t>destinations/pos_includedareas_2018.gdb/melb_included_400m_2018</t>
   </si>
   <si>
-    <t>[address_points/GDA2020_GA_LCC.gdb/gnaf_2018_nsw,address_points/GDA2020_GA_LCC.gdb/gnaf_2018_vic ]</t>
-  </si>
-  <si>
     <t xml:space="preserve">"STATE_NAME" = 'Australian Capital Territory' AND "GCCSA_NAME"  = 'Australian Capital Territory' </t>
   </si>
   <si>
@@ -2923,6 +2920,15 @@
   </si>
   <si>
     <t>osm_10km_WesternSydney_10km_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">address_points/GDA2020_GA_LCC.gdb/gnaf_2018_nsw,address_points/GDA2020_GA_LCC.gdb/gnaf_2018_vic </t>
+  </si>
+  <si>
+    <t>QLD_NSW</t>
+  </si>
+  <si>
+    <t>address_points/GDA2020_GA_LCC.gdb/gnaf_2018_nsw,address_points/GDA2020_GA_LCC.gdb/gnaf_2018_qld</t>
   </si>
 </sst>
 </file>
@@ -4008,12 +4014,12 @@
   <sheetData>
     <row r="1" spans="1:1" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="2" spans="1:1" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="3" spans="1:1" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4021,27 +4027,27 @@
     </row>
     <row r="4" spans="1:1" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="5" spans="1:1" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="8" spans="1:1" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
   </sheetData>
@@ -4068,12 +4074,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B3" s="34" t="s">
         <v>472</v>
@@ -4082,24 +4088,24 @@
         <v>473</v>
       </c>
       <c r="D3" s="56" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B4" s="55"/>
       <c r="C4" s="85"/>
       <c r="D4" s="87" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="91"/>
       <c r="B5" s="92"/>
       <c r="C5" s="52" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D5" s="86"/>
     </row>
@@ -4107,18 +4113,18 @@
       <c r="A6" s="89"/>
       <c r="B6" s="90"/>
       <c r="C6" s="93" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="D6" s="88"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B7" s="49"/>
       <c r="C7" s="58"/>
       <c r="D7" s="63" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -4151,16 +4157,16 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="35"/>
       <c r="B11" s="50" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C11" s="58" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="35"/>
       <c r="B12" s="50" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="C12" s="58" t="s">
         <v>475</v>
@@ -4169,7 +4175,7 @@
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="35"/>
       <c r="B13" s="49" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C13" s="58" t="s">
         <v>471</v>
@@ -4178,7 +4184,7 @@
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="35"/>
       <c r="B14" s="49" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C14" s="58" t="s">
         <v>476</v>
@@ -4187,28 +4193,28 @@
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
       <c r="B15" s="49" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="C15" s="58" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="35"/>
       <c r="B16" s="49" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C16" s="58" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="35"/>
       <c r="B17" s="49" t="s">
+        <v>915</v>
+      </c>
+      <c r="C17" s="58" t="s">
         <v>916</v>
-      </c>
-      <c r="C17" s="58" t="s">
-        <v>917</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4223,7 +4229,7 @@
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="35"/>
       <c r="B19" s="60" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C19" s="58" t="s">
         <v>477</v>
@@ -4232,19 +4238,19 @@
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
       <c r="B20" s="60" t="s">
+        <v>692</v>
+      </c>
+      <c r="C20" s="58" t="s">
         <v>693</v>
-      </c>
-      <c r="C20" s="58" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="35"/>
       <c r="B21" s="60" t="s">
+        <v>830</v>
+      </c>
+      <c r="C21" s="58" t="s">
         <v>831</v>
-      </c>
-      <c r="C21" s="58" t="s">
-        <v>832</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -4262,67 +4268,67 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="59" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B24" s="35"/>
       <c r="C24" s="58"/>
       <c r="D24" s="60" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="60" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="35"/>
       <c r="B26" s="60" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="35"/>
       <c r="B27" s="60" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C27" s="58" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="35"/>
       <c r="B28" s="60" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C28" s="58" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="47"/>
       <c r="B29" s="61" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C29" s="68" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D29" s="61"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="62" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B30" s="60"/>
       <c r="C30" s="58"/>
       <c r="D30" s="60" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -4389,10 +4395,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="62" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="D41" s="63" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -4400,7 +4406,7 @@
         <v>205</v>
       </c>
       <c r="C42" s="64" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -4408,7 +4414,7 @@
         <v>204</v>
       </c>
       <c r="C43" s="64" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -4416,7 +4422,7 @@
         <v>207</v>
       </c>
       <c r="C44" s="64" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4424,7 +4430,7 @@
         <v>298</v>
       </c>
       <c r="C45" s="64" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -4432,7 +4438,7 @@
         <v>424</v>
       </c>
       <c r="C46" s="64" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -4440,7 +4446,7 @@
         <v>300</v>
       </c>
       <c r="C47" s="64" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -4448,7 +4454,7 @@
         <v>323</v>
       </c>
       <c r="C48" s="64" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
@@ -4456,7 +4462,7 @@
         <v>158</v>
       </c>
       <c r="C49" s="64" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="50" spans="2:3" ht="45" x14ac:dyDescent="0.25">
@@ -4464,7 +4470,7 @@
         <v>208</v>
       </c>
       <c r="C50" s="64" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="45" x14ac:dyDescent="0.25">
@@ -4472,7 +4478,7 @@
         <v>209</v>
       </c>
       <c r="C51" s="64" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="52" spans="2:3" ht="75" x14ac:dyDescent="0.25">
@@ -4480,7 +4486,7 @@
         <v>273</v>
       </c>
       <c r="C52" s="64" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="53" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -4488,7 +4494,7 @@
         <v>272</v>
       </c>
       <c r="C53" s="64" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="54" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -4496,7 +4502,7 @@
         <v>278</v>
       </c>
       <c r="C54" s="64" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="55" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
@@ -4504,7 +4510,7 @@
         <v>321</v>
       </c>
       <c r="C55" s="64" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="56" spans="2:3" ht="45" x14ac:dyDescent="0.25">
@@ -4512,7 +4518,7 @@
         <v>316</v>
       </c>
       <c r="C56" s="64" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
   </sheetData>
@@ -4527,85 +4533,85 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" style="69" customWidth="1"/>
+    <col min="2" max="2" width="67.42578125" style="69" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" style="38" customWidth="1"/>
     <col min="4" max="4" width="54.5703125" style="38" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="94" t="s">
+        <v>687</v>
+      </c>
+      <c r="B1" s="95" t="s">
         <v>688</v>
       </c>
-      <c r="B1" s="95" t="s">
-        <v>689</v>
-      </c>
       <c r="C1" s="101" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D1" s="101" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>689</v>
+      </c>
+      <c r="B2" s="69" t="s">
         <v>690</v>
       </c>
-      <c r="B2" s="69" t="s">
-        <v>691</v>
-      </c>
       <c r="C2" s="38" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B3" s="69">
         <v>2016</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B4" s="69" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B5" s="69">
         <v>7845</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4613,584 +4619,584 @@
         <v>321</v>
       </c>
       <c r="B6" s="69" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>703</v>
+      </c>
+      <c r="B7" s="69" t="s">
         <v>704</v>
       </c>
-      <c r="B7" s="69" t="s">
-        <v>705</v>
-      </c>
       <c r="C7" s="38" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B8" s="69">
         <v>10000</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B9" s="69">
         <v>3000</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B10" s="69">
         <v>3000</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>716</v>
+      </c>
+      <c r="B11" s="69" t="s">
         <v>717</v>
       </c>
-      <c r="B11" s="69" t="s">
-        <v>718</v>
-      </c>
       <c r="C11" s="38" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B12" s="69" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B13" s="69">
         <v>5432</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B14" s="69" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C14" s="38" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B15" s="69" t="s">
+        <v>741</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>797</v>
+      </c>
+      <c r="D15" s="38" t="s">
         <v>742</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>798</v>
-      </c>
-      <c r="D15" s="38" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>745</v>
+      </c>
+      <c r="B16" s="69" t="s">
         <v>746</v>
       </c>
-      <c r="B16" s="69" t="s">
-        <v>747</v>
-      </c>
       <c r="C16" s="38" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B17" s="69" t="s">
+        <v>875</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>797</v>
+      </c>
+      <c r="D17" s="38" t="s">
         <v>876</v>
-      </c>
-      <c r="C17" s="38" t="s">
-        <v>798</v>
-      </c>
-      <c r="D17" s="38" t="s">
-        <v>877</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>872</v>
+      </c>
+      <c r="B18" s="69" t="s">
         <v>873</v>
       </c>
-      <c r="B18" s="69" t="s">
+      <c r="C18" s="38" t="s">
+        <v>797</v>
+      </c>
+      <c r="D18" s="38" t="s">
         <v>874</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>798</v>
-      </c>
-      <c r="D18" s="38" t="s">
-        <v>875</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B19" s="69" t="s">
+        <v>718</v>
+      </c>
+      <c r="C19" s="38" t="s">
+        <v>798</v>
+      </c>
+      <c r="D19" s="38" t="s">
         <v>719</v>
-      </c>
-      <c r="C19" s="38" t="s">
-        <v>799</v>
-      </c>
-      <c r="D19" s="38" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>722</v>
+      </c>
+      <c r="B20" s="69" t="s">
         <v>723</v>
       </c>
-      <c r="B20" s="69" t="s">
+      <c r="C20" s="38" t="s">
+        <v>798</v>
+      </c>
+      <c r="D20" s="38" t="s">
         <v>724</v>
-      </c>
-      <c r="C20" s="38" t="s">
-        <v>799</v>
-      </c>
-      <c r="D20" s="38" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>725</v>
+      </c>
+      <c r="B21" s="69" t="s">
         <v>726</v>
       </c>
-      <c r="B21" s="69" t="s">
+      <c r="C21" s="38" t="s">
+        <v>799</v>
+      </c>
+      <c r="D21" s="38" t="s">
         <v>727</v>
-      </c>
-      <c r="C21" s="38" t="s">
-        <v>800</v>
-      </c>
-      <c r="D21" s="38" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B22" s="69" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B23" s="69" t="s">
+        <v>731</v>
+      </c>
+      <c r="C23" s="38" t="s">
+        <v>799</v>
+      </c>
+      <c r="D23" s="38" t="s">
         <v>732</v>
-      </c>
-      <c r="C23" s="38" t="s">
-        <v>800</v>
-      </c>
-      <c r="D23" s="38" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>733</v>
+      </c>
+      <c r="B24" s="69" t="s">
+        <v>735</v>
+      </c>
+      <c r="C24" s="38" t="s">
+        <v>799</v>
+      </c>
+      <c r="D24" s="38" t="s">
         <v>734</v>
-      </c>
-      <c r="B24" s="69" t="s">
-        <v>736</v>
-      </c>
-      <c r="C24" s="38" t="s">
-        <v>800</v>
-      </c>
-      <c r="D24" s="38" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>747</v>
+      </c>
+      <c r="B25" s="69" t="s">
         <v>748</v>
       </c>
-      <c r="B25" s="69" t="s">
-        <v>749</v>
-      </c>
       <c r="C25" s="38" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>749</v>
+      </c>
+      <c r="B26" s="69" t="s">
         <v>750</v>
       </c>
-      <c r="B26" s="69" t="s">
-        <v>751</v>
-      </c>
       <c r="C26" s="38" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>751</v>
+      </c>
+      <c r="B27" s="69" t="s">
         <v>752</v>
       </c>
-      <c r="B27" s="69" t="s">
-        <v>753</v>
-      </c>
       <c r="C27" s="38" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B28" s="69" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B29" s="69" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D29" s="38" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B30" s="69" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B31" s="69" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C31" s="38" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B32" s="69" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C32" s="38" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B33" s="69" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C33" s="38" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B34" s="69" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C34" s="38" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B35" s="69" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B36" s="69" t="s">
         <v>567</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B37" s="69" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C37" s="38" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="B38" s="69" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C38" s="38" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B39" s="69" t="s">
+        <v>803</v>
+      </c>
+      <c r="C39" s="38" t="s">
+        <v>801</v>
+      </c>
+      <c r="D39" s="38" t="s">
         <v>804</v>
-      </c>
-      <c r="C39" s="38" t="s">
-        <v>802</v>
-      </c>
-      <c r="D39" s="38" t="s">
-        <v>805</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B40" s="69">
         <v>7844</v>
       </c>
       <c r="C40" s="38" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>806</v>
+      </c>
+      <c r="B41" s="69" t="s">
         <v>807</v>
       </c>
-      <c r="B41" s="69" t="s">
+      <c r="C41" s="38" t="s">
+        <v>807</v>
+      </c>
+      <c r="D41" s="38" t="s">
         <v>808</v>
-      </c>
-      <c r="C41" s="38" t="s">
-        <v>808</v>
-      </c>
-      <c r="D41" s="38" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B42" s="69" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C42" s="38" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B43" s="69" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="C43" s="38" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B44" s="69" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C44" s="38" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>816</v>
+      </c>
+      <c r="B45" s="69" t="s">
         <v>817</v>
       </c>
-      <c r="B45" s="69" t="s">
+      <c r="C45" s="38" t="s">
+        <v>807</v>
+      </c>
+      <c r="D45" s="38" t="s">
         <v>818</v>
-      </c>
-      <c r="C45" s="38" t="s">
-        <v>808</v>
-      </c>
-      <c r="D45" s="38" t="s">
-        <v>819</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B46" s="69" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C46" s="38" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D46" s="38" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B47" s="69" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C47" s="38" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D47" s="38" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -5201,164 +5207,164 @@
         <v>1600</v>
       </c>
       <c r="C48" s="38" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D48" s="38" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B49" s="69">
         <v>500</v>
       </c>
       <c r="C49" s="38" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D49" s="38" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B50" s="69">
         <v>50</v>
       </c>
       <c r="C50" s="38" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B51" s="69">
         <v>3000</v>
       </c>
       <c r="C51" s="38" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D51" s="38" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B52" s="69">
         <v>3200</v>
       </c>
       <c r="C52" s="38" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D52" s="38" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="B53" s="69">
         <v>5</v>
       </c>
       <c r="C53" s="38" t="s">
+        <v>832</v>
+      </c>
+      <c r="D53" s="38" t="s">
         <v>833</v>
-      </c>
-      <c r="D53" s="38" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B54" s="69">
         <v>50</v>
       </c>
       <c r="C54" s="38" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="D54" s="38" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>842</v>
+      </c>
+      <c r="B55" s="69" t="s">
+        <v>658</v>
+      </c>
+      <c r="C55" s="38" t="s">
+        <v>658</v>
+      </c>
+      <c r="D55" s="38" t="s">
         <v>843</v>
-      </c>
-      <c r="B55" s="69" t="s">
-        <v>659</v>
-      </c>
-      <c r="C55" s="38" t="s">
-        <v>659</v>
-      </c>
-      <c r="D55" s="38" t="s">
-        <v>844</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>844</v>
+      </c>
+      <c r="B56" s="69" t="s">
         <v>845</v>
       </c>
-      <c r="B56" s="69" t="s">
+      <c r="C56" s="38" t="s">
+        <v>658</v>
+      </c>
+      <c r="D56" s="38" t="s">
         <v>846</v>
-      </c>
-      <c r="C56" s="38" t="s">
-        <v>659</v>
-      </c>
-      <c r="D56" s="38" t="s">
-        <v>847</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B57" s="69" t="s">
+        <v>849</v>
+      </c>
+      <c r="C57" s="38" t="s">
+        <v>658</v>
+      </c>
+      <c r="D57" s="38" t="s">
         <v>850</v>
-      </c>
-      <c r="C57" s="38" t="s">
-        <v>659</v>
-      </c>
-      <c r="D57" s="38" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B58" s="69" t="b">
         <v>0</v>
       </c>
       <c r="C58" s="38" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D58" s="38" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>852</v>
+      </c>
+      <c r="B59" s="69" t="s">
+        <v>854</v>
+      </c>
+      <c r="C59" s="38" t="s">
+        <v>658</v>
+      </c>
+      <c r="D59" s="38" t="s">
         <v>853</v>
-      </c>
-      <c r="B59" s="69" t="s">
-        <v>855</v>
-      </c>
-      <c r="C59" s="38" t="s">
-        <v>659</v>
-      </c>
-      <c r="D59" s="38" t="s">
-        <v>854</v>
       </c>
     </row>
   </sheetData>
@@ -5371,10 +5377,10 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J24" sqref="J24"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5382,9 +5388,9 @@
     <col min="1" max="1" width="24" style="36" customWidth="1"/>
     <col min="2" max="2" width="36.140625" style="32" customWidth="1"/>
     <col min="3" max="4" width="20.140625" style="32" customWidth="1"/>
-    <col min="5" max="5" width="86.140625" style="33" customWidth="1"/>
+    <col min="5" max="5" width="99.140625" style="33" customWidth="1"/>
     <col min="6" max="6" width="91.140625" style="32" customWidth="1"/>
-    <col min="7" max="7" width="51.42578125" style="32" customWidth="1"/>
+    <col min="7" max="7" width="90.42578125" style="32" customWidth="1"/>
     <col min="8" max="10" width="41.140625" style="32" customWidth="1"/>
     <col min="11" max="11" width="51.42578125" style="32" customWidth="1"/>
     <col min="12" max="12" width="40.85546875" style="32" customWidth="1"/>
@@ -5404,60 +5410,60 @@
         <v>428</v>
       </c>
       <c r="D1" s="71" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E1" s="72" t="s">
+        <v>757</v>
+      </c>
+      <c r="F1" s="72" t="s">
+        <v>759</v>
+      </c>
+      <c r="G1" s="71" t="s">
         <v>758</v>
       </c>
-      <c r="F1" s="72" t="s">
-        <v>760</v>
-      </c>
-      <c r="G1" s="71" t="s">
-        <v>759</v>
-      </c>
       <c r="H1" s="71" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="I1" s="71" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="J1" s="71" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="K1" s="71" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="L1" s="71" t="s">
         <v>429</v>
       </c>
       <c r="M1" s="71" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="N1" s="73" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="O1" s="73" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="74" t="s">
+        <v>753</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>753</v>
+      </c>
+      <c r="C2" s="75" t="s">
         <v>754</v>
       </c>
-      <c r="B2" s="75" t="s">
-        <v>754</v>
-      </c>
-      <c r="C2" s="75" t="s">
+      <c r="D2" s="75" t="s">
         <v>755</v>
-      </c>
-      <c r="D2" s="75" t="s">
-        <v>756</v>
       </c>
       <c r="E2" s="76" t="s">
         <v>433</v>
       </c>
       <c r="F2" s="76" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="G2" s="75" t="s">
         <v>434</v>
@@ -5467,20 +5473,20 @@
         <v>D:/ntnl_li_2018_template/data/study_region/testing/testing_gccstest_2016_10000m_20181001.osm</v>
       </c>
       <c r="I2" s="75" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J2" s="75" t="str">
         <f>"osm_10km_"&amp;B2&amp;"_10km_pedestrian_"&amp;RIGHT(I2,8)</f>
         <v>osm_10km_testing_10km_pedestrian_20181001</v>
       </c>
       <c r="K2" s="75" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="L2" s="76" t="s">
         <v>439</v>
       </c>
       <c r="M2" s="75" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="N2" s="77"/>
       <c r="O2" s="77">
@@ -5492,13 +5498,13 @@
         <v>430</v>
       </c>
       <c r="B3" s="75" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C3" s="75" t="s">
         <v>431</v>
       </c>
       <c r="D3" s="75" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E3" s="76" t="s">
         <v>433</v>
@@ -5514,10 +5520,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/adelaide/adelaide_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="I3" s="75" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J3" s="75" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="K3" s="75"/>
       <c r="L3" s="75"/>
@@ -5532,13 +5538,13 @@
         <v>435</v>
       </c>
       <c r="B4" s="79" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C4" s="79" t="s">
         <v>436</v>
       </c>
       <c r="D4" s="79" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E4" s="80" t="s">
         <v>433</v>
@@ -5554,13 +5560,13 @@
         <v>D:/ntnl_li_2018_template/data/study_region/bris/bris_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="I4" s="79" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J4" s="79" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="K4" s="79" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="L4" s="80" t="s">
         <v>439</v>
@@ -5575,19 +5581,19 @@
         <v>440</v>
       </c>
       <c r="B5" s="82" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C5" s="82" t="s">
         <v>441</v>
       </c>
       <c r="D5" s="82" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E5" s="83" t="s">
         <v>433</v>
       </c>
       <c r="F5" s="83" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="G5" s="82" t="s">
         <v>442</v>
@@ -5597,10 +5603,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/canberra/canberra_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="I5" s="82" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J5" s="82" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="K5" s="82"/>
       <c r="L5" s="82"/>
@@ -5615,13 +5621,13 @@
         <v>443</v>
       </c>
       <c r="B6" s="79" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C6" s="79" t="s">
         <v>444</v>
       </c>
       <c r="D6" s="79" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E6" s="80" t="s">
         <v>433</v>
@@ -5637,10 +5643,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/darwin/darwin_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="I6" s="79" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J6" s="79" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="K6" s="79"/>
       <c r="L6" s="79"/>
@@ -5654,13 +5660,13 @@
         <v>447</v>
       </c>
       <c r="B7" s="82" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C7" s="82" t="s">
         <v>448</v>
       </c>
       <c r="D7" s="82" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E7" s="83" t="s">
         <v>433</v>
@@ -5676,10 +5682,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/hobart/hobart_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="I7" s="82" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J7" s="82" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="K7" s="82"/>
       <c r="L7" s="82"/>
@@ -5694,13 +5700,13 @@
         <v>451</v>
       </c>
       <c r="B8" s="79" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C8" s="79" t="s">
         <v>452</v>
       </c>
       <c r="D8" s="79" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E8" s="80" t="s">
         <v>433</v>
@@ -5716,13 +5722,13 @@
         <v>D:/ntnl_li_2018_template/data/study_region/melb/melb_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="I8" s="79" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J8" s="79" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="K8" s="79" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="L8" s="80" t="s">
         <v>455</v>
@@ -5739,13 +5745,13 @@
         <v>44</v>
       </c>
       <c r="B9" s="82" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C9" s="82" t="s">
         <v>457</v>
       </c>
       <c r="D9" s="82" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E9" s="83" t="s">
         <v>433</v>
@@ -5761,13 +5767,13 @@
         <v>D:/ntnl_li_2018_template/data/study_region/perth/perth_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="I9" s="82" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J9" s="82" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="K9" s="82" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="L9" s="83" t="s">
         <v>460</v>
@@ -5783,13 +5789,13 @@
         <v>461</v>
       </c>
       <c r="B10" s="79" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C10" s="79" t="s">
         <v>462</v>
       </c>
       <c r="D10" s="79" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E10" s="80" t="s">
         <v>433</v>
@@ -5805,13 +5811,13 @@
         <v>D:/ntnl_li_2018_template/data/study_region/syd/syd_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="I10" s="79" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J10" s="79" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="K10" s="79" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="L10" s="80" t="s">
         <v>465</v>
@@ -5828,13 +5834,13 @@
         <v>466</v>
       </c>
       <c r="B11" s="82" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C11" s="82" t="s">
         <v>452</v>
       </c>
       <c r="D11" s="82" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E11" s="83" t="s">
         <v>567</v>
@@ -5850,10 +5856,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/mitchell/mitchell_lga_2016_10000m_20181001.osm</v>
       </c>
       <c r="I11" s="82" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J11" s="82" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="K11" s="82"/>
       <c r="L11" s="82"/>
@@ -5868,32 +5874,32 @@
         <v>552</v>
       </c>
       <c r="B12" s="79" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="C12" s="79" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D12" s="79" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E12" s="80" t="s">
+        <v>887</v>
+      </c>
+      <c r="F12" s="103" t="s">
         <v>888</v>
       </c>
-      <c r="F12" s="103" t="s">
-        <v>889</v>
-      </c>
       <c r="G12" s="102" t="s">
-        <v>569</v>
+        <v>931</v>
       </c>
       <c r="H12" s="79" t="str">
         <f t="shared" ref="H12:H25" si="1">"D:/ntnl_li_2018_template/data/study_region/"&amp;B12&amp;"/"&amp;B12&amp;"_20181001.osm"</f>
         <v>D:/ntnl_li_2018_template/data/study_region/albury_wodonga/albury_wodonga_20181001.osm</v>
       </c>
       <c r="I12" s="79" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J12" s="82" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="K12" s="84"/>
       <c r="L12" s="80" t="s">
@@ -5909,19 +5915,19 @@
         <v>553</v>
       </c>
       <c r="B13" s="82" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C13" s="82" t="s">
         <v>452</v>
       </c>
       <c r="D13" s="82" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E13" s="83" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="F13" s="83" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="G13" s="82" t="s">
         <v>454</v>
@@ -5931,10 +5937,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/ballarat/ballarat_20181001.osm</v>
       </c>
       <c r="I13" s="82" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J13" s="82" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="K13" s="82"/>
       <c r="L13" s="83" t="s">
@@ -5951,19 +5957,19 @@
         <v>554</v>
       </c>
       <c r="B14" s="79" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C14" s="79" t="s">
         <v>452</v>
       </c>
       <c r="D14" s="79" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E14" s="80" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="F14" s="79" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="G14" s="79" t="s">
         <v>454</v>
@@ -5973,10 +5979,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/bendigo/bendigo_20181001.osm</v>
       </c>
       <c r="I14" s="79" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J14" s="82" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="K14" s="79"/>
       <c r="L14" s="80" t="s">
@@ -5992,19 +5998,19 @@
         <v>555</v>
       </c>
       <c r="B15" s="82" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C15" s="82" t="s">
         <v>436</v>
       </c>
       <c r="D15" s="82" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E15" s="83" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="F15" s="82" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="G15" s="82" t="s">
         <v>438</v>
@@ -6014,10 +6020,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/cairns/cairns_20181001.osm</v>
       </c>
       <c r="I15" s="82" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J15" s="82" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="K15" s="82"/>
       <c r="L15" s="83" t="s">
@@ -6034,19 +6040,19 @@
         <v>556</v>
       </c>
       <c r="B16" s="79" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C16" s="79" t="s">
         <v>452</v>
       </c>
       <c r="D16" s="79" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E16" s="80" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="F16" s="80" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="G16" s="79" t="s">
         <v>454</v>
@@ -6056,10 +6062,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/geelong/geelong_20181001.osm</v>
       </c>
       <c r="I16" s="79" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J16" s="82" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="K16" s="79"/>
       <c r="L16" s="80" t="s">
@@ -6075,32 +6081,32 @@
         <v>557</v>
       </c>
       <c r="B17" s="82" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C17" s="82" t="s">
-        <v>436</v>
+        <v>932</v>
       </c>
       <c r="D17" s="82" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E17" s="83" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="F17" s="82" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="G17" s="82" t="s">
-        <v>438</v>
+        <v>933</v>
       </c>
       <c r="H17" s="82" t="str">
         <f t="shared" si="1"/>
         <v>D:/ntnl_li_2018_template/data/study_region/goldcoast_tweedheads/goldcoast_tweedheads_20181001.osm</v>
       </c>
       <c r="I17" s="82" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J17" s="82" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="K17" s="82"/>
       <c r="L17" s="83" t="s">
@@ -6117,19 +6123,19 @@
         <v>558</v>
       </c>
       <c r="B18" s="79" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C18" s="79" t="s">
         <v>448</v>
       </c>
       <c r="D18" s="79" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E18" s="80" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="F18" s="79" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="G18" s="79" t="s">
         <v>450</v>
@@ -6139,10 +6145,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/launceston/launceston_20181001.osm</v>
       </c>
       <c r="I18" s="79" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J18" s="82" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="K18" s="79"/>
       <c r="L18" s="79" t="s">
@@ -6158,19 +6164,19 @@
         <v>559</v>
       </c>
       <c r="B19" s="82" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C19" s="82" t="s">
         <v>436</v>
       </c>
       <c r="D19" s="82" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E19" s="83" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="F19" s="82" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="G19" s="82" t="s">
         <v>438</v>
@@ -6180,10 +6186,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/mackay/mackay_20181001.osm</v>
       </c>
       <c r="I19" s="82" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J19" s="82" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="K19" s="82"/>
       <c r="L19" s="83" t="s">
@@ -6200,19 +6206,19 @@
         <v>560</v>
       </c>
       <c r="B20" s="79" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="C20" s="79" t="s">
         <v>462</v>
       </c>
       <c r="D20" s="79" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E20" s="80" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="F20" s="79" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G20" s="79" t="s">
         <v>464</v>
@@ -6222,10 +6228,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/newcastle_maitland/newcastle_maitland_20181001.osm</v>
       </c>
       <c r="I20" s="79" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J20" s="82" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="K20" s="79"/>
       <c r="L20" s="80" t="s">
@@ -6241,19 +6247,19 @@
         <v>561</v>
       </c>
       <c r="B21" s="82" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="C21" s="82" t="s">
         <v>436</v>
       </c>
       <c r="D21" s="82" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E21" s="83" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="F21" s="82" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G21" s="82" t="s">
         <v>438</v>
@@ -6263,10 +6269,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/sunshine_coast/sunshine_coast_20181001.osm</v>
       </c>
       <c r="I21" s="82" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J21" s="82" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="K21" s="82"/>
       <c r="L21" s="83" t="s">
@@ -6283,19 +6289,19 @@
         <v>562</v>
       </c>
       <c r="B22" s="79" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C22" s="79" t="s">
         <v>436</v>
       </c>
       <c r="D22" s="79" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E22" s="80" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="F22" s="79" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="G22" s="79" t="s">
         <v>438</v>
@@ -6305,10 +6311,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/toowoomba/toowoomba_20181001.osm</v>
       </c>
       <c r="I22" s="79" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J22" s="82" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="K22" s="79"/>
       <c r="L22" s="80" t="s">
@@ -6324,19 +6330,19 @@
         <v>563</v>
       </c>
       <c r="B23" s="82" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C23" s="82" t="s">
         <v>436</v>
       </c>
       <c r="D23" s="82" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E23" s="83" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="F23" s="82" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="G23" s="82" t="s">
         <v>438</v>
@@ -6346,10 +6352,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/townsville/townsville_20181001.osm</v>
       </c>
       <c r="I23" s="82" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J23" s="82" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="K23" s="82"/>
       <c r="L23" s="83" t="s">
@@ -6366,19 +6372,19 @@
         <v>564</v>
       </c>
       <c r="B24" s="79" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C24" s="79" t="s">
         <v>462</v>
       </c>
       <c r="D24" s="79" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E24" s="80" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="F24" s="79" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="G24" s="79" t="s">
         <v>464</v>
@@ -6388,10 +6394,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/wollongong/wollongong_20181001.osm</v>
       </c>
       <c r="I24" s="79" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J24" s="82" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="K24" s="79"/>
       <c r="L24" s="80" t="s">
@@ -6407,19 +6413,19 @@
         <v>566</v>
       </c>
       <c r="B25" s="82" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C25" s="82" t="s">
         <v>462</v>
       </c>
       <c r="D25" s="82" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E25" s="83" t="s">
         <v>567</v>
       </c>
       <c r="F25" s="84" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="G25" s="83" t="s">
         <v>567</v>
@@ -6429,10 +6435,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/western_sydney/western_sydney_20181001.osm</v>
       </c>
       <c r="I25" s="82" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J25" s="82" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="K25" s="83"/>
       <c r="L25" s="83" t="s">
@@ -6469,19 +6475,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
+        <v>596</v>
+      </c>
+      <c r="B1" s="37" t="s">
         <v>597</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="C1" s="37" t="s">
         <v>598</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="D1" s="39" t="s">
         <v>599</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="E1" s="39" t="s">
         <v>600</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -6489,7 +6495,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C2" t="s">
         <v>151</v>
@@ -6503,7 +6509,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C3" t="s">
         <v>151</v>
@@ -6517,7 +6523,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C4" t="s">
         <v>151</v>
@@ -6531,7 +6537,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C5" t="s">
         <v>151</v>
@@ -6545,7 +6551,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C6" t="s">
         <v>151</v>
@@ -6559,7 +6565,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C7" t="s">
         <v>151</v>
@@ -6573,7 +6579,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C8" t="s">
         <v>151</v>
@@ -6587,7 +6593,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C9" t="s">
         <v>151</v>
@@ -6601,10 +6607,10 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
+        <v>609</v>
+      </c>
+      <c r="C10" t="s">
         <v>610</v>
-      </c>
-      <c r="C10" t="s">
-        <v>611</v>
       </c>
       <c r="D10">
         <v>1600</v>
@@ -6615,10 +6621,10 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C11" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D11">
         <v>1600</v>
@@ -6629,10 +6635,10 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C12" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D12">
         <v>1600</v>
@@ -6643,7 +6649,7 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C13" t="s">
         <v>144</v>
@@ -6657,7 +6663,7 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C14" t="s">
         <v>144</v>
@@ -6674,7 +6680,7 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C15" t="s">
         <v>76</v>
@@ -6688,7 +6694,7 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C16" t="s">
         <v>76</v>
@@ -6702,7 +6708,7 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C17" t="s">
         <v>76</v>
@@ -6716,7 +6722,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C18" t="s">
         <v>76</v>
@@ -6730,7 +6736,7 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C19" t="s">
         <v>76</v>
@@ -6744,7 +6750,7 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C20" t="s">
         <v>76</v>
@@ -6758,7 +6764,7 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C21" t="s">
         <v>76</v>
@@ -6772,7 +6778,7 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C22" t="s">
         <v>76</v>
@@ -6786,7 +6792,7 @@
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C23" t="s">
         <v>76</v>
@@ -6800,7 +6806,7 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C24" t="s">
         <v>76</v>
@@ -6814,7 +6820,7 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C25" t="s">
         <v>76</v>
@@ -6828,7 +6834,7 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C26" t="s">
         <v>76</v>
@@ -6842,7 +6848,7 @@
         <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C27" t="s">
         <v>76</v>
@@ -6856,7 +6862,7 @@
         <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C28" t="s">
         <v>76</v>
@@ -6870,7 +6876,7 @@
         <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C29" t="s">
         <v>76</v>
@@ -6884,7 +6890,7 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C30" t="s">
         <v>76</v>
@@ -6898,7 +6904,7 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C31" t="s">
         <v>76</v>
@@ -6912,7 +6918,7 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C32" t="s">
         <v>76</v>
@@ -6926,7 +6932,7 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C33" t="s">
         <v>76</v>
@@ -6940,7 +6946,7 @@
         <v>14</v>
       </c>
       <c r="B34" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C34" t="s">
         <v>76</v>
@@ -6954,7 +6960,7 @@
         <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C35" t="s">
         <v>76</v>
@@ -6968,7 +6974,7 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C36" t="s">
         <v>76</v>
@@ -6982,7 +6988,7 @@
         <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C37" t="s">
         <v>76</v>
@@ -6996,7 +7002,7 @@
         <v>100</v>
       </c>
       <c r="B38" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C38" t="s">
         <v>16</v>
@@ -7010,7 +7016,7 @@
         <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C39" t="s">
         <v>144</v>
@@ -7024,7 +7030,7 @@
         <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C40" t="s">
         <v>144</v>
@@ -7038,7 +7044,7 @@
         <v>16</v>
       </c>
       <c r="B41" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C41" t="s">
         <v>144</v>
@@ -7052,7 +7058,7 @@
         <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C42" t="s">
         <v>144</v>
@@ -7066,7 +7072,7 @@
         <v>18</v>
       </c>
       <c r="B43" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C43" t="s">
         <v>144</v>
@@ -7080,7 +7086,7 @@
         <v>19</v>
       </c>
       <c r="B44" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C44" t="s">
         <v>144</v>
@@ -7094,7 +7100,7 @@
         <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C45" t="s">
         <v>144</v>
@@ -7108,7 +7114,7 @@
         <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C46" t="s">
         <v>16</v>
@@ -7122,7 +7128,7 @@
         <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C47" t="s">
         <v>16</v>
@@ -7136,7 +7142,7 @@
         <v>22</v>
       </c>
       <c r="B48" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C48" t="s">
         <v>16</v>
@@ -7150,10 +7156,10 @@
         <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C49" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D49">
         <v>1600</v>
@@ -7164,10 +7170,10 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C50" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D50">
         <v>1600</v>
@@ -7178,10 +7184,10 @@
         <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C51" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D51">
         <v>1600</v>
@@ -9464,7 +9470,7 @@
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="98" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D2" s="42" t="s">
         <v>416</v>
@@ -9502,7 +9508,7 @@
         <v>203</v>
       </c>
       <c r="C3" s="98" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D3" s="43" t="s">
         <v>324</v>
@@ -9549,7 +9555,7 @@
         <v>206</v>
       </c>
       <c r="C4" s="98" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D4" s="43" t="s">
         <v>324</v>
@@ -9594,7 +9600,7 @@
       </c>
       <c r="B5" s="23"/>
       <c r="C5" s="98" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D5" s="43" t="s">
         <v>325</v>
@@ -9633,7 +9639,7 @@
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="98" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D6" s="43" t="s">
         <v>326</v>
@@ -9669,7 +9675,7 @@
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="98" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D7" s="43" t="s">
         <v>327</v>
@@ -9705,7 +9711,7 @@
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="98" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D8" s="43" t="s">
         <v>328</v>
@@ -9744,7 +9750,7 @@
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="98" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D9" s="43" t="s">
         <v>369</v>
@@ -9780,7 +9786,7 @@
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="98" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D10" s="43" t="s">
         <v>385</v>
@@ -9816,7 +9822,7 @@
       </c>
       <c r="B11" s="23"/>
       <c r="C11" s="98" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D11" s="43" t="s">
         <v>329</v>
@@ -9855,7 +9861,7 @@
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="98" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D12" s="43" t="s">
         <v>384</v>
@@ -9894,7 +9900,7 @@
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="98" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D13" s="43" t="s">
         <v>331</v>
@@ -9933,7 +9939,7 @@
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>421</v>
@@ -9975,7 +9981,7 @@
       </c>
       <c r="B15" s="23"/>
       <c r="C15" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>422</v>
@@ -10010,7 +10016,7 @@
         <v>203</v>
       </c>
       <c r="C16" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D16" s="23" t="s">
         <v>380</v>
@@ -10054,7 +10060,7 @@
         <v>206</v>
       </c>
       <c r="C17" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D17" s="23" t="s">
         <v>381</v>
@@ -10095,7 +10101,7 @@
         <v>173</v>
       </c>
       <c r="C18" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D18" s="43" t="s">
         <v>382</v>
@@ -10137,7 +10143,7 @@
       </c>
       <c r="B19" s="23"/>
       <c r="C19" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D19" s="23" t="s">
         <v>383</v>
@@ -10181,7 +10187,7 @@
         <v>203</v>
       </c>
       <c r="C20" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D20" s="23" t="s">
         <v>379</v>
@@ -10225,7 +10231,7 @@
         <v>206</v>
       </c>
       <c r="C21" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D21" s="23" t="s">
         <v>386</v>
@@ -10269,7 +10275,7 @@
         <v>203</v>
       </c>
       <c r="C22" s="98" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D22" s="43" t="s">
         <v>378</v>
@@ -10316,7 +10322,7 @@
         <v>206</v>
       </c>
       <c r="C23" s="98" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D23" s="43" t="s">
         <v>388</v>
@@ -10363,7 +10369,7 @@
         <v>203</v>
       </c>
       <c r="C24" s="98" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D24" s="43" t="s">
         <v>377</v>
@@ -10410,7 +10416,7 @@
         <v>206</v>
       </c>
       <c r="C25" s="98" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D25" s="43" t="s">
         <v>387</v>
@@ -10455,7 +10461,7 @@
       </c>
       <c r="B26" s="23"/>
       <c r="C26" s="98" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D26" s="43" t="s">
         <v>376</v>
@@ -10496,7 +10502,7 @@
         <v>203</v>
       </c>
       <c r="C27" s="98" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D27" s="43" t="s">
         <v>375</v>
@@ -10543,7 +10549,7 @@
         <v>206</v>
       </c>
       <c r="C28" s="98" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D28" s="43" t="s">
         <v>389</v>
@@ -10590,7 +10596,7 @@
         <v>203</v>
       </c>
       <c r="C29" s="98" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D29" s="43" t="s">
         <v>402</v>
@@ -10637,7 +10643,7 @@
         <v>206</v>
       </c>
       <c r="C30" s="98" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D30" s="43" t="s">
         <v>401</v>
@@ -10684,7 +10690,7 @@
         <v>203</v>
       </c>
       <c r="C31" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D31" s="43" t="s">
         <v>374</v>
@@ -10728,7 +10734,7 @@
         <v>206</v>
       </c>
       <c r="C32" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D32" s="43" t="s">
         <v>390</v>
@@ -10769,7 +10775,7 @@
         <v>516</v>
       </c>
       <c r="C33" s="98" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D33" s="44" t="s">
         <v>517</v>
@@ -10813,7 +10819,7 @@
         <v>203</v>
       </c>
       <c r="C34" s="98" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D34" s="43" t="s">
         <v>373</v>
@@ -10860,7 +10866,7 @@
         <v>206</v>
       </c>
       <c r="C35" s="98" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D35" s="43" t="s">
         <v>391</v>
@@ -10907,7 +10913,7 @@
         <v>203</v>
       </c>
       <c r="C36" s="98" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D36" s="43" t="s">
         <v>372</v>
@@ -10954,7 +10960,7 @@
         <v>206</v>
       </c>
       <c r="C37" s="98" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D37" s="43" t="s">
         <v>394</v>
@@ -11001,7 +11007,7 @@
         <v>203</v>
       </c>
       <c r="C38" s="98" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D38" s="43" t="s">
         <v>395</v>
@@ -11048,7 +11054,7 @@
         <v>206</v>
       </c>
       <c r="C39" s="98" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D39" s="43" t="s">
         <v>396</v>
@@ -11095,7 +11101,7 @@
         <v>203</v>
       </c>
       <c r="C40" s="98" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D40" s="43" t="s">
         <v>397</v>
@@ -11142,7 +11148,7 @@
         <v>206</v>
       </c>
       <c r="C41" s="98" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D41" s="43" t="s">
         <v>398</v>
@@ -11189,7 +11195,7 @@
         <v>203</v>
       </c>
       <c r="C42" s="98" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D42" s="43" t="s">
         <v>399</v>
@@ -11236,7 +11242,7 @@
         <v>206</v>
       </c>
       <c r="C43" s="98" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D43" s="43" t="s">
         <v>400</v>
@@ -11283,7 +11289,7 @@
         <v>203</v>
       </c>
       <c r="C44" s="98" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D44" s="43" t="s">
         <v>405</v>
@@ -11330,7 +11336,7 @@
         <v>206</v>
       </c>
       <c r="C45" s="98" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D45" s="43" t="s">
         <v>406</v>
@@ -11377,7 +11383,7 @@
         <v>203</v>
       </c>
       <c r="C46" s="98" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D46" s="43" t="s">
         <v>403</v>
@@ -11424,7 +11430,7 @@
         <v>206</v>
       </c>
       <c r="C47" s="98" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D47" s="43" t="s">
         <v>404</v>
@@ -11471,7 +11477,7 @@
         <v>203</v>
       </c>
       <c r="C48" s="98" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D48" s="43" t="s">
         <v>407</v>
@@ -11518,7 +11524,7 @@
         <v>206</v>
       </c>
       <c r="C49" s="98" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D49" s="43" t="s">
         <v>408</v>
@@ -11565,7 +11571,7 @@
         <v>203</v>
       </c>
       <c r="C50" s="98" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D50" s="43" t="s">
         <v>409</v>
@@ -11612,7 +11618,7 @@
         <v>206</v>
       </c>
       <c r="C51" s="98" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D51" s="43" t="s">
         <v>410</v>
@@ -11659,7 +11665,7 @@
         <v>203</v>
       </c>
       <c r="C52" s="98" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D52" s="43" t="s">
         <v>370</v>
@@ -11703,7 +11709,7 @@
         <v>206</v>
       </c>
       <c r="C53" s="98" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D53" s="43" t="s">
         <v>393</v>
@@ -11747,7 +11753,7 @@
         <v>203</v>
       </c>
       <c r="C54" s="98" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D54" s="43" t="s">
         <v>411</v>
@@ -11791,7 +11797,7 @@
         <v>206</v>
       </c>
       <c r="C55" s="98" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D55" s="43" t="s">
         <v>412</v>
@@ -11833,7 +11839,7 @@
       </c>
       <c r="B56" s="23"/>
       <c r="C56" s="98" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D56" s="43" t="s">
         <v>364</v>
@@ -11869,7 +11875,7 @@
       </c>
       <c r="B57" s="23"/>
       <c r="C57" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D57" s="43" t="s">
         <v>365</v>
@@ -11905,7 +11911,7 @@
       </c>
       <c r="B58" s="23"/>
       <c r="C58" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D58" s="43" t="s">
         <v>366</v>
@@ -11941,7 +11947,7 @@
       </c>
       <c r="B59" s="23"/>
       <c r="C59" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D59" s="43" t="s">
         <v>357</v>
@@ -11977,7 +11983,7 @@
       </c>
       <c r="B60" s="23"/>
       <c r="C60" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D60" s="43" t="s">
         <v>358</v>
@@ -12013,7 +12019,7 @@
       </c>
       <c r="B61" s="23"/>
       <c r="C61" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D61" s="43" t="s">
         <v>359</v>
@@ -12049,7 +12055,7 @@
       </c>
       <c r="B62" s="23"/>
       <c r="C62" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D62" s="43" t="s">
         <v>360</v>
@@ -12085,7 +12091,7 @@
       </c>
       <c r="B63" s="23"/>
       <c r="C63" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D63" s="43" t="s">
         <v>361</v>
@@ -12121,7 +12127,7 @@
       </c>
       <c r="B64" s="23"/>
       <c r="C64" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D64" s="43" t="s">
         <v>415</v>
@@ -12163,7 +12169,7 @@
         <v>203</v>
       </c>
       <c r="C65" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D65" s="43" t="s">
         <v>371</v>
@@ -12207,7 +12213,7 @@
         <v>206</v>
       </c>
       <c r="C66" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D66" s="43" t="s">
         <v>392</v>
@@ -12251,7 +12257,7 @@
         <v>203</v>
       </c>
       <c r="C67" s="98" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D67" s="44" t="s">
         <v>481</v>
@@ -12295,7 +12301,7 @@
         <v>206</v>
       </c>
       <c r="C68" s="98" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D68" s="44" t="s">
         <v>481</v>
@@ -12339,7 +12345,7 @@
         <v>203</v>
       </c>
       <c r="C69" s="98" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D69" s="44" t="s">
         <v>487</v>
@@ -12383,7 +12389,7 @@
         <v>206</v>
       </c>
       <c r="C70" s="98" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D70" s="44" t="s">
         <v>487</v>
@@ -12424,7 +12430,7 @@
         <v>492</v>
       </c>
       <c r="C71" s="98" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D71" s="44" t="s">
         <v>493</v>
@@ -12465,7 +12471,7 @@
         <v>496</v>
       </c>
       <c r="C72" s="98" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D72" s="44" t="s">
         <v>497</v>
@@ -12506,7 +12512,7 @@
         <v>500</v>
       </c>
       <c r="C73" s="98" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D73" s="44" t="s">
         <v>501</v>
@@ -12544,7 +12550,7 @@
         <v>505</v>
       </c>
       <c r="C74" s="98" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D74" s="44" t="s">
         <v>506</v>
@@ -12582,7 +12588,7 @@
         <v>510</v>
       </c>
       <c r="C75" s="98" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D75" s="44" t="s">
         <v>511</v>
@@ -12621,7 +12627,7 @@
       </c>
       <c r="B76" s="23"/>
       <c r="C76" s="98" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="D76" s="43" t="s">
         <v>413</v>
@@ -12661,7 +12667,7 @@
       </c>
       <c r="B77" s="23"/>
       <c r="C77" s="98" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="D77" s="43" t="s">
         <v>414</v>
@@ -12700,7 +12706,7 @@
         <v>520</v>
       </c>
       <c r="C78" s="98" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D78" s="44" t="s">
         <v>521</v>
@@ -12741,7 +12747,7 @@
         <v>524</v>
       </c>
       <c r="C79" s="98" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D79" s="44" t="s">
         <v>525</v>
@@ -12785,7 +12791,7 @@
         <v>203</v>
       </c>
       <c r="C80" s="98" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D80" s="44" t="s">
         <v>529</v>
@@ -12829,7 +12835,7 @@
         <v>206</v>
       </c>
       <c r="C81" s="98" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D81" s="44" t="s">
         <v>529</v>
@@ -12870,7 +12876,7 @@
         <v>534</v>
       </c>
       <c r="C82" s="98" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D82" s="44" t="s">
         <v>535</v>
@@ -12914,7 +12920,7 @@
         <v>203</v>
       </c>
       <c r="C83" s="98" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D83" s="44" t="s">
         <v>539</v>
@@ -12958,7 +12964,7 @@
         <v>206</v>
       </c>
       <c r="C84" s="98" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D84" s="44" t="s">
         <v>539</v>
@@ -12999,7 +13005,7 @@
         <v>544</v>
       </c>
       <c r="C85" s="98" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D85" s="44" t="s">
         <v>545</v>
@@ -13040,7 +13046,7 @@
         <v>548</v>
       </c>
       <c r="C86" s="98" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D86" s="44" t="s">
         <v>549</v>
@@ -13078,13 +13084,13 @@
     </row>
     <row r="87" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="22" t="s">
+        <v>867</v>
+      </c>
+      <c r="C87" s="99" t="s">
         <v>868</v>
       </c>
-      <c r="C87" s="99" t="s">
+      <c r="D87" s="42" t="s">
         <v>869</v>
-      </c>
-      <c r="D87" s="42" t="s">
-        <v>870</v>
       </c>
       <c r="E87" t="s">
         <v>425</v>
@@ -13093,13 +13099,13 @@
         <v>308</v>
       </c>
       <c r="G87" s="42" t="s">
+        <v>869</v>
+      </c>
+      <c r="H87" s="42" t="s">
+        <v>869</v>
+      </c>
+      <c r="K87" s="96" t="s">
         <v>870</v>
-      </c>
-      <c r="H87" s="42" t="s">
-        <v>870</v>
-      </c>
-      <c r="K87" s="96" t="s">
-        <v>871</v>
       </c>
       <c r="L87" s="22">
         <v>1</v>
@@ -13130,10 +13136,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>862</v>
+      </c>
+      <c r="B1" t="s">
         <v>863</v>
-      </c>
-      <c r="B1" t="s">
-        <v>864</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates, including fix to avoid div by zero in AOS proportion water, and correct address source for Western Sydney
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97598ED4-D87B-4D05-807E-1E9CCBDCEC7E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290980BF-C56F-4546-AEF6-E711B2382B6C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="3" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
@@ -5377,10 +5377,10 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6428,7 +6428,7 @@
         <v>570</v>
       </c>
       <c r="G25" s="83" t="s">
-        <v>567</v>
+        <v>464</v>
       </c>
       <c r="H25" s="82" t="str">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
od_aos script corrected; working again
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290980BF-C56F-4546-AEF6-E711B2382B6C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C562DD-F00C-4F81-9A53-F2ADE7FA7EE7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="3" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="1" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2064" uniqueCount="934">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2066" uniqueCount="935">
   <si>
     <t>Domain</t>
   </si>
@@ -2877,9 +2877,6 @@
     <t>network folder</t>
   </si>
   <si>
-    <t>folder in locale direc</t>
-  </si>
-  <si>
     <t>osm_10km_AlburyWodonga_10km_pedestrian_20181001</t>
   </si>
   <si>
@@ -2929,6 +2926,12 @@
   </si>
   <si>
     <t>address_points/GDA2020_GA_LCC.gdb/gnaf_2018_nsw,address_points/GDA2020_GA_LCC.gdb/gnaf_2018_qld</t>
+  </si>
+  <si>
+    <t>folder in locale directory where osmnx output road nodes and edges (wgs84 epsg4326) are located</t>
+  </si>
+  <si>
+    <t>path to source feature for public open space analysis relative to data directory</t>
   </si>
 </sst>
 </file>
@@ -4058,10 +4061,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{169A8F36-66C8-40F7-A0A8-79F453EFA097}">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4214,165 +4217,166 @@
         <v>915</v>
       </c>
       <c r="C17" s="58" t="s">
-        <v>916</v>
+        <v>933</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="35"/>
       <c r="B18" s="49" t="s">
+        <v>834</v>
+      </c>
+      <c r="C18" s="58" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="35"/>
+      <c r="B19" s="49" t="s">
         <v>429</v>
       </c>
-      <c r="C18" s="58" t="s">
+      <c r="C19" s="58" t="s">
         <v>474</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
-      <c r="B19" s="60" t="s">
-        <v>860</v>
-      </c>
-      <c r="C19" s="58" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
       <c r="B20" s="60" t="s">
-        <v>692</v>
+        <v>860</v>
       </c>
       <c r="C20" s="58" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="35"/>
       <c r="B21" s="60" t="s">
+        <v>692</v>
+      </c>
+      <c r="C21" s="58" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="35"/>
+      <c r="B22" s="60" t="s">
         <v>830</v>
       </c>
-      <c r="C21" s="58" t="s">
+      <c r="C22" s="58" t="s">
         <v>831</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="58"/>
-    </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
-      <c r="B23" s="47"/>
-      <c r="C23" s="68" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="35"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="58"/>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="47"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="68" t="s">
         <v>478</v>
       </c>
-      <c r="D23" s="61"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="59" t="s">
+      <c r="D24" s="61"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="59" t="s">
         <v>658</v>
       </c>
-      <c r="B24" s="35"/>
-      <c r="C24" s="58"/>
-      <c r="D24" s="60" t="s">
+      <c r="B25" s="35"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="60" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="60" t="s">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="60" t="s">
         <v>596</v>
       </c>
-      <c r="C25" s="58" t="s">
+      <c r="C26" s="58" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
-      <c r="B26" s="60" t="s">
-        <v>597</v>
-      </c>
-      <c r="C26" s="58" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="35"/>
       <c r="B27" s="60" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C27" s="58" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="35"/>
       <c r="B28" s="60" t="s">
+        <v>598</v>
+      </c>
+      <c r="C28" s="58" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="35"/>
+      <c r="B29" s="60" t="s">
         <v>599</v>
       </c>
-      <c r="C28" s="58" t="s">
+      <c r="C29" s="58" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
-      <c r="B29" s="61" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="47"/>
+      <c r="B30" s="61" t="s">
         <v>600</v>
       </c>
-      <c r="C29" s="68" t="s">
+      <c r="C30" s="68" t="s">
         <v>664</v>
       </c>
-      <c r="D29" s="61"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="62" t="s">
+      <c r="D30" s="61"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="62" t="s">
         <v>665</v>
       </c>
-      <c r="B30" s="60"/>
-      <c r="C30" s="58"/>
-      <c r="D30" s="60" t="s">
+      <c r="B31" s="60"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="60" t="s">
         <v>669</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="53" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="53" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="53" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="53" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="53" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B36" s="53" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="54" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="54" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
-      <c r="B37" s="54" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="35"/>
+      <c r="B38" s="54" t="s">
         <v>7</v>
-      </c>
-      <c r="C37" s="58"/>
-      <c r="D37" s="60"/>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="35"/>
-      <c r="B38" s="53" t="s">
-        <v>8</v>
       </c>
       <c r="C38" s="58"/>
       <c r="D38" s="60"/>
@@ -4380,144 +4384,152 @@
     <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="35"/>
       <c r="B39" s="53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C39" s="58"/>
       <c r="D39" s="60"/>
     </row>
     <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="47"/>
-      <c r="B40" s="57" t="s">
+      <c r="A40" s="35"/>
+      <c r="B40" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="58"/>
+      <c r="D40" s="60"/>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="47"/>
+      <c r="B41" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="68"/>
-      <c r="D40" s="61"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="62" t="s">
+      <c r="C41" s="68"/>
+      <c r="D41" s="61"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="62" t="s">
         <v>670</v>
       </c>
-      <c r="D41" s="63" t="s">
+      <c r="D42" s="63" t="s">
         <v>672</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B42" s="60" t="s">
-        <v>205</v>
-      </c>
-      <c r="C42" s="64" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B43" s="60" t="s">
+        <v>205</v>
+      </c>
+      <c r="C43" s="64" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B44" s="60" t="s">
         <v>204</v>
       </c>
-      <c r="C43" s="64" t="s">
+      <c r="C44" s="64" t="s">
         <v>673</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="60" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="60" t="s">
         <v>207</v>
       </c>
-      <c r="C44" s="64" t="s">
+      <c r="C45" s="64" t="s">
         <v>674</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="54" t="s">
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="54" t="s">
         <v>298</v>
       </c>
-      <c r="C45" s="64" t="s">
+      <c r="C46" s="64" t="s">
         <v>675</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="60" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="60" t="s">
         <v>424</v>
       </c>
-      <c r="C46" s="64" t="s">
+      <c r="C47" s="64" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="54" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="54" t="s">
         <v>300</v>
       </c>
-      <c r="C47" s="64" t="s">
+      <c r="C48" s="64" t="s">
         <v>677</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="65" t="s">
-        <v>323</v>
-      </c>
-      <c r="C48" s="64" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="65" t="s">
+        <v>323</v>
+      </c>
+      <c r="C49" s="64" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="65" t="s">
         <v>158</v>
       </c>
-      <c r="C49" s="64" t="s">
+      <c r="C50" s="64" t="s">
         <v>679</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B50" s="65" t="s">
-        <v>208</v>
-      </c>
-      <c r="C50" s="64" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B51" s="65" t="s">
+        <v>208</v>
+      </c>
+      <c r="C51" s="64" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B52" s="65" t="s">
         <v>209</v>
       </c>
-      <c r="C51" s="64" t="s">
+      <c r="C52" s="64" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="52" spans="2:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="B52" s="66" t="s">
+    <row r="53" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B53" s="66" t="s">
         <v>273</v>
       </c>
-      <c r="C52" s="64" t="s">
+      <c r="C53" s="64" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="53" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B53" s="60" t="s">
+    <row r="54" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B54" s="60" t="s">
         <v>272</v>
       </c>
-      <c r="C53" s="64" t="s">
+      <c r="C54" s="64" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="54" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B54" s="66" t="s">
+    <row r="55" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B55" s="66" t="s">
         <v>278</v>
       </c>
-      <c r="C54" s="64" t="s">
+      <c r="C55" s="64" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="55" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B55" s="66" t="s">
+    <row r="56" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B56" s="66" t="s">
         <v>321</v>
       </c>
-      <c r="C55" s="64" t="s">
+      <c r="C56" s="64" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="56" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B56" s="66" t="s">
+    <row r="57" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B57" s="66" t="s">
         <v>316</v>
       </c>
-      <c r="C56" s="64" t="s">
+      <c r="C57" s="64" t="s">
         <v>686</v>
       </c>
     </row>
@@ -5376,11 +5388,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317EB008-F691-4F16-B99A-D5845A82BBBD}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5889,7 +5901,7 @@
         <v>888</v>
       </c>
       <c r="G12" s="102" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="H12" s="79" t="str">
         <f t="shared" ref="H12:H25" si="1">"D:/ntnl_li_2018_template/data/study_region/"&amp;B12&amp;"/"&amp;B12&amp;"_20181001.osm"</f>
@@ -5899,7 +5911,7 @@
         <v>878</v>
       </c>
       <c r="J12" s="82" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="K12" s="84"/>
       <c r="L12" s="80" t="s">
@@ -5940,7 +5952,7 @@
         <v>878</v>
       </c>
       <c r="J13" s="82" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="K13" s="82"/>
       <c r="L13" s="83" t="s">
@@ -5982,7 +5994,7 @@
         <v>878</v>
       </c>
       <c r="J14" s="82" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="K14" s="79"/>
       <c r="L14" s="80" t="s">
@@ -6023,7 +6035,7 @@
         <v>878</v>
       </c>
       <c r="J15" s="82" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="K15" s="82"/>
       <c r="L15" s="83" t="s">
@@ -6065,7 +6077,7 @@
         <v>878</v>
       </c>
       <c r="J16" s="82" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="K16" s="79"/>
       <c r="L16" s="80" t="s">
@@ -6084,7 +6096,7 @@
         <v>883</v>
       </c>
       <c r="C17" s="82" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="D17" s="82" t="s">
         <v>901</v>
@@ -6096,7 +6108,7 @@
         <v>893</v>
       </c>
       <c r="G17" s="82" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="H17" s="82" t="str">
         <f t="shared" si="1"/>
@@ -6106,7 +6118,7 @@
         <v>878</v>
       </c>
       <c r="J17" s="82" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="K17" s="82"/>
       <c r="L17" s="83" t="s">
@@ -6148,7 +6160,7 @@
         <v>878</v>
       </c>
       <c r="J18" s="82" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="K18" s="79"/>
       <c r="L18" s="79" t="s">
@@ -6189,7 +6201,7 @@
         <v>878</v>
       </c>
       <c r="J19" s="82" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="K19" s="82"/>
       <c r="L19" s="83" t="s">
@@ -6231,7 +6243,7 @@
         <v>878</v>
       </c>
       <c r="J20" s="82" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="K20" s="79"/>
       <c r="L20" s="80" t="s">
@@ -6272,7 +6284,7 @@
         <v>878</v>
       </c>
       <c r="J21" s="82" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="K21" s="82"/>
       <c r="L21" s="83" t="s">
@@ -6314,7 +6326,7 @@
         <v>878</v>
       </c>
       <c r="J22" s="82" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="K22" s="79"/>
       <c r="L22" s="80" t="s">
@@ -6355,7 +6367,7 @@
         <v>878</v>
       </c>
       <c r="J23" s="82" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="K23" s="82"/>
       <c r="L23" s="83" t="s">
@@ -6397,7 +6409,7 @@
         <v>878</v>
       </c>
       <c r="J24" s="82" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="K24" s="79"/>
       <c r="L24" s="80" t="s">
@@ -6438,7 +6450,7 @@
         <v>878</v>
       </c>
       <c r="J25" s="82" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="K25" s="83"/>
       <c r="L25" s="83" t="s">

</xml_diff>

<commit_message>
updates -- now you can write 'python who.py' to find out what you need to do
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C987D32C-916E-44C2-8500-FEB1067D7806}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79F62FD-C451-4DEE-BFCA-94E3DE4C7F5F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="3" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -2047,9 +2047,6 @@
     <t>petrolstations_Petrol_2018</t>
   </si>
   <si>
-    <t>Australian National Liveability Indicators, 2016</t>
-  </si>
-  <si>
     <t>June to December 2018</t>
   </si>
   <si>
@@ -2944,6 +2941,9 @@
   </si>
   <si>
     <t>osm_wollongong__sua_2018_10000m_epsg4326_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t>Australian National Liveability Indicators, 2018</t>
   </si>
 </sst>
 </file>
@@ -4018,8 +4018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E850BD-5E22-47F0-A5F7-1D4C00B37AB6}">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4029,12 +4029,12 @@
   <sheetData>
     <row r="1" spans="1:1" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>652</v>
+        <v>938</v>
       </c>
     </row>
     <row r="2" spans="1:1" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="3" spans="1:1" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4047,12 +4047,12 @@
     </row>
     <row r="5" spans="1:1" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="8" spans="1:1" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -4089,12 +4089,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B3" s="34" t="s">
         <v>472</v>
@@ -4103,24 +4103,24 @@
         <v>473</v>
       </c>
       <c r="D3" s="56" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B4" s="55"/>
       <c r="C4" s="85"/>
       <c r="D4" s="87" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="91"/>
       <c r="B5" s="92"/>
       <c r="C5" s="52" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D5" s="86"/>
     </row>
@@ -4128,18 +4128,18 @@
       <c r="A6" s="89"/>
       <c r="B6" s="90"/>
       <c r="C6" s="93" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D6" s="88"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B7" s="49"/>
       <c r="C7" s="58"/>
       <c r="D7" s="63" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -4175,13 +4175,13 @@
         <v>580</v>
       </c>
       <c r="C11" s="58" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="35"/>
       <c r="B12" s="50" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C12" s="58" t="s">
         <v>475</v>
@@ -4190,7 +4190,7 @@
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="35"/>
       <c r="B13" s="49" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C13" s="58" t="s">
         <v>471</v>
@@ -4199,7 +4199,7 @@
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="35"/>
       <c r="B14" s="49" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="C14" s="58" t="s">
         <v>476</v>
@@ -4208,37 +4208,37 @@
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
       <c r="B15" s="49" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C15" s="58" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="35"/>
       <c r="B16" s="49" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="C16" s="58" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="35"/>
       <c r="B17" s="49" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C17" s="58" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="35"/>
       <c r="B18" s="49" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C18" s="58" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -4253,7 +4253,7 @@
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
       <c r="B20" s="60" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C20" s="58" t="s">
         <v>477</v>
@@ -4262,19 +4262,19 @@
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="35"/>
       <c r="B21" s="60" t="s">
+        <v>691</v>
+      </c>
+      <c r="C21" s="58" t="s">
         <v>692</v>
-      </c>
-      <c r="C21" s="58" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="35"/>
       <c r="B22" s="60" t="s">
+        <v>829</v>
+      </c>
+      <c r="C22" s="58" t="s">
         <v>830</v>
-      </c>
-      <c r="C22" s="58" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -4292,12 +4292,12 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="59" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B25" s="35"/>
       <c r="C25" s="58"/>
       <c r="D25" s="60" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4305,7 +4305,7 @@
         <v>596</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -4314,7 +4314,7 @@
         <v>597</v>
       </c>
       <c r="C27" s="58" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -4323,7 +4323,7 @@
         <v>598</v>
       </c>
       <c r="C28" s="58" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -4332,7 +4332,7 @@
         <v>599</v>
       </c>
       <c r="C29" s="58" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -4341,18 +4341,18 @@
         <v>600</v>
       </c>
       <c r="C30" s="68" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D30" s="61"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="62" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B31" s="60"/>
       <c r="C31" s="58"/>
       <c r="D31" s="60" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -4419,10 +4419,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="62" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D42" s="63" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -4430,7 +4430,7 @@
         <v>205</v>
       </c>
       <c r="C43" s="64" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -4438,7 +4438,7 @@
         <v>204</v>
       </c>
       <c r="C44" s="64" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -4446,7 +4446,7 @@
         <v>207</v>
       </c>
       <c r="C45" s="64" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4454,7 +4454,7 @@
         <v>298</v>
       </c>
       <c r="C46" s="64" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -4462,7 +4462,7 @@
         <v>424</v>
       </c>
       <c r="C47" s="64" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -4470,7 +4470,7 @@
         <v>300</v>
       </c>
       <c r="C48" s="64" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
@@ -4478,7 +4478,7 @@
         <v>323</v>
       </c>
       <c r="C49" s="64" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
@@ -4486,7 +4486,7 @@
         <v>158</v>
       </c>
       <c r="C50" s="64" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="45" x14ac:dyDescent="0.25">
@@ -4494,7 +4494,7 @@
         <v>208</v>
       </c>
       <c r="C51" s="64" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="52" spans="2:3" ht="45" x14ac:dyDescent="0.25">
@@ -4502,7 +4502,7 @@
         <v>209</v>
       </c>
       <c r="C52" s="64" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="53" spans="2:3" ht="75" x14ac:dyDescent="0.25">
@@ -4510,7 +4510,7 @@
         <v>273</v>
       </c>
       <c r="C53" s="64" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="54" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -4518,7 +4518,7 @@
         <v>272</v>
       </c>
       <c r="C54" s="64" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="55" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -4526,7 +4526,7 @@
         <v>278</v>
       </c>
       <c r="C55" s="64" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="56" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
@@ -4534,7 +4534,7 @@
         <v>321</v>
       </c>
       <c r="C56" s="64" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="57" spans="2:3" ht="45" x14ac:dyDescent="0.25">
@@ -4542,7 +4542,7 @@
         <v>316</v>
       </c>
       <c r="C57" s="64" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
   </sheetData>
@@ -4570,72 +4570,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="94" t="s">
+        <v>686</v>
+      </c>
+      <c r="B1" s="95" t="s">
         <v>687</v>
       </c>
-      <c r="B1" s="95" t="s">
-        <v>688</v>
-      </c>
       <c r="C1" s="101" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="D1" s="101" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>688</v>
+      </c>
+      <c r="B2" s="69" t="s">
         <v>689</v>
       </c>
-      <c r="B2" s="69" t="s">
-        <v>690</v>
-      </c>
       <c r="C2" s="38" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B3" s="69">
         <v>2018</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B4" s="69" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B5" s="69">
         <v>7845</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4643,584 +4643,584 @@
         <v>321</v>
       </c>
       <c r="B6" s="69" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>702</v>
+      </c>
+      <c r="B7" s="69" t="s">
         <v>703</v>
       </c>
-      <c r="B7" s="69" t="s">
-        <v>704</v>
-      </c>
       <c r="C7" s="38" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B8" s="69">
         <v>10000</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B9" s="69">
         <v>3000</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B10" s="69">
         <v>3000</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>715</v>
+      </c>
+      <c r="B11" s="69" t="s">
         <v>716</v>
       </c>
-      <c r="B11" s="69" t="s">
-        <v>717</v>
-      </c>
       <c r="C11" s="38" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B12" s="69" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B13" s="69">
         <v>5432</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B14" s="69" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C14" s="38" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B15" s="69" t="s">
+        <v>740</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>796</v>
+      </c>
+      <c r="D15" s="38" t="s">
         <v>741</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>797</v>
-      </c>
-      <c r="D15" s="38" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>744</v>
+      </c>
+      <c r="B16" s="69" t="s">
         <v>745</v>
       </c>
-      <c r="B16" s="69" t="s">
-        <v>746</v>
-      </c>
       <c r="C16" s="38" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B17" s="69" t="s">
+        <v>874</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>796</v>
+      </c>
+      <c r="D17" s="38" t="s">
         <v>875</v>
-      </c>
-      <c r="C17" s="38" t="s">
-        <v>797</v>
-      </c>
-      <c r="D17" s="38" t="s">
-        <v>876</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>871</v>
+      </c>
+      <c r="B18" s="69" t="s">
         <v>872</v>
       </c>
-      <c r="B18" s="69" t="s">
+      <c r="C18" s="38" t="s">
+        <v>796</v>
+      </c>
+      <c r="D18" s="38" t="s">
         <v>873</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>797</v>
-      </c>
-      <c r="D18" s="38" t="s">
-        <v>874</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B19" s="69" t="s">
+        <v>717</v>
+      </c>
+      <c r="C19" s="38" t="s">
+        <v>797</v>
+      </c>
+      <c r="D19" s="38" t="s">
         <v>718</v>
-      </c>
-      <c r="C19" s="38" t="s">
-        <v>798</v>
-      </c>
-      <c r="D19" s="38" t="s">
-        <v>719</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>721</v>
+      </c>
+      <c r="B20" s="69" t="s">
         <v>722</v>
       </c>
-      <c r="B20" s="69" t="s">
+      <c r="C20" s="38" t="s">
+        <v>797</v>
+      </c>
+      <c r="D20" s="38" t="s">
         <v>723</v>
-      </c>
-      <c r="C20" s="38" t="s">
-        <v>798</v>
-      </c>
-      <c r="D20" s="38" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>724</v>
+      </c>
+      <c r="B21" s="69" t="s">
         <v>725</v>
       </c>
-      <c r="B21" s="69" t="s">
+      <c r="C21" s="38" t="s">
+        <v>798</v>
+      </c>
+      <c r="D21" s="38" t="s">
         <v>726</v>
-      </c>
-      <c r="C21" s="38" t="s">
-        <v>799</v>
-      </c>
-      <c r="D21" s="38" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B22" s="69" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B23" s="69" t="s">
+        <v>730</v>
+      </c>
+      <c r="C23" s="38" t="s">
+        <v>798</v>
+      </c>
+      <c r="D23" s="38" t="s">
         <v>731</v>
-      </c>
-      <c r="C23" s="38" t="s">
-        <v>799</v>
-      </c>
-      <c r="D23" s="38" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>732</v>
+      </c>
+      <c r="B24" s="69" t="s">
+        <v>734</v>
+      </c>
+      <c r="C24" s="38" t="s">
+        <v>798</v>
+      </c>
+      <c r="D24" s="38" t="s">
         <v>733</v>
-      </c>
-      <c r="B24" s="69" t="s">
-        <v>735</v>
-      </c>
-      <c r="C24" s="38" t="s">
-        <v>799</v>
-      </c>
-      <c r="D24" s="38" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>746</v>
+      </c>
+      <c r="B25" s="69" t="s">
         <v>747</v>
       </c>
-      <c r="B25" s="69" t="s">
-        <v>748</v>
-      </c>
       <c r="C25" s="38" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>748</v>
+      </c>
+      <c r="B26" s="69" t="s">
         <v>749</v>
       </c>
-      <c r="B26" s="69" t="s">
-        <v>750</v>
-      </c>
       <c r="C26" s="38" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>750</v>
+      </c>
+      <c r="B27" s="69" t="s">
         <v>751</v>
       </c>
-      <c r="B27" s="69" t="s">
-        <v>752</v>
-      </c>
       <c r="C27" s="38" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B28" s="69" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B29" s="69" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D29" s="38" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B30" s="69" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B31" s="69" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C31" s="38" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B32" s="69" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C32" s="38" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B33" s="69" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C33" s="38" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B34" s="69" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C34" s="38" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B35" s="69" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B36" s="69" t="s">
         <v>567</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B37" s="69" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="C37" s="38" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B38" s="69" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C38" s="38" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="B39" s="69" t="s">
+        <v>802</v>
+      </c>
+      <c r="C39" s="38" t="s">
+        <v>800</v>
+      </c>
+      <c r="D39" s="38" t="s">
         <v>803</v>
-      </c>
-      <c r="C39" s="38" t="s">
-        <v>801</v>
-      </c>
-      <c r="D39" s="38" t="s">
-        <v>804</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B40" s="69">
         <v>7844</v>
       </c>
       <c r="C40" s="38" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>805</v>
+      </c>
+      <c r="B41" s="69" t="s">
         <v>806</v>
       </c>
-      <c r="B41" s="69" t="s">
+      <c r="C41" s="38" t="s">
+        <v>806</v>
+      </c>
+      <c r="D41" s="38" t="s">
         <v>807</v>
-      </c>
-      <c r="C41" s="38" t="s">
-        <v>807</v>
-      </c>
-      <c r="D41" s="38" t="s">
-        <v>808</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B42" s="69" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C42" s="38" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B43" s="69" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C43" s="38" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B44" s="69" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="C44" s="38" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>815</v>
+      </c>
+      <c r="B45" s="69" t="s">
         <v>816</v>
       </c>
-      <c r="B45" s="69" t="s">
+      <c r="C45" s="38" t="s">
+        <v>806</v>
+      </c>
+      <c r="D45" s="38" t="s">
         <v>817</v>
-      </c>
-      <c r="C45" s="38" t="s">
-        <v>807</v>
-      </c>
-      <c r="D45" s="38" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B46" s="69" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C46" s="38" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="D46" s="38" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B47" s="69" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C47" s="38" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="D47" s="38" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -5231,164 +5231,164 @@
         <v>1600</v>
       </c>
       <c r="C48" s="38" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="D48" s="38" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="B49" s="69">
         <v>500</v>
       </c>
       <c r="C49" s="38" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="D49" s="38" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B50" s="69">
         <v>50</v>
       </c>
       <c r="C50" s="38" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B51" s="69">
         <v>3000</v>
       </c>
       <c r="C51" s="38" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="D51" s="38" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B52" s="69">
         <v>3200</v>
       </c>
       <c r="C52" s="38" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="D52" s="38" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="B53" s="69">
         <v>5</v>
       </c>
       <c r="C53" s="38" t="s">
+        <v>831</v>
+      </c>
+      <c r="D53" s="38" t="s">
         <v>832</v>
-      </c>
-      <c r="D53" s="38" t="s">
-        <v>833</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B54" s="69">
         <v>50</v>
       </c>
       <c r="C54" s="38" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="D54" s="38" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>841</v>
+      </c>
+      <c r="B55" s="69" t="s">
+        <v>657</v>
+      </c>
+      <c r="C55" s="38" t="s">
+        <v>657</v>
+      </c>
+      <c r="D55" s="38" t="s">
         <v>842</v>
-      </c>
-      <c r="B55" s="69" t="s">
-        <v>658</v>
-      </c>
-      <c r="C55" s="38" t="s">
-        <v>658</v>
-      </c>
-      <c r="D55" s="38" t="s">
-        <v>843</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>843</v>
+      </c>
+      <c r="B56" s="69" t="s">
         <v>844</v>
       </c>
-      <c r="B56" s="69" t="s">
+      <c r="C56" s="38" t="s">
+        <v>657</v>
+      </c>
+      <c r="D56" s="38" t="s">
         <v>845</v>
-      </c>
-      <c r="C56" s="38" t="s">
-        <v>658</v>
-      </c>
-      <c r="D56" s="38" t="s">
-        <v>846</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B57" s="69" t="s">
+        <v>848</v>
+      </c>
+      <c r="C57" s="38" t="s">
+        <v>657</v>
+      </c>
+      <c r="D57" s="38" t="s">
         <v>849</v>
-      </c>
-      <c r="C57" s="38" t="s">
-        <v>658</v>
-      </c>
-      <c r="D57" s="38" t="s">
-        <v>850</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B58" s="69" t="b">
         <v>0</v>
       </c>
       <c r="C58" s="38" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D58" s="38" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>851</v>
+      </c>
+      <c r="B59" s="69" t="s">
+        <v>853</v>
+      </c>
+      <c r="C59" s="38" t="s">
+        <v>657</v>
+      </c>
+      <c r="D59" s="38" t="s">
         <v>852</v>
-      </c>
-      <c r="B59" s="69" t="s">
-        <v>854</v>
-      </c>
-      <c r="C59" s="38" t="s">
-        <v>658</v>
-      </c>
-      <c r="D59" s="38" t="s">
-        <v>853</v>
       </c>
     </row>
   </sheetData>
@@ -5400,7 +5400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317EB008-F691-4F16-B99A-D5845A82BBBD}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -5432,7 +5432,7 @@
         <v>207</v>
       </c>
       <c r="C1" s="71" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="D1" s="71" t="s">
         <v>428</v>
@@ -5441,58 +5441,58 @@
         <v>580</v>
       </c>
       <c r="F1" s="72" t="s">
+        <v>756</v>
+      </c>
+      <c r="G1" s="72" t="s">
+        <v>758</v>
+      </c>
+      <c r="H1" s="71" t="s">
         <v>757</v>
       </c>
-      <c r="G1" s="72" t="s">
-        <v>759</v>
-      </c>
-      <c r="H1" s="71" t="s">
-        <v>758</v>
-      </c>
       <c r="I1" s="71" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="J1" s="71" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="K1" s="71" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="L1" s="71" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="M1" s="71" t="s">
         <v>429</v>
       </c>
       <c r="N1" s="71" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="O1" s="73" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="P1" s="73" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="74" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B2" s="75" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C2" s="75"/>
       <c r="D2" s="75" t="s">
+        <v>753</v>
+      </c>
+      <c r="E2" s="75" t="s">
         <v>754</v>
-      </c>
-      <c r="E2" s="75" t="s">
-        <v>755</v>
       </c>
       <c r="F2" s="76" t="s">
         <v>433</v>
       </c>
       <c r="G2" s="76" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="H2" s="75" t="s">
         <v>434</v>
@@ -5502,20 +5502,20 @@
         <v>D:/ntnl_li_2018_template/data/study_region/testing/testing_gccstest_2016_10000m_20181001.osm</v>
       </c>
       <c r="J2" s="75" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K2" s="75" t="str">
         <f>"osm_10km_"&amp;B2&amp;"_10km_pedestrian_"&amp;RIGHT(J2,8)</f>
         <v>osm_10km_testing_10km_pedestrian_20181001</v>
       </c>
       <c r="L2" s="75" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="M2" s="76" t="s">
         <v>439</v>
       </c>
       <c r="N2" s="75" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="O2" s="77"/>
       <c r="P2" s="77">
@@ -5530,7 +5530,7 @@
         <v>585</v>
       </c>
       <c r="C3" s="75" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D3" s="75" t="s">
         <v>431</v>
@@ -5552,10 +5552,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/adelaide/adelaide_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="J3" s="75" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K3" s="75" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="L3" s="75"/>
       <c r="M3" s="75"/>
@@ -5573,7 +5573,7 @@
         <v>584</v>
       </c>
       <c r="C4" s="79" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D4" s="79" t="s">
         <v>436</v>
@@ -5595,13 +5595,13 @@
         <v>D:/ntnl_li_2018_template/data/study_region/bris/bris_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="J4" s="79" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K4" s="79" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="L4" s="79" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="M4" s="80" t="s">
         <v>439</v>
@@ -5619,7 +5619,7 @@
         <v>586</v>
       </c>
       <c r="C5" s="82" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D5" s="82" t="s">
         <v>441</v>
@@ -5641,10 +5641,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/canberra/canberra_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="J5" s="82" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K5" s="82" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="L5" s="82"/>
       <c r="M5" s="82"/>
@@ -5662,7 +5662,7 @@
         <v>587</v>
       </c>
       <c r="C6" s="79" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D6" s="79" t="s">
         <v>444</v>
@@ -5684,10 +5684,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/darwin/darwin_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="J6" s="79" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K6" s="79" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="L6" s="79"/>
       <c r="M6" s="79"/>
@@ -5704,7 +5704,7 @@
         <v>588</v>
       </c>
       <c r="C7" s="82" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D7" s="82" t="s">
         <v>448</v>
@@ -5726,10 +5726,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/hobart/hobart_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="J7" s="82" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K7" s="82" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="L7" s="82"/>
       <c r="M7" s="82"/>
@@ -5747,7 +5747,7 @@
         <v>589</v>
       </c>
       <c r="C8" s="79" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D8" s="79" t="s">
         <v>452</v>
@@ -5769,13 +5769,13 @@
         <v>D:/ntnl_li_2018_template/data/study_region/melb/melb_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="J8" s="79" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K8" s="79" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="L8" s="79" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="M8" s="80" t="s">
         <v>455</v>
@@ -5795,7 +5795,7 @@
         <v>590</v>
       </c>
       <c r="C9" s="82" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D9" s="82" t="s">
         <v>457</v>
@@ -5817,13 +5817,13 @@
         <v>D:/ntnl_li_2018_template/data/study_region/perth/perth_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="J9" s="82" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K9" s="82" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="L9" s="82" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="M9" s="83" t="s">
         <v>460</v>
@@ -5842,7 +5842,7 @@
         <v>591</v>
       </c>
       <c r="C10" s="79" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D10" s="79" t="s">
         <v>462</v>
@@ -5864,13 +5864,13 @@
         <v>D:/ntnl_li_2018_template/data/study_region/syd/syd_gccsa_2016_10000m_20181001.osm</v>
       </c>
       <c r="J10" s="79" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K10" s="79" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="L10" s="79" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="M10" s="80" t="s">
         <v>465</v>
@@ -5890,7 +5890,7 @@
         <v>592</v>
       </c>
       <c r="C11" s="82" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D11" s="82" t="s">
         <v>452</v>
@@ -5912,10 +5912,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/mitchell/mitchell_lga_2016_10000m_20181001.osm</v>
       </c>
       <c r="J11" s="82" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K11" s="82" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="L11" s="82"/>
       <c r="M11" s="82"/>
@@ -5930,35 +5930,35 @@
         <v>552</v>
       </c>
       <c r="B12" s="79" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="C12" s="79" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D12" s="79" t="s">
         <v>583</v>
       </c>
       <c r="E12" s="79" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="F12" s="80" t="s">
+        <v>886</v>
+      </c>
+      <c r="G12" s="103" t="s">
         <v>887</v>
       </c>
-      <c r="G12" s="103" t="s">
-        <v>888</v>
-      </c>
       <c r="H12" s="102" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="I12" s="79" t="str">
         <f t="shared" ref="I12:I25" si="1">"D:/ntnl_li_2018_template/data/study_region/"&amp;B12&amp;"/"&amp;B12&amp;"_20181001.osm"</f>
         <v>D:/ntnl_li_2018_template/data/study_region/albury_wodonga/albury_wodonga_20181001.osm</v>
       </c>
       <c r="J12" s="79" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K12" s="82" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="L12" s="84"/>
       <c r="M12" s="80" t="s">
@@ -5977,19 +5977,19 @@
         <v>571</v>
       </c>
       <c r="C13" s="82" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D13" s="82" t="s">
         <v>452</v>
       </c>
       <c r="E13" s="82" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="F13" s="83" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="G13" s="83" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="H13" s="82" t="s">
         <v>454</v>
@@ -5999,10 +5999,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/ballarat/ballarat_20181001.osm</v>
       </c>
       <c r="J13" s="82" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K13" s="82" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="L13" s="82"/>
       <c r="M13" s="83" t="s">
@@ -6022,19 +6022,19 @@
         <v>572</v>
       </c>
       <c r="C14" s="79" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D14" s="79" t="s">
         <v>452</v>
       </c>
       <c r="E14" s="79" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="F14" s="80" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="G14" s="79" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="H14" s="79" t="s">
         <v>454</v>
@@ -6044,10 +6044,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/bendigo/bendigo_20181001.osm</v>
       </c>
       <c r="J14" s="79" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K14" s="82" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="L14" s="79"/>
       <c r="M14" s="80" t="s">
@@ -6066,19 +6066,19 @@
         <v>573</v>
       </c>
       <c r="C15" s="82" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D15" s="82" t="s">
         <v>436</v>
       </c>
       <c r="E15" s="82" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="F15" s="83" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="G15" s="82" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="H15" s="82" t="s">
         <v>438</v>
@@ -6088,10 +6088,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/cairns/cairns_20181001.osm</v>
       </c>
       <c r="J15" s="82" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K15" s="82" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="L15" s="82"/>
       <c r="M15" s="83" t="s">
@@ -6111,19 +6111,19 @@
         <v>574</v>
       </c>
       <c r="C16" s="79" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D16" s="79" t="s">
         <v>452</v>
       </c>
       <c r="E16" s="79" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="F16" s="80" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="G16" s="80" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="H16" s="79" t="s">
         <v>454</v>
@@ -6133,10 +6133,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/geelong/geelong_20181001.osm</v>
       </c>
       <c r="J16" s="79" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K16" s="82" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="L16" s="79"/>
       <c r="M16" s="80" t="s">
@@ -6152,35 +6152,35 @@
         <v>557</v>
       </c>
       <c r="B17" s="82" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C17" s="82" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D17" s="82" t="s">
+        <v>907</v>
+      </c>
+      <c r="E17" s="82" t="s">
+        <v>900</v>
+      </c>
+      <c r="F17" s="83" t="s">
+        <v>886</v>
+      </c>
+      <c r="G17" s="82" t="s">
+        <v>892</v>
+      </c>
+      <c r="H17" s="82" t="s">
         <v>908</v>
-      </c>
-      <c r="E17" s="82" t="s">
-        <v>901</v>
-      </c>
-      <c r="F17" s="83" t="s">
-        <v>887</v>
-      </c>
-      <c r="G17" s="82" t="s">
-        <v>893</v>
-      </c>
-      <c r="H17" s="82" t="s">
-        <v>909</v>
       </c>
       <c r="I17" s="82" t="str">
         <f t="shared" si="1"/>
         <v>D:/ntnl_li_2018_template/data/study_region/goldcoast_tweedheads/goldcoast_tweedheads_20181001.osm</v>
       </c>
       <c r="J17" s="82" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K17" s="82" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="L17" s="82"/>
       <c r="M17" s="83" t="s">
@@ -6200,19 +6200,19 @@
         <v>575</v>
       </c>
       <c r="C18" s="79" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D18" s="79" t="s">
         <v>448</v>
       </c>
       <c r="E18" s="79" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="F18" s="80" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="G18" s="79" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="H18" s="79" t="s">
         <v>450</v>
@@ -6222,10 +6222,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/launceston/launceston_20181001.osm</v>
       </c>
       <c r="J18" s="79" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K18" s="82" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="L18" s="79"/>
       <c r="M18" s="79" t="s">
@@ -6244,19 +6244,19 @@
         <v>576</v>
       </c>
       <c r="C19" s="82" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D19" s="82" t="s">
         <v>436</v>
       </c>
       <c r="E19" s="82" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="F19" s="83" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="G19" s="82" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="H19" s="82" t="s">
         <v>438</v>
@@ -6266,10 +6266,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/mackay/mackay_20181001.osm</v>
       </c>
       <c r="J19" s="82" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K19" s="82" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="L19" s="82"/>
       <c r="M19" s="83" t="s">
@@ -6286,22 +6286,22 @@
         <v>560</v>
       </c>
       <c r="B20" s="79" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="C20" s="79" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D20" s="79" t="s">
         <v>462</v>
       </c>
       <c r="E20" s="79" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="F20" s="80" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="G20" s="79" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="H20" s="79" t="s">
         <v>464</v>
@@ -6311,10 +6311,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/newcastle_maitland/newcastle_maitland_20181001.osm</v>
       </c>
       <c r="J20" s="79" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K20" s="82" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="L20" s="79"/>
       <c r="M20" s="80" t="s">
@@ -6330,22 +6330,22 @@
         <v>561</v>
       </c>
       <c r="B21" s="82" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="C21" s="82" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D21" s="82" t="s">
         <v>436</v>
       </c>
       <c r="E21" s="82" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="F21" s="83" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="G21" s="82" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="H21" s="82" t="s">
         <v>438</v>
@@ -6355,10 +6355,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/sunshine_coast/sunshine_coast_20181001.osm</v>
       </c>
       <c r="J21" s="82" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K21" s="82" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="L21" s="82"/>
       <c r="M21" s="83" t="s">
@@ -6378,19 +6378,19 @@
         <v>577</v>
       </c>
       <c r="C22" s="79" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D22" s="79" t="s">
         <v>436</v>
       </c>
       <c r="E22" s="79" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="F22" s="80" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="G22" s="79" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="H22" s="79" t="s">
         <v>438</v>
@@ -6400,10 +6400,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/toowoomba/toowoomba_20181001.osm</v>
       </c>
       <c r="J22" s="79" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K22" s="82" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="L22" s="79"/>
       <c r="M22" s="80" t="s">
@@ -6422,19 +6422,19 @@
         <v>578</v>
       </c>
       <c r="C23" s="82" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D23" s="82" t="s">
         <v>436</v>
       </c>
       <c r="E23" s="82" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="F23" s="83" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="G23" s="82" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="H23" s="82" t="s">
         <v>438</v>
@@ -6444,10 +6444,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/townsville/townsville_20181001.osm</v>
       </c>
       <c r="J23" s="82" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K23" s="82" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="L23" s="82"/>
       <c r="M23" s="83" t="s">
@@ -6467,19 +6467,19 @@
         <v>579</v>
       </c>
       <c r="C24" s="79" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D24" s="79" t="s">
         <v>462</v>
       </c>
       <c r="E24" s="79" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="F24" s="80" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="G24" s="79" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="H24" s="79" t="s">
         <v>464</v>
@@ -6489,10 +6489,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/wollongong/wollongong_20181001.osm</v>
       </c>
       <c r="J24" s="79" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K24" s="82" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="L24" s="79"/>
       <c r="M24" s="80" t="s">
@@ -6508,16 +6508,16 @@
         <v>566</v>
       </c>
       <c r="B25" s="82" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="C25" s="82" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D25" s="82" t="s">
         <v>462</v>
       </c>
       <c r="E25" s="82" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="F25" s="83" t="s">
         <v>567</v>
@@ -6533,10 +6533,10 @@
         <v>D:/ntnl_li_2018_template/data/study_region/western_sydney/western_sydney_20181001.osm</v>
       </c>
       <c r="J25" s="82" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K25" s="82" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="L25" s="83"/>
       <c r="M25" s="83" t="s">
@@ -10037,7 +10037,7 @@
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="98" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>421</v>
@@ -10079,7 +10079,7 @@
       </c>
       <c r="B15" s="23"/>
       <c r="C15" s="98" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>422</v>
@@ -10114,7 +10114,7 @@
         <v>203</v>
       </c>
       <c r="C16" s="98" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D16" s="23" t="s">
         <v>380</v>
@@ -10158,7 +10158,7 @@
         <v>206</v>
       </c>
       <c r="C17" s="98" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D17" s="23" t="s">
         <v>381</v>
@@ -10199,7 +10199,7 @@
         <v>173</v>
       </c>
       <c r="C18" s="98" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D18" s="43" t="s">
         <v>382</v>
@@ -10241,7 +10241,7 @@
       </c>
       <c r="B19" s="23"/>
       <c r="C19" s="98" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D19" s="23" t="s">
         <v>383</v>
@@ -10285,7 +10285,7 @@
         <v>203</v>
       </c>
       <c r="C20" s="98" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D20" s="23" t="s">
         <v>379</v>
@@ -10329,7 +10329,7 @@
         <v>206</v>
       </c>
       <c r="C21" s="98" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D21" s="23" t="s">
         <v>386</v>
@@ -10788,7 +10788,7 @@
         <v>203</v>
       </c>
       <c r="C31" s="98" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D31" s="43" t="s">
         <v>374</v>
@@ -10832,7 +10832,7 @@
         <v>206</v>
       </c>
       <c r="C32" s="98" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D32" s="43" t="s">
         <v>390</v>
@@ -11763,7 +11763,7 @@
         <v>203</v>
       </c>
       <c r="C52" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D52" s="43" t="s">
         <v>370</v>
@@ -11807,7 +11807,7 @@
         <v>206</v>
       </c>
       <c r="C53" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D53" s="43" t="s">
         <v>393</v>
@@ -11851,7 +11851,7 @@
         <v>203</v>
       </c>
       <c r="C54" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D54" s="43" t="s">
         <v>411</v>
@@ -11895,7 +11895,7 @@
         <v>206</v>
       </c>
       <c r="C55" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D55" s="43" t="s">
         <v>412</v>
@@ -11937,7 +11937,7 @@
       </c>
       <c r="B56" s="23"/>
       <c r="C56" s="98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D56" s="43" t="s">
         <v>364</v>
@@ -11973,7 +11973,7 @@
       </c>
       <c r="B57" s="23"/>
       <c r="C57" s="98" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D57" s="43" t="s">
         <v>365</v>
@@ -12009,7 +12009,7 @@
       </c>
       <c r="B58" s="23"/>
       <c r="C58" s="98" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D58" s="43" t="s">
         <v>366</v>
@@ -12045,7 +12045,7 @@
       </c>
       <c r="B59" s="23"/>
       <c r="C59" s="98" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D59" s="43" t="s">
         <v>357</v>
@@ -12081,7 +12081,7 @@
       </c>
       <c r="B60" s="23"/>
       <c r="C60" s="98" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D60" s="43" t="s">
         <v>358</v>
@@ -12117,7 +12117,7 @@
       </c>
       <c r="B61" s="23"/>
       <c r="C61" s="98" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D61" s="43" t="s">
         <v>359</v>
@@ -12153,7 +12153,7 @@
       </c>
       <c r="B62" s="23"/>
       <c r="C62" s="98" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D62" s="43" t="s">
         <v>360</v>
@@ -12189,7 +12189,7 @@
       </c>
       <c r="B63" s="23"/>
       <c r="C63" s="98" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D63" s="43" t="s">
         <v>361</v>
@@ -12225,7 +12225,7 @@
       </c>
       <c r="B64" s="23"/>
       <c r="C64" s="98" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D64" s="43" t="s">
         <v>415</v>
@@ -12267,7 +12267,7 @@
         <v>203</v>
       </c>
       <c r="C65" s="98" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D65" s="43" t="s">
         <v>371</v>
@@ -12311,7 +12311,7 @@
         <v>206</v>
       </c>
       <c r="C66" s="98" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D66" s="43" t="s">
         <v>392</v>
@@ -12725,7 +12725,7 @@
       </c>
       <c r="B76" s="23"/>
       <c r="C76" s="98" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D76" s="43" t="s">
         <v>413</v>
@@ -12765,7 +12765,7 @@
       </c>
       <c r="B77" s="23"/>
       <c r="C77" s="98" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D77" s="43" t="s">
         <v>414</v>
@@ -13182,13 +13182,13 @@
     </row>
     <row r="87" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="22" t="s">
+        <v>866</v>
+      </c>
+      <c r="C87" s="99" t="s">
         <v>867</v>
       </c>
-      <c r="C87" s="99" t="s">
+      <c r="D87" s="42" t="s">
         <v>868</v>
-      </c>
-      <c r="D87" s="42" t="s">
-        <v>869</v>
       </c>
       <c r="E87" t="s">
         <v>425</v>
@@ -13197,13 +13197,13 @@
         <v>308</v>
       </c>
       <c r="G87" s="42" t="s">
+        <v>868</v>
+      </c>
+      <c r="H87" s="42" t="s">
+        <v>868</v>
+      </c>
+      <c r="K87" s="96" t="s">
         <v>869</v>
-      </c>
-      <c r="H87" s="42" t="s">
-        <v>869</v>
-      </c>
-      <c r="K87" s="96" t="s">
-        <v>870</v>
       </c>
       <c r="L87" s="22">
         <v>1</v>
@@ -13234,10 +13234,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>861</v>
+      </c>
+      <c r="B1" t="s">
         <v>862</v>
-      </c>
-      <c r="B1" t="s">
-        <v>863</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added in batch script for processing scripts 1 to 5, which cautiously we can try out
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFAC5CF8-DCF1-4E7C-AAC5-27D7E1CFD6A5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9B451F-C7F4-417B-A354-432256A54E3E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="2" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="3" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -2874,76 +2874,76 @@
     <t>Carl</t>
   </si>
   <si>
-    <t xml:space="preserve">osm_adelaide_gccsa_2018_10000m_epsg4326_pedestrian_20181001 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">osm_bris_gccsa_2018_10000m_epsg4326_pedestrian_20181001 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">osm_canberra_gccsa_2018_10000m_epsg4326_pedestrian_20181001 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">osm_darwin_gccsa_2018_10000m_epsg4326_pedestrian_20181001 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">osm_hobart_gccsa_2018_10000m_epsg4326_pedestrian_20181001 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">osm_melb_gccsa_2018_10000m_epsg4326_pedestrian_20181001 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">osm_perth_gccsa_2018_10000m_epsg4326_pedestrian_20181001 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">osm_syd_gccsa_2018_10000m_epsg4326_pedestrian_20181001 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">osm_mitchell_lga_2018_10000m_epsg4326_pedestrian_20181001 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">osm_alburywodonga__sua_2018_10000m_epsg4326_pedestrian_20181001 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">osm_ballarat__sua_2018_10000m_epsg4326_pedestrian_20181001 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">osm_bendigo__sua_2018_10000m_epsg4326_pedestrian_20181001 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">osm_cairns__sua_2018_10000m_epsg4326_pedestrian_20181001 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">osm_geelong__sua_2018_10000m_epsg4326_pedestrian_20181001 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">osm_goldcoast__sua_2018_10000m_epsg4326_pedestrian_20181001 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">osm_launceston__sua_2018_10000m_epsg4326_pedestrian_20181001 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">osm_mackay__sua_2018_10000m_epsg4326_pedestrian_20181001 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">osm_newcastle__sua_2018_10000m_epsg4326_pedestrian_20181001 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">osm_sunshinecoast__sua_2018_10000m_epsg4326_pedestrian_20181001 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">osm_toowoomba__sua_2018_10000m_epsg4326_pedestrian_20181001 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">osm_townsville__sua_2018_10000m_epsg4326_pedestrian_20181001 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">osm_westernsydney__sua_2018_10000m_epsg4326_pedestrian_20181001 </t>
-  </si>
-  <si>
     <t>osm_wollongong__sua_2018_10000m_epsg4326_pedestrian_20181001</t>
   </si>
   <si>
     <t>Australian National Liveability Indicators, 2018</t>
+  </si>
+  <si>
+    <t>osm_adelaide_gccsa_2018_10000m_epsg4326_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t>osm_bris_gccsa_2018_10000m_epsg4326_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t>osm_canberra_gccsa_2018_10000m_epsg4326_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t>osm_darwin_gccsa_2018_10000m_epsg4326_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t>osm_hobart_gccsa_2018_10000m_epsg4326_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t>osm_melb_gccsa_2018_10000m_epsg4326_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t>osm_perth_gccsa_2018_10000m_epsg4326_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t>osm_syd_gccsa_2018_10000m_epsg4326_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t>osm_mitchell_lga_2018_10000m_epsg4326_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t>osm_alburywodonga__sua_2018_10000m_epsg4326_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t>osm_ballarat__sua_2018_10000m_epsg4326_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t>osm_bendigo__sua_2018_10000m_epsg4326_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t>osm_cairns__sua_2018_10000m_epsg4326_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t>osm_geelong__sua_2018_10000m_epsg4326_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t>osm_goldcoast__sua_2018_10000m_epsg4326_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t>osm_launceston__sua_2018_10000m_epsg4326_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t>osm_mackay__sua_2018_10000m_epsg4326_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t>osm_newcastle__sua_2018_10000m_epsg4326_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t>osm_sunshinecoast__sua_2018_10000m_epsg4326_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t>osm_toowoomba__sua_2018_10000m_epsg4326_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t>osm_townsville__sua_2018_10000m_epsg4326_pedestrian_20181001</t>
+  </si>
+  <si>
+    <t>osm_westernsydney__sua_2018_10000m_epsg4326_pedestrian_20181001</t>
   </si>
 </sst>
 </file>
@@ -4029,7 +4029,7 @@
   <sheetData>
     <row r="1" spans="1:1" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>938</v>
+        <v>916</v>
       </c>
     </row>
     <row r="2" spans="1:1" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4555,7 +4555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3E5F03-EC28-486B-BA51-9D83D1ACCD02}">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
@@ -5400,11 +5400,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317EB008-F691-4F16-B99A-D5845A82BBBD}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C33" sqref="C33"/>
+      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5555,7 +5555,7 @@
         <v>877</v>
       </c>
       <c r="K3" s="75" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="L3" s="75"/>
       <c r="M3" s="75"/>
@@ -5598,7 +5598,7 @@
         <v>877</v>
       </c>
       <c r="K4" s="79" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="L4" s="79" t="s">
         <v>834</v>
@@ -5644,7 +5644,7 @@
         <v>877</v>
       </c>
       <c r="K5" s="82" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="L5" s="82"/>
       <c r="M5" s="82"/>
@@ -5687,7 +5687,7 @@
         <v>877</v>
       </c>
       <c r="K6" s="79" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="L6" s="79"/>
       <c r="M6" s="79"/>
@@ -5729,7 +5729,7 @@
         <v>877</v>
       </c>
       <c r="K7" s="82" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="L7" s="82"/>
       <c r="M7" s="82"/>
@@ -5772,7 +5772,7 @@
         <v>877</v>
       </c>
       <c r="K8" s="79" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="L8" s="79" t="s">
         <v>835</v>
@@ -5820,7 +5820,7 @@
         <v>877</v>
       </c>
       <c r="K9" s="82" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="L9" s="82" t="s">
         <v>837</v>
@@ -5867,7 +5867,7 @@
         <v>877</v>
       </c>
       <c r="K10" s="79" t="s">
-        <v>922</v>
+        <v>924</v>
       </c>
       <c r="L10" s="79" t="s">
         <v>836</v>
@@ -5915,7 +5915,7 @@
         <v>877</v>
       </c>
       <c r="K11" s="82" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="L11" s="82"/>
       <c r="M11" s="82"/>
@@ -5958,7 +5958,7 @@
         <v>877</v>
       </c>
       <c r="K12" s="82" t="s">
-        <v>924</v>
+        <v>926</v>
       </c>
       <c r="L12" s="84"/>
       <c r="M12" s="80" t="s">
@@ -6002,7 +6002,7 @@
         <v>877</v>
       </c>
       <c r="K13" s="82" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="L13" s="82"/>
       <c r="M13" s="83" t="s">
@@ -6047,7 +6047,7 @@
         <v>877</v>
       </c>
       <c r="K14" s="82" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="L14" s="79"/>
       <c r="M14" s="80" t="s">
@@ -6091,7 +6091,7 @@
         <v>877</v>
       </c>
       <c r="K15" s="82" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="L15" s="82"/>
       <c r="M15" s="83" t="s">
@@ -6136,7 +6136,7 @@
         <v>877</v>
       </c>
       <c r="K16" s="82" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="L16" s="79"/>
       <c r="M16" s="80" t="s">
@@ -6180,7 +6180,7 @@
         <v>877</v>
       </c>
       <c r="K17" s="82" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
       <c r="L17" s="82"/>
       <c r="M17" s="83" t="s">
@@ -6225,7 +6225,7 @@
         <v>877</v>
       </c>
       <c r="K18" s="82" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="L18" s="79"/>
       <c r="M18" s="79" t="s">
@@ -6269,7 +6269,7 @@
         <v>877</v>
       </c>
       <c r="K19" s="82" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="L19" s="82"/>
       <c r="M19" s="83" t="s">
@@ -6314,7 +6314,7 @@
         <v>877</v>
       </c>
       <c r="K20" s="82" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="L20" s="79"/>
       <c r="M20" s="80" t="s">
@@ -6358,7 +6358,7 @@
         <v>877</v>
       </c>
       <c r="K21" s="82" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="L21" s="82"/>
       <c r="M21" s="83" t="s">
@@ -6403,7 +6403,7 @@
         <v>877</v>
       </c>
       <c r="K22" s="82" t="s">
-        <v>934</v>
+        <v>936</v>
       </c>
       <c r="L22" s="79"/>
       <c r="M22" s="80" t="s">
@@ -6447,7 +6447,7 @@
         <v>877</v>
       </c>
       <c r="K23" s="82" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="L23" s="82"/>
       <c r="M23" s="83" t="s">
@@ -6492,7 +6492,7 @@
         <v>877</v>
       </c>
       <c r="K24" s="82" t="s">
-        <v>937</v>
+        <v>915</v>
       </c>
       <c r="L24" s="79"/>
       <c r="M24" s="80" t="s">
@@ -6536,7 +6536,7 @@
         <v>877</v>
       </c>
       <c r="K25" s="82" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="L25" s="83"/>
       <c r="M25" s="83" t="s">

</xml_diff>

<commit_message>
updated the ind spreadsheet to divvy out Western syd to julianna
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9B451F-C7F4-417B-A354-432256A54E3E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFD550C-1686-4ED3-BB41-9510D24699B8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="3" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
@@ -4019,7 +4019,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5401,10 +5401,10 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
+      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6511,7 +6511,7 @@
         <v>881</v>
       </c>
       <c r="C25" s="82" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="D25" s="82" t="s">
         <v>462</v>

</xml_diff>

<commit_message>
the 21 cities notebook's clean intersections processing is confirmed to work programatically (with exception of requirement to manually run the printed call to ogr2ogr); now to validate with Bec
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DFB7DA-BC50-4856-A5E1-13C6B3D6DA91}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C66DD61-3E2D-429C-9B1F-B1EE9BDADD53}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="1" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -3196,16 +3196,10 @@
     <t>linear_feature_criteria_AND</t>
   </si>
   <si>
-    <t>amal_toarea_ratio &gt; 140</t>
-  </si>
-  <si>
     <t>area_ha &gt; 0.5</t>
   </si>
   <si>
     <t>medial_axis_length &gt; 300</t>
-  </si>
-  <si>
-    <t>num_symdiff_convull_geoms &gt; 0</t>
   </si>
   <si>
     <t>roundness &lt; 0.25</t>
@@ -3334,6 +3328,12 @@
   </si>
   <si>
     <t>A list of OSM and derived data columns which should be included as open_space feature tags (in addition to existing tags) when collating open space features to an Area of Open Space.</t>
+  </si>
+  <si>
+    <t>amal_to_area_ratio &gt; 140</t>
+  </si>
+  <si>
+    <t>num_symdiff_convhull_geoms &gt; 0</t>
   </si>
 </sst>
 </file>
@@ -4077,6 +4077,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4091,12 +4097,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4471,7 +4471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{169A8F36-66C8-40F7-A0A8-79F453EFA097}">
   <dimension ref="A1:D16445"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A54" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A54" workbookViewId="0">
       <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
@@ -4935,7 +4935,7 @@
     </row>
     <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="47"/>
-      <c r="B57" s="109" t="s">
+      <c r="B57" s="104" t="s">
         <v>316</v>
       </c>
       <c r="C57" s="68" t="s">
@@ -4944,10 +4944,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="D58" s="63" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -4955,7 +4955,7 @@
         <v>968</v>
       </c>
       <c r="C59" s="64" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4963,7 +4963,7 @@
         <v>950</v>
       </c>
       <c r="C60" s="64" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -4971,7 +4971,7 @@
         <v>975</v>
       </c>
       <c r="C61" s="64" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -4979,7 +4979,7 @@
         <v>969</v>
       </c>
       <c r="C62" s="64" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -4987,7 +4987,7 @@
         <v>976</v>
       </c>
       <c r="C63" s="64" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -4995,7 +4995,7 @@
         <v>1008</v>
       </c>
       <c r="C64" s="64" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5003,34 +5003,34 @@
         <v>1021</v>
       </c>
       <c r="C65" s="64" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B66" s="63" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="C66" s="64" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B67" s="63" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="C67" s="64" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B68" s="110"/>
+      <c r="B68" s="105"/>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B69" s="110"/>
+      <c r="B69" s="105"/>
       <c r="C69"/>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B70" s="110"/>
+      <c r="B70" s="105"/>
       <c r="C70"/>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
@@ -55014,10 +55014,10 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomRight" activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56914,8 +56914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:I1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56954,10 +56954,10 @@
         <v>1021</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="I1" s="37" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -56980,13 +56980,13 @@
         <v>1009</v>
       </c>
       <c r="G2" t="s">
-        <v>1022</v>
+        <v>1066</v>
       </c>
       <c r="H2" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="I2" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -57009,13 +57009,13 @@
         <v>1010</v>
       </c>
       <c r="G3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="H3" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="I3" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -57032,13 +57032,13 @@
         <v>1011</v>
       </c>
       <c r="G4" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="H4" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="I4" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -57055,10 +57055,10 @@
         <v>1012</v>
       </c>
       <c r="G5" t="s">
-        <v>1025</v>
+        <v>1067</v>
       </c>
       <c r="H5" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="I5" t="s">
         <v>944</v>
@@ -57078,10 +57078,10 @@
         <v>1013</v>
       </c>
       <c r="G6" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="H6" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="I6" t="s">
         <v>948</v>
@@ -57101,7 +57101,7 @@
         <v>1014</v>
       </c>
       <c r="H7" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="I7" t="s">
         <v>945</v>
@@ -57121,7 +57121,7 @@
         <v>1015</v>
       </c>
       <c r="H8" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="I8" t="s">
         <v>946</v>
@@ -57141,7 +57141,7 @@
         <v>1016</v>
       </c>
       <c r="H9" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="I9" t="s">
         <v>947</v>
@@ -57181,7 +57181,7 @@
         <v>1017</v>
       </c>
       <c r="H11" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="I11" t="s">
         <v>967</v>
@@ -57201,10 +57201,10 @@
         <v>1018</v>
       </c>
       <c r="H12" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="I12" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -57218,10 +57218,10 @@
         <v>1019</v>
       </c>
       <c r="H13" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="I13" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -57235,10 +57235,10 @@
         <v>1020</v>
       </c>
       <c r="H14" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="I14" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -57249,10 +57249,10 @@
         <v>989</v>
       </c>
       <c r="H15" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="I15" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -57263,10 +57263,10 @@
         <v>990</v>
       </c>
       <c r="H16" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="I16" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -57277,10 +57277,10 @@
         <v>991</v>
       </c>
       <c r="H17" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="I17" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -57291,10 +57291,10 @@
         <v>992</v>
       </c>
       <c r="H18" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="I18" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -57305,10 +57305,10 @@
         <v>962</v>
       </c>
       <c r="H19" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="I19" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -57457,31 +57457,31 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="104" t="s">
+      <c r="G1" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="105"/>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
-      <c r="Q1" s="105"/>
-      <c r="R1" s="105"/>
-      <c r="S1" s="105"/>
-      <c r="T1" s="105"/>
-      <c r="U1" s="105"/>
-      <c r="V1" s="105"/>
-      <c r="W1" s="105"/>
-      <c r="X1" s="106"/>
-      <c r="Y1" s="107" t="s">
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="107"/>
+      <c r="S1" s="107"/>
+      <c r="T1" s="107"/>
+      <c r="U1" s="107"/>
+      <c r="V1" s="107"/>
+      <c r="W1" s="107"/>
+      <c r="X1" s="108"/>
+      <c r="Y1" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="Z1" s="105"/>
-      <c r="AA1" s="108"/>
+      <c r="Z1" s="107"/>
+      <c r="AA1" s="110"/>
       <c r="AB1" s="2" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
fixed some bugs in externalised variables for AOS set up script
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C66DD61-3E2D-429C-9B1F-B1EE9BDADD53}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354B11B3-1783-4700-A358-A147D651EE17}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
@@ -56915,7 +56915,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
improved specific inclusion criteria logic (was broken when externalised; now fixed -- specifically to recognise potential for landuse to be legitimately null as alternative when checking that landuse is not military)
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354B11B3-1783-4700-A358-A147D651EE17}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EC569A-D0AE-4DBB-9BA5-8362C79793A2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" firstSheet="1" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -3049,9 +3049,6 @@
     <t>p.access IS NULL OR p.access NOT IN('no','private')</t>
   </si>
   <si>
-    <t>p.landuse NOT IN ('military')</t>
-  </si>
-  <si>
     <t>inclusion explanation (p. is shorthand for the 'park' table where the open space data is)</t>
   </si>
   <si>
@@ -3334,6 +3331,9 @@
   </si>
   <si>
     <t>num_symdiff_convhull_geoms &gt; 0</t>
+  </si>
+  <si>
+    <t>p.landuse IS NULL OR p.landuse NOT IN ('military')</t>
   </si>
 </sst>
 </file>
@@ -4944,10 +4944,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D58" s="63" t="s">
         <v>1025</v>
-      </c>
-      <c r="D58" s="63" t="s">
-        <v>1026</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -4955,7 +4955,7 @@
         <v>968</v>
       </c>
       <c r="C59" s="64" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4963,15 +4963,15 @@
         <v>950</v>
       </c>
       <c r="C60" s="64" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B61" s="63" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="C61" s="64" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -4979,47 +4979,47 @@
         <v>969</v>
       </c>
       <c r="C62" s="64" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B63" s="63" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="C63" s="64" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="63" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C64" s="64" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="63" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="C65" s="64" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B66" s="63" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="C66" s="64" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B67" s="63" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="C67" s="64" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
@@ -55014,10 +55014,10 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H30" sqref="H30"/>
+      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56914,8 +56914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56939,25 +56939,25 @@
         <v>950</v>
       </c>
       <c r="C1" s="37" t="s">
+        <v>974</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>973</v>
+      </c>
+      <c r="E1" s="37" t="s">
         <v>975</v>
       </c>
-      <c r="D1" s="37" t="s">
-        <v>974</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>976</v>
-      </c>
       <c r="F1" s="37" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="G1" s="37" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="I1" s="37" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -56974,19 +56974,19 @@
         <v>970</v>
       </c>
       <c r="E2" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="F2" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="G2" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="H2" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="I2" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -56997,25 +56997,25 @@
         <v>952</v>
       </c>
       <c r="C3" t="s">
-        <v>973</v>
+        <v>1067</v>
       </c>
       <c r="D3" t="s">
         <v>971</v>
       </c>
       <c r="E3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="F3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="G3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="H3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="I3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -57026,19 +57026,19 @@
         <v>953</v>
       </c>
       <c r="E4" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="F4" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="G4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="H4" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="I4" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -57052,13 +57052,13 @@
         <v>939</v>
       </c>
       <c r="F5" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="G5" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="H5" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="I5" t="s">
         <v>944</v>
@@ -57072,16 +57072,16 @@
         <v>955</v>
       </c>
       <c r="E6" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="F6" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="G6" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="H6" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="I6" t="s">
         <v>948</v>
@@ -57095,13 +57095,13 @@
         <v>956</v>
       </c>
       <c r="E7" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="F7" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="H7" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="I7" t="s">
         <v>945</v>
@@ -57115,13 +57115,13 @@
         <v>957</v>
       </c>
       <c r="E8" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="F8" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="H8" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="I8" t="s">
         <v>946</v>
@@ -57135,13 +57135,13 @@
         <v>945</v>
       </c>
       <c r="E9" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="F9" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="H9" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="I9" t="s">
         <v>947</v>
@@ -57155,10 +57155,10 @@
         <v>958</v>
       </c>
       <c r="E10" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="F10" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="H10" t="s">
         <v>695</v>
@@ -57175,13 +57175,13 @@
         <v>959</v>
       </c>
       <c r="E11" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F11" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="H11" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="I11" t="s">
         <v>967</v>
@@ -57195,16 +57195,16 @@
         <v>960</v>
       </c>
       <c r="E12" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="F12" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="H12" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="I12" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -57212,16 +57212,16 @@
         <v>961</v>
       </c>
       <c r="E13" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="F13" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="H13" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="I13" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -57229,16 +57229,16 @@
         <v>962</v>
       </c>
       <c r="E14" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="F14" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="H14" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="I14" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -57246,13 +57246,13 @@
         <v>963</v>
       </c>
       <c r="E15" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="H15" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="I15" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -57260,13 +57260,13 @@
         <v>947</v>
       </c>
       <c r="E16" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="H16" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="I16" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -57274,13 +57274,13 @@
         <v>964</v>
       </c>
       <c r="E17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="H17" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="I17" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -57288,13 +57288,13 @@
         <v>965</v>
       </c>
       <c r="E18" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="H18" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="I18" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -57305,10 +57305,10 @@
         <v>962</v>
       </c>
       <c r="H19" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="I19" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -57324,62 +57324,62 @@
         <v>967</v>
       </c>
       <c r="E21" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="33" spans="5:5" x14ac:dyDescent="0.25">
@@ -57389,17 +57389,17 @@
     </row>
     <row r="34" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="35" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="36" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="37" spans="5:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added in brisbane testing sketch to testing branch
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EC569A-D0AE-4DBB-9BA5-8362C79793A2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C348FEB-BCDE-4AFA-9E36-BDC0C7EE20B6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" firstSheet="1" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2245" uniqueCount="1068">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2261" uniqueCount="1081">
   <si>
     <t>Domain</t>
   </si>
@@ -3334,6 +3334,45 @@
   </si>
   <si>
     <t>p.landuse IS NULL OR p.landuse NOT IN ('military')</t>
+  </si>
+  <si>
+    <t>recreation_ground</t>
+  </si>
+  <si>
+    <t>village_green</t>
+  </si>
+  <si>
+    <t>cemetary</t>
+  </si>
+  <si>
+    <t>os_boundary</t>
+  </si>
+  <si>
+    <t>nature_reserve</t>
+  </si>
+  <si>
+    <t>protected_area</t>
+  </si>
+  <si>
+    <t>national_park</t>
+  </si>
+  <si>
+    <t>water_protection_area</t>
+  </si>
+  <si>
+    <t>boundary</t>
+  </si>
+  <si>
+    <t>state_forest</t>
+  </si>
+  <si>
+    <t>state_park</t>
+  </si>
+  <si>
+    <t>regional_park</t>
+  </si>
+  <si>
+    <t>county_park</t>
   </si>
 </sst>
 </file>
@@ -56912,26 +56951,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="45.140625" customWidth="1"/>
-    <col min="4" max="4" width="94.5703125" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="31" customWidth="1"/>
-    <col min="8" max="8" width="29.140625" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" customWidth="1"/>
+    <col min="2" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" customWidth="1"/>
+    <col min="5" max="5" width="94.5703125" customWidth="1"/>
+    <col min="6" max="6" width="41.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="31" customWidth="1"/>
+    <col min="9" max="9" width="29.140625" customWidth="1"/>
+    <col min="10" max="10" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>968</v>
       </c>
@@ -56939,28 +56978,31 @@
         <v>950</v>
       </c>
       <c r="C1" s="37" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D1" s="37" t="s">
         <v>974</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="E1" s="37" t="s">
         <v>973</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="F1" s="37" t="s">
         <v>975</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="G1" s="37" t="s">
         <v>1007</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="H1" s="37" t="s">
         <v>1020</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="I1" s="37" t="s">
         <v>1046</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="J1" s="37" t="s">
         <v>1058</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>939</v>
       </c>
@@ -56968,447 +57010,492 @@
         <v>951</v>
       </c>
       <c r="C2" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D2" t="s">
         <v>972</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>970</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>976</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>1008</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>1065</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>1029</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>1047</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>940</v>
       </c>
       <c r="B3" t="s">
-        <v>952</v>
+        <v>1070</v>
       </c>
       <c r="C3" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D3" t="s">
         <v>1067</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>971</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>977</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>1009</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>1021</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>1030</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>1048</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>941</v>
       </c>
       <c r="B4" t="s">
-        <v>953</v>
-      </c>
-      <c r="E4" t="s">
+        <v>952</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F4" t="s">
         <v>978</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>1010</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>1022</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>1031</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>1052</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>942</v>
       </c>
       <c r="B5" t="s">
+        <v>953</v>
+      </c>
+      <c r="C5" t="s">
         <v>954</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>939</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>1011</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>1066</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>1032</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>944</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>943</v>
       </c>
       <c r="B6" t="s">
-        <v>955</v>
-      </c>
-      <c r="E6" t="s">
+        <v>954</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1075</v>
+      </c>
+      <c r="F6" t="s">
         <v>979</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>1012</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>1023</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>1033</v>
       </c>
-      <c r="I6" t="s">
-        <v>948</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>944</v>
       </c>
       <c r="B7" t="s">
-        <v>956</v>
-      </c>
-      <c r="E7" t="s">
+        <v>955</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F7" t="s">
         <v>980</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>1013</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>1034</v>
       </c>
-      <c r="I7" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>945</v>
       </c>
       <c r="B8" t="s">
-        <v>957</v>
-      </c>
-      <c r="E8" t="s">
+        <v>956</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F8" t="s">
         <v>981</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>1014</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>1035</v>
       </c>
-      <c r="I8" t="s">
-        <v>946</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>946</v>
       </c>
       <c r="B9" t="s">
-        <v>945</v>
-      </c>
-      <c r="E9" t="s">
+        <v>957</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F9" t="s">
         <v>982</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>1015</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>1036</v>
       </c>
-      <c r="I9" t="s">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>947</v>
       </c>
       <c r="B10" t="s">
-        <v>958</v>
-      </c>
-      <c r="E10" t="s">
+        <v>945</v>
+      </c>
+      <c r="C10" t="s">
+        <v>960</v>
+      </c>
+      <c r="F10" t="s">
         <v>983</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>1007</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>695</v>
       </c>
-      <c r="I10" t="s">
-        <v>942</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>948</v>
       </c>
       <c r="B11" t="s">
-        <v>959</v>
-      </c>
-      <c r="E11" t="s">
+        <v>958</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1080</v>
+      </c>
+      <c r="F11" t="s">
         <v>984</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>1016</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>1037</v>
       </c>
-      <c r="I11" t="s">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>949</v>
       </c>
       <c r="B12" t="s">
+        <v>959</v>
+      </c>
+      <c r="F12" t="s">
+        <v>985</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1017</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1038</v>
+      </c>
+      <c r="J12" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B13" t="s">
         <v>960</v>
       </c>
-      <c r="E12" t="s">
-        <v>985</v>
-      </c>
-      <c r="F12" t="s">
-        <v>1017</v>
-      </c>
-      <c r="H12" t="s">
-        <v>1038</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="F13" t="s">
+        <v>986</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1018</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1039</v>
+      </c>
+      <c r="J13" t="s">
         <v>1053</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>961</v>
       </c>
-      <c r="E13" t="s">
-        <v>986</v>
-      </c>
-      <c r="F13" t="s">
-        <v>1018</v>
-      </c>
-      <c r="H13" t="s">
-        <v>1039</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="F14" t="s">
+        <v>987</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1019</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1040</v>
+      </c>
+      <c r="J14" t="s">
         <v>1054</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>962</v>
       </c>
-      <c r="E14" t="s">
-        <v>987</v>
-      </c>
-      <c r="F14" t="s">
-        <v>1019</v>
-      </c>
-      <c r="H14" t="s">
-        <v>1040</v>
-      </c>
-      <c r="I14" t="s">
+      <c r="F15" t="s">
+        <v>988</v>
+      </c>
+      <c r="I15" t="s">
+        <v>1041</v>
+      </c>
+      <c r="J15" t="s">
         <v>1055</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>963</v>
       </c>
-      <c r="E15" t="s">
-        <v>988</v>
-      </c>
-      <c r="H15" t="s">
-        <v>1041</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="F16" t="s">
+        <v>989</v>
+      </c>
+      <c r="I16" t="s">
+        <v>1042</v>
+      </c>
+      <c r="J16" t="s">
         <v>1049</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>1068</v>
+      </c>
+      <c r="F17" t="s">
+        <v>990</v>
+      </c>
+      <c r="I17" t="s">
+        <v>1043</v>
+      </c>
+      <c r="J17" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>947</v>
       </c>
-      <c r="E16" t="s">
-        <v>989</v>
-      </c>
-      <c r="H16" t="s">
-        <v>1042</v>
-      </c>
-      <c r="I16" t="s">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="F18" t="s">
+        <v>991</v>
+      </c>
+      <c r="I18" t="s">
+        <v>1044</v>
+      </c>
+      <c r="J18" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>964</v>
       </c>
-      <c r="E17" t="s">
-        <v>990</v>
-      </c>
-      <c r="H17" t="s">
-        <v>1043</v>
-      </c>
-      <c r="I17" t="s">
-        <v>1051</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="F19" t="s">
+        <v>962</v>
+      </c>
+      <c r="I19" t="s">
+        <v>1045</v>
+      </c>
+      <c r="J19" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F20" t="s">
+        <v>940</v>
+      </c>
+      <c r="J20" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>965</v>
       </c>
-      <c r="E18" t="s">
-        <v>991</v>
-      </c>
-      <c r="H18" t="s">
-        <v>1044</v>
-      </c>
-      <c r="I18" t="s">
-        <v>1056</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="F21" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>941</v>
       </c>
-      <c r="E19" t="s">
-        <v>962</v>
-      </c>
-      <c r="H19" t="s">
-        <v>1045</v>
-      </c>
-      <c r="I19" t="s">
-        <v>1057</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="F22" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>966</v>
       </c>
-      <c r="E20" t="s">
-        <v>940</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="F23" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>967</v>
       </c>
-      <c r="E21" t="s">
-        <v>992</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
-        <v>993</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E23" t="s">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>995</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E25" t="s">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
         <v>996</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E26" t="s">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
         <v>997</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E27" t="s">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
         <v>998</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E28" t="s">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
         <v>999</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E29" t="s">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
         <v>1000</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E30" t="s">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
         <v>1001</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E31" t="s">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
         <v>1002</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E32" t="s">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
         <v>1003</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E33" t="s">
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
         <v>941</v>
       </c>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E34" t="s">
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
         <v>1004</v>
       </c>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E35" t="s">
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
         <v>1005</v>
       </c>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E36" t="s">
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
         <v>1006</v>
       </c>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E37" t="s">
+    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
         <v>942</v>
       </c>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E38" t="s">
+    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
         <v>943</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated files in test branch with important changes relevant to all --- ie. nWorkers is now a configuration parameter (multiprocessing), and also some changes to the AOS set up script
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C348FEB-BCDE-4AFA-9E36-BDC0C7EE20B6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAC0264-5A68-4CED-B67A-D124387FB875}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" firstSheet="1" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="2" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2261" uniqueCount="1081">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2264" uniqueCount="1083">
   <si>
     <t>Domain</t>
   </si>
@@ -3373,6 +3373,12 @@
   </si>
   <si>
     <t>county_park</t>
+  </si>
+  <si>
+    <t>multiprocessing</t>
+  </si>
+  <si>
+    <t>Number of processors to use in multiprocessing scripts</t>
   </si>
 </sst>
 </file>
@@ -54205,11 +54211,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3E5F03-EC28-486B-BA51-9D83D1ACCD02}">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54376,38 +54382,38 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>735</v>
-      </c>
-      <c r="B12" s="69" t="s">
-        <v>738</v>
+        <v>1081</v>
+      </c>
+      <c r="B12" s="69">
+        <v>7</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>796</v>
+        <v>801</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>742</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>736</v>
-      </c>
-      <c r="B13" s="69">
-        <v>5432</v>
+        <v>735</v>
+      </c>
+      <c r="B13" s="69" t="s">
+        <v>738</v>
       </c>
       <c r="C13" s="38" t="s">
         <v>796</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>737</v>
-      </c>
-      <c r="B14" s="69" t="s">
-        <v>739</v>
+        <v>736</v>
+      </c>
+      <c r="B14" s="69">
+        <v>5432</v>
       </c>
       <c r="C14" s="38" t="s">
         <v>796</v>
@@ -54418,10 +54424,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>854</v>
+        <v>737</v>
       </c>
       <c r="B15" s="69" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C15" s="38" t="s">
         <v>796</v>
@@ -54432,10 +54438,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>744</v>
+        <v>854</v>
       </c>
       <c r="B16" s="69" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="C16" s="38" t="s">
         <v>796</v>
@@ -54446,94 +54452,94 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>870</v>
+        <v>744</v>
       </c>
       <c r="B17" s="69" t="s">
-        <v>874</v>
+        <v>745</v>
       </c>
       <c r="C17" s="38" t="s">
         <v>796</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>875</v>
+        <v>741</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B18" s="69" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="C18" s="38" t="s">
         <v>796</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>720</v>
+        <v>871</v>
       </c>
       <c r="B19" s="69" t="s">
-        <v>717</v>
+        <v>872</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>718</v>
+        <v>873</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B20" s="69" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
       <c r="C20" s="38" t="s">
         <v>797</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="B21" s="69" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="B22" s="69" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="C22" s="38" t="s">
         <v>798</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B23" s="69" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C23" s="38" t="s">
         <v>798</v>
@@ -54544,287 +54550,287 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="B24" s="69" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="C24" s="38" t="s">
         <v>798</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>746</v>
+        <v>732</v>
       </c>
       <c r="B25" s="69" t="s">
-        <v>747</v>
+        <v>734</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>773</v>
+        <v>733</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="B26" s="69" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="C26" s="38" t="s">
         <v>799</v>
       </c>
+      <c r="D26" s="38" t="s">
+        <v>773</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B27" s="69" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="C27" s="38" t="s">
         <v>799</v>
       </c>
-      <c r="D27" s="38" t="s">
-        <v>771</v>
-      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>759</v>
+        <v>750</v>
       </c>
       <c r="B28" s="69" t="s">
-        <v>764</v>
+        <v>751</v>
       </c>
       <c r="C28" s="38" t="s">
         <v>799</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B29" s="69" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C29" s="38" t="s">
         <v>799</v>
       </c>
       <c r="D29" s="38" t="s">
-        <v>768</v>
+        <v>772</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B30" s="69" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C30" s="38" t="s">
         <v>799</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B31" s="69" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C31" s="38" t="s">
         <v>799</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B32" s="69" t="s">
-        <v>774</v>
+        <v>767</v>
       </c>
       <c r="C32" s="38" t="s">
         <v>799</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>786</v>
+        <v>770</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>778</v>
+        <v>763</v>
       </c>
       <c r="B33" s="69" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C33" s="38" t="s">
         <v>799</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B34" s="69" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C34" s="38" t="s">
         <v>799</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B35" s="69" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C35" s="38" t="s">
         <v>799</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B36" s="69" t="s">
-        <v>567</v>
+        <v>777</v>
       </c>
       <c r="C36" s="38" t="s">
         <v>799</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B37" s="69" t="s">
-        <v>784</v>
+        <v>567</v>
       </c>
       <c r="C37" s="38" t="s">
         <v>799</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B38" s="69" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="C38" s="38" t="s">
         <v>799</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>793</v>
+        <v>783</v>
       </c>
       <c r="B39" s="69" t="s">
-        <v>802</v>
+        <v>785</v>
       </c>
       <c r="C39" s="38" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D39" s="38" t="s">
-        <v>803</v>
+        <v>792</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>794</v>
-      </c>
-      <c r="B40" s="69">
-        <v>7844</v>
+        <v>793</v>
+      </c>
+      <c r="B40" s="69" t="s">
+        <v>802</v>
       </c>
       <c r="C40" s="38" t="s">
         <v>800</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>805</v>
-      </c>
-      <c r="B41" s="69" t="s">
-        <v>806</v>
+        <v>794</v>
+      </c>
+      <c r="B41" s="69">
+        <v>7844</v>
       </c>
       <c r="C41" s="38" t="s">
-        <v>806</v>
+        <v>800</v>
       </c>
       <c r="D41" s="38" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="B42" s="69" t="s">
-        <v>811</v>
+        <v>806</v>
       </c>
       <c r="C42" s="38" t="s">
         <v>806</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>814</v>
+        <v>807</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B43" s="69" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C43" s="38" t="s">
         <v>806</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>741</v>
+        <v>814</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B44" s="69" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C44" s="38" t="s">
         <v>806</v>
@@ -54835,38 +54841,38 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>815</v>
+        <v>810</v>
       </c>
       <c r="B45" s="69" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="C45" s="38" t="s">
         <v>806</v>
       </c>
       <c r="D45" s="38" t="s">
-        <v>817</v>
+        <v>741</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="B46" s="69" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="C46" s="38" t="s">
-        <v>798</v>
+        <v>806</v>
       </c>
       <c r="D46" s="38" t="s">
-        <v>857</v>
+        <v>817</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B47" s="69" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C47" s="38" t="s">
         <v>798</v>
@@ -54877,169 +54883,183 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>282</v>
-      </c>
-      <c r="B48" s="69">
-        <v>1600</v>
+        <v>819</v>
+      </c>
+      <c r="B48" s="69" t="s">
+        <v>821</v>
       </c>
       <c r="C48" s="38" t="s">
-        <v>823</v>
+        <v>798</v>
       </c>
       <c r="D48" s="38" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>822</v>
+        <v>282</v>
       </c>
       <c r="B49" s="69">
-        <v>500</v>
+        <v>1600</v>
       </c>
       <c r="C49" s="38" t="s">
         <v>823</v>
       </c>
       <c r="D49" s="38" t="s">
-        <v>827</v>
+        <v>856</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>855</v>
+        <v>822</v>
       </c>
       <c r="B50" s="69">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="C50" s="38" t="s">
         <v>823</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>824</v>
+        <v>855</v>
       </c>
       <c r="B51" s="69">
-        <v>3000</v>
+        <v>50</v>
       </c>
       <c r="C51" s="38" t="s">
         <v>823</v>
       </c>
       <c r="D51" s="38" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>884</v>
+        <v>824</v>
       </c>
       <c r="B52" s="69">
-        <v>3200</v>
+        <v>3000</v>
       </c>
       <c r="C52" s="38" t="s">
         <v>823</v>
       </c>
       <c r="D52" s="38" t="s">
-        <v>885</v>
+        <v>825</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>828</v>
+        <v>884</v>
       </c>
       <c r="B53" s="69">
-        <v>5</v>
+        <v>3200</v>
       </c>
       <c r="C53" s="38" t="s">
-        <v>831</v>
+        <v>823</v>
       </c>
       <c r="D53" s="38" t="s">
-        <v>832</v>
+        <v>885</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>838</v>
+        <v>828</v>
       </c>
       <c r="B54" s="69">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C54" s="38" t="s">
-        <v>840</v>
+        <v>831</v>
       </c>
       <c r="D54" s="38" t="s">
-        <v>839</v>
+        <v>832</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>841</v>
-      </c>
-      <c r="B55" s="69" t="s">
-        <v>657</v>
+        <v>838</v>
+      </c>
+      <c r="B55" s="69">
+        <v>50</v>
       </c>
       <c r="C55" s="38" t="s">
-        <v>657</v>
+        <v>840</v>
       </c>
       <c r="D55" s="38" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="B56" s="69" t="s">
-        <v>844</v>
+        <v>657</v>
       </c>
       <c r="C56" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D56" s="38" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="B57" s="69" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="C57" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D57" s="38" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>847</v>
-      </c>
-      <c r="B58" s="69" t="b">
-        <v>0</v>
+        <v>846</v>
+      </c>
+      <c r="B58" s="69" t="s">
+        <v>848</v>
       </c>
       <c r="C58" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D58" s="38" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>851</v>
-      </c>
-      <c r="B59" s="69" t="s">
-        <v>853</v>
+        <v>847</v>
+      </c>
+      <c r="B59" s="69" t="b">
+        <v>0</v>
       </c>
       <c r="C59" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D59" s="38" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>851</v>
+      </c>
+      <c r="B60" s="69" t="s">
+        <v>853</v>
+      </c>
+      <c r="C60" s="38" t="s">
+        <v>657</v>
+      </c>
+      <c r="D60" s="38" t="s">
         <v>852</v>
       </c>
     </row>
@@ -55056,7 +55076,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomRight" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56953,8 +56973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated geelong to reflect no foward edge issues
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAC0264-5A68-4CED-B67A-D124387FB875}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA65BE6-1A4E-4CCE-A7B3-110D16821200}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="2" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="3" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -54213,9 +54213,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3E5F03-EC28-486B-BA51-9D83D1ACCD02}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55072,11 +55072,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317EB008-F691-4F16-B99A-D5845A82BBBD}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L4" sqref="L4"/>
+      <selection pane="bottomRight" activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55816,7 +55816,7 @@
       </c>
       <c r="N16" s="79"/>
       <c r="P16" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
school script is minimally functioning
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAC0264-5A68-4CED-B67A-D124387FB875}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5922137-CCDC-4120-B784-D00721B8A8B0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="2" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2264" uniqueCount="1083">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2276" uniqueCount="1092">
   <si>
     <t>Domain</t>
   </si>
@@ -3379,6 +3379,33 @@
   </si>
   <si>
     <t>Number of processors to use in multiprocessing scripts</t>
+  </si>
+  <si>
+    <t>school_destinations</t>
+  </si>
+  <si>
+    <t>All schools; these will be associated with OSM school polygons where possible</t>
+  </si>
+  <si>
+    <t>school_id</t>
+  </si>
+  <si>
+    <t>ACARA_Scho</t>
+  </si>
+  <si>
+    <t>The school id, as found in the source data</t>
+  </si>
+  <si>
+    <t>school_id_type</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>The data type of the source data (technically, in our case it is double, but I'm hoping we can treat as int; let's see)</t>
+  </si>
+  <si>
+    <t>all_schools2018</t>
   </si>
 </sst>
 </file>
@@ -54211,11 +54238,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3E5F03-EC28-486B-BA51-9D83D1ACCD02}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55061,6 +55088,48 @@
       </c>
       <c r="D60" s="38" t="s">
         <v>852</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B61" s="69" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C61" s="38" t="s">
+        <v>657</v>
+      </c>
+      <c r="D61" s="38" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B62" s="69" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C62" s="38" t="s">
+        <v>657</v>
+      </c>
+      <c r="D62" s="38" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B63" s="69" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C63" s="38" t="s">
+        <v>657</v>
+      </c>
+      <c r="D63" s="38" t="s">
+        <v>1090</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the set up schools script, but more work is needed to integrate the schools not matched to an osm polygon
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5922137-CCDC-4120-B784-D00721B8A8B0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA3E613-6ED8-4BF2-87B4-C5E4EB3DBB4E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="2" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2276" uniqueCount="1092">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2274" uniqueCount="1090">
   <si>
     <t>Domain</t>
   </si>
@@ -3019,13 +3019,7 @@
     <t>pond</t>
   </si>
   <si>
-    <t>recreation ground</t>
-  </si>
-  <si>
     <t>trees</t>
-  </si>
-  <si>
-    <t>village green</t>
   </si>
   <si>
     <t>winter_sports</t>
@@ -5016,18 +5010,18 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="D58" s="63" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B59" s="63" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="C59" s="64" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -5035,63 +5029,63 @@
         <v>950</v>
       </c>
       <c r="C60" s="64" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B61" s="63" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="C61" s="64" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" s="63" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="C62" s="64" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B63" s="63" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="C63" s="64" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="63" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="C64" s="64" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="63" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="C65" s="64" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B66" s="63" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="C66" s="64" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B67" s="63" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="C67" s="64" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
@@ -54240,8 +54234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3E5F03-EC28-486B-BA51-9D83D1ACCD02}">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
@@ -54409,7 +54403,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="B12" s="69">
         <v>7</v>
@@ -54418,7 +54412,7 @@
         <v>801</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -55092,44 +55086,44 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="B61" s="69" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="C61" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D61" s="38" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="B62" s="69" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="C62" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D62" s="38" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="B63" s="69" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="C63" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D63" s="38" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
     </row>
   </sheetData>
@@ -57042,8 +57036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57061,34 +57055,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="B1" s="37" t="s">
         <v>950</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="E1" s="37" t="s">
+        <v>971</v>
+      </c>
+      <c r="F1" s="37" t="s">
         <v>973</v>
       </c>
-      <c r="F1" s="37" t="s">
-        <v>975</v>
-      </c>
       <c r="G1" s="37" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="I1" s="37" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -57099,28 +57093,28 @@
         <v>951</v>
       </c>
       <c r="C2" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="D2" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="E2" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="F2" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="G2" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="H2" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="I2" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="J2" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -57128,31 +57122,31 @@
         <v>940</v>
       </c>
       <c r="B3" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="C3" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="D3" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="E3" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="F3" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="G3" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="H3" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="I3" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="J3" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -57163,22 +57157,22 @@
         <v>952</v>
       </c>
       <c r="C4" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="F4" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="G4" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="H4" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="I4" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="J4" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -57195,13 +57189,13 @@
         <v>939</v>
       </c>
       <c r="G5" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="H5" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="I5" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="J5" t="s">
         <v>944</v>
@@ -57215,22 +57209,22 @@
         <v>954</v>
       </c>
       <c r="C6" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="F6" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="G6" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="H6" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="I6" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="J6" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -57241,16 +57235,16 @@
         <v>955</v>
       </c>
       <c r="C7" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="F7" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="G7" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="I7" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="J7" t="s">
         <v>948</v>
@@ -57264,16 +57258,16 @@
         <v>956</v>
       </c>
       <c r="C8" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="F8" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="G8" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="I8" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="J8" t="s">
         <v>945</v>
@@ -57287,16 +57281,16 @@
         <v>957</v>
       </c>
       <c r="C9" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="F9" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="G9" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="I9" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="J9" t="s">
         <v>946</v>
@@ -57313,10 +57307,10 @@
         <v>960</v>
       </c>
       <c r="F10" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="G10" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="I10" t="s">
         <v>695</v>
@@ -57333,16 +57327,16 @@
         <v>958</v>
       </c>
       <c r="C11" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="F11" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="G11" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="I11" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="J11" t="s">
         <v>942</v>
@@ -57356,36 +57350,36 @@
         <v>959</v>
       </c>
       <c r="F12" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="G12" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="I12" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="J12" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="B13" t="s">
         <v>960</v>
       </c>
       <c r="F13" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="G13" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="I13" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="J13" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -57393,16 +57387,16 @@
         <v>961</v>
       </c>
       <c r="F14" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="G14" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="I14" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="J14" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -57410,152 +57404,146 @@
         <v>962</v>
       </c>
       <c r="F15" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="I15" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="J15" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>963</v>
+        <v>1066</v>
       </c>
       <c r="F16" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="I16" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="J16" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>1068</v>
+        <v>947</v>
       </c>
       <c r="F17" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="I17" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="J17" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>947</v>
+        <v>963</v>
       </c>
       <c r="F18" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="I18" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="J18" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>964</v>
+        <v>1067</v>
       </c>
       <c r="F19" t="s">
         <v>962</v>
       </c>
       <c r="I19" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="J19" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>1069</v>
+        <v>941</v>
       </c>
       <c r="F20" t="s">
         <v>940</v>
       </c>
       <c r="J20" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="F21" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>941</v>
+        <v>965</v>
       </c>
       <c r="F22" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
         <v>993</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>966</v>
-      </c>
-      <c r="F23" t="s">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>967</v>
-      </c>
-      <c r="F24" t="s">
-        <v>995</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.25">
@@ -57565,17 +57553,17 @@
     </row>
     <row r="34" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="35" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="36" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="37" spans="6:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated street connectivity to use OSMnx derived clean intersections, following advice from Bec that these are good
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA3E613-6ED8-4BF2-87B4-C5E4EB3DBB4E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1180E2B0-4147-44BB-822E-04C236B56EB0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="2" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2274" uniqueCount="1090">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2303" uniqueCount="1100">
   <si>
     <t>Domain</t>
   </si>
@@ -3400,6 +3400,36 @@
   </si>
   <si>
     <t>all_schools2018</t>
+  </si>
+  <si>
+    <t>clean_intersections_gpkg</t>
+  </si>
+  <si>
+    <t>A set of clean intersections pre-prepared for each study region using osmnx (see 21 cities .ipynb jupyter notebook in process folder)</t>
+  </si>
+  <si>
+    <t>alburywodonga</t>
+  </si>
+  <si>
+    <t>goldcoast</t>
+  </si>
+  <si>
+    <t>newcastle</t>
+  </si>
+  <si>
+    <t>sunshinecoast</t>
+  </si>
+  <si>
+    <t>westernsydney</t>
+  </si>
+  <si>
+    <t>nada</t>
+  </si>
+  <si>
+    <t>clean_intersections_locale</t>
+  </si>
+  <si>
+    <t>roads/li_intersections_2018.gpkg</t>
   </si>
 </sst>
 </file>
@@ -54232,11 +54262,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3E5F03-EC28-486B-BA51-9D83D1ACCD02}">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54834,38 +54864,38 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>808</v>
+        <v>1090</v>
       </c>
       <c r="B43" s="69" t="s">
-        <v>811</v>
+        <v>1099</v>
       </c>
       <c r="C43" s="38" t="s">
         <v>806</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>814</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B44" s="69" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C44" s="38" t="s">
         <v>806</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>741</v>
+        <v>814</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B45" s="69" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C45" s="38" t="s">
         <v>806</v>
@@ -54876,38 +54906,38 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>815</v>
+        <v>810</v>
       </c>
       <c r="B46" s="69" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="C46" s="38" t="s">
         <v>806</v>
       </c>
       <c r="D46" s="38" t="s">
-        <v>817</v>
+        <v>741</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="B47" s="69" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="C47" s="38" t="s">
-        <v>798</v>
+        <v>806</v>
       </c>
       <c r="D47" s="38" t="s">
-        <v>857</v>
+        <v>817</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B48" s="69" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C48" s="38" t="s">
         <v>798</v>
@@ -54918,211 +54948,225 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>282</v>
-      </c>
-      <c r="B49" s="69">
-        <v>1600</v>
+        <v>819</v>
+      </c>
+      <c r="B49" s="69" t="s">
+        <v>821</v>
       </c>
       <c r="C49" s="38" t="s">
-        <v>823</v>
+        <v>798</v>
       </c>
       <c r="D49" s="38" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>822</v>
+        <v>282</v>
       </c>
       <c r="B50" s="69">
-        <v>500</v>
+        <v>1600</v>
       </c>
       <c r="C50" s="38" t="s">
         <v>823</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>827</v>
+        <v>856</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>855</v>
+        <v>822</v>
       </c>
       <c r="B51" s="69">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="C51" s="38" t="s">
         <v>823</v>
       </c>
       <c r="D51" s="38" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>824</v>
+        <v>855</v>
       </c>
       <c r="B52" s="69">
-        <v>3000</v>
+        <v>50</v>
       </c>
       <c r="C52" s="38" t="s">
         <v>823</v>
       </c>
       <c r="D52" s="38" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>884</v>
+        <v>824</v>
       </c>
       <c r="B53" s="69">
-        <v>3200</v>
+        <v>3000</v>
       </c>
       <c r="C53" s="38" t="s">
         <v>823</v>
       </c>
       <c r="D53" s="38" t="s">
-        <v>885</v>
+        <v>825</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>828</v>
+        <v>884</v>
       </c>
       <c r="B54" s="69">
-        <v>5</v>
+        <v>3200</v>
       </c>
       <c r="C54" s="38" t="s">
-        <v>831</v>
+        <v>823</v>
       </c>
       <c r="D54" s="38" t="s">
-        <v>832</v>
+        <v>885</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>838</v>
+        <v>828</v>
       </c>
       <c r="B55" s="69">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C55" s="38" t="s">
-        <v>840</v>
+        <v>831</v>
       </c>
       <c r="D55" s="38" t="s">
-        <v>839</v>
+        <v>832</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>841</v>
-      </c>
-      <c r="B56" s="69" t="s">
-        <v>657</v>
+        <v>838</v>
+      </c>
+      <c r="B56" s="69">
+        <v>50</v>
       </c>
       <c r="C56" s="38" t="s">
-        <v>657</v>
+        <v>840</v>
       </c>
       <c r="D56" s="38" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="B57" s="69" t="s">
-        <v>844</v>
+        <v>657</v>
       </c>
       <c r="C57" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D57" s="38" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="B58" s="69" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="C58" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D58" s="38" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>847</v>
-      </c>
-      <c r="B59" s="69" t="b">
-        <v>0</v>
+        <v>846</v>
+      </c>
+      <c r="B59" s="69" t="s">
+        <v>848</v>
       </c>
       <c r="C59" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D59" s="38" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>851</v>
-      </c>
-      <c r="B60" s="69" t="s">
-        <v>853</v>
+        <v>847</v>
+      </c>
+      <c r="B60" s="69" t="b">
+        <v>0</v>
       </c>
       <c r="C60" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D60" s="38" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>1081</v>
+        <v>851</v>
       </c>
       <c r="B61" s="69" t="s">
-        <v>1089</v>
+        <v>853</v>
       </c>
       <c r="C61" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D61" s="38" t="s">
-        <v>1082</v>
+        <v>852</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="B62" s="69" t="s">
-        <v>1084</v>
+        <v>1089</v>
       </c>
       <c r="C62" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D62" s="38" t="s">
-        <v>1085</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="B63" s="69" t="s">
-        <v>1087</v>
+        <v>1084</v>
       </c>
       <c r="C63" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D63" s="38" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B64" s="69" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C64" s="38" t="s">
+        <v>657</v>
+      </c>
+      <c r="D64" s="38" t="s">
         <v>1088</v>
       </c>
     </row>
@@ -55133,13 +55177,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317EB008-F691-4F16-B99A-D5845A82BBBD}">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L4" sqref="L4"/>
+      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55151,15 +55195,15 @@
     <col min="7" max="7" width="91.140625" style="32" customWidth="1"/>
     <col min="8" max="8" width="90.42578125" style="32" customWidth="1"/>
     <col min="9" max="10" width="41.140625" style="32" customWidth="1"/>
-    <col min="11" max="11" width="60.140625" style="32" customWidth="1"/>
-    <col min="12" max="12" width="51.42578125" style="32" customWidth="1"/>
-    <col min="13" max="13" width="40.85546875" style="32" customWidth="1"/>
-    <col min="14" max="14" width="67.28515625" style="32" customWidth="1"/>
-    <col min="15" max="16" width="9.140625" style="32"/>
-    <col min="17" max="16384" width="9.140625" style="21"/>
+    <col min="11" max="11" width="77.28515625" style="32" customWidth="1"/>
+    <col min="12" max="13" width="41.140625" style="32" customWidth="1"/>
+    <col min="14" max="14" width="40.85546875" style="32" customWidth="1"/>
+    <col min="15" max="15" width="67.28515625" style="32" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="32"/>
+    <col min="18" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
         <v>427</v>
       </c>
@@ -55194,22 +55238,25 @@
         <v>901</v>
       </c>
       <c r="L1" s="71" t="s">
+        <v>1098</v>
+      </c>
+      <c r="M1" s="71" t="s">
         <v>833</v>
       </c>
-      <c r="M1" s="71" t="s">
+      <c r="N1" s="71" t="s">
         <v>429</v>
       </c>
-      <c r="N1" s="71" t="s">
+      <c r="O1" s="71" t="s">
         <v>859</v>
       </c>
-      <c r="O1" s="73" t="s">
+      <c r="P1" s="73" t="s">
         <v>691</v>
       </c>
-      <c r="P1" s="73" t="s">
+      <c r="Q1" s="73" t="s">
         <v>829</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="74" t="s">
         <v>752</v>
       </c>
@@ -55244,20 +55291,23 @@
         <v>osm_10km_testing_10km_pedestrian_20181001</v>
       </c>
       <c r="L2" s="75" t="s">
+        <v>1097</v>
+      </c>
+      <c r="M2" s="75" t="s">
         <v>858</v>
       </c>
-      <c r="M2" s="76" t="s">
+      <c r="N2" s="76" t="s">
         <v>439</v>
       </c>
-      <c r="N2" s="75" t="s">
+      <c r="O2" s="75" t="s">
         <v>860</v>
       </c>
-      <c r="O2" s="77"/>
-      <c r="P2" s="77">
+      <c r="P2" s="77"/>
+      <c r="Q2" s="77">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="74" t="s">
         <v>430</v>
       </c>
@@ -55292,15 +55342,18 @@
       <c r="K3" s="75" t="s">
         <v>917</v>
       </c>
-      <c r="L3" s="75"/>
+      <c r="L3" s="75" t="s">
+        <v>585</v>
+      </c>
       <c r="M3" s="75"/>
       <c r="N3" s="75"/>
-      <c r="O3" s="77"/>
-      <c r="P3" s="77">
+      <c r="O3" s="75"/>
+      <c r="P3" s="77"/>
+      <c r="Q3" s="77">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="78" t="s">
         <v>435</v>
       </c>
@@ -55336,17 +55389,20 @@
         <v>918</v>
       </c>
       <c r="L4" s="79" t="s">
+        <v>584</v>
+      </c>
+      <c r="M4" s="79" t="s">
         <v>834</v>
       </c>
-      <c r="M4" s="80" t="s">
+      <c r="N4" s="80" t="s">
         <v>439</v>
       </c>
-      <c r="N4" s="79"/>
-      <c r="P4" s="32">
+      <c r="O4" s="79"/>
+      <c r="Q4" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="81" t="s">
         <v>440</v>
       </c>
@@ -55381,15 +55437,18 @@
       <c r="K5" s="82" t="s">
         <v>919</v>
       </c>
-      <c r="L5" s="82"/>
+      <c r="L5" s="82" t="s">
+        <v>586</v>
+      </c>
       <c r="M5" s="82"/>
       <c r="N5" s="82"/>
-      <c r="O5" s="51"/>
-      <c r="P5" s="51">
+      <c r="O5" s="82"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="51">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="78" t="s">
         <v>443</v>
       </c>
@@ -55424,14 +55483,17 @@
       <c r="K6" s="79" t="s">
         <v>920</v>
       </c>
-      <c r="L6" s="79"/>
+      <c r="L6" s="79" t="s">
+        <v>587</v>
+      </c>
       <c r="M6" s="79"/>
       <c r="N6" s="79"/>
-      <c r="P6" s="32">
+      <c r="O6" s="79"/>
+      <c r="Q6" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="81" t="s">
         <v>447</v>
       </c>
@@ -55466,15 +55528,18 @@
       <c r="K7" s="82" t="s">
         <v>921</v>
       </c>
-      <c r="L7" s="82"/>
+      <c r="L7" s="82" t="s">
+        <v>588</v>
+      </c>
       <c r="M7" s="82"/>
       <c r="N7" s="82"/>
-      <c r="O7" s="51"/>
-      <c r="P7" s="51">
+      <c r="O7" s="82"/>
+      <c r="P7" s="51"/>
+      <c r="Q7" s="51">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="78" t="s">
         <v>451</v>
       </c>
@@ -55510,19 +55575,22 @@
         <v>922</v>
       </c>
       <c r="L8" s="79" t="s">
+        <v>589</v>
+      </c>
+      <c r="M8" s="79" t="s">
         <v>835</v>
       </c>
-      <c r="M8" s="80" t="s">
+      <c r="N8" s="80" t="s">
         <v>455</v>
       </c>
-      <c r="N8" s="79" t="s">
+      <c r="O8" s="79" t="s">
         <v>568</v>
       </c>
-      <c r="P8" s="32">
+      <c r="Q8" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="81" t="s">
         <v>44</v>
       </c>
@@ -55558,18 +55626,21 @@
         <v>923</v>
       </c>
       <c r="L9" s="82" t="s">
+        <v>590</v>
+      </c>
+      <c r="M9" s="82" t="s">
         <v>837</v>
       </c>
-      <c r="M9" s="83" t="s">
+      <c r="N9" s="83" t="s">
         <v>460</v>
       </c>
-      <c r="N9" s="82"/>
-      <c r="O9" s="51"/>
-      <c r="P9" s="51">
+      <c r="O9" s="82"/>
+      <c r="P9" s="51"/>
+      <c r="Q9" s="51">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="78" t="s">
         <v>461</v>
       </c>
@@ -55605,19 +55676,22 @@
         <v>924</v>
       </c>
       <c r="L10" s="79" t="s">
+        <v>591</v>
+      </c>
+      <c r="M10" s="79" t="s">
         <v>836</v>
       </c>
-      <c r="M10" s="80" t="s">
+      <c r="N10" s="80" t="s">
         <v>465</v>
       </c>
-      <c r="N10" s="79" t="s">
+      <c r="O10" s="79" t="s">
         <v>456</v>
       </c>
-      <c r="P10" s="32">
+      <c r="Q10" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="81" t="s">
         <v>466</v>
       </c>
@@ -55652,15 +55726,18 @@
       <c r="K11" s="82" t="s">
         <v>925</v>
       </c>
-      <c r="L11" s="82"/>
+      <c r="L11" s="82" t="s">
+        <v>592</v>
+      </c>
       <c r="M11" s="82"/>
       <c r="N11" s="82"/>
-      <c r="O11" s="51"/>
-      <c r="P11" s="51">
+      <c r="O11" s="82"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="51">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="78" t="s">
         <v>552</v>
       </c>
@@ -55692,19 +55769,22 @@
       <c r="J12" s="79" t="s">
         <v>877</v>
       </c>
-      <c r="K12" s="82" t="s">
+      <c r="K12" s="79" t="s">
         <v>926</v>
       </c>
-      <c r="L12" s="84"/>
-      <c r="M12" s="80" t="s">
+      <c r="L12" s="79" t="s">
+        <v>1092</v>
+      </c>
+      <c r="M12" s="79"/>
+      <c r="N12" s="80" t="s">
         <v>465</v>
       </c>
-      <c r="N12" s="79"/>
-      <c r="P12" s="32">
+      <c r="O12" s="79"/>
+      <c r="Q12" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="81" t="s">
         <v>553</v>
       </c>
@@ -55739,17 +55819,20 @@
       <c r="K13" s="82" t="s">
         <v>927</v>
       </c>
-      <c r="L13" s="82"/>
-      <c r="M13" s="83" t="s">
+      <c r="L13" s="82" t="s">
+        <v>571</v>
+      </c>
+      <c r="M13" s="82"/>
+      <c r="N13" s="83" t="s">
         <v>455</v>
       </c>
-      <c r="N13" s="82"/>
-      <c r="O13" s="51"/>
-      <c r="P13" s="51">
+      <c r="O13" s="82"/>
+      <c r="P13" s="51"/>
+      <c r="Q13" s="51">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="78" t="s">
         <v>554</v>
       </c>
@@ -55781,19 +55864,22 @@
       <c r="J14" s="79" t="s">
         <v>877</v>
       </c>
-      <c r="K14" s="82" t="s">
+      <c r="K14" s="79" t="s">
         <v>928</v>
       </c>
-      <c r="L14" s="79"/>
-      <c r="M14" s="80" t="s">
+      <c r="L14" s="79" t="s">
+        <v>572</v>
+      </c>
+      <c r="M14" s="79"/>
+      <c r="N14" s="80" t="s">
         <v>455</v>
       </c>
-      <c r="N14" s="79"/>
-      <c r="P14" s="32">
+      <c r="O14" s="79"/>
+      <c r="Q14" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="81" t="s">
         <v>555</v>
       </c>
@@ -55828,17 +55914,20 @@
       <c r="K15" s="82" t="s">
         <v>929</v>
       </c>
-      <c r="L15" s="82"/>
-      <c r="M15" s="83" t="s">
+      <c r="L15" s="82" t="s">
+        <v>573</v>
+      </c>
+      <c r="M15" s="82"/>
+      <c r="N15" s="83" t="s">
         <v>439</v>
       </c>
-      <c r="N15" s="82"/>
-      <c r="O15" s="51"/>
-      <c r="P15" s="51">
+      <c r="O15" s="82"/>
+      <c r="P15" s="51"/>
+      <c r="Q15" s="51">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="78" t="s">
         <v>556</v>
       </c>
@@ -55870,19 +55959,22 @@
       <c r="J16" s="79" t="s">
         <v>877</v>
       </c>
-      <c r="K16" s="82" t="s">
+      <c r="K16" s="79" t="s">
         <v>930</v>
       </c>
-      <c r="L16" s="79"/>
-      <c r="M16" s="80" t="s">
+      <c r="L16" s="79" t="s">
+        <v>574</v>
+      </c>
+      <c r="M16" s="79"/>
+      <c r="N16" s="80" t="s">
         <v>455</v>
       </c>
-      <c r="N16" s="79"/>
-      <c r="P16" s="32">
+      <c r="O16" s="79"/>
+      <c r="Q16" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="81" t="s">
         <v>557</v>
       </c>
@@ -55917,17 +56009,20 @@
       <c r="K17" s="82" t="s">
         <v>931</v>
       </c>
-      <c r="L17" s="82"/>
-      <c r="M17" s="83" t="s">
+      <c r="L17" s="82" t="s">
+        <v>1093</v>
+      </c>
+      <c r="M17" s="82"/>
+      <c r="N17" s="83" t="s">
         <v>439</v>
       </c>
-      <c r="N17" s="82"/>
-      <c r="O17" s="51"/>
-      <c r="P17" s="51">
+      <c r="O17" s="82"/>
+      <c r="P17" s="51"/>
+      <c r="Q17" s="51">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="78" t="s">
         <v>558</v>
       </c>
@@ -55959,19 +56054,22 @@
       <c r="J18" s="79" t="s">
         <v>877</v>
       </c>
-      <c r="K18" s="82" t="s">
+      <c r="K18" s="79" t="s">
         <v>932</v>
       </c>
-      <c r="L18" s="79"/>
-      <c r="M18" s="79" t="s">
+      <c r="L18" s="79" t="s">
+        <v>575</v>
+      </c>
+      <c r="M18" s="79"/>
+      <c r="N18" s="79" t="s">
         <v>565</v>
       </c>
-      <c r="N18" s="79"/>
-      <c r="P18" s="32">
+      <c r="O18" s="79"/>
+      <c r="Q18" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="81" t="s">
         <v>559</v>
       </c>
@@ -56006,17 +56104,20 @@
       <c r="K19" s="82" t="s">
         <v>933</v>
       </c>
-      <c r="L19" s="82"/>
-      <c r="M19" s="83" t="s">
+      <c r="L19" s="82" t="s">
+        <v>576</v>
+      </c>
+      <c r="M19" s="82"/>
+      <c r="N19" s="83" t="s">
         <v>439</v>
       </c>
-      <c r="N19" s="82"/>
-      <c r="O19" s="51"/>
-      <c r="P19" s="51">
+      <c r="O19" s="82"/>
+      <c r="P19" s="51"/>
+      <c r="Q19" s="51">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="78" t="s">
         <v>560</v>
       </c>
@@ -56048,19 +56149,22 @@
       <c r="J20" s="79" t="s">
         <v>877</v>
       </c>
-      <c r="K20" s="82" t="s">
+      <c r="K20" s="79" t="s">
         <v>934</v>
       </c>
-      <c r="L20" s="79"/>
-      <c r="M20" s="80" t="s">
+      <c r="L20" s="79" t="s">
+        <v>1094</v>
+      </c>
+      <c r="M20" s="79"/>
+      <c r="N20" s="80" t="s">
         <v>465</v>
       </c>
-      <c r="N20" s="79"/>
-      <c r="P20" s="32">
+      <c r="O20" s="79"/>
+      <c r="Q20" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="81" t="s">
         <v>561</v>
       </c>
@@ -56095,17 +56199,20 @@
       <c r="K21" s="82" t="s">
         <v>935</v>
       </c>
-      <c r="L21" s="82"/>
-      <c r="M21" s="83" t="s">
+      <c r="L21" s="82" t="s">
+        <v>1095</v>
+      </c>
+      <c r="M21" s="82"/>
+      <c r="N21" s="83" t="s">
         <v>439</v>
       </c>
-      <c r="N21" s="82"/>
-      <c r="O21" s="51"/>
-      <c r="P21" s="51">
+      <c r="O21" s="82"/>
+      <c r="P21" s="51"/>
+      <c r="Q21" s="51">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="78" t="s">
         <v>562</v>
       </c>
@@ -56137,19 +56244,22 @@
       <c r="J22" s="79" t="s">
         <v>877</v>
       </c>
-      <c r="K22" s="82" t="s">
+      <c r="K22" s="79" t="s">
         <v>936</v>
       </c>
-      <c r="L22" s="79"/>
-      <c r="M22" s="80" t="s">
+      <c r="L22" s="79" t="s">
+        <v>577</v>
+      </c>
+      <c r="M22" s="79"/>
+      <c r="N22" s="80" t="s">
         <v>439</v>
       </c>
-      <c r="N22" s="79"/>
-      <c r="P22" s="32">
+      <c r="O22" s="79"/>
+      <c r="Q22" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="81" t="s">
         <v>563</v>
       </c>
@@ -56184,17 +56294,20 @@
       <c r="K23" s="82" t="s">
         <v>937</v>
       </c>
-      <c r="L23" s="82"/>
-      <c r="M23" s="83" t="s">
+      <c r="L23" s="82" t="s">
+        <v>578</v>
+      </c>
+      <c r="M23" s="82"/>
+      <c r="N23" s="83" t="s">
         <v>439</v>
       </c>
-      <c r="N23" s="82"/>
-      <c r="O23" s="51"/>
-      <c r="P23" s="51">
+      <c r="O23" s="82"/>
+      <c r="P23" s="51"/>
+      <c r="Q23" s="51">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="78" t="s">
         <v>564</v>
       </c>
@@ -56226,19 +56339,22 @@
       <c r="J24" s="79" t="s">
         <v>877</v>
       </c>
-      <c r="K24" s="82" t="s">
+      <c r="K24" s="79" t="s">
         <v>915</v>
       </c>
-      <c r="L24" s="79"/>
-      <c r="M24" s="80" t="s">
+      <c r="L24" s="79" t="s">
+        <v>579</v>
+      </c>
+      <c r="M24" s="79"/>
+      <c r="N24" s="80" t="s">
         <v>465</v>
       </c>
-      <c r="N24" s="79"/>
-      <c r="P24" s="32">
+      <c r="O24" s="79"/>
+      <c r="Q24" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="81" t="s">
         <v>566</v>
       </c>
@@ -56273,15 +56389,18 @@
       <c r="K25" s="82" t="s">
         <v>938</v>
       </c>
-      <c r="L25" s="83"/>
-      <c r="M25" s="83" t="s">
+      <c r="L25" s="82" t="s">
+        <v>1096</v>
+      </c>
+      <c r="M25" s="82"/>
+      <c r="N25" s="83" t="s">
         <v>465</v>
       </c>
-      <c r="N25" s="82" t="s">
+      <c r="O25" s="82" t="s">
         <v>456</v>
       </c>
-      <c r="O25" s="51"/>
-      <c r="P25" s="51">
+      <c r="P25" s="51"/>
+      <c r="Q25" s="51">
         <v>0</v>
       </c>
     </row>
@@ -57036,7 +57155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
corrected osm_source in ind_study_region_matrix
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1180E2B0-4147-44BB-822E-04C236B56EB0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2D2B3A-6EE3-4F40-8AE5-7061B273A41D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="2" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="3" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -54264,7 +54264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3E5F03-EC28-486B-BA51-9D83D1ACCD02}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
     </sheetView>
@@ -55179,11 +55179,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317EB008-F691-4F16-B99A-D5845A82BBBD}">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
+      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55193,8 +55193,8 @@
     <col min="4" max="5" width="20.140625" style="32" customWidth="1"/>
     <col min="6" max="6" width="99.140625" style="33" customWidth="1"/>
     <col min="7" max="7" width="91.140625" style="32" customWidth="1"/>
-    <col min="8" max="8" width="90.42578125" style="32" customWidth="1"/>
-    <col min="9" max="10" width="41.140625" style="32" customWidth="1"/>
+    <col min="8" max="9" width="90.42578125" style="32" customWidth="1"/>
+    <col min="10" max="10" width="41.140625" style="32" customWidth="1"/>
     <col min="11" max="11" width="77.28515625" style="32" customWidth="1"/>
     <col min="12" max="13" width="41.140625" style="32" customWidth="1"/>
     <col min="14" max="14" width="40.85546875" style="32" customWidth="1"/>
@@ -55762,9 +55762,9 @@
       <c r="H12" s="102" t="s">
         <v>906</v>
       </c>
-      <c r="I12" s="79" t="str">
-        <f t="shared" ref="I12:I25" si="1">"D:/ntnl_li_2018_template/data/study_region/"&amp;B12&amp;"/"&amp;B12&amp;"_20181001.osm"</f>
-        <v>D:/ntnl_li_2018_template/data/study_region/albury_wodonga/albury_wodonga_20181001.osm</v>
+      <c r="I12" s="102" t="str">
+        <f>"D:/ntnl_li_2018_template/data/study_region/"&amp;B12&amp;"/"&amp;L12&amp;"_20181001.osm"</f>
+        <v>D:/ntnl_li_2018_template/data/study_region/albury_wodonga/alburywodonga_20181001.osm</v>
       </c>
       <c r="J12" s="79" t="s">
         <v>877</v>
@@ -55810,7 +55810,7 @@
         <v>454</v>
       </c>
       <c r="I13" s="82" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I13:I25" si="1">"D:/ntnl_li_2018_template/data/study_region/"&amp;B13&amp;"/"&amp;L13&amp;"_20181001.osm"</f>
         <v>D:/ntnl_li_2018_template/data/study_region/ballarat/ballarat_20181001.osm</v>
       </c>
       <c r="J13" s="82" t="s">
@@ -56001,7 +56001,7 @@
       </c>
       <c r="I17" s="82" t="str">
         <f t="shared" si="1"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/goldcoast_tweedheads/goldcoast_tweedheads_20181001.osm</v>
+        <v>D:/ntnl_li_2018_template/data/study_region/goldcoast_tweedheads/goldcoast_20181001.osm</v>
       </c>
       <c r="J17" s="82" t="s">
         <v>877</v>
@@ -56144,7 +56144,7 @@
       </c>
       <c r="I20" s="79" t="str">
         <f t="shared" si="1"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/newcastle_maitland/newcastle_maitland_20181001.osm</v>
+        <v>D:/ntnl_li_2018_template/data/study_region/newcastle_maitland/newcastle_20181001.osm</v>
       </c>
       <c r="J20" s="79" t="s">
         <v>877</v>
@@ -56191,7 +56191,7 @@
       </c>
       <c r="I21" s="82" t="str">
         <f t="shared" si="1"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/sunshine_coast/sunshine_coast_20181001.osm</v>
+        <v>D:/ntnl_li_2018_template/data/study_region/sunshine_coast/sunshinecoast_20181001.osm</v>
       </c>
       <c r="J21" s="82" t="s">
         <v>877</v>
@@ -56379,9 +56379,9 @@
       <c r="H25" s="83" t="s">
         <v>464</v>
       </c>
-      <c r="I25" s="82" t="str">
+      <c r="I25" s="83" t="str">
         <f t="shared" si="1"/>
-        <v>D:/ntnl_li_2018_template/data/study_region/western_sydney/western_sydney_20181001.osm</v>
+        <v>D:/ntnl_li_2018_template/data/study_region/western_sydney/westernsydney_20181001.osm</v>
       </c>
       <c r="J25" s="82" t="s">
         <v>877</v>

</xml_diff>

<commit_message>
updated open space scripts
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2D2B3A-6EE3-4F40-8AE5-7061B273A41D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20193566-E588-4616-A43F-65E2866BED41}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="3" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2303" uniqueCount="1100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2304" uniqueCount="1101">
   <si>
     <t>Domain</t>
   </si>
@@ -3430,6 +3430,9 @@
   </si>
   <si>
     <t>roads/li_intersections_2018.gpkg</t>
+  </si>
+  <si>
+    <t>school_tags</t>
   </si>
 </sst>
 </file>
@@ -55179,7 +55182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317EB008-F691-4F16-B99A-D5845A82BBBD}">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -57155,8 +57158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57529,7 +57532,7 @@
         <v>1039</v>
       </c>
       <c r="J15" t="s">
-        <v>1053</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -57543,7 +57546,7 @@
         <v>1040</v>
       </c>
       <c r="J16" t="s">
-        <v>1047</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -57557,7 +57560,7 @@
         <v>1041</v>
       </c>
       <c r="J17" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -57571,7 +57574,7 @@
         <v>1042</v>
       </c>
       <c r="J18" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -57585,7 +57588,7 @@
         <v>1043</v>
       </c>
       <c r="J19" t="s">
-        <v>1054</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -57596,7 +57599,7 @@
         <v>940</v>
       </c>
       <c r="J20" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
@@ -57605,6 +57608,9 @@
       </c>
       <c r="F21" t="s">
         <v>990</v>
+      </c>
+      <c r="J21" t="s">
+        <v>1055</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
tuned the sausage buffer script to use some more efficient progress tracking, and group in larger sizes; also removed the fixed parameterisation of workers -- should be set in config file
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20193566-E588-4616-A43F-65E2866BED41}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FB344C-5F93-46FD-9ED9-1B628EA3A65E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="2" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -54267,9 +54267,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3E5F03-EC28-486B-BA51-9D83D1ACCD02}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54439,7 +54439,7 @@
         <v>1079</v>
       </c>
       <c r="B12" s="69">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="38" t="s">
         <v>801</v>
@@ -57158,7 +57158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated study region matrix
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FB344C-5F93-46FD-9ED9-1B628EA3A65E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B94BCD-45A0-49A2-9E5B-4EC6B27C8836}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="2" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
@@ -54269,7 +54269,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54439,7 +54439,7 @@
         <v>1079</v>
       </c>
       <c r="B12" s="69">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" s="38" t="s">
         <v>801</v>

</xml_diff>

<commit_message>
added in a playground sketch
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B94BCD-45A0-49A2-9E5B-4EC6B27C8836}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A202447-812D-4FB9-B9B6-7090AFFAC2DF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="2" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2304" uniqueCount="1101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2310" uniqueCount="1107">
   <si>
     <t>Domain</t>
   </si>
@@ -3040,9 +3040,6 @@
     <t>Military installations can at times be mistaken for open spaces (e.g. shooting ranges in natural woodlands)</t>
   </si>
   <si>
-    <t>p.access IS NULL OR p.access NOT IN('no','private')</t>
-  </si>
-  <si>
     <t>inclusion explanation (p. is shorthand for the 'park' table where the open space data is)</t>
   </si>
   <si>
@@ -3185,15 +3182,6 @@
   </si>
   <si>
     <t>linear_feature_criteria_AND</t>
-  </si>
-  <si>
-    <t>area_ha &gt; 0.5</t>
-  </si>
-  <si>
-    <t>medial_axis_length &gt; 300</t>
-  </si>
-  <si>
-    <t>roundness &lt; 0.25</t>
   </si>
   <si>
     <t>open_space_defs</t>
@@ -3321,12 +3309,6 @@
     <t>A list of OSM and derived data columns which should be included as open_space feature tags (in addition to existing tags) when collating open space features to an Area of Open Space.</t>
   </si>
   <si>
-    <t>amal_to_area_ratio &gt; 140</t>
-  </si>
-  <si>
-    <t>num_symdiff_convhull_geoms &gt; 0</t>
-  </si>
-  <si>
     <t>p.landuse IS NULL OR p.landuse NOT IN ('military')</t>
   </si>
   <si>
@@ -3433,6 +3415,42 @@
   </si>
   <si>
     <t>school_tags</t>
+  </si>
+  <si>
+    <t>(amal_to_area_ratio &gt; 140</t>
+  </si>
+  <si>
+    <t>AND area_ha &gt; 0.5</t>
+  </si>
+  <si>
+    <t>AND medial_axis_length &gt; 300</t>
+  </si>
+  <si>
+    <t>AND num_symdiff_convhull_geoms &gt; 0</t>
+  </si>
+  <si>
+    <t>AND roundness &lt; 0.25)</t>
+  </si>
+  <si>
+    <t>OR (</t>
+  </si>
+  <si>
+    <t>waterway IS NOT NULL</t>
+  </si>
+  <si>
+    <t>OR river IS NOT NULL</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>min_bounding_circle_area</t>
+  </si>
+  <si>
+    <t>min_bounding_circle_diameter</t>
+  </si>
+  <si>
+    <t>p.access IS NULL OR p.access NOT IN('customers','designated','employee','no','private','privates','staff')</t>
   </si>
 </sst>
 </file>
@@ -5043,10 +5061,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="D58" s="63" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -5054,7 +5072,7 @@
         <v>966</v>
       </c>
       <c r="C59" s="64" t="s">
-        <v>1024</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -5062,15 +5080,15 @@
         <v>950</v>
       </c>
       <c r="C60" s="64" t="s">
-        <v>1025</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B61" s="63" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="C61" s="64" t="s">
-        <v>1026</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -5078,47 +5096,47 @@
         <v>967</v>
       </c>
       <c r="C62" s="64" t="s">
-        <v>1057</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B63" s="63" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="C63" s="64" t="s">
-        <v>1058</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="63" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="C64" s="64" t="s">
-        <v>1059</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="63" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="C65" s="64" t="s">
-        <v>1060</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B66" s="63" t="s">
-        <v>1044</v>
+        <v>1040</v>
       </c>
       <c r="C66" s="64" t="s">
-        <v>1061</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B67" s="63" t="s">
-        <v>1056</v>
+        <v>1052</v>
       </c>
       <c r="C67" s="64" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
@@ -54267,7 +54285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3E5F03-EC28-486B-BA51-9D83D1ACCD02}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
@@ -54436,7 +54454,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1079</v>
+        <v>1073</v>
       </c>
       <c r="B12" s="69">
         <v>7</v>
@@ -54445,7 +54463,7 @@
         <v>801</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>1080</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -54867,16 +54885,16 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1090</v>
+        <v>1084</v>
       </c>
       <c r="B43" s="69" t="s">
-        <v>1099</v>
+        <v>1093</v>
       </c>
       <c r="C43" s="38" t="s">
         <v>806</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>1091</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -55133,44 +55151,44 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1081</v>
+        <v>1075</v>
       </c>
       <c r="B62" s="69" t="s">
-        <v>1089</v>
+        <v>1083</v>
       </c>
       <c r="C62" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D62" s="38" t="s">
-        <v>1082</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>1083</v>
+        <v>1077</v>
       </c>
       <c r="B63" s="69" t="s">
-        <v>1084</v>
+        <v>1078</v>
       </c>
       <c r="C63" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D63" s="38" t="s">
-        <v>1085</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>1086</v>
+        <v>1080</v>
       </c>
       <c r="B64" s="69" t="s">
-        <v>1087</v>
+        <v>1081</v>
       </c>
       <c r="C64" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D64" s="38" t="s">
-        <v>1088</v>
+        <v>1082</v>
       </c>
     </row>
   </sheetData>
@@ -55241,7 +55259,7 @@
         <v>901</v>
       </c>
       <c r="L1" s="71" t="s">
-        <v>1098</v>
+        <v>1092</v>
       </c>
       <c r="M1" s="71" t="s">
         <v>833</v>
@@ -55294,7 +55312,7 @@
         <v>osm_10km_testing_10km_pedestrian_20181001</v>
       </c>
       <c r="L2" s="75" t="s">
-        <v>1097</v>
+        <v>1091</v>
       </c>
       <c r="M2" s="75" t="s">
         <v>858</v>
@@ -55776,7 +55794,7 @@
         <v>926</v>
       </c>
       <c r="L12" s="79" t="s">
-        <v>1092</v>
+        <v>1086</v>
       </c>
       <c r="M12" s="79"/>
       <c r="N12" s="80" t="s">
@@ -56013,7 +56031,7 @@
         <v>931</v>
       </c>
       <c r="L17" s="82" t="s">
-        <v>1093</v>
+        <v>1087</v>
       </c>
       <c r="M17" s="82"/>
       <c r="N17" s="83" t="s">
@@ -56156,7 +56174,7 @@
         <v>934</v>
       </c>
       <c r="L20" s="79" t="s">
-        <v>1094</v>
+        <v>1088</v>
       </c>
       <c r="M20" s="79"/>
       <c r="N20" s="80" t="s">
@@ -56203,7 +56221,7 @@
         <v>935</v>
       </c>
       <c r="L21" s="82" t="s">
-        <v>1095</v>
+        <v>1089</v>
       </c>
       <c r="M21" s="82"/>
       <c r="N21" s="83" t="s">
@@ -56393,7 +56411,7 @@
         <v>938</v>
       </c>
       <c r="L25" s="82" t="s">
-        <v>1096</v>
+        <v>1090</v>
       </c>
       <c r="M25" s="82"/>
       <c r="N25" s="83" t="s">
@@ -57158,8 +57176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57183,28 +57201,28 @@
         <v>950</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>1069</v>
+        <v>1063</v>
       </c>
       <c r="D1" s="37" t="s">
+        <v>971</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>970</v>
+      </c>
+      <c r="F1" s="37" t="s">
         <v>972</v>
       </c>
-      <c r="E1" s="37" t="s">
-        <v>971</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>973</v>
-      </c>
       <c r="G1" s="37" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="I1" s="37" t="s">
-        <v>1044</v>
+        <v>1040</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>1056</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -57215,28 +57233,28 @@
         <v>951</v>
       </c>
       <c r="C2" t="s">
-        <v>1071</v>
+        <v>1065</v>
       </c>
       <c r="D2" t="s">
-        <v>970</v>
+        <v>1106</v>
       </c>
       <c r="E2" t="s">
         <v>968</v>
       </c>
       <c r="F2" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="G2" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="H2" t="s">
-        <v>1063</v>
+        <v>1095</v>
       </c>
       <c r="I2" t="s">
-        <v>1027</v>
+        <v>1023</v>
       </c>
       <c r="J2" t="s">
-        <v>1045</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -57244,31 +57262,31 @@
         <v>940</v>
       </c>
       <c r="B3" t="s">
-        <v>1068</v>
+        <v>1062</v>
       </c>
       <c r="C3" t="s">
-        <v>1072</v>
+        <v>1066</v>
       </c>
       <c r="D3" t="s">
-        <v>1065</v>
+        <v>1059</v>
       </c>
       <c r="E3" t="s">
         <v>969</v>
       </c>
       <c r="F3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="G3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="H3" t="s">
-        <v>1019</v>
+        <v>1096</v>
       </c>
       <c r="I3" t="s">
-        <v>1028</v>
+        <v>1024</v>
       </c>
       <c r="J3" t="s">
-        <v>1046</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -57279,22 +57297,22 @@
         <v>952</v>
       </c>
       <c r="C4" t="s">
-        <v>1070</v>
+        <v>1064</v>
       </c>
       <c r="F4" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="G4" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="H4" t="s">
-        <v>1020</v>
+        <v>1097</v>
       </c>
       <c r="I4" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J4" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -57311,13 +57329,13 @@
         <v>939</v>
       </c>
       <c r="G5" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="H5" t="s">
-        <v>1064</v>
+        <v>1098</v>
       </c>
       <c r="I5" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
       <c r="J5" t="s">
         <v>944</v>
@@ -57331,22 +57349,22 @@
         <v>954</v>
       </c>
       <c r="C6" t="s">
-        <v>1073</v>
+        <v>1067</v>
       </c>
       <c r="F6" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="G6" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="H6" t="s">
-        <v>1021</v>
+        <v>1099</v>
       </c>
       <c r="I6" t="s">
-        <v>1031</v>
+        <v>1027</v>
       </c>
       <c r="J6" t="s">
-        <v>1074</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -57357,16 +57375,19 @@
         <v>955</v>
       </c>
       <c r="C7" t="s">
-        <v>1075</v>
+        <v>1069</v>
       </c>
       <c r="F7" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="G7" t="s">
-        <v>1011</v>
+        <v>1010</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1100</v>
       </c>
       <c r="I7" t="s">
-        <v>1032</v>
+        <v>1028</v>
       </c>
       <c r="J7" t="s">
         <v>948</v>
@@ -57380,16 +57401,19 @@
         <v>956</v>
       </c>
       <c r="C8" t="s">
-        <v>1076</v>
+        <v>1070</v>
       </c>
       <c r="F8" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="G8" t="s">
-        <v>1012</v>
+        <v>1011</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1101</v>
       </c>
       <c r="I8" t="s">
-        <v>1033</v>
+        <v>1029</v>
       </c>
       <c r="J8" t="s">
         <v>945</v>
@@ -57403,16 +57427,19 @@
         <v>957</v>
       </c>
       <c r="C9" t="s">
-        <v>1077</v>
+        <v>1071</v>
       </c>
       <c r="F9" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="G9" t="s">
-        <v>1013</v>
+        <v>1012</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1102</v>
       </c>
       <c r="I9" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
       <c r="J9" t="s">
         <v>946</v>
@@ -57429,10 +57456,13 @@
         <v>960</v>
       </c>
       <c r="F10" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="G10" t="s">
-        <v>1005</v>
+        <v>1004</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1103</v>
       </c>
       <c r="I10" t="s">
         <v>695</v>
@@ -57449,16 +57479,16 @@
         <v>958</v>
       </c>
       <c r="C11" t="s">
-        <v>1078</v>
+        <v>1072</v>
       </c>
       <c r="F11" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="G11" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="I11" t="s">
-        <v>1035</v>
+        <v>1031</v>
       </c>
       <c r="J11" t="s">
         <v>942</v>
@@ -57472,13 +57502,13 @@
         <v>959</v>
       </c>
       <c r="F12" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="G12" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="I12" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
       <c r="J12" t="s">
         <v>965</v>
@@ -57486,22 +57516,22 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1074</v>
+        <v>1068</v>
       </c>
       <c r="B13" t="s">
         <v>960</v>
       </c>
       <c r="F13" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="G13" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="I13" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
       <c r="J13" t="s">
-        <v>1051</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -57509,16 +57539,16 @@
         <v>961</v>
       </c>
       <c r="F14" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="G14" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="I14" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="J14" t="s">
-        <v>1052</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -57526,27 +57556,27 @@
         <v>962</v>
       </c>
       <c r="F15" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="I15" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
       <c r="J15" t="s">
-        <v>1100</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>1066</v>
+        <v>1060</v>
       </c>
       <c r="F16" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="I16" t="s">
-        <v>1040</v>
+        <v>1036</v>
       </c>
       <c r="J16" t="s">
-        <v>1053</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -57554,13 +57584,13 @@
         <v>947</v>
       </c>
       <c r="F17" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="I17" t="s">
-        <v>1041</v>
+        <v>1037</v>
       </c>
       <c r="J17" t="s">
-        <v>1047</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -57568,27 +57598,27 @@
         <v>963</v>
       </c>
       <c r="F18" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="I18" t="s">
-        <v>1042</v>
+        <v>1038</v>
       </c>
       <c r="J18" t="s">
-        <v>1048</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>1067</v>
+        <v>1061</v>
       </c>
       <c r="F19" t="s">
         <v>962</v>
       </c>
       <c r="I19" t="s">
-        <v>1043</v>
+        <v>1039</v>
       </c>
       <c r="J19" t="s">
-        <v>1049</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -57599,7 +57629,7 @@
         <v>940</v>
       </c>
       <c r="J20" t="s">
-        <v>1054</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
@@ -57607,10 +57637,10 @@
         <v>964</v>
       </c>
       <c r="F21" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="J21" t="s">
-        <v>1055</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -57618,57 +57648,63 @@
         <v>965</v>
       </c>
       <c r="F22" t="s">
-        <v>991</v>
+        <v>990</v>
+      </c>
+      <c r="J22" t="s">
+        <v>1050</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
-        <v>992</v>
+        <v>991</v>
+      </c>
+      <c r="J23" t="s">
+        <v>1051</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.25">
@@ -57678,17 +57714,17 @@
     </row>
     <row r="34" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="35" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="36" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="37" spans="6:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added in Australia to ind_study_region_matrix
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A202447-812D-4FB9-B9B6-7090AFFAC2DF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28F4E8B-48C9-4131-8558-3102309F3810}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="3" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2310" uniqueCount="1107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2323" uniqueCount="1113">
   <si>
     <t>Domain</t>
   </si>
@@ -3451,6 +3451,24 @@
   </si>
   <si>
     <t>p.access IS NULL OR p.access NOT IN('customers','designated','employee','no','private','privates','staff')</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>australia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>study_region/australia/Australia_gda2020_epsg7845.shp</t>
+  </si>
+  <si>
+    <t>"OBJECT ID" IS NOT NULL</t>
+  </si>
+  <si>
+    <t>_</t>
   </si>
 </sst>
 </file>
@@ -55198,13 +55216,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317EB008-F691-4F16-B99A-D5845A82BBBD}">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="I20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
+      <selection pane="bottomRight" activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56422,6 +56440,52 @@
       </c>
       <c r="P25" s="51"/>
       <c r="Q25" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="78" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B26" s="79" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C26" s="79" t="s">
+        <v>912</v>
+      </c>
+      <c r="D26" s="79" t="s">
+        <v>1112</v>
+      </c>
+      <c r="E26" s="79" t="s">
+        <v>1112</v>
+      </c>
+      <c r="F26" s="80" t="s">
+        <v>1110</v>
+      </c>
+      <c r="G26" s="79" t="s">
+        <v>1111</v>
+      </c>
+      <c r="H26" s="79" t="s">
+        <v>1109</v>
+      </c>
+      <c r="I26" s="79" t="s">
+        <v>1109</v>
+      </c>
+      <c r="J26" s="79" t="s">
+        <v>877</v>
+      </c>
+      <c r="K26" s="79" t="s">
+        <v>1109</v>
+      </c>
+      <c r="L26" s="79" t="s">
+        <v>1109</v>
+      </c>
+      <c r="M26" s="79"/>
+      <c r="N26" s="80" t="s">
+        <v>465</v>
+      </c>
+      <c r="O26" s="79"/>
+      <c r="Q26" s="32">
         <v>0</v>
       </c>
     </row>
@@ -57176,8 +57240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59941,10 +60005,10 @@
   <dimension ref="A1:O87"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C72" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D92" sqref="D92"/>
+      <selection pane="bottomRight" activeCell="M89" sqref="M89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update with change to script 11 for Australia
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EF6123-AE33-43EF-89BB-CCD2935BA4DF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DEAD48-74D0-4593-AC06-B37A6DA32B2C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="3" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2323" uniqueCount="1113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2323" uniqueCount="1114">
   <si>
     <t>Domain</t>
   </si>
@@ -3469,6 +3469,9 @@
   </si>
   <si>
     <t>OBJECTID IS NOT NULL;</t>
+  </si>
+  <si>
+    <t>D:/ntnl_li_2018_template/data/study_region/australia/Australia_20181001.osm</t>
   </si>
 </sst>
 </file>
@@ -55219,10 +55222,10 @@
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G26" sqref="G26"/>
+      <selection pane="bottomRight" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55849,7 +55852,7 @@
         <v>454</v>
       </c>
       <c r="I13" s="82" t="str">
-        <f t="shared" ref="I13:I25" si="1">"D:/ntnl_li_2018_template/data/study_region/"&amp;B13&amp;"/"&amp;L13&amp;"_20181001.osm"</f>
+        <f t="shared" ref="I13:I26" si="1">"D:/ntnl_li_2018_template/data/study_region/"&amp;B13&amp;"/"&amp;L13&amp;"_20181001.osm"</f>
         <v>D:/ntnl_li_2018_template/data/study_region/ballarat/ballarat_20181001.osm</v>
       </c>
       <c r="J13" s="82" t="s">
@@ -56469,7 +56472,7 @@
         <v>1109</v>
       </c>
       <c r="I26" s="79" t="s">
-        <v>1109</v>
+        <v>1113</v>
       </c>
       <c r="J26" s="79" t="s">
         <v>877</v>

</xml_diff>

<commit_message>
added in idea for update, i'm not sure if i'll implement
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70186089-7431-49D1-8521-5A699FE86668}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF55F5C-CB53-4E76-BB74-2DB5A226130B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="2" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -4284,6 +4284,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4299,7 +4300,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -54370,7 +54370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3E5F03-EC28-486B-BA51-9D83D1ACCD02}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
@@ -54542,7 +54542,7 @@
         <v>1073</v>
       </c>
       <c r="B12" s="69">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="38" t="s">
         <v>801</v>
@@ -57307,7 +57307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -57399,7 +57399,7 @@
       <c r="K2" t="s">
         <v>1046</v>
       </c>
-      <c r="L2" s="111" t="s">
+      <c r="L2" s="106" t="s">
         <v>1128</v>
       </c>
       <c r="M2" t="s">
@@ -57440,7 +57440,7 @@
       <c r="K3" t="s">
         <v>945</v>
       </c>
-      <c r="L3" s="111" t="s">
+      <c r="L3" s="106" t="s">
         <v>1129</v>
       </c>
       <c r="M3" t="s">
@@ -57481,7 +57481,7 @@
       <c r="K4" t="s">
         <v>1115</v>
       </c>
-      <c r="L4" s="111" t="s">
+      <c r="L4" s="106" t="s">
         <v>1130</v>
       </c>
     </row>
@@ -57513,7 +57513,7 @@
       <c r="K5" t="s">
         <v>1060</v>
       </c>
-      <c r="L5" s="111" t="s">
+      <c r="L5" s="106" t="s">
         <v>1133</v>
       </c>
     </row>
@@ -57545,7 +57545,7 @@
       <c r="K6" t="s">
         <v>947</v>
       </c>
-      <c r="L6" s="111" t="s">
+      <c r="L6" s="106" t="s">
         <v>1131</v>
       </c>
     </row>
@@ -57577,7 +57577,7 @@
       <c r="K7" t="s">
         <v>944</v>
       </c>
-      <c r="L7" s="111" t="s">
+      <c r="L7" s="106" t="s">
         <v>1132</v>
       </c>
     </row>
@@ -58000,31 +58000,31 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="106" t="s">
+      <c r="G1" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
-      <c r="M1" s="107"/>
-      <c r="N1" s="107"/>
-      <c r="O1" s="107"/>
-      <c r="P1" s="107"/>
-      <c r="Q1" s="107"/>
-      <c r="R1" s="107"/>
-      <c r="S1" s="107"/>
-      <c r="T1" s="107"/>
-      <c r="U1" s="107"/>
-      <c r="V1" s="107"/>
-      <c r="W1" s="107"/>
-      <c r="X1" s="108"/>
-      <c r="Y1" s="109" t="s">
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="108"/>
+      <c r="L1" s="108"/>
+      <c r="M1" s="108"/>
+      <c r="N1" s="108"/>
+      <c r="O1" s="108"/>
+      <c r="P1" s="108"/>
+      <c r="Q1" s="108"/>
+      <c r="R1" s="108"/>
+      <c r="S1" s="108"/>
+      <c r="T1" s="108"/>
+      <c r="U1" s="108"/>
+      <c r="V1" s="108"/>
+      <c r="W1" s="108"/>
+      <c r="X1" s="109"/>
+      <c r="Y1" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="Z1" s="107"/>
-      <c r="AA1" s="110"/>
+      <c r="Z1" s="108"/>
+      <c r="AA1" s="111"/>
       <c r="AB1" s="2" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
updated canberra no forward edges
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B58F15-4DC6-4F2F-AC87-AFE12CAEDC52}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493C9ADA-3F9C-4F55-8242-ED021AEF3419}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="3" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -4284,6 +4284,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4299,7 +4300,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -55285,11 +55285,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317EB008-F691-4F16-B99A-D5845A82BBBD}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G23" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I27" sqref="I27"/>
+      <selection pane="bottomRight" activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55551,7 +55551,7 @@
       <c r="O5" s="82"/>
       <c r="P5" s="51"/>
       <c r="Q5" s="51">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -57307,7 +57307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -57399,7 +57399,7 @@
       <c r="K2" t="s">
         <v>1046</v>
       </c>
-      <c r="L2" s="111" t="s">
+      <c r="L2" s="106" t="s">
         <v>1128</v>
       </c>
       <c r="M2" t="s">
@@ -57440,7 +57440,7 @@
       <c r="K3" t="s">
         <v>945</v>
       </c>
-      <c r="L3" s="111" t="s">
+      <c r="L3" s="106" t="s">
         <v>1129</v>
       </c>
       <c r="M3" t="s">
@@ -57481,7 +57481,7 @@
       <c r="K4" t="s">
         <v>1115</v>
       </c>
-      <c r="L4" s="111" t="s">
+      <c r="L4" s="106" t="s">
         <v>1130</v>
       </c>
     </row>
@@ -57513,7 +57513,7 @@
       <c r="K5" t="s">
         <v>1060</v>
       </c>
-      <c r="L5" s="111" t="s">
+      <c r="L5" s="106" t="s">
         <v>1133</v>
       </c>
     </row>
@@ -57545,7 +57545,7 @@
       <c r="K6" t="s">
         <v>947</v>
       </c>
-      <c r="L6" s="111" t="s">
+      <c r="L6" s="106" t="s">
         <v>1131</v>
       </c>
     </row>
@@ -57577,7 +57577,7 @@
       <c r="K7" t="s">
         <v>944</v>
       </c>
-      <c r="L7" s="111" t="s">
+      <c r="L7" s="106" t="s">
         <v>1132</v>
       </c>
     </row>
@@ -58000,31 +58000,31 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="106" t="s">
+      <c r="G1" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
-      <c r="M1" s="107"/>
-      <c r="N1" s="107"/>
-      <c r="O1" s="107"/>
-      <c r="P1" s="107"/>
-      <c r="Q1" s="107"/>
-      <c r="R1" s="107"/>
-      <c r="S1" s="107"/>
-      <c r="T1" s="107"/>
-      <c r="U1" s="107"/>
-      <c r="V1" s="107"/>
-      <c r="W1" s="107"/>
-      <c r="X1" s="108"/>
-      <c r="Y1" s="109" t="s">
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="108"/>
+      <c r="L1" s="108"/>
+      <c r="M1" s="108"/>
+      <c r="N1" s="108"/>
+      <c r="O1" s="108"/>
+      <c r="P1" s="108"/>
+      <c r="Q1" s="108"/>
+      <c r="R1" s="108"/>
+      <c r="S1" s="108"/>
+      <c r="T1" s="108"/>
+      <c r="U1" s="108"/>
+      <c r="V1" s="108"/>
+      <c r="W1" s="108"/>
+      <c r="X1" s="109"/>
+      <c r="Y1" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="Z1" s="107"/>
-      <c r="AA1" s="110"/>
+      <c r="Z1" s="108"/>
+      <c r="AA1" s="111"/>
       <c r="AB1" s="2" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
updated the 15c script for area level summary to use vicmap network
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CE9C8C-F870-4025-B884-5FF1A8080850}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D022DA0-3506-4B5E-B06B-E8DFB0501D62}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="3" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -55285,7 +55285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317EB008-F691-4F16-B99A-D5845A82BBBD}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -57307,8 +57307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated the OD AOS process to work more efficiently and better account for intersections in light of recent lessons from Melb comparison analyses
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D022DA0-3506-4B5E-B06B-E8DFB0501D62}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76508D7-2A34-4C42-B343-B6001442B10B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2352" uniqueCount="1135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2348" uniqueCount="1131">
   <si>
     <t>Domain</t>
   </si>
@@ -3001,12 +3001,6 @@
     <t>grass</t>
   </si>
   <si>
-    <t>green</t>
-  </si>
-  <si>
-    <t>meadow</t>
-  </si>
-  <si>
     <t>orchard</t>
   </si>
   <si>
@@ -3309,9 +3303,6 @@
     <t>A list of OSM and derived data columns which should be included as open_space feature tags (in addition to existing tags) when collating open space features to an Area of Open Space.</t>
   </si>
   <si>
-    <t>p.landuse IS NULL OR p.landuse NOT IN ('military')</t>
-  </si>
-  <si>
     <t>recreation_ground</t>
   </si>
   <si>
@@ -3507,12 +3498,6 @@
     <t>reservoir</t>
   </si>
   <si>
-    <t>sand</t>
-  </si>
-  <si>
-    <t>salt_pond</t>
-  </si>
-  <si>
     <t>sports_centre</t>
   </si>
   <si>
@@ -3535,6 +3520,9 @@
   </si>
   <si>
     <t>public_access</t>
+  </si>
+  <si>
+    <t>p.landuse IS NULL OR p.landuse NOT IN ('military','industrial')</t>
   </si>
 </sst>
 </file>
@@ -5146,18 +5134,18 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="D58" s="63" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B59" s="63" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="C59" s="64" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -5165,63 +5153,63 @@
         <v>950</v>
       </c>
       <c r="C60" s="64" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B61" s="63" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="C61" s="64" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" s="63" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="C62" s="64" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B63" s="63" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="C63" s="64" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="63" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="C64" s="64" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="63" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="C65" s="64" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B66" s="63" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="C66" s="64" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B67" s="63" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="C67" s="64" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
@@ -54539,7 +54527,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="B12" s="69">
         <v>6</v>
@@ -54548,7 +54536,7 @@
         <v>801</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>1074</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -54970,16 +54958,16 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1084</v>
+        <v>1081</v>
       </c>
       <c r="B43" s="69" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
       <c r="C43" s="38" t="s">
         <v>806</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>1085</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -55236,44 +55224,44 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1075</v>
+        <v>1072</v>
       </c>
       <c r="B62" s="69" t="s">
-        <v>1083</v>
+        <v>1080</v>
       </c>
       <c r="C62" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D62" s="38" t="s">
-        <v>1076</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>1077</v>
+        <v>1074</v>
       </c>
       <c r="B63" s="69" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="C63" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D63" s="38" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="B64" s="69" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="C64" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D64" s="38" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
     </row>
   </sheetData>
@@ -55344,7 +55332,7 @@
         <v>901</v>
       </c>
       <c r="L1" s="71" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
       <c r="M1" s="71" t="s">
         <v>833</v>
@@ -55397,7 +55385,7 @@
         <v>osm_10km_testing_10km_pedestrian_20181001</v>
       </c>
       <c r="L2" s="75" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="M2" s="75" t="s">
         <v>858</v>
@@ -55879,7 +55867,7 @@
         <v>926</v>
       </c>
       <c r="L12" s="79" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="M12" s="79"/>
       <c r="N12" s="80" t="s">
@@ -56116,7 +56104,7 @@
         <v>931</v>
       </c>
       <c r="L17" s="82" t="s">
-        <v>1087</v>
+        <v>1084</v>
       </c>
       <c r="M17" s="82"/>
       <c r="N17" s="83" t="s">
@@ -56259,7 +56247,7 @@
         <v>934</v>
       </c>
       <c r="L20" s="79" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="M20" s="79"/>
       <c r="N20" s="80" t="s">
@@ -56306,7 +56294,7 @@
         <v>935</v>
       </c>
       <c r="L21" s="82" t="s">
-        <v>1089</v>
+        <v>1086</v>
       </c>
       <c r="M21" s="82"/>
       <c r="N21" s="83" t="s">
@@ -56496,7 +56484,7 @@
         <v>938</v>
       </c>
       <c r="L25" s="82" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
       <c r="M25" s="82"/>
       <c r="N25" s="83" t="s">
@@ -56512,40 +56500,40 @@
     </row>
     <row r="26" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="78" t="s">
-        <v>1106</v>
+        <v>1103</v>
       </c>
       <c r="B26" s="79" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
       <c r="C26" s="79" t="s">
         <v>912</v>
       </c>
       <c r="D26" s="79" t="s">
-        <v>1110</v>
+        <v>1107</v>
       </c>
       <c r="E26" s="79" t="s">
-        <v>1110</v>
+        <v>1107</v>
       </c>
       <c r="F26" s="80" t="s">
+        <v>1106</v>
+      </c>
+      <c r="G26" s="79" t="s">
+        <v>1108</v>
+      </c>
+      <c r="H26" s="79" t="s">
+        <v>1105</v>
+      </c>
+      <c r="I26" s="79" t="s">
         <v>1109</v>
-      </c>
-      <c r="G26" s="79" t="s">
-        <v>1111</v>
-      </c>
-      <c r="H26" s="79" t="s">
-        <v>1108</v>
-      </c>
-      <c r="I26" s="79" t="s">
-        <v>1112</v>
       </c>
       <c r="J26" s="79" t="s">
         <v>877</v>
       </c>
       <c r="K26" s="79" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
       <c r="L26" s="79" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
       <c r="M26" s="79"/>
       <c r="N26" s="80" t="s">
@@ -57307,8 +57295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57326,43 +57314,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="B1" s="37" t="s">
         <v>950</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="E1" s="37" t="s">
+        <v>968</v>
+      </c>
+      <c r="F1" s="37" t="s">
         <v>970</v>
       </c>
-      <c r="F1" s="37" t="s">
-        <v>972</v>
-      </c>
       <c r="G1" s="37" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="H1" s="37" t="s">
+        <v>1113</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>1038</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>1050</v>
+      </c>
+      <c r="K1" s="37" t="s">
+        <v>1115</v>
+      </c>
+      <c r="L1" s="37" t="s">
         <v>1116</v>
       </c>
-      <c r="I1" s="37" t="s">
-        <v>1040</v>
-      </c>
-      <c r="J1" s="37" t="s">
-        <v>1052</v>
-      </c>
-      <c r="K1" s="37" t="s">
-        <v>1118</v>
-      </c>
-      <c r="L1" s="37" t="s">
-        <v>1119</v>
-      </c>
       <c r="M1" s="37" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -57373,37 +57361,37 @@
         <v>951</v>
       </c>
       <c r="C2" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="D2" t="s">
-        <v>1120</v>
+        <v>1117</v>
       </c>
       <c r="E2" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="F2" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="G2" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="H2" t="s">
-        <v>1095</v>
+        <v>1092</v>
       </c>
       <c r="I2" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="J2" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="K2" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="L2" s="106" t="s">
-        <v>1128</v>
+        <v>1123</v>
       </c>
       <c r="M2" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -57411,40 +57399,40 @@
         <v>940</v>
       </c>
       <c r="B3" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="C3" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="D3" t="s">
-        <v>1059</v>
+        <v>1130</v>
       </c>
       <c r="E3" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="F3" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="G3" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="H3" t="s">
-        <v>1096</v>
+        <v>1093</v>
       </c>
       <c r="I3" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="J3" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="K3" t="s">
         <v>945</v>
       </c>
       <c r="L3" s="106" t="s">
-        <v>1129</v>
+        <v>1124</v>
       </c>
       <c r="M3" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -57455,34 +57443,34 @@
         <v>952</v>
       </c>
       <c r="C4" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="D4" t="s">
-        <v>1113</v>
+        <v>1110</v>
       </c>
       <c r="E4" t="s">
-        <v>1114</v>
+        <v>1111</v>
       </c>
       <c r="F4" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="G4" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="H4" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
       <c r="I4" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="J4" t="s">
-        <v>1134</v>
+        <v>1129</v>
       </c>
       <c r="K4" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="L4" s="106" t="s">
-        <v>1130</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -57499,22 +57487,22 @@
         <v>939</v>
       </c>
       <c r="G5" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="H5" t="s">
-        <v>1098</v>
+        <v>1095</v>
       </c>
       <c r="I5" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="J5" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="K5" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
       <c r="L5" s="106" t="s">
-        <v>1133</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -57525,19 +57513,19 @@
         <v>954</v>
       </c>
       <c r="C6" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="F6" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="G6" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="H6" t="s">
-        <v>1099</v>
+        <v>1096</v>
       </c>
       <c r="I6" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="J6" t="s">
         <v>944</v>
@@ -57546,7 +57534,7 @@
         <v>947</v>
       </c>
       <c r="L6" s="106" t="s">
-        <v>1131</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -57557,28 +57545,28 @@
         <v>955</v>
       </c>
       <c r="C7" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="F7" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="G7" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="H7" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
       <c r="I7" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="J7" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
       <c r="K7" t="s">
         <v>944</v>
       </c>
       <c r="L7" s="106" t="s">
-        <v>1132</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -57589,19 +57577,19 @@
         <v>956</v>
       </c>
       <c r="C8" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="F8" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="G8" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="H8" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
       <c r="I8" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="J8" t="s">
         <v>948</v>
@@ -57612,22 +57600,22 @@
         <v>946</v>
       </c>
       <c r="B9" t="s">
-        <v>957</v>
+        <v>945</v>
       </c>
       <c r="C9" t="s">
-        <v>1071</v>
+        <v>1068</v>
       </c>
       <c r="F9" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="G9" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="H9" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
       <c r="I9" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="J9" t="s">
         <v>945</v>
@@ -57638,19 +57626,19 @@
         <v>947</v>
       </c>
       <c r="B10" t="s">
-        <v>945</v>
+        <v>957</v>
       </c>
       <c r="C10" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="F10" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="G10" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="H10" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
       <c r="I10" t="s">
         <v>695</v>
@@ -57667,16 +57655,16 @@
         <v>958</v>
       </c>
       <c r="C11" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="F11" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="G11" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="I11" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="J11" t="s">
         <v>947</v>
@@ -57690,13 +57678,13 @@
         <v>959</v>
       </c>
       <c r="F12" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="G12" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="I12" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="J12" t="s">
         <v>942</v>
@@ -57704,225 +57692,213 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
       <c r="B13" t="s">
         <v>960</v>
       </c>
       <c r="F13" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="G13" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="I13" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="J13" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
       <c r="B14" t="s">
-        <v>961</v>
+        <v>1057</v>
       </c>
       <c r="F14" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="G14" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="I14" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="J14" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>962</v>
+        <v>947</v>
       </c>
       <c r="F15" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="I15" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="J15" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>1060</v>
+        <v>961</v>
       </c>
       <c r="F16" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="I16" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="J16" t="s">
-        <v>1094</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>947</v>
+        <v>1058</v>
       </c>
       <c r="F17" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="I17" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="J17" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>963</v>
+        <v>941</v>
       </c>
       <c r="F18" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="I18" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="J18" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>1061</v>
+        <v>962</v>
       </c>
       <c r="F19" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="I19" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="J19" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>941</v>
+        <v>963</v>
       </c>
       <c r="F20" t="s">
         <v>940</v>
       </c>
       <c r="J20" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>964</v>
+        <v>1118</v>
       </c>
       <c r="F21" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="J21" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>965</v>
+        <v>1119</v>
       </c>
       <c r="F22" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="J22" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>1121</v>
+        <v>1061</v>
       </c>
       <c r="F23" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="J23" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="F24" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="J24" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>1064</v>
+        <v>1121</v>
       </c>
       <c r="F25" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="F26" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
         <v>994</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>1124</v>
-      </c>
-      <c r="F27" t="s">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
         <v>995</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>1125</v>
-      </c>
-      <c r="F28" t="s">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
         <v>996</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>1126</v>
-      </c>
-      <c r="F29" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>1127</v>
-      </c>
-      <c r="F30" t="s">
-        <v>998</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.25">
@@ -57932,17 +57908,17 @@
     </row>
     <row r="34" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
     </row>
     <row r="35" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="36" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="37" spans="6:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
identified and fixed an error where by park nodes for 'any' pos comparison analysis were not restricted to Public indicated open spaces.  Of course, they should have been.  This issue impacted all POS regardless of network, but only for the any analysis.  The new results should be available by 10 am on Friday 16 Nov.
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76508D7-2A34-4C42-B343-B6001442B10B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A707007-4E67-494E-990F-4E750FBC48FB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="6" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -19,12 +19,13 @@
     <sheet name="study_regions" sheetId="3" r:id="rId4"/>
     <sheet name="destinations" sheetId="6" r:id="rId5"/>
     <sheet name="open_space_defs" sheetId="10" r:id="rId6"/>
-    <sheet name="indicators" sheetId="1" r:id="rId7"/>
-    <sheet name="ind_study_region_matrix" sheetId="2" r:id="rId8"/>
-    <sheet name="local_environments" sheetId="9" r:id="rId9"/>
+    <sheet name="ULI" sheetId="11" r:id="rId7"/>
+    <sheet name="indicators" sheetId="1" r:id="rId8"/>
+    <sheet name="ind_study_region_matrix" sheetId="2" r:id="rId9"/>
+    <sheet name="local_environments" sheetId="9" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">indicators!$A$2:$AC$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">indicators!$A$2:$AC$48</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2348" uniqueCount="1131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2432" uniqueCount="1165">
   <si>
     <t>Domain</t>
   </si>
@@ -3524,12 +3525,114 @@
   <si>
     <t>p.landuse IS NULL OR p.landuse NOT IN ('military','industrial')</t>
   </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>TAS</t>
+  </si>
+  <si>
+    <t>VIC</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Gtfs transport</t>
+  </si>
+  <si>
+    <t>processing</t>
+  </si>
+  <si>
+    <t>GTFS</t>
+  </si>
+  <si>
+    <t>Supermarket</t>
+  </si>
+  <si>
+    <t>acquired</t>
+  </si>
+  <si>
+    <t>scraped / OSM?</t>
+  </si>
+  <si>
+    <t>Community centre</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>open data / osm?</t>
+  </si>
+  <si>
+    <t>Museum / Art gallery</t>
+  </si>
+  <si>
+    <t>Cinema / Theatre</t>
+  </si>
+  <si>
+    <t>Library</t>
+  </si>
+  <si>
+    <t>https://data.gov.au/dataset/queensland-public-libraries</t>
+  </si>
+  <si>
+    <t>D:/ntnl_li_2018_template/data/destinations/libraries/QLD/publiclibrarybranches-with-coordinates6march18slq.csv</t>
+  </si>
+  <si>
+    <t>https://data.gov.au/dataset/western-australia-public-library-network</t>
+  </si>
+  <si>
+    <t>D:/ntnl_li_2018_template/data/destinations/libraries/WA/libraries20160206.csv</t>
+  </si>
+  <si>
+    <t>Childcare</t>
+  </si>
+  <si>
+    <t>yes?</t>
+  </si>
+  <si>
+    <t>acequa?</t>
+  </si>
+  <si>
+    <t>Childcare OSH</t>
+  </si>
+  <si>
+    <t>State secondary school</t>
+  </si>
+  <si>
+    <t>acequa</t>
+  </si>
+  <si>
+    <t>State primary school</t>
+  </si>
+  <si>
+    <t>Aged care</t>
+  </si>
+  <si>
+    <t>nhsd</t>
+  </si>
+  <si>
+    <t>Community health centre</t>
+  </si>
+  <si>
+    <t>nhsd?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3647,6 +3750,14 @@
       <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3982,10 +4093,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -4288,8 +4400,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4657,6 +4774,33 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0682DDBC-BDF5-465A-84E8-EDD50FC1290A}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="61.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>861</v>
+      </c>
+      <c r="B1" t="s">
+        <v>862</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{169A8F36-66C8-40F7-A0A8-79F453EFA097}">
   <dimension ref="A1:D16445"/>
@@ -57295,7 +57439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9:B26"/>
     </sheetView>
   </sheetViews>
@@ -57938,6 +58082,346 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00663411-69BA-4AA2-8F13-6278DC3BD89D}">
+  <dimension ref="A1:AB14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="28" width="9.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>598</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>597</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E1" s="112" t="s">
+        <v>441</v>
+      </c>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112" t="s">
+        <v>462</v>
+      </c>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112" t="s">
+        <v>444</v>
+      </c>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112" t="s">
+        <v>1133</v>
+      </c>
+      <c r="O1" s="112"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112" t="s">
+        <v>436</v>
+      </c>
+      <c r="R1" s="112"/>
+      <c r="S1" s="112"/>
+      <c r="T1" s="112" t="s">
+        <v>431</v>
+      </c>
+      <c r="U1" s="112"/>
+      <c r="V1" s="112"/>
+      <c r="W1" s="112" t="s">
+        <v>1134</v>
+      </c>
+      <c r="X1" s="112"/>
+      <c r="Y1" s="112"/>
+      <c r="Z1" s="112" t="s">
+        <v>457</v>
+      </c>
+      <c r="AA1" s="112"/>
+      <c r="AB1" s="112"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>1132</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>1137</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="J2" s="37" t="s">
+        <v>1136</v>
+      </c>
+      <c r="K2" s="37" t="s">
+        <v>1137</v>
+      </c>
+      <c r="L2" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="M2" s="37" t="s">
+        <v>1136</v>
+      </c>
+      <c r="N2" s="37" t="s">
+        <v>1137</v>
+      </c>
+      <c r="O2" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="P2" s="37" t="s">
+        <v>1136</v>
+      </c>
+      <c r="Q2" s="37" t="s">
+        <v>1137</v>
+      </c>
+      <c r="R2" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="S2" s="37" t="s">
+        <v>1136</v>
+      </c>
+      <c r="T2" s="37" t="s">
+        <v>1137</v>
+      </c>
+      <c r="U2" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="V2" s="37" t="s">
+        <v>1136</v>
+      </c>
+      <c r="W2" s="37" t="s">
+        <v>1137</v>
+      </c>
+      <c r="X2" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="Y2" s="37" t="s">
+        <v>1136</v>
+      </c>
+      <c r="Z2" s="37" t="s">
+        <v>1137</v>
+      </c>
+      <c r="AA2" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="AB2" s="37" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1140</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1140</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1140</v>
+      </c>
+      <c r="O3" t="s">
+        <v>1140</v>
+      </c>
+      <c r="R3" t="s">
+        <v>1140</v>
+      </c>
+      <c r="U3" t="s">
+        <v>1140</v>
+      </c>
+      <c r="X3" t="s">
+        <v>1140</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1146</v>
+      </c>
+      <c r="Q8">
+        <v>2018</v>
+      </c>
+      <c r="R8" s="113" t="s">
+        <v>1150</v>
+      </c>
+      <c r="S8" t="s">
+        <v>1151</v>
+      </c>
+      <c r="Z8">
+        <v>2016</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>1152</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="T1:V1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="R8" r:id="rId1" xr:uid="{880BC495-9AE4-466F-8181-3A3C0C200010}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA10FF44-D24D-4AD6-829C-327E640FAE4C}">
   <dimension ref="A1:AC48"/>
   <sheetViews>
@@ -60130,7 +60614,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E520E13B-C7CF-4991-8581-C25916074E3A}">
   <dimension ref="A1:O87"/>
   <sheetViews>
@@ -63856,31 +64340,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0682DDBC-BDF5-465A-84E8-EDD50FC1290A}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="61.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>861</v>
-      </c>
-      <c r="B1" t="s">
-        <v>862</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
amended the AOS set up script; more changes to definition are coming in future push
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A707007-4E67-494E-990F-4E750FBC48FB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8ADA34-E63C-4B85-90E9-0FF2435F8DF3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="6" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2432" uniqueCount="1165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="1173">
   <si>
     <t>Domain</t>
   </si>
@@ -3463,21 +3463,12 @@
     <t>D:/ntnl_li_2018_template/data/study_region/australia/Australia_20181001.osm</t>
   </si>
   <si>
-    <t>p.tourism IS NULL or p.tourism NOT IN ('zoo')</t>
-  </si>
-  <si>
-    <t>Enclosed animal spaces were decided to be excluded; also, most cases private</t>
-  </si>
-  <si>
     <t>area</t>
   </si>
   <si>
     <t>linear_feature_criteria</t>
   </si>
   <si>
-    <t>optional_exclusions</t>
-  </si>
-  <si>
     <t>public_field</t>
   </si>
   <si>
@@ -3505,9 +3496,6 @@
     <t>'aged_care','animal_boarding','allotments','animal_boarding','bank','bar','biergarten','boatyard','carpark','childcare','casino','church','club','club_house','college','conference_centre','embassy','fast_food','garden_centre','grave_yard','hospital','gym','kindergarten','monastery','motel','nursing home','parking','parking_space','prison','retirement','retirement_home','retirement_village','school','scout_hut','university'</t>
   </si>
   <si>
-    <t>'golf_course','horse_riding', 'racetrack','summer_camp','sports_club'</t>
-  </si>
-  <si>
     <t>'school'</t>
   </si>
   <si>
@@ -3626,6 +3614,42 @@
   </si>
   <si>
     <t>nhsd?</t>
+  </si>
+  <si>
+    <t>https://www.data.vic.gov.au/data/dataset/libraries</t>
+  </si>
+  <si>
+    <t>D:/ntnl_li_2018_template/data/destinations/libraries/VIC/fileslibraries.csv</t>
+  </si>
+  <si>
+    <t>D:/ntnl_li_2018_template/data/destinations/libraries/ACT/Library_Locations.csv</t>
+  </si>
+  <si>
+    <t>https://www.data.act.gov.au/Government-and-Transparency/Library-Locations/hssi-h7fk</t>
+  </si>
+  <si>
+    <t>e-mail</t>
+  </si>
+  <si>
+    <t>D:/ntnl_li_2018_template/data/destinations/libraries/NSW/Library-Export  - NSW official library data  - XY coord seperated_20160301.xlsx</t>
+  </si>
+  <si>
+    <t>'golf_course','horse_riding', 'racetrack','summer_camp','sports_club','stadium','sports_centre'</t>
+  </si>
+  <si>
+    <t>golf</t>
+  </si>
+  <si>
+    <t>golf IS NULL</t>
+  </si>
+  <si>
+    <t>additional_public_criteria</t>
+  </si>
+  <si>
+    <t>Previously we had another clause 'p.tourism IS NULL or p.tourism NOT IN ('zoo')' for the reason 'Enclosed animal spaces were decided to be excluded; also, most cases private'; However, but not including it we lose the bounding 'zoo' box which we can  distinguish as being private --- because we lose that we are unable to distinguish the individual animal enclosures and other zoo features which appear natural as also being private (by virtue of being enclosed in a private space).  So, we must include zoos as open space in order to flag them as public.</t>
+  </si>
+  <si>
+    <t>within_public</t>
   </si>
 </sst>
 </file>
@@ -4097,7 +4121,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -4403,13 +4427,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -57439,21 +57482,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="2" max="3" width="21.28515625" customWidth="1"/>
-    <col min="4" max="4" width="91.5703125" customWidth="1"/>
+    <col min="4" max="4" width="70.42578125" customWidth="1"/>
     <col min="5" max="5" width="94.5703125" customWidth="1"/>
     <col min="6" max="6" width="41.5703125" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="41" customWidth="1"/>
     <col min="9" max="9" width="29.140625" customWidth="1"/>
     <col min="10" max="10" width="26.85546875" customWidth="1"/>
+    <col min="12" max="12" width="27.28515625" customWidth="1"/>
+    <col min="13" max="13" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -57479,7 +57524,7 @@
         <v>1002</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="I1" s="37" t="s">
         <v>1038</v>
@@ -57488,13 +57533,13 @@
         <v>1050</v>
       </c>
       <c r="K1" s="37" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="L1" s="37" t="s">
-        <v>1116</v>
+        <v>1113</v>
       </c>
       <c r="M1" s="37" t="s">
-        <v>1114</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -57508,7 +57553,7 @@
         <v>1062</v>
       </c>
       <c r="D2" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
       <c r="E2" t="s">
         <v>966</v>
@@ -57532,10 +57577,10 @@
         <v>1044</v>
       </c>
       <c r="L2" s="106" t="s">
-        <v>1123</v>
+        <v>1120</v>
       </c>
       <c r="M2" t="s">
-        <v>1003</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -57549,7 +57594,7 @@
         <v>1063</v>
       </c>
       <c r="D3" t="s">
-        <v>1130</v>
+        <v>1126</v>
       </c>
       <c r="E3" t="s">
         <v>967</v>
@@ -57573,10 +57618,7 @@
         <v>945</v>
       </c>
       <c r="L3" s="106" t="s">
-        <v>1124</v>
-      </c>
-      <c r="M3" t="s">
-        <v>995</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -57589,11 +57631,8 @@
       <c r="C4" t="s">
         <v>1061</v>
       </c>
-      <c r="D4" t="s">
-        <v>1110</v>
-      </c>
       <c r="E4" t="s">
-        <v>1111</v>
+        <v>1171</v>
       </c>
       <c r="F4" t="s">
         <v>973</v>
@@ -57608,13 +57647,13 @@
         <v>1023</v>
       </c>
       <c r="J4" t="s">
-        <v>1129</v>
+        <v>1125</v>
       </c>
       <c r="K4" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="L4" s="106" t="s">
-        <v>1125</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -57640,13 +57679,13 @@
         <v>1024</v>
       </c>
       <c r="J5" t="s">
-        <v>1044</v>
+        <v>1172</v>
       </c>
       <c r="K5" t="s">
         <v>1057</v>
       </c>
       <c r="L5" s="106" t="s">
-        <v>1128</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -57672,13 +57711,13 @@
         <v>1025</v>
       </c>
       <c r="J6" t="s">
-        <v>944</v>
+        <v>1044</v>
       </c>
       <c r="K6" t="s">
         <v>947</v>
       </c>
       <c r="L6" s="106" t="s">
-        <v>1126</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -57704,13 +57743,13 @@
         <v>1026</v>
       </c>
       <c r="J7" t="s">
-        <v>1065</v>
+        <v>944</v>
       </c>
       <c r="K7" t="s">
         <v>944</v>
       </c>
       <c r="L7" s="106" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -57736,7 +57775,7 @@
         <v>1027</v>
       </c>
       <c r="J8" t="s">
-        <v>948</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -57762,7 +57801,7 @@
         <v>1028</v>
       </c>
       <c r="J9" t="s">
-        <v>945</v>
+        <v>948</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -57788,7 +57827,7 @@
         <v>695</v>
       </c>
       <c r="J10" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -57811,7 +57850,7 @@
         <v>1029</v>
       </c>
       <c r="J11" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -57831,7 +57870,7 @@
         <v>1030</v>
       </c>
       <c r="J12" t="s">
-        <v>942</v>
+        <v>947</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -57851,7 +57890,7 @@
         <v>1031</v>
       </c>
       <c r="J13" t="s">
-        <v>963</v>
+        <v>942</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -57871,10 +57910,13 @@
         <v>1032</v>
       </c>
       <c r="J14" t="s">
-        <v>1045</v>
+        <v>963</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1168</v>
+      </c>
       <c r="B15" t="s">
         <v>947</v>
       </c>
@@ -57885,7 +57927,7 @@
         <v>1033</v>
       </c>
       <c r="J15" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -57899,7 +57941,7 @@
         <v>1034</v>
       </c>
       <c r="J16" t="s">
-        <v>1091</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -57913,7 +57955,7 @@
         <v>1035</v>
       </c>
       <c r="J17" t="s">
-        <v>1047</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -57927,7 +57969,7 @@
         <v>1036</v>
       </c>
       <c r="J18" t="s">
-        <v>1041</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -57941,7 +57983,7 @@
         <v>1037</v>
       </c>
       <c r="J19" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -57952,29 +57994,29 @@
         <v>940</v>
       </c>
       <c r="J20" t="s">
-        <v>1101</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="F21" t="s">
         <v>987</v>
       </c>
       <c r="J21" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>1119</v>
+        <v>1116</v>
       </c>
       <c r="F22" t="s">
         <v>988</v>
       </c>
       <c r="J22" t="s">
-        <v>1043</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
@@ -57985,31 +58027,34 @@
         <v>989</v>
       </c>
       <c r="J23" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>1120</v>
+        <v>1117</v>
       </c>
       <c r="F24" t="s">
         <v>990</v>
       </c>
       <c r="J24" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="F25" t="s">
         <v>991</v>
       </c>
+      <c r="J25" t="s">
+        <v>1049</v>
+      </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
       <c r="F26" t="s">
         <v>992</v>
@@ -58085,8 +58130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00663411-69BA-4AA2-8F13-6278DC3BD89D}">
   <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58094,21 +58139,21 @@
     <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="28" width="9.7109375" customWidth="1"/>
+    <col min="5" max="28" width="9.7109375" style="69" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:28" s="116" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="115" t="s">
         <v>598</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="115" t="s">
         <v>597</v>
       </c>
-      <c r="C1" s="37" t="s">
-        <v>1131</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>1132</v>
+      <c r="C1" s="115" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D1" s="115" t="s">
+        <v>1128</v>
       </c>
       <c r="E1" s="112" t="s">
         <v>441</v>
@@ -58126,7 +58171,7 @@
       <c r="L1" s="112"/>
       <c r="M1" s="112"/>
       <c r="N1" s="112" t="s">
-        <v>1133</v>
+        <v>1129</v>
       </c>
       <c r="O1" s="112"/>
       <c r="P1" s="112"/>
@@ -58141,7 +58186,7 @@
       <c r="U1" s="112"/>
       <c r="V1" s="112"/>
       <c r="W1" s="112" t="s">
-        <v>1134</v>
+        <v>1130</v>
       </c>
       <c r="X1" s="112"/>
       <c r="Y1" s="112"/>
@@ -58156,251 +58201,302 @@
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
       <c r="D2" s="37"/>
-      <c r="E2" s="37" t="s">
-        <v>1135</v>
-      </c>
-      <c r="F2" s="37" t="s">
+      <c r="E2" s="113" t="s">
+        <v>1131</v>
+      </c>
+      <c r="F2" s="113" t="s">
+        <v>1128</v>
+      </c>
+      <c r="G2" s="113" t="s">
         <v>1132</v>
       </c>
-      <c r="G2" s="37" t="s">
-        <v>1136</v>
-      </c>
-      <c r="H2" s="37" t="s">
-        <v>1137</v>
-      </c>
-      <c r="I2" s="37" t="s">
+      <c r="H2" s="113" t="s">
+        <v>1133</v>
+      </c>
+      <c r="I2" s="113" t="s">
         <v>209</v>
       </c>
-      <c r="J2" s="37" t="s">
-        <v>1136</v>
-      </c>
-      <c r="K2" s="37" t="s">
-        <v>1137</v>
-      </c>
-      <c r="L2" s="37" t="s">
+      <c r="J2" s="113" t="s">
+        <v>1132</v>
+      </c>
+      <c r="K2" s="113" t="s">
+        <v>1133</v>
+      </c>
+      <c r="L2" s="113" t="s">
         <v>209</v>
       </c>
-      <c r="M2" s="37" t="s">
-        <v>1136</v>
-      </c>
-      <c r="N2" s="37" t="s">
-        <v>1137</v>
-      </c>
-      <c r="O2" s="37" t="s">
+      <c r="M2" s="113" t="s">
+        <v>1132</v>
+      </c>
+      <c r="N2" s="113" t="s">
+        <v>1133</v>
+      </c>
+      <c r="O2" s="113" t="s">
         <v>209</v>
       </c>
-      <c r="P2" s="37" t="s">
-        <v>1136</v>
-      </c>
-      <c r="Q2" s="37" t="s">
-        <v>1137</v>
-      </c>
-      <c r="R2" s="37" t="s">
+      <c r="P2" s="113" t="s">
+        <v>1132</v>
+      </c>
+      <c r="Q2" s="113" t="s">
+        <v>1133</v>
+      </c>
+      <c r="R2" s="113" t="s">
         <v>209</v>
       </c>
-      <c r="S2" s="37" t="s">
-        <v>1136</v>
-      </c>
-      <c r="T2" s="37" t="s">
-        <v>1137</v>
-      </c>
-      <c r="U2" s="37" t="s">
+      <c r="S2" s="113" t="s">
+        <v>1132</v>
+      </c>
+      <c r="T2" s="113" t="s">
+        <v>1133</v>
+      </c>
+      <c r="U2" s="113" t="s">
         <v>209</v>
       </c>
-      <c r="V2" s="37" t="s">
-        <v>1136</v>
-      </c>
-      <c r="W2" s="37" t="s">
-        <v>1137</v>
-      </c>
-      <c r="X2" s="37" t="s">
+      <c r="V2" s="113" t="s">
+        <v>1132</v>
+      </c>
+      <c r="W2" s="113" t="s">
+        <v>1133</v>
+      </c>
+      <c r="X2" s="113" t="s">
         <v>209</v>
       </c>
-      <c r="Y2" s="37" t="s">
-        <v>1136</v>
-      </c>
-      <c r="Z2" s="37" t="s">
-        <v>1137</v>
-      </c>
-      <c r="AA2" s="37" t="s">
+      <c r="Y2" s="113" t="s">
+        <v>1132</v>
+      </c>
+      <c r="Z2" s="113" t="s">
+        <v>1133</v>
+      </c>
+      <c r="AA2" s="113" t="s">
         <v>209</v>
       </c>
-      <c r="AB2" s="37" t="s">
-        <v>1136</v>
+      <c r="AB2" s="113" t="s">
+        <v>1132</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>1138</v>
+        <v>1134</v>
       </c>
       <c r="C3" t="s">
-        <v>1139</v>
+        <v>1135</v>
       </c>
       <c r="D3" t="s">
-        <v>1140</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1140</v>
-      </c>
-      <c r="I3" t="s">
-        <v>1140</v>
-      </c>
-      <c r="L3" t="s">
-        <v>1140</v>
-      </c>
-      <c r="O3" t="s">
-        <v>1140</v>
-      </c>
-      <c r="R3" t="s">
-        <v>1140</v>
-      </c>
-      <c r="U3" t="s">
-        <v>1140</v>
-      </c>
-      <c r="X3" t="s">
-        <v>1140</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>1140</v>
+        <v>1136</v>
+      </c>
+      <c r="E3" s="69">
+        <v>2018</v>
+      </c>
+      <c r="F3" s="69" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H3" s="69">
+        <v>2018</v>
+      </c>
+      <c r="I3" s="69" t="s">
+        <v>1136</v>
+      </c>
+      <c r="K3" s="69">
+        <v>2018</v>
+      </c>
+      <c r="L3" s="69" t="s">
+        <v>1136</v>
+      </c>
+      <c r="N3" s="69">
+        <v>2018</v>
+      </c>
+      <c r="O3" s="69" t="s">
+        <v>1136</v>
+      </c>
+      <c r="Q3" s="69">
+        <v>2018</v>
+      </c>
+      <c r="R3" s="69" t="s">
+        <v>1136</v>
+      </c>
+      <c r="T3" s="69">
+        <v>2018</v>
+      </c>
+      <c r="U3" s="69" t="s">
+        <v>1136</v>
+      </c>
+      <c r="W3" s="69">
+        <v>2018</v>
+      </c>
+      <c r="X3" s="69" t="s">
+        <v>1136</v>
+      </c>
+      <c r="Z3" s="69">
+        <v>2018</v>
+      </c>
+      <c r="AA3" s="69" t="s">
+        <v>1136</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>1141</v>
+        <v>1137</v>
       </c>
       <c r="C4" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="D4" t="s">
-        <v>1143</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
       <c r="C5" t="s">
-        <v>1145</v>
+        <v>1141</v>
       </c>
       <c r="D5" t="s">
-        <v>1146</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>1147</v>
+        <v>1143</v>
       </c>
       <c r="C6" t="s">
-        <v>1145</v>
+        <v>1141</v>
       </c>
       <c r="D6" t="s">
-        <v>1146</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="C7" t="s">
-        <v>1145</v>
+        <v>1141</v>
       </c>
       <c r="D7" t="s">
-        <v>1146</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E8" s="69">
+        <v>2017</v>
+      </c>
+      <c r="F8" s="114" t="s">
+        <v>1164</v>
+      </c>
+      <c r="G8" s="69" t="s">
+        <v>1163</v>
+      </c>
+      <c r="H8" s="69">
+        <v>2016</v>
+      </c>
+      <c r="I8" s="69" t="s">
+        <v>1165</v>
+      </c>
+      <c r="J8" s="69" t="s">
+        <v>1166</v>
+      </c>
+      <c r="Q8" s="69">
+        <v>2018</v>
+      </c>
+      <c r="R8" s="114" t="s">
+        <v>1146</v>
+      </c>
+      <c r="S8" s="69" t="s">
+        <v>1147</v>
+      </c>
+      <c r="W8" s="69">
+        <v>2016</v>
+      </c>
+      <c r="X8" s="114" t="s">
+        <v>1161</v>
+      </c>
+      <c r="Y8" s="69" t="s">
+        <v>1162</v>
+      </c>
+      <c r="Z8" s="69">
+        <v>2016</v>
+      </c>
+      <c r="AA8" s="69" t="s">
+        <v>1148</v>
+      </c>
+      <c r="AB8" s="69" t="s">
         <v>1149</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1145</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1146</v>
-      </c>
-      <c r="Q8">
-        <v>2018</v>
-      </c>
-      <c r="R8" s="113" t="s">
-        <v>1150</v>
-      </c>
-      <c r="S8" t="s">
-        <v>1151</v>
-      </c>
-      <c r="Z8">
-        <v>2016</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>1152</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>1153</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="C9" t="s">
-        <v>1155</v>
+        <v>1151</v>
       </c>
       <c r="D9" t="s">
-        <v>1156</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>1157</v>
+        <v>1153</v>
       </c>
       <c r="C10" t="s">
-        <v>1155</v>
+        <v>1151</v>
       </c>
       <c r="D10" t="s">
-        <v>1156</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>1158</v>
+        <v>1154</v>
       </c>
       <c r="C11" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="D11" t="s">
-        <v>1159</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>1160</v>
+        <v>1156</v>
       </c>
       <c r="C12" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="D12" t="s">
-        <v>1159</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>1161</v>
+        <v>1157</v>
       </c>
       <c r="C13" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="D13" t="s">
-        <v>1162</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>1163</v>
+        <v>1159</v>
       </c>
       <c r="C14" t="s">
-        <v>1145</v>
+        <v>1141</v>
       </c>
       <c r="D14" t="s">
-        <v>1164</v>
+        <v>1160</v>
       </c>
     </row>
   </sheetData>
@@ -58414,8 +58510,15 @@
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="T1:V1"/>
   </mergeCells>
+  <conditionalFormatting sqref="E3:AB14">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(E3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="R8" r:id="rId1" xr:uid="{880BC495-9AE4-466F-8181-3A3C0C200010}"/>
+    <hyperlink ref="X8" r:id="rId2" xr:uid="{FB261EBD-990A-4D37-B19E-DDDA92832966}"/>
+    <hyperlink ref="F8" r:id="rId3" xr:uid="{FA499368-B6DC-442D-ABFF-FA03548B9B6A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
drafted up new AOS construction with exclusion areas
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8ADA34-E63C-4B85-90E9-0FF2435F8DF3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3427680-DB02-4798-BD51-0D5B145AFACD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="1173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2440" uniqueCount="1174">
   <si>
     <t>Domain</t>
   </si>
@@ -2990,19 +2990,10 @@
     <t>conservation</t>
   </si>
   <si>
-    <t>field</t>
-  </si>
-  <si>
     <t>forest</t>
   </si>
   <si>
     <t>garden</t>
-  </si>
-  <si>
-    <t>grass</t>
-  </si>
-  <si>
-    <t>orchard</t>
   </si>
   <si>
     <t>park</t>
@@ -3310,9 +3301,6 @@
     <t>village_green</t>
   </si>
   <si>
-    <t>cemetary</t>
-  </si>
-  <si>
     <t>os_boundary</t>
   </si>
   <si>
@@ -3475,21 +3463,12 @@
     <t>public_not_in</t>
   </si>
   <si>
-    <t>p.access IS NULL OR p.access NOT IN('employee','no','private','privates','staff')</t>
-  </si>
-  <si>
-    <t>basin</t>
-  </si>
-  <si>
     <t>dog_park</t>
   </si>
   <si>
     <t xml:space="preserve">off_leash </t>
   </si>
   <si>
-    <t>reservoir</t>
-  </si>
-  <si>
     <t>sports_centre</t>
   </si>
   <si>
@@ -3511,9 +3490,6 @@
     <t>public_access</t>
   </si>
   <si>
-    <t>p.landuse IS NULL OR p.landuse NOT IN ('military','industrial')</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
@@ -3650,6 +3626,33 @@
   </si>
   <si>
     <t>within_public</t>
+  </si>
+  <si>
+    <t>exclusion_field</t>
+  </si>
+  <si>
+    <t>exclusion_list</t>
+  </si>
+  <si>
+    <t>('employee','no','private','privates','staff')</t>
+  </si>
+  <si>
+    <t>('military','industrial')</t>
+  </si>
+  <si>
+    <t>exclusion_key</t>
+  </si>
+  <si>
+    <t>agricultural</t>
+  </si>
+  <si>
+    <t>forestry</t>
+  </si>
+  <si>
+    <t>military</t>
+  </si>
+  <si>
+    <t>possible_tags</t>
   </si>
 </sst>
 </file>
@@ -4409,6 +4412,21 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4423,21 +4441,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5321,18 +5324,18 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="D58" s="63" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B59" s="63" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="C59" s="64" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -5340,63 +5343,63 @@
         <v>950</v>
       </c>
       <c r="C60" s="64" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B61" s="63" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="C61" s="64" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" s="63" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="C62" s="64" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B63" s="63" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="C63" s="64" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="63" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C64" s="64" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="63" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="C65" s="64" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B66" s="63" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="C66" s="64" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B67" s="63" t="s">
-        <v>1050</v>
+        <v>1047</v>
       </c>
       <c r="C67" s="64" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
@@ -54714,7 +54717,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1070</v>
+        <v>1066</v>
       </c>
       <c r="B12" s="69">
         <v>6</v>
@@ -54723,7 +54726,7 @@
         <v>801</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>1071</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -55145,16 +55148,16 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1081</v>
+        <v>1077</v>
       </c>
       <c r="B43" s="69" t="s">
-        <v>1090</v>
+        <v>1086</v>
       </c>
       <c r="C43" s="38" t="s">
         <v>806</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>1082</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -55411,44 +55414,44 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1072</v>
+        <v>1068</v>
       </c>
       <c r="B62" s="69" t="s">
-        <v>1080</v>
+        <v>1076</v>
       </c>
       <c r="C62" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D62" s="38" t="s">
-        <v>1073</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>1074</v>
+        <v>1070</v>
       </c>
       <c r="B63" s="69" t="s">
-        <v>1075</v>
+        <v>1071</v>
       </c>
       <c r="C63" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D63" s="38" t="s">
-        <v>1076</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>1077</v>
+        <v>1073</v>
       </c>
       <c r="B64" s="69" t="s">
-        <v>1078</v>
+        <v>1074</v>
       </c>
       <c r="C64" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D64" s="38" t="s">
-        <v>1079</v>
+        <v>1075</v>
       </c>
     </row>
   </sheetData>
@@ -55519,7 +55522,7 @@
         <v>901</v>
       </c>
       <c r="L1" s="71" t="s">
-        <v>1089</v>
+        <v>1085</v>
       </c>
       <c r="M1" s="71" t="s">
         <v>833</v>
@@ -55572,7 +55575,7 @@
         <v>osm_10km_testing_10km_pedestrian_20181001</v>
       </c>
       <c r="L2" s="75" t="s">
-        <v>1088</v>
+        <v>1084</v>
       </c>
       <c r="M2" s="75" t="s">
         <v>858</v>
@@ -56054,7 +56057,7 @@
         <v>926</v>
       </c>
       <c r="L12" s="79" t="s">
-        <v>1083</v>
+        <v>1079</v>
       </c>
       <c r="M12" s="79"/>
       <c r="N12" s="80" t="s">
@@ -56291,7 +56294,7 @@
         <v>931</v>
       </c>
       <c r="L17" s="82" t="s">
-        <v>1084</v>
+        <v>1080</v>
       </c>
       <c r="M17" s="82"/>
       <c r="N17" s="83" t="s">
@@ -56434,7 +56437,7 @@
         <v>934</v>
       </c>
       <c r="L20" s="79" t="s">
-        <v>1085</v>
+        <v>1081</v>
       </c>
       <c r="M20" s="79"/>
       <c r="N20" s="80" t="s">
@@ -56481,7 +56484,7 @@
         <v>935</v>
       </c>
       <c r="L21" s="82" t="s">
-        <v>1086</v>
+        <v>1082</v>
       </c>
       <c r="M21" s="82"/>
       <c r="N21" s="83" t="s">
@@ -56671,7 +56674,7 @@
         <v>938</v>
       </c>
       <c r="L25" s="82" t="s">
-        <v>1087</v>
+        <v>1083</v>
       </c>
       <c r="M25" s="82"/>
       <c r="N25" s="83" t="s">
@@ -56687,40 +56690,40 @@
     </row>
     <row r="26" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="78" t="s">
-        <v>1103</v>
+        <v>1099</v>
       </c>
       <c r="B26" s="79" t="s">
-        <v>1104</v>
+        <v>1100</v>
       </c>
       <c r="C26" s="79" t="s">
         <v>912</v>
       </c>
       <c r="D26" s="79" t="s">
-        <v>1107</v>
+        <v>1103</v>
       </c>
       <c r="E26" s="79" t="s">
-        <v>1107</v>
+        <v>1103</v>
       </c>
       <c r="F26" s="80" t="s">
-        <v>1106</v>
+        <v>1102</v>
       </c>
       <c r="G26" s="79" t="s">
-        <v>1108</v>
+        <v>1104</v>
       </c>
       <c r="H26" s="79" t="s">
+        <v>1101</v>
+      </c>
+      <c r="I26" s="79" t="s">
         <v>1105</v>
-      </c>
-      <c r="I26" s="79" t="s">
-        <v>1109</v>
       </c>
       <c r="J26" s="79" t="s">
         <v>877</v>
       </c>
       <c r="K26" s="79" t="s">
-        <v>1105</v>
+        <v>1101</v>
       </c>
       <c r="L26" s="79" t="s">
-        <v>1105</v>
+        <v>1101</v>
       </c>
       <c r="M26" s="79"/>
       <c r="N26" s="80" t="s">
@@ -57480,69 +57483,74 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="3" width="21.28515625" customWidth="1"/>
-    <col min="4" max="4" width="70.42578125" customWidth="1"/>
-    <col min="5" max="5" width="94.5703125" customWidth="1"/>
-    <col min="6" max="6" width="41.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="41" customWidth="1"/>
-    <col min="9" max="9" width="29.140625" customWidth="1"/>
-    <col min="10" max="10" width="26.85546875" customWidth="1"/>
-    <col min="12" max="12" width="27.28515625" customWidth="1"/>
-    <col min="13" max="13" width="29.140625" customWidth="1"/>
+    <col min="2" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="94.5703125" customWidth="1"/>
+    <col min="8" max="8" width="41.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="41" customWidth="1"/>
+    <col min="11" max="11" width="29.140625" customWidth="1"/>
+    <col min="12" max="12" width="26.85546875" customWidth="1"/>
+    <col min="14" max="14" width="27.28515625" customWidth="1"/>
+    <col min="15" max="15" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>964</v>
+        <v>1173</v>
       </c>
       <c r="B1" s="37" t="s">
         <v>950</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>1060</v>
+        <v>1056</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>969</v>
+        <v>1169</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>968</v>
+        <v>1165</v>
       </c>
       <c r="F1" s="37" t="s">
-        <v>970</v>
+        <v>1166</v>
       </c>
       <c r="G1" s="37" t="s">
-        <v>1002</v>
+        <v>965</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>1111</v>
+        <v>967</v>
       </c>
       <c r="I1" s="37" t="s">
-        <v>1038</v>
+        <v>999</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>1050</v>
+        <v>1107</v>
       </c>
       <c r="K1" s="37" t="s">
-        <v>1112</v>
+        <v>1035</v>
       </c>
       <c r="L1" s="37" t="s">
-        <v>1113</v>
+        <v>1047</v>
       </c>
       <c r="M1" s="37" t="s">
-        <v>1170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1108</v>
+      </c>
+      <c r="N1" s="37" t="s">
+        <v>1109</v>
+      </c>
+      <c r="O1" s="37" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>939</v>
       </c>
@@ -57550,177 +57558,192 @@
         <v>951</v>
       </c>
       <c r="C2" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="D2" t="s">
-        <v>1114</v>
+        <v>1172</v>
       </c>
       <c r="E2" t="s">
-        <v>966</v>
+        <v>944</v>
       </c>
       <c r="F2" t="s">
-        <v>971</v>
+        <v>1167</v>
       </c>
       <c r="G2" t="s">
-        <v>1003</v>
+        <v>963</v>
       </c>
       <c r="H2" t="s">
-        <v>1092</v>
+        <v>968</v>
       </c>
       <c r="I2" t="s">
-        <v>1021</v>
+        <v>1000</v>
       </c>
       <c r="J2" t="s">
-        <v>1039</v>
+        <v>1088</v>
       </c>
       <c r="K2" t="s">
-        <v>1044</v>
-      </c>
-      <c r="L2" s="106" t="s">
-        <v>1120</v>
+        <v>1018</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1036</v>
       </c>
       <c r="M2" t="s">
-        <v>1169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1041</v>
+      </c>
+      <c r="N2" s="106" t="s">
+        <v>1113</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>940</v>
       </c>
       <c r="B3" t="s">
+        <v>952</v>
+      </c>
+      <c r="C3" t="s">
         <v>1059</v>
       </c>
-      <c r="C3" t="s">
-        <v>1063</v>
-      </c>
       <c r="D3" t="s">
-        <v>1126</v>
+        <v>1170</v>
       </c>
       <c r="E3" t="s">
-        <v>967</v>
+        <v>948</v>
       </c>
       <c r="F3" t="s">
-        <v>972</v>
+        <v>1168</v>
       </c>
       <c r="G3" t="s">
-        <v>1004</v>
+        <v>964</v>
       </c>
       <c r="H3" t="s">
-        <v>1093</v>
+        <v>969</v>
       </c>
       <c r="I3" t="s">
-        <v>1022</v>
+        <v>1001</v>
       </c>
       <c r="J3" t="s">
-        <v>1040</v>
+        <v>1089</v>
       </c>
       <c r="K3" t="s">
+        <v>1019</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="M3" t="s">
         <v>945</v>
       </c>
-      <c r="L3" s="106" t="s">
-        <v>1167</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" s="106" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>941</v>
       </c>
       <c r="B4" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="C4" t="s">
-        <v>1061</v>
-      </c>
-      <c r="E4" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D4" t="s">
         <v>1171</v>
       </c>
-      <c r="F4" t="s">
-        <v>973</v>
-      </c>
       <c r="G4" t="s">
-        <v>1005</v>
+        <v>1163</v>
       </c>
       <c r="H4" t="s">
-        <v>1094</v>
+        <v>970</v>
       </c>
       <c r="I4" t="s">
-        <v>1023</v>
+        <v>1002</v>
       </c>
       <c r="J4" t="s">
-        <v>1125</v>
+        <v>1090</v>
       </c>
       <c r="K4" t="s">
-        <v>1110</v>
-      </c>
-      <c r="L4" s="106" t="s">
-        <v>1121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1020</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="N4" s="106" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>942</v>
       </c>
       <c r="B5" t="s">
+        <v>954</v>
+      </c>
+      <c r="C5" t="s">
         <v>953</v>
       </c>
-      <c r="C5" t="s">
-        <v>954</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>939</v>
       </c>
-      <c r="G5" t="s">
-        <v>1006</v>
-      </c>
-      <c r="H5" t="s">
-        <v>1095</v>
-      </c>
       <c r="I5" t="s">
-        <v>1024</v>
+        <v>1003</v>
       </c>
       <c r="J5" t="s">
-        <v>1172</v>
+        <v>1091</v>
       </c>
       <c r="K5" t="s">
-        <v>1057</v>
-      </c>
-      <c r="L5" s="106" t="s">
-        <v>1124</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1021</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1164</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1054</v>
+      </c>
+      <c r="N5" s="106" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>943</v>
       </c>
       <c r="B6" t="s">
-        <v>954</v>
+        <v>945</v>
       </c>
       <c r="C6" t="s">
-        <v>1064</v>
-      </c>
-      <c r="F6" t="s">
-        <v>974</v>
-      </c>
-      <c r="G6" t="s">
-        <v>1007</v>
+        <v>1060</v>
       </c>
       <c r="H6" t="s">
-        <v>1096</v>
+        <v>971</v>
       </c>
       <c r="I6" t="s">
-        <v>1025</v>
+        <v>1004</v>
       </c>
       <c r="J6" t="s">
-        <v>1044</v>
+        <v>1092</v>
       </c>
       <c r="K6" t="s">
+        <v>1022</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1041</v>
+      </c>
+      <c r="M6" t="s">
         <v>947</v>
       </c>
-      <c r="L6" s="106" t="s">
-        <v>1122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" s="106" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>944</v>
       </c>
@@ -57728,31 +57751,31 @@
         <v>955</v>
       </c>
       <c r="C7" t="s">
-        <v>1066</v>
-      </c>
-      <c r="F7" t="s">
-        <v>975</v>
-      </c>
-      <c r="G7" t="s">
-        <v>1008</v>
+        <v>1062</v>
       </c>
       <c r="H7" t="s">
-        <v>1097</v>
+        <v>972</v>
       </c>
       <c r="I7" t="s">
-        <v>1026</v>
+        <v>1005</v>
       </c>
       <c r="J7" t="s">
+        <v>1093</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1023</v>
+      </c>
+      <c r="L7" t="s">
         <v>944</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>944</v>
       </c>
-      <c r="L7" s="106" t="s">
-        <v>1123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="106" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>945</v>
       </c>
@@ -57760,77 +57783,77 @@
         <v>956</v>
       </c>
       <c r="C8" t="s">
-        <v>1067</v>
-      </c>
-      <c r="F8" t="s">
-        <v>976</v>
-      </c>
-      <c r="G8" t="s">
-        <v>1009</v>
+        <v>1063</v>
       </c>
       <c r="H8" t="s">
-        <v>1098</v>
+        <v>973</v>
       </c>
       <c r="I8" t="s">
-        <v>1027</v>
+        <v>1006</v>
       </c>
       <c r="J8" t="s">
-        <v>1065</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1094</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1024</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>946</v>
       </c>
       <c r="B9" t="s">
-        <v>945</v>
+        <v>1054</v>
       </c>
       <c r="C9" t="s">
-        <v>1068</v>
-      </c>
-      <c r="F9" t="s">
-        <v>977</v>
-      </c>
-      <c r="G9" t="s">
-        <v>1010</v>
+        <v>1064</v>
       </c>
       <c r="H9" t="s">
-        <v>1099</v>
+        <v>974</v>
       </c>
       <c r="I9" t="s">
-        <v>1028</v>
+        <v>1007</v>
       </c>
       <c r="J9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1025</v>
+      </c>
+      <c r="L9" t="s">
         <v>948</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>947</v>
       </c>
       <c r="B10" t="s">
-        <v>957</v>
+        <v>947</v>
       </c>
       <c r="C10" t="s">
-        <v>958</v>
-      </c>
-      <c r="F10" t="s">
-        <v>978</v>
-      </c>
-      <c r="G10" t="s">
-        <v>1002</v>
+        <v>955</v>
       </c>
       <c r="H10" t="s">
-        <v>1100</v>
+        <v>975</v>
       </c>
       <c r="I10" t="s">
+        <v>999</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1096</v>
+      </c>
+      <c r="K10" t="s">
         <v>695</v>
       </c>
-      <c r="J10" t="s">
+      <c r="L10" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>948</v>
       </c>
@@ -57838,285 +57861,270 @@
         <v>958</v>
       </c>
       <c r="C11" t="s">
-        <v>1069</v>
-      </c>
-      <c r="F11" t="s">
-        <v>979</v>
-      </c>
-      <c r="G11" t="s">
-        <v>1011</v>
+        <v>1065</v>
+      </c>
+      <c r="H11" t="s">
+        <v>976</v>
       </c>
       <c r="I11" t="s">
-        <v>1029</v>
-      </c>
-      <c r="J11" t="s">
+        <v>1008</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1026</v>
+      </c>
+      <c r="L11" t="s">
         <v>946</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>949</v>
       </c>
       <c r="B12" t="s">
+        <v>1055</v>
+      </c>
+      <c r="H12" t="s">
+        <v>977</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1009</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1027</v>
+      </c>
+      <c r="L12" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B13" t="s">
         <v>959</v>
       </c>
-      <c r="F12" t="s">
+      <c r="H13" t="s">
+        <v>978</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1010</v>
+      </c>
+      <c r="K13" t="s">
+        <v>1028</v>
+      </c>
+      <c r="L13" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B14" t="s">
+        <v>960</v>
+      </c>
+      <c r="H14" t="s">
+        <v>979</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1011</v>
+      </c>
+      <c r="K14" t="s">
+        <v>1029</v>
+      </c>
+      <c r="L14" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1110</v>
+      </c>
+      <c r="H15" t="s">
         <v>980</v>
       </c>
-      <c r="G12" t="s">
-        <v>1012</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="K15" t="s">
         <v>1030</v>
       </c>
-      <c r="J12" t="s">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>1065</v>
-      </c>
-      <c r="B13" t="s">
-        <v>960</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="L15" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1057</v>
+      </c>
+      <c r="H16" t="s">
         <v>981</v>
       </c>
-      <c r="G13" t="s">
-        <v>1013</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="K16" t="s">
         <v>1031</v>
       </c>
-      <c r="J13" t="s">
+      <c r="L16" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1111</v>
+      </c>
+      <c r="H17" t="s">
+        <v>982</v>
+      </c>
+      <c r="K17" t="s">
+        <v>1032</v>
+      </c>
+      <c r="L17" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1112</v>
+      </c>
+      <c r="H18" t="s">
+        <v>983</v>
+      </c>
+      <c r="K18" t="s">
+        <v>1033</v>
+      </c>
+      <c r="L18" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>957</v>
+      </c>
+      <c r="K19" t="s">
+        <v>1034</v>
+      </c>
+      <c r="L19" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>940</v>
+      </c>
+      <c r="L20" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>984</v>
+      </c>
+      <c r="L21" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>985</v>
+      </c>
+      <c r="L22" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>986</v>
+      </c>
+      <c r="L23" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>987</v>
+      </c>
+      <c r="L24" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>988</v>
+      </c>
+      <c r="L25" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H35" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="36" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H36" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="37" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H37" t="s">
         <v>942</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>1057</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1057</v>
-      </c>
-      <c r="F14" t="s">
-        <v>982</v>
-      </c>
-      <c r="G14" t="s">
-        <v>1014</v>
-      </c>
-      <c r="I14" t="s">
-        <v>1032</v>
-      </c>
-      <c r="J14" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>1168</v>
-      </c>
-      <c r="B15" t="s">
-        <v>947</v>
-      </c>
-      <c r="F15" t="s">
-        <v>983</v>
-      </c>
-      <c r="I15" t="s">
-        <v>1033</v>
-      </c>
-      <c r="J15" t="s">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>961</v>
-      </c>
-      <c r="F16" t="s">
-        <v>984</v>
-      </c>
-      <c r="I16" t="s">
-        <v>1034</v>
-      </c>
-      <c r="J16" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>1058</v>
-      </c>
-      <c r="F17" t="s">
-        <v>985</v>
-      </c>
-      <c r="I17" t="s">
-        <v>1035</v>
-      </c>
-      <c r="J17" t="s">
-        <v>1091</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>941</v>
-      </c>
-      <c r="F18" t="s">
-        <v>986</v>
-      </c>
-      <c r="I18" t="s">
-        <v>1036</v>
-      </c>
-      <c r="J18" t="s">
-        <v>1047</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>962</v>
-      </c>
-      <c r="F19" t="s">
-        <v>960</v>
-      </c>
-      <c r="I19" t="s">
-        <v>1037</v>
-      </c>
-      <c r="J19" t="s">
-        <v>1041</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>963</v>
-      </c>
-      <c r="F20" t="s">
-        <v>940</v>
-      </c>
-      <c r="J20" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>1115</v>
-      </c>
-      <c r="F21" t="s">
-        <v>987</v>
-      </c>
-      <c r="J21" t="s">
-        <v>1101</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>1116</v>
-      </c>
-      <c r="F22" t="s">
-        <v>988</v>
-      </c>
-      <c r="J22" t="s">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>1061</v>
-      </c>
-      <c r="F23" t="s">
-        <v>989</v>
-      </c>
-      <c r="J23" t="s">
-        <v>1043</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>1117</v>
-      </c>
-      <c r="F24" t="s">
-        <v>990</v>
-      </c>
-      <c r="J24" t="s">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>1118</v>
-      </c>
-      <c r="F25" t="s">
-        <v>991</v>
-      </c>
-      <c r="J25" t="s">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>1119</v>
-      </c>
-      <c r="F26" t="s">
-        <v>992</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F27" t="s">
-        <v>993</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F28" t="s">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F29" t="s">
-        <v>995</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F30" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F31" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F32" t="s">
-        <v>998</v>
-      </c>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F33" t="s">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F34" t="s">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F35" t="s">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F36" t="s">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F37" t="s">
-        <v>942</v>
-      </c>
-    </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F38" t="s">
+    <row r="38" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H38" t="s">
         <v>943</v>
       </c>
     </row>
@@ -58142,361 +58150,361 @@
     <col min="5" max="28" width="9.7109375" style="69" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="116" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="115" t="s">
+    <row r="1" spans="1:28" s="110" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="109" t="s">
         <v>598</v>
       </c>
-      <c r="B1" s="115" t="s">
+      <c r="B1" s="109" t="s">
         <v>597</v>
       </c>
-      <c r="C1" s="115" t="s">
-        <v>1127</v>
-      </c>
-      <c r="D1" s="115" t="s">
-        <v>1128</v>
-      </c>
-      <c r="E1" s="112" t="s">
+      <c r="C1" s="109" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D1" s="109" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E1" s="111" t="s">
         <v>441</v>
       </c>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112" t="s">
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111" t="s">
         <v>462</v>
       </c>
-      <c r="I1" s="112"/>
-      <c r="J1" s="112"/>
-      <c r="K1" s="112" t="s">
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111" t="s">
         <v>444</v>
       </c>
-      <c r="L1" s="112"/>
-      <c r="M1" s="112"/>
-      <c r="N1" s="112" t="s">
-        <v>1129</v>
-      </c>
-      <c r="O1" s="112"/>
-      <c r="P1" s="112"/>
-      <c r="Q1" s="112" t="s">
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111" t="s">
+        <v>1121</v>
+      </c>
+      <c r="O1" s="111"/>
+      <c r="P1" s="111"/>
+      <c r="Q1" s="111" t="s">
         <v>436</v>
       </c>
-      <c r="R1" s="112"/>
-      <c r="S1" s="112"/>
-      <c r="T1" s="112" t="s">
+      <c r="R1" s="111"/>
+      <c r="S1" s="111"/>
+      <c r="T1" s="111" t="s">
         <v>431</v>
       </c>
-      <c r="U1" s="112"/>
-      <c r="V1" s="112"/>
-      <c r="W1" s="112" t="s">
-        <v>1130</v>
-      </c>
-      <c r="X1" s="112"/>
-      <c r="Y1" s="112"/>
-      <c r="Z1" s="112" t="s">
+      <c r="U1" s="111"/>
+      <c r="V1" s="111"/>
+      <c r="W1" s="111" t="s">
+        <v>1122</v>
+      </c>
+      <c r="X1" s="111"/>
+      <c r="Y1" s="111"/>
+      <c r="Z1" s="111" t="s">
         <v>457</v>
       </c>
-      <c r="AA1" s="112"/>
-      <c r="AB1" s="112"/>
+      <c r="AA1" s="111"/>
+      <c r="AB1" s="111"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="37"/>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
       <c r="D2" s="37"/>
-      <c r="E2" s="113" t="s">
-        <v>1131</v>
-      </c>
-      <c r="F2" s="113" t="s">
-        <v>1128</v>
-      </c>
-      <c r="G2" s="113" t="s">
-        <v>1132</v>
-      </c>
-      <c r="H2" s="113" t="s">
-        <v>1133</v>
-      </c>
-      <c r="I2" s="113" t="s">
+      <c r="E2" s="107" t="s">
+        <v>1123</v>
+      </c>
+      <c r="F2" s="107" t="s">
+        <v>1120</v>
+      </c>
+      <c r="G2" s="107" t="s">
+        <v>1124</v>
+      </c>
+      <c r="H2" s="107" t="s">
+        <v>1125</v>
+      </c>
+      <c r="I2" s="107" t="s">
         <v>209</v>
       </c>
-      <c r="J2" s="113" t="s">
-        <v>1132</v>
-      </c>
-      <c r="K2" s="113" t="s">
-        <v>1133</v>
-      </c>
-      <c r="L2" s="113" t="s">
+      <c r="J2" s="107" t="s">
+        <v>1124</v>
+      </c>
+      <c r="K2" s="107" t="s">
+        <v>1125</v>
+      </c>
+      <c r="L2" s="107" t="s">
         <v>209</v>
       </c>
-      <c r="M2" s="113" t="s">
-        <v>1132</v>
-      </c>
-      <c r="N2" s="113" t="s">
-        <v>1133</v>
-      </c>
-      <c r="O2" s="113" t="s">
+      <c r="M2" s="107" t="s">
+        <v>1124</v>
+      </c>
+      <c r="N2" s="107" t="s">
+        <v>1125</v>
+      </c>
+      <c r="O2" s="107" t="s">
         <v>209</v>
       </c>
-      <c r="P2" s="113" t="s">
-        <v>1132</v>
-      </c>
-      <c r="Q2" s="113" t="s">
-        <v>1133</v>
-      </c>
-      <c r="R2" s="113" t="s">
+      <c r="P2" s="107" t="s">
+        <v>1124</v>
+      </c>
+      <c r="Q2" s="107" t="s">
+        <v>1125</v>
+      </c>
+      <c r="R2" s="107" t="s">
         <v>209</v>
       </c>
-      <c r="S2" s="113" t="s">
-        <v>1132</v>
-      </c>
-      <c r="T2" s="113" t="s">
-        <v>1133</v>
-      </c>
-      <c r="U2" s="113" t="s">
+      <c r="S2" s="107" t="s">
+        <v>1124</v>
+      </c>
+      <c r="T2" s="107" t="s">
+        <v>1125</v>
+      </c>
+      <c r="U2" s="107" t="s">
         <v>209</v>
       </c>
-      <c r="V2" s="113" t="s">
-        <v>1132</v>
-      </c>
-      <c r="W2" s="113" t="s">
-        <v>1133</v>
-      </c>
-      <c r="X2" s="113" t="s">
+      <c r="V2" s="107" t="s">
+        <v>1124</v>
+      </c>
+      <c r="W2" s="107" t="s">
+        <v>1125</v>
+      </c>
+      <c r="X2" s="107" t="s">
         <v>209</v>
       </c>
-      <c r="Y2" s="113" t="s">
-        <v>1132</v>
-      </c>
-      <c r="Z2" s="113" t="s">
-        <v>1133</v>
-      </c>
-      <c r="AA2" s="113" t="s">
+      <c r="Y2" s="107" t="s">
+        <v>1124</v>
+      </c>
+      <c r="Z2" s="107" t="s">
+        <v>1125</v>
+      </c>
+      <c r="AA2" s="107" t="s">
         <v>209</v>
       </c>
-      <c r="AB2" s="113" t="s">
-        <v>1132</v>
+      <c r="AB2" s="107" t="s">
+        <v>1124</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>1134</v>
+        <v>1126</v>
       </c>
       <c r="C3" t="s">
-        <v>1135</v>
+        <v>1127</v>
       </c>
       <c r="D3" t="s">
-        <v>1136</v>
+        <v>1128</v>
       </c>
       <c r="E3" s="69">
         <v>2018</v>
       </c>
       <c r="F3" s="69" t="s">
-        <v>1136</v>
+        <v>1128</v>
       </c>
       <c r="H3" s="69">
         <v>2018</v>
       </c>
       <c r="I3" s="69" t="s">
-        <v>1136</v>
+        <v>1128</v>
       </c>
       <c r="K3" s="69">
         <v>2018</v>
       </c>
       <c r="L3" s="69" t="s">
-        <v>1136</v>
+        <v>1128</v>
       </c>
       <c r="N3" s="69">
         <v>2018</v>
       </c>
       <c r="O3" s="69" t="s">
-        <v>1136</v>
+        <v>1128</v>
       </c>
       <c r="Q3" s="69">
         <v>2018</v>
       </c>
       <c r="R3" s="69" t="s">
-        <v>1136</v>
+        <v>1128</v>
       </c>
       <c r="T3" s="69">
         <v>2018</v>
       </c>
       <c r="U3" s="69" t="s">
-        <v>1136</v>
+        <v>1128</v>
       </c>
       <c r="W3" s="69">
         <v>2018</v>
       </c>
       <c r="X3" s="69" t="s">
-        <v>1136</v>
+        <v>1128</v>
       </c>
       <c r="Z3" s="69">
         <v>2018</v>
       </c>
       <c r="AA3" s="69" t="s">
-        <v>1136</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>1137</v>
+        <v>1129</v>
       </c>
       <c r="C4" t="s">
-        <v>1138</v>
+        <v>1130</v>
       </c>
       <c r="D4" t="s">
-        <v>1139</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>1140</v>
+        <v>1132</v>
       </c>
       <c r="C5" t="s">
-        <v>1141</v>
+        <v>1133</v>
       </c>
       <c r="D5" t="s">
-        <v>1142</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>1143</v>
+        <v>1135</v>
       </c>
       <c r="C6" t="s">
-        <v>1141</v>
+        <v>1133</v>
       </c>
       <c r="D6" t="s">
-        <v>1142</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>1144</v>
+        <v>1136</v>
       </c>
       <c r="C7" t="s">
-        <v>1141</v>
+        <v>1133</v>
       </c>
       <c r="D7" t="s">
-        <v>1142</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>1145</v>
+        <v>1137</v>
       </c>
       <c r="C8" t="s">
-        <v>1141</v>
+        <v>1133</v>
       </c>
       <c r="D8" t="s">
-        <v>1142</v>
+        <v>1134</v>
       </c>
       <c r="E8" s="69">
         <v>2017</v>
       </c>
-      <c r="F8" s="114" t="s">
-        <v>1164</v>
+      <c r="F8" s="108" t="s">
+        <v>1156</v>
       </c>
       <c r="G8" s="69" t="s">
-        <v>1163</v>
+        <v>1155</v>
       </c>
       <c r="H8" s="69">
         <v>2016</v>
       </c>
       <c r="I8" s="69" t="s">
-        <v>1165</v>
+        <v>1157</v>
       </c>
       <c r="J8" s="69" t="s">
-        <v>1166</v>
+        <v>1158</v>
       </c>
       <c r="Q8" s="69">
         <v>2018</v>
       </c>
-      <c r="R8" s="114" t="s">
-        <v>1146</v>
+      <c r="R8" s="108" t="s">
+        <v>1138</v>
       </c>
       <c r="S8" s="69" t="s">
-        <v>1147</v>
+        <v>1139</v>
       </c>
       <c r="W8" s="69">
         <v>2016</v>
       </c>
-      <c r="X8" s="114" t="s">
-        <v>1161</v>
+      <c r="X8" s="108" t="s">
+        <v>1153</v>
       </c>
       <c r="Y8" s="69" t="s">
-        <v>1162</v>
+        <v>1154</v>
       </c>
       <c r="Z8" s="69">
         <v>2016</v>
       </c>
       <c r="AA8" s="69" t="s">
-        <v>1148</v>
+        <v>1140</v>
       </c>
       <c r="AB8" s="69" t="s">
-        <v>1149</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>1150</v>
+        <v>1142</v>
       </c>
       <c r="C9" t="s">
-        <v>1151</v>
+        <v>1143</v>
       </c>
       <c r="D9" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>1153</v>
+        <v>1145</v>
       </c>
       <c r="C10" t="s">
-        <v>1151</v>
+        <v>1143</v>
       </c>
       <c r="D10" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>1154</v>
+        <v>1146</v>
       </c>
       <c r="C11" t="s">
-        <v>1138</v>
+        <v>1130</v>
       </c>
       <c r="D11" t="s">
-        <v>1155</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>1156</v>
+        <v>1148</v>
       </c>
       <c r="C12" t="s">
-        <v>1138</v>
+        <v>1130</v>
       </c>
       <c r="D12" t="s">
-        <v>1155</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>1157</v>
+        <v>1149</v>
       </c>
       <c r="C13" t="s">
-        <v>1138</v>
+        <v>1130</v>
       </c>
       <c r="D13" t="s">
-        <v>1158</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>1159</v>
+        <v>1151</v>
       </c>
       <c r="C14" t="s">
-        <v>1141</v>
+        <v>1133</v>
       </c>
       <c r="D14" t="s">
-        <v>1160</v>
+        <v>1152</v>
       </c>
     </row>
   </sheetData>
@@ -58563,31 +58571,31 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="107" t="s">
+      <c r="G1" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="108"/>
-      <c r="I1" s="108"/>
-      <c r="J1" s="108"/>
-      <c r="K1" s="108"/>
-      <c r="L1" s="108"/>
-      <c r="M1" s="108"/>
-      <c r="N1" s="108"/>
-      <c r="O1" s="108"/>
-      <c r="P1" s="108"/>
-      <c r="Q1" s="108"/>
-      <c r="R1" s="108"/>
-      <c r="S1" s="108"/>
-      <c r="T1" s="108"/>
-      <c r="U1" s="108"/>
-      <c r="V1" s="108"/>
-      <c r="W1" s="108"/>
-      <c r="X1" s="109"/>
-      <c r="Y1" s="110" t="s">
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
+      <c r="O1" s="113"/>
+      <c r="P1" s="113"/>
+      <c r="Q1" s="113"/>
+      <c r="R1" s="113"/>
+      <c r="S1" s="113"/>
+      <c r="T1" s="113"/>
+      <c r="U1" s="113"/>
+      <c r="V1" s="113"/>
+      <c r="W1" s="113"/>
+      <c r="X1" s="114"/>
+      <c r="Y1" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="Z1" s="108"/>
-      <c r="AA1" s="111"/>
+      <c r="Z1" s="113"/>
+      <c r="AA1" s="116"/>
       <c r="AB1" s="2" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
some changes before i edit heavily the aos creation script to deal with problematic medial axis function
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3427680-DB02-4798-BD51-0D5B145AFACD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53B0A25-18CE-4203-B74A-0D6E12F8BACB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
@@ -57485,8 +57485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
re-wrote the AOS set up to define linearity in terms predominantly of roundness, area and diameter --- not using medial axis of convex hulls.  Medial axis length calculation had issues with complex geometries and was expensive to run, was not an intuitive or easy to explain measure of linearity, and 'roundness' of < 0.25 seemed both a simpler to understand , caulculate and more effective predictor of linearity.
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53B0A25-18CE-4203-B74A-0D6E12F8BACB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E81629-942A-4FF3-B3CB-9AE6111E56C6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2440" uniqueCount="1174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2436" uniqueCount="1170">
   <si>
     <t>Domain</t>
   </si>
@@ -3247,12 +3247,6 @@
     <t>area_ha</t>
   </si>
   <si>
-    <t>medial_axis_length</t>
-  </si>
-  <si>
-    <t>num_symdiff_convhull_geoms</t>
-  </si>
-  <si>
     <t>roundness</t>
   </si>
   <si>
@@ -3397,18 +3391,6 @@
     <t>school_tags</t>
   </si>
   <si>
-    <t>(amal_to_area_ratio &gt; 140</t>
-  </si>
-  <si>
-    <t>AND area_ha &gt; 0.5</t>
-  </si>
-  <si>
-    <t>AND medial_axis_length &gt; 300</t>
-  </si>
-  <si>
-    <t>AND num_symdiff_convhull_geoms &gt; 0</t>
-  </si>
-  <si>
     <t>AND roundness &lt; 0.25)</t>
   </si>
   <si>
@@ -3653,6 +3635,12 @@
   </si>
   <si>
     <t>possible_tags</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> area_ha &gt; 0.5</t>
   </si>
 </sst>
 </file>
@@ -5359,7 +5347,7 @@
         <v>962</v>
       </c>
       <c r="C62" s="64" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -5367,7 +5355,7 @@
         <v>967</v>
       </c>
       <c r="C63" s="64" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -5375,7 +5363,7 @@
         <v>999</v>
       </c>
       <c r="C64" s="64" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5383,7 +5371,7 @@
         <v>1012</v>
       </c>
       <c r="C65" s="64" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -5391,15 +5379,15 @@
         <v>1035</v>
       </c>
       <c r="C66" s="64" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B67" s="63" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="C67" s="64" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
@@ -54717,7 +54705,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="B12" s="69">
         <v>6</v>
@@ -54726,7 +54714,7 @@
         <v>801</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -55148,16 +55136,16 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="B43" s="69" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="C43" s="38" t="s">
         <v>806</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -55414,44 +55402,44 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="B62" s="69" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="C62" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D62" s="38" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="B63" s="69" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="C63" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D63" s="38" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="B64" s="69" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="C64" s="38" t="s">
         <v>657</v>
       </c>
       <c r="D64" s="38" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
     </row>
   </sheetData>
@@ -55522,7 +55510,7 @@
         <v>901</v>
       </c>
       <c r="L1" s="71" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="M1" s="71" t="s">
         <v>833</v>
@@ -55575,7 +55563,7 @@
         <v>osm_10km_testing_10km_pedestrian_20181001</v>
       </c>
       <c r="L2" s="75" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="M2" s="75" t="s">
         <v>858</v>
@@ -56057,7 +56045,7 @@
         <v>926</v>
       </c>
       <c r="L12" s="79" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="M12" s="79"/>
       <c r="N12" s="80" t="s">
@@ -56294,7 +56282,7 @@
         <v>931</v>
       </c>
       <c r="L17" s="82" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="M17" s="82"/>
       <c r="N17" s="83" t="s">
@@ -56437,7 +56425,7 @@
         <v>934</v>
       </c>
       <c r="L20" s="79" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="M20" s="79"/>
       <c r="N20" s="80" t="s">
@@ -56484,7 +56472,7 @@
         <v>935</v>
       </c>
       <c r="L21" s="82" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="M21" s="82"/>
       <c r="N21" s="83" t="s">
@@ -56674,7 +56662,7 @@
         <v>938</v>
       </c>
       <c r="L25" s="82" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="M25" s="82"/>
       <c r="N25" s="83" t="s">
@@ -56690,40 +56678,40 @@
     </row>
     <row r="26" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="78" t="s">
-        <v>1099</v>
+        <v>1093</v>
       </c>
       <c r="B26" s="79" t="s">
-        <v>1100</v>
+        <v>1094</v>
       </c>
       <c r="C26" s="79" t="s">
         <v>912</v>
       </c>
       <c r="D26" s="79" t="s">
-        <v>1103</v>
+        <v>1097</v>
       </c>
       <c r="E26" s="79" t="s">
-        <v>1103</v>
+        <v>1097</v>
       </c>
       <c r="F26" s="80" t="s">
-        <v>1102</v>
+        <v>1096</v>
       </c>
       <c r="G26" s="79" t="s">
-        <v>1104</v>
+        <v>1098</v>
       </c>
       <c r="H26" s="79" t="s">
-        <v>1101</v>
+        <v>1095</v>
       </c>
       <c r="I26" s="79" t="s">
-        <v>1105</v>
+        <v>1099</v>
       </c>
       <c r="J26" s="79" t="s">
         <v>877</v>
       </c>
       <c r="K26" s="79" t="s">
-        <v>1101</v>
+        <v>1095</v>
       </c>
       <c r="L26" s="79" t="s">
-        <v>1101</v>
+        <v>1095</v>
       </c>
       <c r="M26" s="79"/>
       <c r="N26" s="80" t="s">
@@ -57485,8 +57473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57505,22 +57493,22 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>1173</v>
+        <v>1167</v>
       </c>
       <c r="B1" s="37" t="s">
         <v>950</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>1169</v>
+        <v>1163</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>1165</v>
+        <v>1159</v>
       </c>
       <c r="F1" s="37" t="s">
-        <v>1166</v>
+        <v>1160</v>
       </c>
       <c r="G1" s="37" t="s">
         <v>965</v>
@@ -57532,22 +57520,22 @@
         <v>999</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>1107</v>
+        <v>1101</v>
       </c>
       <c r="K1" s="37" t="s">
         <v>1035</v>
       </c>
       <c r="L1" s="37" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="M1" s="37" t="s">
-        <v>1108</v>
+        <v>1102</v>
       </c>
       <c r="N1" s="37" t="s">
-        <v>1109</v>
+        <v>1103</v>
       </c>
       <c r="O1" s="37" t="s">
-        <v>1162</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -57558,16 +57546,16 @@
         <v>951</v>
       </c>
       <c r="C2" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="D2" t="s">
-        <v>1172</v>
+        <v>1166</v>
       </c>
       <c r="E2" t="s">
         <v>944</v>
       </c>
       <c r="F2" t="s">
-        <v>1167</v>
+        <v>1161</v>
       </c>
       <c r="G2" t="s">
         <v>963</v>
@@ -57579,7 +57567,7 @@
         <v>1000</v>
       </c>
       <c r="J2" t="s">
-        <v>1088</v>
+        <v>1168</v>
       </c>
       <c r="K2" t="s">
         <v>1018</v>
@@ -57588,13 +57576,13 @@
         <v>1036</v>
       </c>
       <c r="M2" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="N2" s="106" t="s">
-        <v>1113</v>
+        <v>1107</v>
       </c>
       <c r="O2" t="s">
-        <v>1161</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -57605,16 +57593,16 @@
         <v>952</v>
       </c>
       <c r="C3" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="D3" t="s">
-        <v>1170</v>
+        <v>1164</v>
       </c>
       <c r="E3" t="s">
         <v>948</v>
       </c>
       <c r="F3" t="s">
-        <v>1168</v>
+        <v>1162</v>
       </c>
       <c r="G3" t="s">
         <v>964</v>
@@ -57626,7 +57614,7 @@
         <v>1001</v>
       </c>
       <c r="J3" t="s">
-        <v>1089</v>
+        <v>1169</v>
       </c>
       <c r="K3" t="s">
         <v>1019</v>
@@ -57638,7 +57626,7 @@
         <v>945</v>
       </c>
       <c r="N3" s="106" t="s">
-        <v>1159</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -57649,13 +57637,13 @@
         <v>953</v>
       </c>
       <c r="C4" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="D4" t="s">
-        <v>1171</v>
+        <v>1165</v>
       </c>
       <c r="G4" t="s">
-        <v>1163</v>
+        <v>1157</v>
       </c>
       <c r="H4" t="s">
         <v>970</v>
@@ -57664,19 +57652,19 @@
         <v>1002</v>
       </c>
       <c r="J4" t="s">
-        <v>1090</v>
+        <v>1086</v>
       </c>
       <c r="K4" t="s">
         <v>1020</v>
       </c>
       <c r="L4" t="s">
-        <v>1118</v>
+        <v>1112</v>
       </c>
       <c r="M4" t="s">
-        <v>1106</v>
+        <v>1100</v>
       </c>
       <c r="N4" s="106" t="s">
-        <v>1114</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -57696,19 +57684,19 @@
         <v>1003</v>
       </c>
       <c r="J5" t="s">
-        <v>1091</v>
+        <v>1087</v>
       </c>
       <c r="K5" t="s">
         <v>1021</v>
       </c>
       <c r="L5" t="s">
-        <v>1164</v>
+        <v>1158</v>
       </c>
       <c r="M5" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="N5" s="106" t="s">
-        <v>1117</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -57719,7 +57707,7 @@
         <v>945</v>
       </c>
       <c r="C6" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="H6" t="s">
         <v>971</v>
@@ -57728,19 +57716,19 @@
         <v>1004</v>
       </c>
       <c r="J6" t="s">
-        <v>1092</v>
+        <v>1088</v>
       </c>
       <c r="K6" t="s">
         <v>1022</v>
       </c>
       <c r="L6" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="M6" t="s">
         <v>947</v>
       </c>
       <c r="N6" s="106" t="s">
-        <v>1115</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -57751,7 +57739,7 @@
         <v>955</v>
       </c>
       <c r="C7" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="H7" t="s">
         <v>972</v>
@@ -57760,7 +57748,7 @@
         <v>1005</v>
       </c>
       <c r="J7" t="s">
-        <v>1093</v>
+        <v>1089</v>
       </c>
       <c r="K7" t="s">
         <v>1023</v>
@@ -57772,7 +57760,7 @@
         <v>944</v>
       </c>
       <c r="N7" s="106" t="s">
-        <v>1116</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -57783,7 +57771,7 @@
         <v>956</v>
       </c>
       <c r="C8" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="H8" t="s">
         <v>973</v>
@@ -57792,13 +57780,13 @@
         <v>1006</v>
       </c>
       <c r="J8" t="s">
-        <v>1094</v>
+        <v>1090</v>
       </c>
       <c r="K8" t="s">
         <v>1024</v>
       </c>
       <c r="L8" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -57806,19 +57794,16 @@
         <v>946</v>
       </c>
       <c r="B9" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="C9" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="H9" t="s">
         <v>974</v>
       </c>
       <c r="I9" t="s">
         <v>1007</v>
-      </c>
-      <c r="J9" t="s">
-        <v>1095</v>
       </c>
       <c r="K9" t="s">
         <v>1025</v>
@@ -57843,9 +57828,6 @@
       <c r="I10" t="s">
         <v>999</v>
       </c>
-      <c r="J10" t="s">
-        <v>1096</v>
-      </c>
       <c r="K10" t="s">
         <v>695</v>
       </c>
@@ -57861,7 +57843,7 @@
         <v>958</v>
       </c>
       <c r="C11" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="H11" t="s">
         <v>976</v>
@@ -57881,7 +57863,7 @@
         <v>949</v>
       </c>
       <c r="B12" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="H12" t="s">
         <v>977</v>
@@ -57898,7 +57880,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="B13" t="s">
         <v>959</v>
@@ -57918,7 +57900,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="B14" t="s">
         <v>960</v>
@@ -57938,10 +57920,10 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1160</v>
+        <v>1154</v>
       </c>
       <c r="B15" t="s">
-        <v>1110</v>
+        <v>1104</v>
       </c>
       <c r="H15" t="s">
         <v>980</v>
@@ -57950,15 +57932,15 @@
         <v>1030</v>
       </c>
       <c r="L15" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1172</v>
+        <v>1166</v>
       </c>
       <c r="B16" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="H16" t="s">
         <v>981</v>
@@ -57967,15 +57949,15 @@
         <v>1031</v>
       </c>
       <c r="L16" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1170</v>
+        <v>1164</v>
       </c>
       <c r="B17" t="s">
-        <v>1111</v>
+        <v>1105</v>
       </c>
       <c r="H17" t="s">
         <v>982</v>
@@ -57984,15 +57966,15 @@
         <v>1032</v>
       </c>
       <c r="L17" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1171</v>
+        <v>1165</v>
       </c>
       <c r="B18" t="s">
-        <v>1112</v>
+        <v>1106</v>
       </c>
       <c r="H18" t="s">
         <v>983</v>
@@ -58001,7 +57983,7 @@
         <v>1033</v>
       </c>
       <c r="L18" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -58012,7 +57994,7 @@
         <v>1034</v>
       </c>
       <c r="L19" t="s">
-        <v>1038</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -58020,7 +58002,7 @@
         <v>940</v>
       </c>
       <c r="L20" t="s">
-        <v>1039</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -58028,7 +58010,7 @@
         <v>984</v>
       </c>
       <c r="L21" t="s">
-        <v>1097</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -58036,7 +58018,7 @@
         <v>985</v>
       </c>
       <c r="L22" t="s">
-        <v>1098</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -58044,23 +58026,17 @@
         <v>986</v>
       </c>
       <c r="L23" t="s">
-        <v>1040</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H24" t="s">
         <v>987</v>
       </c>
-      <c r="L24" t="s">
-        <v>1045</v>
-      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H25" t="s">
         <v>988</v>
-      </c>
-      <c r="L25" t="s">
-        <v>1046</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -58158,10 +58134,10 @@
         <v>597</v>
       </c>
       <c r="C1" s="109" t="s">
-        <v>1119</v>
+        <v>1113</v>
       </c>
       <c r="D1" s="109" t="s">
-        <v>1120</v>
+        <v>1114</v>
       </c>
       <c r="E1" s="111" t="s">
         <v>441</v>
@@ -58179,7 +58155,7 @@
       <c r="L1" s="111"/>
       <c r="M1" s="111"/>
       <c r="N1" s="111" t="s">
-        <v>1121</v>
+        <v>1115</v>
       </c>
       <c r="O1" s="111"/>
       <c r="P1" s="111"/>
@@ -58194,7 +58170,7 @@
       <c r="U1" s="111"/>
       <c r="V1" s="111"/>
       <c r="W1" s="111" t="s">
-        <v>1122</v>
+        <v>1116</v>
       </c>
       <c r="X1" s="111"/>
       <c r="Y1" s="111"/>
@@ -58210,301 +58186,301 @@
       <c r="C2" s="37"/>
       <c r="D2" s="37"/>
       <c r="E2" s="107" t="s">
-        <v>1123</v>
+        <v>1117</v>
       </c>
       <c r="F2" s="107" t="s">
-        <v>1120</v>
+        <v>1114</v>
       </c>
       <c r="G2" s="107" t="s">
-        <v>1124</v>
+        <v>1118</v>
       </c>
       <c r="H2" s="107" t="s">
-        <v>1125</v>
+        <v>1119</v>
       </c>
       <c r="I2" s="107" t="s">
         <v>209</v>
       </c>
       <c r="J2" s="107" t="s">
-        <v>1124</v>
+        <v>1118</v>
       </c>
       <c r="K2" s="107" t="s">
-        <v>1125</v>
+        <v>1119</v>
       </c>
       <c r="L2" s="107" t="s">
         <v>209</v>
       </c>
       <c r="M2" s="107" t="s">
-        <v>1124</v>
+        <v>1118</v>
       </c>
       <c r="N2" s="107" t="s">
-        <v>1125</v>
+        <v>1119</v>
       </c>
       <c r="O2" s="107" t="s">
         <v>209</v>
       </c>
       <c r="P2" s="107" t="s">
-        <v>1124</v>
+        <v>1118</v>
       </c>
       <c r="Q2" s="107" t="s">
-        <v>1125</v>
+        <v>1119</v>
       </c>
       <c r="R2" s="107" t="s">
         <v>209</v>
       </c>
       <c r="S2" s="107" t="s">
-        <v>1124</v>
+        <v>1118</v>
       </c>
       <c r="T2" s="107" t="s">
-        <v>1125</v>
+        <v>1119</v>
       </c>
       <c r="U2" s="107" t="s">
         <v>209</v>
       </c>
       <c r="V2" s="107" t="s">
-        <v>1124</v>
+        <v>1118</v>
       </c>
       <c r="W2" s="107" t="s">
-        <v>1125</v>
+        <v>1119</v>
       </c>
       <c r="X2" s="107" t="s">
         <v>209</v>
       </c>
       <c r="Y2" s="107" t="s">
-        <v>1124</v>
+        <v>1118</v>
       </c>
       <c r="Z2" s="107" t="s">
-        <v>1125</v>
+        <v>1119</v>
       </c>
       <c r="AA2" s="107" t="s">
         <v>209</v>
       </c>
       <c r="AB2" s="107" t="s">
-        <v>1124</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>1126</v>
+        <v>1120</v>
       </c>
       <c r="C3" t="s">
-        <v>1127</v>
+        <v>1121</v>
       </c>
       <c r="D3" t="s">
-        <v>1128</v>
+        <v>1122</v>
       </c>
       <c r="E3" s="69">
         <v>2018</v>
       </c>
       <c r="F3" s="69" t="s">
-        <v>1128</v>
+        <v>1122</v>
       </c>
       <c r="H3" s="69">
         <v>2018</v>
       </c>
       <c r="I3" s="69" t="s">
-        <v>1128</v>
+        <v>1122</v>
       </c>
       <c r="K3" s="69">
         <v>2018</v>
       </c>
       <c r="L3" s="69" t="s">
-        <v>1128</v>
+        <v>1122</v>
       </c>
       <c r="N3" s="69">
         <v>2018</v>
       </c>
       <c r="O3" s="69" t="s">
-        <v>1128</v>
+        <v>1122</v>
       </c>
       <c r="Q3" s="69">
         <v>2018</v>
       </c>
       <c r="R3" s="69" t="s">
-        <v>1128</v>
+        <v>1122</v>
       </c>
       <c r="T3" s="69">
         <v>2018</v>
       </c>
       <c r="U3" s="69" t="s">
-        <v>1128</v>
+        <v>1122</v>
       </c>
       <c r="W3" s="69">
         <v>2018</v>
       </c>
       <c r="X3" s="69" t="s">
-        <v>1128</v>
+        <v>1122</v>
       </c>
       <c r="Z3" s="69">
         <v>2018</v>
       </c>
       <c r="AA3" s="69" t="s">
-        <v>1128</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>1129</v>
+        <v>1123</v>
       </c>
       <c r="C4" t="s">
-        <v>1130</v>
+        <v>1124</v>
       </c>
       <c r="D4" t="s">
-        <v>1131</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>1132</v>
+        <v>1126</v>
       </c>
       <c r="C5" t="s">
-        <v>1133</v>
+        <v>1127</v>
       </c>
       <c r="D5" t="s">
-        <v>1134</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>1135</v>
+        <v>1129</v>
       </c>
       <c r="C6" t="s">
-        <v>1133</v>
+        <v>1127</v>
       </c>
       <c r="D6" t="s">
-        <v>1134</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>1136</v>
+        <v>1130</v>
       </c>
       <c r="C7" t="s">
-        <v>1133</v>
+        <v>1127</v>
       </c>
       <c r="D7" t="s">
-        <v>1134</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>1137</v>
+        <v>1131</v>
       </c>
       <c r="C8" t="s">
-        <v>1133</v>
+        <v>1127</v>
       </c>
       <c r="D8" t="s">
-        <v>1134</v>
+        <v>1128</v>
       </c>
       <c r="E8" s="69">
         <v>2017</v>
       </c>
       <c r="F8" s="108" t="s">
-        <v>1156</v>
+        <v>1150</v>
       </c>
       <c r="G8" s="69" t="s">
-        <v>1155</v>
+        <v>1149</v>
       </c>
       <c r="H8" s="69">
         <v>2016</v>
       </c>
       <c r="I8" s="69" t="s">
-        <v>1157</v>
+        <v>1151</v>
       </c>
       <c r="J8" s="69" t="s">
-        <v>1158</v>
+        <v>1152</v>
       </c>
       <c r="Q8" s="69">
         <v>2018</v>
       </c>
       <c r="R8" s="108" t="s">
-        <v>1138</v>
+        <v>1132</v>
       </c>
       <c r="S8" s="69" t="s">
-        <v>1139</v>
+        <v>1133</v>
       </c>
       <c r="W8" s="69">
         <v>2016</v>
       </c>
       <c r="X8" s="108" t="s">
-        <v>1153</v>
+        <v>1147</v>
       </c>
       <c r="Y8" s="69" t="s">
-        <v>1154</v>
+        <v>1148</v>
       </c>
       <c r="Z8" s="69">
         <v>2016</v>
       </c>
       <c r="AA8" s="69" t="s">
-        <v>1140</v>
+        <v>1134</v>
       </c>
       <c r="AB8" s="69" t="s">
-        <v>1141</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>1142</v>
+        <v>1136</v>
       </c>
       <c r="C9" t="s">
-        <v>1143</v>
+        <v>1137</v>
       </c>
       <c r="D9" t="s">
-        <v>1144</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>1145</v>
+        <v>1139</v>
       </c>
       <c r="C10" t="s">
-        <v>1143</v>
+        <v>1137</v>
       </c>
       <c r="D10" t="s">
-        <v>1144</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>1146</v>
+        <v>1140</v>
       </c>
       <c r="C11" t="s">
-        <v>1130</v>
+        <v>1124</v>
       </c>
       <c r="D11" t="s">
-        <v>1147</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>1148</v>
+        <v>1142</v>
       </c>
       <c r="C12" t="s">
-        <v>1130</v>
+        <v>1124</v>
       </c>
       <c r="D12" t="s">
-        <v>1147</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>1149</v>
+        <v>1143</v>
       </c>
       <c r="C13" t="s">
-        <v>1130</v>
+        <v>1124</v>
       </c>
       <c r="D13" t="s">
-        <v>1150</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>1151</v>
+        <v>1145</v>
       </c>
       <c r="C14" t="s">
-        <v>1133</v>
+        <v>1127</v>
       </c>
       <c r="D14" t="s">
-        <v>1152</v>
+        <v>1146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added in script for retrieving coordinates from google map urls (short or long)
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E81629-942A-4FF3-B3CB-9AE6111E56C6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D36BA6-8935-4A0D-8946-EFDF8B167D1E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
@@ -18,8 +18,8 @@
     <sheet name="parameters" sheetId="8" r:id="rId3"/>
     <sheet name="study_regions" sheetId="3" r:id="rId4"/>
     <sheet name="destinations" sheetId="6" r:id="rId5"/>
-    <sheet name="open_space_defs" sheetId="10" r:id="rId6"/>
-    <sheet name="ULI" sheetId="11" r:id="rId7"/>
+    <sheet name="ULI" sheetId="11" r:id="rId6"/>
+    <sheet name="open_space_defs" sheetId="10" r:id="rId7"/>
     <sheet name="indicators" sheetId="1" r:id="rId8"/>
     <sheet name="ind_study_region_matrix" sheetId="2" r:id="rId9"/>
     <sheet name="local_environments" sheetId="9" r:id="rId10"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2436" uniqueCount="1170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2453" uniqueCount="1179">
   <si>
     <t>Domain</t>
   </si>
@@ -3641,6 +3641,33 @@
   </si>
   <si>
     <t xml:space="preserve"> area_ha &gt; 0.5</t>
+  </si>
+  <si>
+    <t>tourism</t>
+  </si>
+  <si>
+    <t>'alpine_hut','apartment','aquarium','bed_and_breakfast','caravan_site','chalet','gallery','guest_house','hostel','hotel','information','motel','museum','theme_park','zoo'</t>
+  </si>
+  <si>
+    <t>https://data.gov.au/dataset/libraries-tasmania-locations</t>
+  </si>
+  <si>
+    <t>D:/ntnl_li_2018_template/data/destinations/libraries/Tas/libraries-tasmania.geojson</t>
+  </si>
+  <si>
+    <t>http://www.libraries.sa.gov.au/webdata/resources/files/All-Library-Locations.xlsx</t>
+  </si>
+  <si>
+    <t>D:/ntnl_li_2018_template/data/destinations/libraries/SA/SA_All-Library-Locations_2017_geocoded.csv</t>
+  </si>
+  <si>
+    <t>https://nt.gov.au/leisure/arts-culture-heritage/find-a-library-in-the-nt</t>
+  </si>
+  <si>
+    <t>D:/ntnl_li_2018_template/data/destinations/libraries/NT/NT libraries list - manually geocoded - 2018.xlsx</t>
+  </si>
+  <si>
+    <t>state government data</t>
   </si>
 </sst>
 </file>
@@ -56733,7 +56760,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD1048576"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57470,652 +57497,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
-  <dimension ref="A1:O38"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="7" width="94.5703125" customWidth="1"/>
-    <col min="8" max="8" width="41.5703125" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1"/>
-    <col min="10" max="10" width="41" customWidth="1"/>
-    <col min="11" max="11" width="29.140625" customWidth="1"/>
-    <col min="12" max="12" width="26.85546875" customWidth="1"/>
-    <col min="14" max="14" width="27.28515625" customWidth="1"/>
-    <col min="15" max="15" width="29.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
-        <v>1167</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>950</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>1054</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>1163</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>1159</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>1160</v>
-      </c>
-      <c r="G1" s="37" t="s">
-        <v>965</v>
-      </c>
-      <c r="H1" s="37" t="s">
-        <v>967</v>
-      </c>
-      <c r="I1" s="37" t="s">
-        <v>999</v>
-      </c>
-      <c r="J1" s="37" t="s">
-        <v>1101</v>
-      </c>
-      <c r="K1" s="37" t="s">
-        <v>1035</v>
-      </c>
-      <c r="L1" s="37" t="s">
-        <v>1045</v>
-      </c>
-      <c r="M1" s="37" t="s">
-        <v>1102</v>
-      </c>
-      <c r="N1" s="37" t="s">
-        <v>1103</v>
-      </c>
-      <c r="O1" s="37" t="s">
-        <v>1156</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>939</v>
-      </c>
-      <c r="B2" t="s">
-        <v>951</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1056</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E2" t="s">
-        <v>944</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1161</v>
-      </c>
-      <c r="G2" t="s">
-        <v>963</v>
-      </c>
-      <c r="H2" t="s">
-        <v>968</v>
-      </c>
-      <c r="I2" t="s">
-        <v>1000</v>
-      </c>
-      <c r="J2" t="s">
-        <v>1168</v>
-      </c>
-      <c r="K2" t="s">
-        <v>1018</v>
-      </c>
-      <c r="L2" t="s">
-        <v>1036</v>
-      </c>
-      <c r="M2" t="s">
-        <v>1039</v>
-      </c>
-      <c r="N2" s="106" t="s">
-        <v>1107</v>
-      </c>
-      <c r="O2" t="s">
-        <v>1155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>940</v>
-      </c>
-      <c r="B3" t="s">
-        <v>952</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1057</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1164</v>
-      </c>
-      <c r="E3" t="s">
-        <v>948</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1162</v>
-      </c>
-      <c r="G3" t="s">
-        <v>964</v>
-      </c>
-      <c r="H3" t="s">
-        <v>969</v>
-      </c>
-      <c r="I3" t="s">
-        <v>1001</v>
-      </c>
-      <c r="J3" t="s">
-        <v>1169</v>
-      </c>
-      <c r="K3" t="s">
-        <v>1019</v>
-      </c>
-      <c r="L3" t="s">
-        <v>1037</v>
-      </c>
-      <c r="M3" t="s">
-        <v>945</v>
-      </c>
-      <c r="N3" s="106" t="s">
-        <v>1153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>941</v>
-      </c>
-      <c r="B4" t="s">
-        <v>953</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1055</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1165</v>
-      </c>
-      <c r="G4" t="s">
-        <v>1157</v>
-      </c>
-      <c r="H4" t="s">
-        <v>970</v>
-      </c>
-      <c r="I4" t="s">
-        <v>1002</v>
-      </c>
-      <c r="J4" t="s">
-        <v>1086</v>
-      </c>
-      <c r="K4" t="s">
-        <v>1020</v>
-      </c>
-      <c r="L4" t="s">
-        <v>1112</v>
-      </c>
-      <c r="M4" t="s">
-        <v>1100</v>
-      </c>
-      <c r="N4" s="106" t="s">
-        <v>1108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>942</v>
-      </c>
-      <c r="B5" t="s">
-        <v>954</v>
-      </c>
-      <c r="C5" t="s">
-        <v>953</v>
-      </c>
-      <c r="H5" t="s">
-        <v>939</v>
-      </c>
-      <c r="I5" t="s">
-        <v>1003</v>
-      </c>
-      <c r="J5" t="s">
-        <v>1087</v>
-      </c>
-      <c r="K5" t="s">
-        <v>1021</v>
-      </c>
-      <c r="L5" t="s">
-        <v>1158</v>
-      </c>
-      <c r="M5" t="s">
-        <v>1052</v>
-      </c>
-      <c r="N5" s="106" t="s">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>943</v>
-      </c>
-      <c r="B6" t="s">
-        <v>945</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1058</v>
-      </c>
-      <c r="H6" t="s">
-        <v>971</v>
-      </c>
-      <c r="I6" t="s">
-        <v>1004</v>
-      </c>
-      <c r="J6" t="s">
-        <v>1088</v>
-      </c>
-      <c r="K6" t="s">
-        <v>1022</v>
-      </c>
-      <c r="L6" t="s">
-        <v>1039</v>
-      </c>
-      <c r="M6" t="s">
-        <v>947</v>
-      </c>
-      <c r="N6" s="106" t="s">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>944</v>
-      </c>
-      <c r="B7" t="s">
-        <v>955</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1060</v>
-      </c>
-      <c r="H7" t="s">
-        <v>972</v>
-      </c>
-      <c r="I7" t="s">
-        <v>1005</v>
-      </c>
-      <c r="J7" t="s">
-        <v>1089</v>
-      </c>
-      <c r="K7" t="s">
-        <v>1023</v>
-      </c>
-      <c r="L7" t="s">
-        <v>944</v>
-      </c>
-      <c r="M7" t="s">
-        <v>944</v>
-      </c>
-      <c r="N7" s="106" t="s">
-        <v>1110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>945</v>
-      </c>
-      <c r="B8" t="s">
-        <v>956</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1061</v>
-      </c>
-      <c r="H8" t="s">
-        <v>973</v>
-      </c>
-      <c r="I8" t="s">
-        <v>1006</v>
-      </c>
-      <c r="J8" t="s">
-        <v>1090</v>
-      </c>
-      <c r="K8" t="s">
-        <v>1024</v>
-      </c>
-      <c r="L8" t="s">
-        <v>1059</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>946</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1052</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1062</v>
-      </c>
-      <c r="H9" t="s">
-        <v>974</v>
-      </c>
-      <c r="I9" t="s">
-        <v>1007</v>
-      </c>
-      <c r="K9" t="s">
-        <v>1025</v>
-      </c>
-      <c r="L9" t="s">
-        <v>948</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>947</v>
-      </c>
-      <c r="B10" t="s">
-        <v>947</v>
-      </c>
-      <c r="C10" t="s">
-        <v>955</v>
-      </c>
-      <c r="H10" t="s">
-        <v>975</v>
-      </c>
-      <c r="I10" t="s">
-        <v>999</v>
-      </c>
-      <c r="K10" t="s">
-        <v>695</v>
-      </c>
-      <c r="L10" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>948</v>
-      </c>
-      <c r="B11" t="s">
-        <v>958</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1063</v>
-      </c>
-      <c r="H11" t="s">
-        <v>976</v>
-      </c>
-      <c r="I11" t="s">
-        <v>1008</v>
-      </c>
-      <c r="K11" t="s">
-        <v>1026</v>
-      </c>
-      <c r="L11" t="s">
-        <v>946</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>949</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1053</v>
-      </c>
-      <c r="H12" t="s">
-        <v>977</v>
-      </c>
-      <c r="I12" t="s">
-        <v>1009</v>
-      </c>
-      <c r="K12" t="s">
-        <v>1027</v>
-      </c>
-      <c r="L12" t="s">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>1059</v>
-      </c>
-      <c r="B13" t="s">
-        <v>959</v>
-      </c>
-      <c r="H13" t="s">
-        <v>978</v>
-      </c>
-      <c r="I13" t="s">
-        <v>1010</v>
-      </c>
-      <c r="K13" t="s">
-        <v>1028</v>
-      </c>
-      <c r="L13" t="s">
-        <v>942</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>1052</v>
-      </c>
-      <c r="B14" t="s">
-        <v>960</v>
-      </c>
-      <c r="H14" t="s">
-        <v>979</v>
-      </c>
-      <c r="I14" t="s">
-        <v>1011</v>
-      </c>
-      <c r="K14" t="s">
-        <v>1029</v>
-      </c>
-      <c r="L14" t="s">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>1154</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1104</v>
-      </c>
-      <c r="H15" t="s">
-        <v>980</v>
-      </c>
-      <c r="K15" t="s">
-        <v>1030</v>
-      </c>
-      <c r="L15" t="s">
-        <v>1040</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>1166</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1055</v>
-      </c>
-      <c r="H16" t="s">
-        <v>981</v>
-      </c>
-      <c r="K16" t="s">
-        <v>1031</v>
-      </c>
-      <c r="L16" t="s">
-        <v>1041</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>1164</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1105</v>
-      </c>
-      <c r="H17" t="s">
-        <v>982</v>
-      </c>
-      <c r="K17" t="s">
-        <v>1032</v>
-      </c>
-      <c r="L17" t="s">
-        <v>1085</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>1165</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1106</v>
-      </c>
-      <c r="H18" t="s">
-        <v>983</v>
-      </c>
-      <c r="K18" t="s">
-        <v>1033</v>
-      </c>
-      <c r="L18" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H19" t="s">
-        <v>957</v>
-      </c>
-      <c r="K19" t="s">
-        <v>1034</v>
-      </c>
-      <c r="L19" t="s">
-        <v>1091</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H20" t="s">
-        <v>940</v>
-      </c>
-      <c r="L20" t="s">
-        <v>1092</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H21" t="s">
-        <v>984</v>
-      </c>
-      <c r="L21" t="s">
-        <v>1038</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H22" t="s">
-        <v>985</v>
-      </c>
-      <c r="L22" t="s">
-        <v>1043</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H23" t="s">
-        <v>986</v>
-      </c>
-      <c r="L23" t="s">
-        <v>1044</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H24" t="s">
-        <v>987</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H25" t="s">
-        <v>988</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H26" t="s">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H27" t="s">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H28" t="s">
-        <v>991</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H29" t="s">
-        <v>992</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H30" t="s">
-        <v>993</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H31" t="s">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H32" t="s">
-        <v>995</v>
-      </c>
-    </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H33" t="s">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H34" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H35" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H36" t="s">
-        <v>998</v>
-      </c>
-    </row>
-    <row r="37" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H37" t="s">
-        <v>942</v>
-      </c>
-    </row>
-    <row r="38" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H38" t="s">
-        <v>943</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00663411-69BA-4AA2-8F13-6278DC3BD89D}">
   <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58369,7 +57755,7 @@
         <v>1127</v>
       </c>
       <c r="D8" t="s">
-        <v>1128</v>
+        <v>1178</v>
       </c>
       <c r="E8" s="69">
         <v>2017</v>
@@ -58389,6 +57775,24 @@
       <c r="J8" s="69" t="s">
         <v>1152</v>
       </c>
+      <c r="K8" s="69">
+        <v>2018</v>
+      </c>
+      <c r="L8" s="108" t="s">
+        <v>1176</v>
+      </c>
+      <c r="M8" s="69" t="s">
+        <v>1177</v>
+      </c>
+      <c r="N8" s="69">
+        <v>2018</v>
+      </c>
+      <c r="O8" s="108" t="s">
+        <v>1172</v>
+      </c>
+      <c r="P8" s="69" t="s">
+        <v>1173</v>
+      </c>
       <c r="Q8" s="69">
         <v>2018</v>
       </c>
@@ -58397,6 +57801,15 @@
       </c>
       <c r="S8" s="69" t="s">
         <v>1133</v>
+      </c>
+      <c r="T8" s="69">
+        <v>2017</v>
+      </c>
+      <c r="U8" s="108" t="s">
+        <v>1174</v>
+      </c>
+      <c r="V8" s="69" t="s">
+        <v>1175</v>
       </c>
       <c r="W8" s="69">
         <v>2016</v>
@@ -58503,8 +57916,685 @@
     <hyperlink ref="R8" r:id="rId1" xr:uid="{880BC495-9AE4-466F-8181-3A3C0C200010}"/>
     <hyperlink ref="X8" r:id="rId2" xr:uid="{FB261EBD-990A-4D37-B19E-DDDA92832966}"/>
     <hyperlink ref="F8" r:id="rId3" xr:uid="{FA499368-B6DC-442D-ABFF-FA03548B9B6A}"/>
+    <hyperlink ref="O8" r:id="rId4" xr:uid="{FB001105-C264-4FE6-A8C9-1F5CE7AF21EE}"/>
+    <hyperlink ref="U8" r:id="rId5" xr:uid="{ED6B062F-F3D0-41C9-B69B-F82CF3BAFEB4}"/>
+    <hyperlink ref="L8" r:id="rId6" xr:uid="{92A13B5C-F8F8-41E1-876B-79DCF21DAD1F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
+  <dimension ref="A1:O38"/>
+  <sheetViews>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="94.5703125" customWidth="1"/>
+    <col min="8" max="8" width="41.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="41" customWidth="1"/>
+    <col min="11" max="11" width="29.140625" customWidth="1"/>
+    <col min="12" max="12" width="26.85546875" customWidth="1"/>
+    <col min="14" max="14" width="27.28515625" customWidth="1"/>
+    <col min="15" max="15" width="29.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>950</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>1160</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>965</v>
+      </c>
+      <c r="H1" s="37" t="s">
+        <v>967</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>999</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>1101</v>
+      </c>
+      <c r="K1" s="37" t="s">
+        <v>1035</v>
+      </c>
+      <c r="L1" s="37" t="s">
+        <v>1045</v>
+      </c>
+      <c r="M1" s="37" t="s">
+        <v>1102</v>
+      </c>
+      <c r="N1" s="37" t="s">
+        <v>1103</v>
+      </c>
+      <c r="O1" s="37" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>939</v>
+      </c>
+      <c r="B2" t="s">
+        <v>951</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1166</v>
+      </c>
+      <c r="E2" t="s">
+        <v>944</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1161</v>
+      </c>
+      <c r="G2" t="s">
+        <v>963</v>
+      </c>
+      <c r="H2" t="s">
+        <v>968</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1000</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1168</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1018</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1036</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1039</v>
+      </c>
+      <c r="N2" s="106" t="s">
+        <v>1107</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>940</v>
+      </c>
+      <c r="B3" t="s">
+        <v>952</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E3" t="s">
+        <v>948</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G3" t="s">
+        <v>964</v>
+      </c>
+      <c r="H3" t="s">
+        <v>969</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1001</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1169</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1019</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="M3" t="s">
+        <v>945</v>
+      </c>
+      <c r="N3" s="106" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>941</v>
+      </c>
+      <c r="B4" t="s">
+        <v>953</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1165</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1157</v>
+      </c>
+      <c r="H4" t="s">
+        <v>970</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1002</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1086</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1020</v>
+      </c>
+      <c r="L4" t="s">
+        <v>939</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1100</v>
+      </c>
+      <c r="N4" s="106" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>942</v>
+      </c>
+      <c r="B5" t="s">
+        <v>954</v>
+      </c>
+      <c r="C5" t="s">
+        <v>953</v>
+      </c>
+      <c r="H5" t="s">
+        <v>939</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1003</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1087</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1021</v>
+      </c>
+      <c r="L5" t="s">
+        <v>940</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1052</v>
+      </c>
+      <c r="N5" s="106" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>943</v>
+      </c>
+      <c r="B6" t="s">
+        <v>945</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1058</v>
+      </c>
+      <c r="H6" t="s">
+        <v>971</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1004</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1088</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1022</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1112</v>
+      </c>
+      <c r="M6" t="s">
+        <v>947</v>
+      </c>
+      <c r="N6" s="106" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>944</v>
+      </c>
+      <c r="B7" t="s">
+        <v>955</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1060</v>
+      </c>
+      <c r="H7" t="s">
+        <v>972</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1005</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1089</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1023</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1158</v>
+      </c>
+      <c r="M7" t="s">
+        <v>944</v>
+      </c>
+      <c r="N7" s="106" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>945</v>
+      </c>
+      <c r="B8" t="s">
+        <v>956</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1061</v>
+      </c>
+      <c r="H8" t="s">
+        <v>973</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1006</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1090</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1024</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1039</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1170</v>
+      </c>
+      <c r="N8" s="106" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>946</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1062</v>
+      </c>
+      <c r="H9" t="s">
+        <v>974</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1007</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1025</v>
+      </c>
+      <c r="L9" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>947</v>
+      </c>
+      <c r="B10" t="s">
+        <v>947</v>
+      </c>
+      <c r="C10" t="s">
+        <v>955</v>
+      </c>
+      <c r="H10" t="s">
+        <v>975</v>
+      </c>
+      <c r="I10" t="s">
+        <v>999</v>
+      </c>
+      <c r="K10" t="s">
+        <v>695</v>
+      </c>
+      <c r="L10" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>948</v>
+      </c>
+      <c r="B11" t="s">
+        <v>958</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1063</v>
+      </c>
+      <c r="H11" t="s">
+        <v>976</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1008</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1026</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>949</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1053</v>
+      </c>
+      <c r="H12" t="s">
+        <v>977</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1009</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1027</v>
+      </c>
+      <c r="L12" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B13" t="s">
+        <v>959</v>
+      </c>
+      <c r="H13" t="s">
+        <v>978</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1010</v>
+      </c>
+      <c r="K13" t="s">
+        <v>1028</v>
+      </c>
+      <c r="L13" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B14" t="s">
+        <v>960</v>
+      </c>
+      <c r="H14" t="s">
+        <v>979</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1011</v>
+      </c>
+      <c r="K14" t="s">
+        <v>1029</v>
+      </c>
+      <c r="L14" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1104</v>
+      </c>
+      <c r="H15" t="s">
+        <v>980</v>
+      </c>
+      <c r="K15" t="s">
+        <v>1030</v>
+      </c>
+      <c r="L15" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1055</v>
+      </c>
+      <c r="H16" t="s">
+        <v>981</v>
+      </c>
+      <c r="K16" t="s">
+        <v>1031</v>
+      </c>
+      <c r="L16" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1105</v>
+      </c>
+      <c r="H17" t="s">
+        <v>982</v>
+      </c>
+      <c r="K17" t="s">
+        <v>1032</v>
+      </c>
+      <c r="L17" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1106</v>
+      </c>
+      <c r="H18" t="s">
+        <v>983</v>
+      </c>
+      <c r="K18" t="s">
+        <v>1033</v>
+      </c>
+      <c r="L18" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1170</v>
+      </c>
+      <c r="H19" t="s">
+        <v>957</v>
+      </c>
+      <c r="K19" t="s">
+        <v>1034</v>
+      </c>
+      <c r="L19" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>940</v>
+      </c>
+      <c r="L20" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>984</v>
+      </c>
+      <c r="L21" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>985</v>
+      </c>
+      <c r="L22" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>986</v>
+      </c>
+      <c r="L23" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>987</v>
+      </c>
+      <c r="L24" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>988</v>
+      </c>
+      <c r="L25" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>989</v>
+      </c>
+      <c r="L26" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>990</v>
+      </c>
+      <c r="L27" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>991</v>
+      </c>
+      <c r="L28" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>992</v>
+      </c>
+      <c r="L29" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>993</v>
+      </c>
+      <c r="L30" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>994</v>
+      </c>
+      <c r="L31" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H35" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="36" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H36" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="37" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H37" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="38" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H38" t="s">
+        <v>943</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fixed up division of public, not public and combined geometries for open space areas
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D36BA6-8935-4A0D-8946-EFDF8B167D1E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885AD9FC-A11E-4026-9E13-1803C2AF20A0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="4" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -56759,8 +56759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E323C290-C88C-4E5C-B55A-017ED14783D9}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57500,8 +57500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00663411-69BA-4AA2-8F13-6278DC3BD89D}">
   <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57509,7 +57509,22 @@
     <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="28" width="9.7109375" style="69" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="69" customWidth="1"/>
+    <col min="6" max="7" width="9.7109375" style="69" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" style="69" customWidth="1"/>
+    <col min="9" max="10" width="9.7109375" style="69" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="69" customWidth="1"/>
+    <col min="12" max="13" width="9.7109375" style="69" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" style="69" customWidth="1"/>
+    <col min="15" max="16" width="9.7109375" style="69" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" style="69" customWidth="1"/>
+    <col min="18" max="19" width="9.7109375" style="69" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" style="69" customWidth="1"/>
+    <col min="21" max="22" width="9.7109375" style="69" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="9.7109375" style="69" customWidth="1"/>
+    <col min="24" max="25" width="9.7109375" style="69" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="9.7109375" style="69" customWidth="1"/>
+    <col min="27" max="28" width="9.7109375" style="69" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="110" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ensured that if a linear feature is within a public feature it is absorbed, and not repeated as a seperate linear feature when aggregated to AOS layer
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885AD9FC-A11E-4026-9E13-1803C2AF20A0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F60B7EA-45FD-4B3F-8854-716B69A979D8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="4" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="6" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -56759,7 +56759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E323C290-C88C-4E5C-B55A-017ED14783D9}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
@@ -57943,8 +57943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57957,7 +57957,7 @@
     <col min="10" max="10" width="41" customWidth="1"/>
     <col min="11" max="11" width="29.140625" customWidth="1"/>
     <col min="12" max="12" width="26.85546875" customWidth="1"/>
-    <col min="14" max="14" width="27.28515625" customWidth="1"/>
+    <col min="14" max="14" width="64.7109375" customWidth="1"/>
     <col min="15" max="15" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
amended scripts: OSM import (add GIST indices to transformed geom of point, line and polygon features) and open_space_areas (associate open spaces with intersecting point and line attributes and better differentiate linear water way features as a distinct class (which has high potential for unintentional aggregation on proximity across large areas; hence, seperated)
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F60B7EA-45FD-4B3F-8854-716B69A979D8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD68EF9-BF2D-42D0-ABFE-6FE066067CDD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="6" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
@@ -27,7 +27,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">indicators!$A$2:$AC$48</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2453" uniqueCount="1179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2475" uniqueCount="1190">
   <si>
     <t>Domain</t>
   </si>
@@ -3668,6 +3668,39 @@
   </si>
   <si>
     <t>state government data</t>
+  </si>
+  <si>
+    <t>linear_waterway</t>
+  </si>
+  <si>
+    <t>point_line_fields</t>
+  </si>
+  <si>
+    <t>"natural"</t>
+  </si>
+  <si>
+    <t>ditch</t>
+  </si>
+  <si>
+    <t>drain</t>
+  </si>
+  <si>
+    <t>canal</t>
+  </si>
+  <si>
+    <t>rapids</t>
+  </si>
+  <si>
+    <t>drystream</t>
+  </si>
+  <si>
+    <t>brook</t>
+  </si>
+  <si>
+    <t>derelict_canal</t>
+  </si>
+  <si>
+    <t>fairway</t>
   </si>
 </sst>
 </file>
@@ -57941,10 +57974,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
-  <dimension ref="A1:O38"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57953,15 +57986,17 @@
     <col min="2" max="6" width="21.28515625" customWidth="1"/>
     <col min="7" max="7" width="94.5703125" customWidth="1"/>
     <col min="8" max="8" width="41.5703125" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1"/>
-    <col min="10" max="10" width="41" customWidth="1"/>
-    <col min="11" max="11" width="29.140625" customWidth="1"/>
-    <col min="12" max="12" width="26.85546875" customWidth="1"/>
-    <col min="14" max="14" width="64.7109375" customWidth="1"/>
-    <col min="15" max="15" width="29.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="33.85546875" customWidth="1"/>
+    <col min="12" max="12" width="41" customWidth="1"/>
+    <col min="13" max="13" width="29.140625" customWidth="1"/>
+    <col min="14" max="14" width="26.85546875" customWidth="1"/>
+    <col min="16" max="16" width="64.7109375" customWidth="1"/>
+    <col min="17" max="17" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>1167</v>
       </c>
@@ -57987,28 +58022,34 @@
         <v>967</v>
       </c>
       <c r="I1" s="37" t="s">
+        <v>1179</v>
+      </c>
+      <c r="J1" s="37" t="s">
         <v>999</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="K1" s="37" t="s">
+        <v>1180</v>
+      </c>
+      <c r="L1" s="37" t="s">
         <v>1101</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="M1" s="37" t="s">
         <v>1035</v>
       </c>
-      <c r="L1" s="37" t="s">
+      <c r="N1" s="37" t="s">
         <v>1045</v>
       </c>
-      <c r="M1" s="37" t="s">
+      <c r="O1" s="37" t="s">
         <v>1102</v>
       </c>
-      <c r="N1" s="37" t="s">
+      <c r="P1" s="37" t="s">
         <v>1103</v>
       </c>
-      <c r="O1" s="37" t="s">
+      <c r="Q1" s="37" t="s">
         <v>1156</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>939</v>
       </c>
@@ -58034,28 +58075,34 @@
         <v>968</v>
       </c>
       <c r="I2" t="s">
+        <v>940</v>
+      </c>
+      <c r="J2" t="s">
         <v>1000</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>1039</v>
+      </c>
+      <c r="L2" t="s">
         <v>1168</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>1018</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>1036</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>1039</v>
       </c>
-      <c r="N2" s="106" t="s">
+      <c r="P2" s="106" t="s">
         <v>1107</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>1155</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>940</v>
       </c>
@@ -58081,25 +58128,31 @@
         <v>969</v>
       </c>
       <c r="I3" t="s">
+        <v>985</v>
+      </c>
+      <c r="J3" t="s">
         <v>1001</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
+        <v>945</v>
+      </c>
+      <c r="L3" t="s">
         <v>1169</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>1019</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>1037</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>945</v>
       </c>
-      <c r="N3" s="106" t="s">
+      <c r="P3" s="106" t="s">
         <v>1153</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>941</v>
       </c>
@@ -58119,25 +58172,31 @@
         <v>970</v>
       </c>
       <c r="I4" t="s">
+        <v>986</v>
+      </c>
+      <c r="J4" t="s">
         <v>1002</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
+        <v>1181</v>
+      </c>
+      <c r="L4" t="s">
         <v>1086</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>1020</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>939</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>1100</v>
       </c>
-      <c r="N4" s="106" t="s">
+      <c r="P4" s="106" t="s">
         <v>1108</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>942</v>
       </c>
@@ -58151,25 +58210,31 @@
         <v>939</v>
       </c>
       <c r="I5" t="s">
+        <v>989</v>
+      </c>
+      <c r="J5" t="s">
         <v>1003</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
+        <v>1170</v>
+      </c>
+      <c r="L5" t="s">
         <v>1087</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>1021</v>
       </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
         <v>940</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>1052</v>
       </c>
-      <c r="N5" s="106" t="s">
+      <c r="P5" s="106" t="s">
         <v>1111</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>943</v>
       </c>
@@ -58183,25 +58248,31 @@
         <v>971</v>
       </c>
       <c r="I6" t="s">
+        <v>942</v>
+      </c>
+      <c r="J6" t="s">
         <v>1004</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
+        <v>942</v>
+      </c>
+      <c r="L6" t="s">
         <v>1088</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>1022</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>1112</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>947</v>
       </c>
-      <c r="N6" s="106" t="s">
+      <c r="P6" s="106" t="s">
         <v>1109</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>944</v>
       </c>
@@ -58215,25 +58286,28 @@
         <v>972</v>
       </c>
       <c r="I7" t="s">
+        <v>990</v>
+      </c>
+      <c r="J7" t="s">
         <v>1005</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>1089</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>1023</v>
       </c>
-      <c r="L7" t="s">
+      <c r="N7" t="s">
         <v>1158</v>
       </c>
-      <c r="M7" t="s">
+      <c r="O7" t="s">
         <v>944</v>
       </c>
-      <c r="N7" s="106" t="s">
+      <c r="P7" s="106" t="s">
         <v>1110</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>945</v>
       </c>
@@ -58247,25 +58321,28 @@
         <v>973</v>
       </c>
       <c r="I8" t="s">
+        <v>1182</v>
+      </c>
+      <c r="J8" t="s">
         <v>1006</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>1090</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>1024</v>
       </c>
-      <c r="L8" t="s">
+      <c r="N8" t="s">
         <v>1039</v>
       </c>
-      <c r="M8" t="s">
+      <c r="O8" t="s">
         <v>1170</v>
       </c>
-      <c r="N8" s="106" t="s">
+      <c r="P8" s="106" t="s">
         <v>1171</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>946</v>
       </c>
@@ -58279,16 +58356,19 @@
         <v>974</v>
       </c>
       <c r="I9" t="s">
+        <v>940</v>
+      </c>
+      <c r="J9" t="s">
         <v>1007</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>1025</v>
       </c>
-      <c r="L9" t="s">
+      <c r="N9" t="s">
         <v>944</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>947</v>
       </c>
@@ -58302,16 +58382,19 @@
         <v>975</v>
       </c>
       <c r="I10" t="s">
+        <v>1183</v>
+      </c>
+      <c r="J10" t="s">
         <v>999</v>
       </c>
-      <c r="K10" t="s">
+      <c r="M10" t="s">
         <v>695</v>
       </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
         <v>1059</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>948</v>
       </c>
@@ -58325,16 +58408,19 @@
         <v>976</v>
       </c>
       <c r="I11" t="s">
+        <v>1184</v>
+      </c>
+      <c r="J11" t="s">
         <v>1008</v>
       </c>
-      <c r="K11" t="s">
+      <c r="M11" t="s">
         <v>1026</v>
       </c>
-      <c r="L11" t="s">
+      <c r="N11" t="s">
         <v>1154</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>949</v>
       </c>
@@ -58345,16 +58431,19 @@
         <v>977</v>
       </c>
       <c r="I12" t="s">
+        <v>1185</v>
+      </c>
+      <c r="J12" t="s">
         <v>1009</v>
       </c>
-      <c r="K12" t="s">
+      <c r="M12" t="s">
         <v>1027</v>
       </c>
-      <c r="L12" t="s">
+      <c r="N12" t="s">
         <v>948</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1059</v>
       </c>
@@ -58365,16 +58454,19 @@
         <v>978</v>
       </c>
       <c r="I13" t="s">
+        <v>1186</v>
+      </c>
+      <c r="J13" t="s">
         <v>1010</v>
       </c>
-      <c r="K13" t="s">
+      <c r="M13" t="s">
         <v>1028</v>
       </c>
-      <c r="L13" t="s">
+      <c r="N13" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1052</v>
       </c>
@@ -58385,16 +58477,19 @@
         <v>979</v>
       </c>
       <c r="I14" t="s">
+        <v>1187</v>
+      </c>
+      <c r="J14" t="s">
         <v>1011</v>
       </c>
-      <c r="K14" t="s">
+      <c r="M14" t="s">
         <v>1029</v>
       </c>
-      <c r="L14" t="s">
+      <c r="N14" t="s">
         <v>946</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1154</v>
       </c>
@@ -58404,14 +58499,17 @@
       <c r="H15" t="s">
         <v>980</v>
       </c>
-      <c r="K15" t="s">
+      <c r="I15" t="s">
+        <v>1188</v>
+      </c>
+      <c r="M15" t="s">
         <v>1030</v>
       </c>
-      <c r="L15" t="s">
+      <c r="N15" t="s">
         <v>949</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1166</v>
       </c>
@@ -58421,14 +58519,17 @@
       <c r="H16" t="s">
         <v>981</v>
       </c>
-      <c r="K16" t="s">
+      <c r="I16" t="s">
+        <v>1189</v>
+      </c>
+      <c r="M16" t="s">
         <v>1031</v>
       </c>
-      <c r="L16" t="s">
+      <c r="N16" t="s">
         <v>1052</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1164</v>
       </c>
@@ -58438,14 +58539,14 @@
       <c r="H17" t="s">
         <v>982</v>
       </c>
-      <c r="K17" t="s">
+      <c r="M17" t="s">
         <v>1032</v>
       </c>
-      <c r="L17" t="s">
+      <c r="N17" t="s">
         <v>947</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1165</v>
       </c>
@@ -58455,124 +58556,124 @@
       <c r="H18" t="s">
         <v>983</v>
       </c>
-      <c r="K18" t="s">
+      <c r="M18" t="s">
         <v>1033</v>
       </c>
-      <c r="L18" t="s">
+      <c r="N18" t="s">
         <v>1170</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1170</v>
       </c>
       <c r="H19" t="s">
         <v>957</v>
       </c>
-      <c r="K19" t="s">
+      <c r="M19" t="s">
         <v>1034</v>
       </c>
-      <c r="L19" t="s">
+      <c r="N19" t="s">
         <v>941</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H20" t="s">
         <v>940</v>
       </c>
-      <c r="L20" t="s">
+      <c r="N20" t="s">
         <v>943</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H21" t="s">
         <v>984</v>
       </c>
-      <c r="L21" t="s">
+      <c r="N21" t="s">
         <v>942</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H22" t="s">
         <v>985</v>
       </c>
-      <c r="L22" t="s">
+      <c r="N22" t="s">
         <v>960</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H23" t="s">
         <v>986</v>
       </c>
-      <c r="L23" t="s">
+      <c r="N23" t="s">
         <v>1040</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H24" t="s">
         <v>987</v>
       </c>
-      <c r="L24" t="s">
+      <c r="N24" t="s">
         <v>1041</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H25" t="s">
         <v>988</v>
       </c>
-      <c r="L25" t="s">
+      <c r="N25" t="s">
         <v>1085</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H26" t="s">
         <v>989</v>
       </c>
-      <c r="L26" t="s">
+      <c r="N26" t="s">
         <v>1042</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H27" t="s">
         <v>990</v>
       </c>
-      <c r="L27" t="s">
+      <c r="N27" t="s">
         <v>1091</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
         <v>991</v>
       </c>
-      <c r="L28" t="s">
+      <c r="N28" t="s">
         <v>1092</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H29" t="s">
         <v>992</v>
       </c>
-      <c r="L29" t="s">
+      <c r="N29" t="s">
         <v>1038</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H30" t="s">
         <v>993</v>
       </c>
-      <c r="L30" t="s">
+      <c r="N30" t="s">
         <v>1043</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H31" t="s">
         <v>994</v>
       </c>
-      <c r="L31" t="s">
+      <c r="N31" t="s">
         <v>1044</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H32" t="s">
         <v>995</v>
       </c>

</xml_diff>

<commit_message>
fixed up the config file so it doesn't crash with the new part-formed destination data
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FE2D60-86C3-4979-AFEE-718850953202}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B3068B-50FB-4465-8BAA-5C787A0ABD50}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="5" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
@@ -59104,8 +59104,8 @@
   <dimension ref="A1:M87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C83" sqref="C83:C87"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61148,6 +61148,9 @@
       <c r="F83" t="s">
         <v>1431</v>
       </c>
+      <c r="K83">
+        <v>2018</v>
+      </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
@@ -61162,6 +61165,9 @@
       <c r="F84" t="s">
         <v>1435</v>
       </c>
+      <c r="K84">
+        <v>2018</v>
+      </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
@@ -61176,6 +61182,9 @@
       <c r="F85" t="s">
         <v>1432</v>
       </c>
+      <c r="K85">
+        <v>2018</v>
+      </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
@@ -61190,6 +61199,9 @@
       <c r="F86" t="s">
         <v>1433</v>
       </c>
+      <c r="K86">
+        <v>2018</v>
+      </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
@@ -61203,6 +61215,9 @@
       </c>
       <c r="F87" t="s">
         <v>1434</v>
+      </c>
+      <c r="K87">
+        <v>2018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
part way with a new recompile destinations script; its not currently finished - but want to commit before i make more big changes
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3A33D7-7DFF-4937-9F50-514ECA8F0086}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4CB5A3-824D-4FE3-9FA3-0E48C0260AB0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="7" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="4" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -62204,8 +62204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB9F8A8-BF9D-4E84-929F-4B49CA2CC7BE}">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62216,8 +62216,7 @@
     <col min="4" max="4" width="19" style="21" customWidth="1"/>
     <col min="5" max="5" width="19" style="64" customWidth="1"/>
     <col min="6" max="7" width="9.140625" style="21"/>
-    <col min="8" max="8" width="19" style="21" customWidth="1"/>
-    <col min="9" max="9" width="19" style="64" customWidth="1"/>
+    <col min="8" max="9" width="19" style="21" customWidth="1"/>
     <col min="10" max="10" width="25" style="64" customWidth="1"/>
     <col min="11" max="11" width="72.85546875" style="64" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="21"/>
@@ -62248,7 +62247,7 @@
       <c r="H1" s="126" t="s">
         <v>1430</v>
       </c>
-      <c r="I1" s="128" t="s">
+      <c r="I1" s="126" t="s">
         <v>1431</v>
       </c>
       <c r="J1" s="128" t="s">
@@ -62283,7 +62282,7 @@
       <c r="H2" s="21">
         <v>20170704</v>
       </c>
-      <c r="I2" s="64" t="s">
+      <c r="I2" s="21" t="s">
         <v>1403</v>
       </c>
       <c r="J2" s="64" t="s">
@@ -62318,7 +62317,7 @@
       <c r="H3" s="21">
         <v>20170704</v>
       </c>
-      <c r="I3" s="64" t="s">
+      <c r="I3" s="21" t="s">
         <v>1403</v>
       </c>
       <c r="J3" s="64" t="s">
@@ -62350,7 +62349,7 @@
       <c r="H4" s="21">
         <v>20170704</v>
       </c>
-      <c r="I4" s="64" t="s">
+      <c r="I4" s="21" t="s">
         <v>1403</v>
       </c>
       <c r="J4" s="64" t="s">
@@ -62466,7 +62465,7 @@
       <c r="H13" s="21">
         <v>20181001</v>
       </c>
-      <c r="I13" s="64" t="s">
+      <c r="I13" s="21" t="s">
         <v>1403</v>
       </c>
       <c r="J13" s="64" t="s">
@@ -62476,647 +62475,284 @@
         <v>1435</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="64" t="s">
-        <v>1399</v>
-      </c>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="21" t="s">
-        <v>806</v>
+        <v>657</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>823</v>
-      </c>
-      <c r="D14" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F14" s="129"/>
-      <c r="G14" s="129"/>
-      <c r="I14" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>601</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
-        <v>1439</v>
+        <v>657</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>1440</v>
-      </c>
-      <c r="D15" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F15" s="129"/>
-      <c r="G15" s="129"/>
-      <c r="I15" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>602</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>1322</v>
-      </c>
-      <c r="D16" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F16" s="129"/>
-      <c r="G16" s="129"/>
-      <c r="I16" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>603</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>1323</v>
-      </c>
-      <c r="D17" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F17" s="129"/>
-      <c r="G17" s="129"/>
-      <c r="I17" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>604</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>1324</v>
-      </c>
-      <c r="D18" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F18" s="129"/>
-      <c r="G18" s="129"/>
-      <c r="I18" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>605</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>1325</v>
-      </c>
-      <c r="D19" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F19" s="129"/>
-      <c r="G19" s="129"/>
-      <c r="I19" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>606</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>1326</v>
-      </c>
-      <c r="D20" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F20" s="129"/>
-      <c r="G20" s="129"/>
-      <c r="I20" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>607</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>1327</v>
-      </c>
-      <c r="D21" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F21" s="129"/>
-      <c r="G21" s="129"/>
-      <c r="I21" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>608</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>1396</v>
-      </c>
-      <c r="D22" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F22" s="129"/>
-      <c r="G22" s="129"/>
-      <c r="I22" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>609</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>1413</v>
-      </c>
-      <c r="D23" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F23" s="129"/>
-      <c r="G23" s="129"/>
-      <c r="I23" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>611</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>1328</v>
-      </c>
-      <c r="D24" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F24" s="129"/>
-      <c r="G24" s="129"/>
-      <c r="I24" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>612</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>1329</v>
-      </c>
-      <c r="D25" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F25" s="129"/>
-      <c r="G25" s="129"/>
-      <c r="I25" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>613</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>1330</v>
-      </c>
-      <c r="D26" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F26" s="129"/>
-      <c r="G26" s="129"/>
-      <c r="I26" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>614</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>1331</v>
-      </c>
-      <c r="D27" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F27" s="129"/>
-      <c r="G27" s="129"/>
-      <c r="I27" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>615</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>1332</v>
-      </c>
-      <c r="D28" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F28" s="129"/>
-      <c r="G28" s="129"/>
-      <c r="I28" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>616</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>1333</v>
-      </c>
-      <c r="D29" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F29" s="129"/>
-      <c r="G29" s="129"/>
-      <c r="I29" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>617</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>1334</v>
-      </c>
-      <c r="D30" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F30" s="129"/>
-      <c r="G30" s="129"/>
-      <c r="I30" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>618</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>1335</v>
-      </c>
-      <c r="D31" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F31" s="129"/>
-      <c r="G31" s="129"/>
-      <c r="I31" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>619</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>1336</v>
-      </c>
-      <c r="D32" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F32" s="129"/>
-      <c r="G32" s="129"/>
-      <c r="I32" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>620</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>1337</v>
-      </c>
-      <c r="D33" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F33" s="129"/>
-      <c r="G33" s="129"/>
-      <c r="I33" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>621</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>1338</v>
-      </c>
-      <c r="D34" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F34" s="129"/>
-      <c r="G34" s="129"/>
-      <c r="I34" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>622</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>1339</v>
-      </c>
-      <c r="D35" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F35" s="129"/>
-      <c r="G35" s="129"/>
-      <c r="I35" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>623</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>1340</v>
-      </c>
-      <c r="D36" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F36" s="129"/>
-      <c r="G36" s="129"/>
-      <c r="I36" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>624</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>1341</v>
-      </c>
-      <c r="D37" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F37" s="129"/>
-      <c r="G37" s="129"/>
-      <c r="I37" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>625</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>1342</v>
-      </c>
-      <c r="D38" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F38" s="129"/>
-      <c r="G38" s="129"/>
-      <c r="I38" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>626</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>1343</v>
-      </c>
-      <c r="D39" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F39" s="129"/>
-      <c r="G39" s="129"/>
-      <c r="I39" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>627</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>1344</v>
-      </c>
-      <c r="D40" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F40" s="129"/>
-      <c r="G40" s="129"/>
-      <c r="I40" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>628</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>1345</v>
-      </c>
-      <c r="D41" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F41" s="129"/>
-      <c r="G41" s="129"/>
-      <c r="I41" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>629</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>1346</v>
-      </c>
-      <c r="D42" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F42" s="129"/>
-      <c r="G42" s="129"/>
-      <c r="I42" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>630</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>1347</v>
-      </c>
-      <c r="D43" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F43" s="129"/>
-      <c r="G43" s="129"/>
-      <c r="I43" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>631</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>1348</v>
-      </c>
-      <c r="D44" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F44" s="129"/>
-      <c r="G44" s="129"/>
-      <c r="I44" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>632</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>1349</v>
-      </c>
-      <c r="D45" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F45" s="129"/>
-      <c r="G45" s="129"/>
-      <c r="I45" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="64" t="s">
-        <v>1399</v>
-      </c>
+        <v>633</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>1350</v>
-      </c>
-      <c r="D46" s="21">
-        <v>2018</v>
-      </c>
-      <c r="F46" s="129"/>
-      <c r="G46" s="129"/>
-      <c r="I46" s="64" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>602</v>
+        <v>636</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
@@ -63124,7 +62760,7 @@
         <v>657</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>603</v>
+        <v>637</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
@@ -63132,7 +62768,7 @@
         <v>657</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>604</v>
+        <v>638</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
@@ -63140,7 +62776,7 @@
         <v>657</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>605</v>
+        <v>639</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
@@ -63148,7 +62784,7 @@
         <v>657</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>606</v>
+        <v>640</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
@@ -63156,7 +62792,7 @@
         <v>657</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>607</v>
+        <v>641</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
@@ -63164,7 +62800,7 @@
         <v>657</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>608</v>
+        <v>642</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
@@ -63172,7 +62808,7 @@
         <v>657</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>609</v>
+        <v>643</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
@@ -63180,7 +62816,7 @@
         <v>657</v>
       </c>
       <c r="C56" s="21" t="s">
-        <v>611</v>
+        <v>644</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
@@ -63188,7 +62824,7 @@
         <v>657</v>
       </c>
       <c r="C57" s="21" t="s">
-        <v>612</v>
+        <v>645</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
@@ -63196,7 +62832,7 @@
         <v>657</v>
       </c>
       <c r="C58" s="21" t="s">
-        <v>613</v>
+        <v>646</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
@@ -63204,7 +62840,7 @@
         <v>657</v>
       </c>
       <c r="C59" s="21" t="s">
-        <v>614</v>
+        <v>647</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
@@ -63212,7 +62848,7 @@
         <v>657</v>
       </c>
       <c r="C60" s="21" t="s">
-        <v>615</v>
+        <v>648</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
@@ -63220,7 +62856,7 @@
         <v>657</v>
       </c>
       <c r="C61" s="21" t="s">
-        <v>616</v>
+        <v>649</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
@@ -63228,7 +62864,7 @@
         <v>657</v>
       </c>
       <c r="C62" s="21" t="s">
-        <v>617</v>
+        <v>650</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
@@ -63236,7 +62872,7 @@
         <v>657</v>
       </c>
       <c r="C63" s="21" t="s">
-        <v>618</v>
+        <v>651</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
@@ -63244,303 +62880,666 @@
         <v>657</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B65" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C65" s="21" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B66" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C66" s="21" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B67" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C67" s="21" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B68" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C68" s="21" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B69" s="21" t="s">
-        <v>657</v>
+        <v>806</v>
       </c>
       <c r="C69" s="21" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+        <v>823</v>
+      </c>
+      <c r="D69" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F69" s="129"/>
+      <c r="G69" s="129"/>
+      <c r="I69" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B70" s="21" t="s">
-        <v>657</v>
+        <v>1439</v>
       </c>
       <c r="C70" s="21" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1440</v>
+      </c>
+      <c r="D70" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F70" s="129"/>
+      <c r="G70" s="129"/>
+      <c r="I70" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B71" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C71" s="21" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1322</v>
+      </c>
+      <c r="D71" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F71" s="129"/>
+      <c r="G71" s="129"/>
+      <c r="I71" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B72" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C72" s="21" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1323</v>
+      </c>
+      <c r="D72" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F72" s="129"/>
+      <c r="G72" s="129"/>
+      <c r="I72" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B73" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C73" s="21" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1324</v>
+      </c>
+      <c r="D73" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F73" s="129"/>
+      <c r="G73" s="129"/>
+      <c r="I73" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B74" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C74" s="21" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1325</v>
+      </c>
+      <c r="D74" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F74" s="129"/>
+      <c r="G74" s="129"/>
+      <c r="I74" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B75" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C75" s="21" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1326</v>
+      </c>
+      <c r="D75" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F75" s="129"/>
+      <c r="G75" s="129"/>
+      <c r="I75" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B76" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C76" s="21" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1327</v>
+      </c>
+      <c r="D76" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F76" s="129"/>
+      <c r="G76" s="129"/>
+      <c r="I76" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B77" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C77" s="21" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1396</v>
+      </c>
+      <c r="D77" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F77" s="129"/>
+      <c r="G77" s="129"/>
+      <c r="I77" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B78" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C78" s="21" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1413</v>
+      </c>
+      <c r="D78" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F78" s="129"/>
+      <c r="G78" s="129"/>
+      <c r="I78" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B79" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C79" s="21" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1328</v>
+      </c>
+      <c r="D79" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F79" s="129"/>
+      <c r="G79" s="129"/>
+      <c r="I79" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B80" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C80" s="21" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1329</v>
+      </c>
+      <c r="D80" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F80" s="129"/>
+      <c r="G80" s="129"/>
+      <c r="I80" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B81" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C81" s="21" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1330</v>
+      </c>
+      <c r="D81" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F81" s="129"/>
+      <c r="G81" s="129"/>
+      <c r="I81" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B82" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C82" s="21" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1331</v>
+      </c>
+      <c r="D82" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F82" s="129"/>
+      <c r="G82" s="129"/>
+      <c r="I82" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B83" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C83" s="21" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1332</v>
+      </c>
+      <c r="D83" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F83" s="129"/>
+      <c r="G83" s="129"/>
+      <c r="I83" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B84" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C84" s="21" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1333</v>
+      </c>
+      <c r="D84" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F84" s="129"/>
+      <c r="G84" s="129"/>
+      <c r="I84" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B85" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C85" s="21" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1334</v>
+      </c>
+      <c r="D85" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F85" s="129"/>
+      <c r="G85" s="129"/>
+      <c r="I85" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B86" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C86" s="21" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1335</v>
+      </c>
+      <c r="D86" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F86" s="129"/>
+      <c r="G86" s="129"/>
+      <c r="I86" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B87" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C87" s="21" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1336</v>
+      </c>
+      <c r="D87" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F87" s="129"/>
+      <c r="G87" s="129"/>
+      <c r="I87" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B88" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C88" s="21" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1337</v>
+      </c>
+      <c r="D88" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F88" s="129"/>
+      <c r="G88" s="129"/>
+      <c r="I88" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B89" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C89" s="21" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1338</v>
+      </c>
+      <c r="D89" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F89" s="129"/>
+      <c r="G89" s="129"/>
+      <c r="I89" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B90" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C90" s="21" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1339</v>
+      </c>
+      <c r="D90" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F90" s="129"/>
+      <c r="G90" s="129"/>
+      <c r="I90" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B91" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C91" s="21" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1340</v>
+      </c>
+      <c r="D91" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F91" s="129"/>
+      <c r="G91" s="129"/>
+      <c r="I91" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B92" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C92" s="21" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1341</v>
+      </c>
+      <c r="D92" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F92" s="129"/>
+      <c r="G92" s="129"/>
+      <c r="I92" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B93" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C93" s="21" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1342</v>
+      </c>
+      <c r="D93" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F93" s="129"/>
+      <c r="G93" s="129"/>
+      <c r="I93" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B94" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C94" s="21" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1343</v>
+      </c>
+      <c r="D94" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F94" s="129"/>
+      <c r="G94" s="129"/>
+      <c r="I94" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B95" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C95" s="21" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1344</v>
+      </c>
+      <c r="D95" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F95" s="129"/>
+      <c r="G95" s="129"/>
+      <c r="I95" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B96" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C96" s="21" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1345</v>
+      </c>
+      <c r="D96" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F96" s="129"/>
+      <c r="G96" s="129"/>
+      <c r="I96" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B97" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C97" s="21" t="s">
-        <v>1074</v>
-      </c>
-    </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1346</v>
+      </c>
+      <c r="D97" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F97" s="129"/>
+      <c r="G97" s="129"/>
+      <c r="I97" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B98" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C98" s="21" t="s">
-        <v>1414</v>
-      </c>
-    </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1347</v>
+      </c>
+      <c r="D98" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F98" s="129"/>
+      <c r="G98" s="129"/>
+      <c r="I98" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B99" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C99" s="21" t="s">
-        <v>1415</v>
-      </c>
-    </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1348</v>
+      </c>
+      <c r="D99" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F99" s="129"/>
+      <c r="G99" s="129"/>
+      <c r="I99" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B100" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C100" s="21" t="s">
-        <v>1416</v>
-      </c>
-    </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1349</v>
+      </c>
+      <c r="D100" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F100" s="129"/>
+      <c r="G100" s="129"/>
+      <c r="I100" s="21" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="64" t="s">
+        <v>1399</v>
+      </c>
       <c r="B101" s="21" t="s">
         <v>657</v>
       </c>
       <c r="C101" s="21" t="s">
-        <v>1417</v>
+        <v>1350</v>
+      </c>
+      <c r="D101" s="21">
+        <v>2018</v>
+      </c>
+      <c r="F101" s="129"/>
+      <c r="G101" s="129"/>
+      <c r="I101" s="21" t="s">
+        <v>1403</v>
       </c>
     </row>
   </sheetData>
@@ -66279,8 +66278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E323C290-C88C-4E5C-B55A-017ED14783D9}">
   <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
committing in case i made changes to ind_study_region_matrix without previously committing
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4CB5A3-824D-4FE3-9FA3-0E48C0260AB0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0301E5EA-7D64-4193-AAF1-D2C5F615032A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="4" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="6" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3349" uniqueCount="1479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3349" uniqueCount="1480">
   <si>
     <t>Domain</t>
   </si>
@@ -4572,6 +4572,9 @@
   </si>
   <si>
     <t>alcohol outlet (onlicence)</t>
+  </si>
+  <si>
+    <t>CH</t>
   </si>
 </sst>
 </file>
@@ -60010,7 +60013,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62204,8 +62207,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB9F8A8-BF9D-4E84-929F-4B49CA2CC7BE}">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62283,7 +62287,7 @@
         <v>20170704</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>1403</v>
+        <v>1479</v>
       </c>
       <c r="J2" s="64" t="s">
         <v>1451</v>
@@ -62318,7 +62322,7 @@
         <v>20170704</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>1403</v>
+        <v>1479</v>
       </c>
       <c r="J3" s="64" t="s">
         <v>1452</v>
@@ -62350,7 +62354,7 @@
         <v>20170704</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>1403</v>
+        <v>1479</v>
       </c>
       <c r="J4" s="64" t="s">
         <v>1453</v>
@@ -62466,7 +62470,7 @@
         <v>20181001</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>1403</v>
+        <v>1479</v>
       </c>
       <c r="J13" s="64" t="s">
         <v>1402</v>
@@ -63551,8 +63555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F76923-BFD4-452D-9FF1-F8A040A2A833}">
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64317,8 +64321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C271BA-CB23-45E6-8B41-63042B9AE792}">
   <dimension ref="A1:K111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -66279,8 +66283,8 @@
   <dimension ref="A1:F87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A21:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
filled in cutoff and count distances for destinations which didn't have these in the ind_study_region_matrix
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0301E5EA-7D64-4193-AAF1-D2C5F615032A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B75B0D-6AB4-4A12-B2B4-D7308E6C17C7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="6" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="7" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -5382,6 +5382,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -5399,21 +5414,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9565,46 +9565,46 @@
       <c r="D1" s="109" t="s">
         <v>1114</v>
       </c>
-      <c r="E1" s="125" t="s">
+      <c r="E1" s="130" t="s">
         <v>441</v>
       </c>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125" t="s">
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130" t="s">
         <v>462</v>
       </c>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125" t="s">
+      <c r="I1" s="130"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="130" t="s">
         <v>444</v>
       </c>
-      <c r="L1" s="125"/>
-      <c r="M1" s="125"/>
-      <c r="N1" s="125" t="s">
+      <c r="L1" s="130"/>
+      <c r="M1" s="130"/>
+      <c r="N1" s="130" t="s">
         <v>1115</v>
       </c>
-      <c r="O1" s="125"/>
-      <c r="P1" s="125"/>
-      <c r="Q1" s="125" t="s">
+      <c r="O1" s="130"/>
+      <c r="P1" s="130"/>
+      <c r="Q1" s="130" t="s">
         <v>436</v>
       </c>
-      <c r="R1" s="125"/>
-      <c r="S1" s="125"/>
-      <c r="T1" s="125" t="s">
+      <c r="R1" s="130"/>
+      <c r="S1" s="130"/>
+      <c r="T1" s="130" t="s">
         <v>431</v>
       </c>
-      <c r="U1" s="125"/>
-      <c r="V1" s="125"/>
-      <c r="W1" s="125" t="s">
+      <c r="U1" s="130"/>
+      <c r="V1" s="130"/>
+      <c r="W1" s="130" t="s">
         <v>1116</v>
       </c>
-      <c r="X1" s="125"/>
-      <c r="Y1" s="125"/>
-      <c r="Z1" s="125" t="s">
+      <c r="X1" s="130"/>
+      <c r="Y1" s="130"/>
+      <c r="Z1" s="130" t="s">
         <v>457</v>
       </c>
-      <c r="AA1" s="125"/>
-      <c r="AB1" s="125"/>
+      <c r="AA1" s="130"/>
+      <c r="AB1" s="130"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="37"/>
@@ -62227,37 +62227,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="122" t="s">
         <v>1442</v>
       </c>
-      <c r="B1" s="126" t="s">
+      <c r="B1" s="120" t="s">
         <v>1433</v>
       </c>
-      <c r="C1" s="126" t="s">
+      <c r="C1" s="120" t="s">
         <v>1434</v>
       </c>
-      <c r="D1" s="126" t="s">
+      <c r="D1" s="120" t="s">
         <v>1429</v>
       </c>
-      <c r="E1" s="128" t="s">
+      <c r="E1" s="122" t="s">
         <v>1437</v>
       </c>
-      <c r="F1" s="127" t="s">
+      <c r="F1" s="121" t="s">
         <v>1401</v>
       </c>
-      <c r="G1" s="127" t="s">
+      <c r="G1" s="121" t="s">
         <v>1114</v>
       </c>
-      <c r="H1" s="126" t="s">
+      <c r="H1" s="120" t="s">
         <v>1430</v>
       </c>
-      <c r="I1" s="126" t="s">
+      <c r="I1" s="120" t="s">
         <v>1431</v>
       </c>
-      <c r="J1" s="128" t="s">
+      <c r="J1" s="122" t="s">
         <v>1118</v>
       </c>
-      <c r="K1" s="128" t="s">
+      <c r="K1" s="122" t="s">
         <v>1432</v>
       </c>
     </row>
@@ -62277,10 +62277,10 @@
       <c r="E2" s="64" t="s">
         <v>1441</v>
       </c>
-      <c r="F2" s="129" t="s">
+      <c r="F2" s="123" t="s">
         <v>1450</v>
       </c>
-      <c r="G2" s="130" t="s">
+      <c r="G2" s="124" t="s">
         <v>1445</v>
       </c>
       <c r="H2" s="21">
@@ -62312,10 +62312,10 @@
       <c r="E3" s="64" t="s">
         <v>1441</v>
       </c>
-      <c r="F3" s="129" t="s">
+      <c r="F3" s="123" t="s">
         <v>1450</v>
       </c>
-      <c r="G3" s="130" t="s">
+      <c r="G3" s="124" t="s">
         <v>1448</v>
       </c>
       <c r="H3" s="21">
@@ -62344,10 +62344,10 @@
       <c r="E4" s="64" t="s">
         <v>1441</v>
       </c>
-      <c r="F4" s="129" t="s">
+      <c r="F4" s="123" t="s">
         <v>1450</v>
       </c>
-      <c r="G4" s="130" t="s">
+      <c r="G4" s="124" t="s">
         <v>1449</v>
       </c>
       <c r="H4" s="21">
@@ -62376,8 +62376,8 @@
       <c r="D5" s="21">
         <v>2016</v>
       </c>
-      <c r="F5" s="129"/>
-      <c r="G5" s="130"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="124"/>
       <c r="K5" s="64" t="s">
         <v>1458</v>
       </c>
@@ -62395,8 +62395,8 @@
       <c r="D6" s="21">
         <v>2016</v>
       </c>
-      <c r="F6" s="129"/>
-      <c r="G6" s="130"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="124"/>
       <c r="K6" s="64" t="s">
         <v>1459</v>
       </c>
@@ -62414,43 +62414,43 @@
       <c r="E7" s="64" t="s">
         <v>1441</v>
       </c>
-      <c r="F7" s="129"/>
-      <c r="G7" s="129"/>
+      <c r="F7" s="123"/>
+      <c r="G7" s="123"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="64" t="s">
         <v>1441</v>
       </c>
-      <c r="F8" s="129"/>
-      <c r="G8" s="129"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="123"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="64" t="s">
         <v>1441</v>
       </c>
-      <c r="F9" s="129"/>
-      <c r="G9" s="129"/>
+      <c r="F9" s="123"/>
+      <c r="G9" s="123"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="64" t="s">
         <v>1441</v>
       </c>
-      <c r="F10" s="129"/>
-      <c r="G10" s="129"/>
+      <c r="F10" s="123"/>
+      <c r="G10" s="123"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="64" t="s">
         <v>1441</v>
       </c>
-      <c r="F11" s="129"/>
-      <c r="G11" s="129"/>
+      <c r="F11" s="123"/>
+      <c r="G11" s="123"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="64" t="s">
         <v>1441</v>
       </c>
-      <c r="F12" s="129"/>
-      <c r="G12" s="129"/>
+      <c r="F12" s="123"/>
+      <c r="G12" s="123"/>
     </row>
     <row r="13" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A13" s="64" t="s">
@@ -62462,10 +62462,10 @@
       <c r="E13" s="64" t="s">
         <v>1438</v>
       </c>
-      <c r="F13" s="129" t="s">
+      <c r="F13" s="123" t="s">
         <v>1400</v>
       </c>
-      <c r="G13" s="129"/>
+      <c r="G13" s="123"/>
       <c r="H13" s="21">
         <v>20181001</v>
       </c>
@@ -62932,8 +62932,8 @@
       <c r="D69" s="21">
         <v>2018</v>
       </c>
-      <c r="F69" s="129"/>
-      <c r="G69" s="129"/>
+      <c r="F69" s="123"/>
+      <c r="G69" s="123"/>
       <c r="I69" s="21" t="s">
         <v>1403</v>
       </c>
@@ -62951,8 +62951,8 @@
       <c r="D70" s="21">
         <v>2018</v>
       </c>
-      <c r="F70" s="129"/>
-      <c r="G70" s="129"/>
+      <c r="F70" s="123"/>
+      <c r="G70" s="123"/>
       <c r="I70" s="21" t="s">
         <v>1403</v>
       </c>
@@ -62970,8 +62970,8 @@
       <c r="D71" s="21">
         <v>2018</v>
       </c>
-      <c r="F71" s="129"/>
-      <c r="G71" s="129"/>
+      <c r="F71" s="123"/>
+      <c r="G71" s="123"/>
       <c r="I71" s="21" t="s">
         <v>1403</v>
       </c>
@@ -62989,8 +62989,8 @@
       <c r="D72" s="21">
         <v>2018</v>
       </c>
-      <c r="F72" s="129"/>
-      <c r="G72" s="129"/>
+      <c r="F72" s="123"/>
+      <c r="G72" s="123"/>
       <c r="I72" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63008,8 +63008,8 @@
       <c r="D73" s="21">
         <v>2018</v>
       </c>
-      <c r="F73" s="129"/>
-      <c r="G73" s="129"/>
+      <c r="F73" s="123"/>
+      <c r="G73" s="123"/>
       <c r="I73" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63027,8 +63027,8 @@
       <c r="D74" s="21">
         <v>2018</v>
       </c>
-      <c r="F74" s="129"/>
-      <c r="G74" s="129"/>
+      <c r="F74" s="123"/>
+      <c r="G74" s="123"/>
       <c r="I74" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63046,8 +63046,8 @@
       <c r="D75" s="21">
         <v>2018</v>
       </c>
-      <c r="F75" s="129"/>
-      <c r="G75" s="129"/>
+      <c r="F75" s="123"/>
+      <c r="G75" s="123"/>
       <c r="I75" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63065,8 +63065,8 @@
       <c r="D76" s="21">
         <v>2018</v>
       </c>
-      <c r="F76" s="129"/>
-      <c r="G76" s="129"/>
+      <c r="F76" s="123"/>
+      <c r="G76" s="123"/>
       <c r="I76" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63084,8 +63084,8 @@
       <c r="D77" s="21">
         <v>2018</v>
       </c>
-      <c r="F77" s="129"/>
-      <c r="G77" s="129"/>
+      <c r="F77" s="123"/>
+      <c r="G77" s="123"/>
       <c r="I77" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63103,8 +63103,8 @@
       <c r="D78" s="21">
         <v>2018</v>
       </c>
-      <c r="F78" s="129"/>
-      <c r="G78" s="129"/>
+      <c r="F78" s="123"/>
+      <c r="G78" s="123"/>
       <c r="I78" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63122,8 +63122,8 @@
       <c r="D79" s="21">
         <v>2018</v>
       </c>
-      <c r="F79" s="129"/>
-      <c r="G79" s="129"/>
+      <c r="F79" s="123"/>
+      <c r="G79" s="123"/>
       <c r="I79" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63141,8 +63141,8 @@
       <c r="D80" s="21">
         <v>2018</v>
       </c>
-      <c r="F80" s="129"/>
-      <c r="G80" s="129"/>
+      <c r="F80" s="123"/>
+      <c r="G80" s="123"/>
       <c r="I80" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63160,8 +63160,8 @@
       <c r="D81" s="21">
         <v>2018</v>
       </c>
-      <c r="F81" s="129"/>
-      <c r="G81" s="129"/>
+      <c r="F81" s="123"/>
+      <c r="G81" s="123"/>
       <c r="I81" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63179,8 +63179,8 @@
       <c r="D82" s="21">
         <v>2018</v>
       </c>
-      <c r="F82" s="129"/>
-      <c r="G82" s="129"/>
+      <c r="F82" s="123"/>
+      <c r="G82" s="123"/>
       <c r="I82" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63198,8 +63198,8 @@
       <c r="D83" s="21">
         <v>2018</v>
       </c>
-      <c r="F83" s="129"/>
-      <c r="G83" s="129"/>
+      <c r="F83" s="123"/>
+      <c r="G83" s="123"/>
       <c r="I83" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63217,8 +63217,8 @@
       <c r="D84" s="21">
         <v>2018</v>
       </c>
-      <c r="F84" s="129"/>
-      <c r="G84" s="129"/>
+      <c r="F84" s="123"/>
+      <c r="G84" s="123"/>
       <c r="I84" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63236,8 +63236,8 @@
       <c r="D85" s="21">
         <v>2018</v>
       </c>
-      <c r="F85" s="129"/>
-      <c r="G85" s="129"/>
+      <c r="F85" s="123"/>
+      <c r="G85" s="123"/>
       <c r="I85" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63255,8 +63255,8 @@
       <c r="D86" s="21">
         <v>2018</v>
       </c>
-      <c r="F86" s="129"/>
-      <c r="G86" s="129"/>
+      <c r="F86" s="123"/>
+      <c r="G86" s="123"/>
       <c r="I86" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63274,8 +63274,8 @@
       <c r="D87" s="21">
         <v>2018</v>
       </c>
-      <c r="F87" s="129"/>
-      <c r="G87" s="129"/>
+      <c r="F87" s="123"/>
+      <c r="G87" s="123"/>
       <c r="I87" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63293,8 +63293,8 @@
       <c r="D88" s="21">
         <v>2018</v>
       </c>
-      <c r="F88" s="129"/>
-      <c r="G88" s="129"/>
+      <c r="F88" s="123"/>
+      <c r="G88" s="123"/>
       <c r="I88" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63312,8 +63312,8 @@
       <c r="D89" s="21">
         <v>2018</v>
       </c>
-      <c r="F89" s="129"/>
-      <c r="G89" s="129"/>
+      <c r="F89" s="123"/>
+      <c r="G89" s="123"/>
       <c r="I89" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63331,8 +63331,8 @@
       <c r="D90" s="21">
         <v>2018</v>
       </c>
-      <c r="F90" s="129"/>
-      <c r="G90" s="129"/>
+      <c r="F90" s="123"/>
+      <c r="G90" s="123"/>
       <c r="I90" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63350,8 +63350,8 @@
       <c r="D91" s="21">
         <v>2018</v>
       </c>
-      <c r="F91" s="129"/>
-      <c r="G91" s="129"/>
+      <c r="F91" s="123"/>
+      <c r="G91" s="123"/>
       <c r="I91" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63369,8 +63369,8 @@
       <c r="D92" s="21">
         <v>2018</v>
       </c>
-      <c r="F92" s="129"/>
-      <c r="G92" s="129"/>
+      <c r="F92" s="123"/>
+      <c r="G92" s="123"/>
       <c r="I92" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63388,8 +63388,8 @@
       <c r="D93" s="21">
         <v>2018</v>
       </c>
-      <c r="F93" s="129"/>
-      <c r="G93" s="129"/>
+      <c r="F93" s="123"/>
+      <c r="G93" s="123"/>
       <c r="I93" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63407,8 +63407,8 @@
       <c r="D94" s="21">
         <v>2018</v>
       </c>
-      <c r="F94" s="129"/>
-      <c r="G94" s="129"/>
+      <c r="F94" s="123"/>
+      <c r="G94" s="123"/>
       <c r="I94" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63426,8 +63426,8 @@
       <c r="D95" s="21">
         <v>2018</v>
       </c>
-      <c r="F95" s="129"/>
-      <c r="G95" s="129"/>
+      <c r="F95" s="123"/>
+      <c r="G95" s="123"/>
       <c r="I95" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63445,8 +63445,8 @@
       <c r="D96" s="21">
         <v>2018</v>
       </c>
-      <c r="F96" s="129"/>
-      <c r="G96" s="129"/>
+      <c r="F96" s="123"/>
+      <c r="G96" s="123"/>
       <c r="I96" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63464,8 +63464,8 @@
       <c r="D97" s="21">
         <v>2018</v>
       </c>
-      <c r="F97" s="129"/>
-      <c r="G97" s="129"/>
+      <c r="F97" s="123"/>
+      <c r="G97" s="123"/>
       <c r="I97" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63483,8 +63483,8 @@
       <c r="D98" s="21">
         <v>2018</v>
       </c>
-      <c r="F98" s="129"/>
-      <c r="G98" s="129"/>
+      <c r="F98" s="123"/>
+      <c r="G98" s="123"/>
       <c r="I98" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63502,8 +63502,8 @@
       <c r="D99" s="21">
         <v>2018</v>
       </c>
-      <c r="F99" s="129"/>
-      <c r="G99" s="129"/>
+      <c r="F99" s="123"/>
+      <c r="G99" s="123"/>
       <c r="I99" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63521,8 +63521,8 @@
       <c r="D100" s="21">
         <v>2018</v>
       </c>
-      <c r="F100" s="129"/>
-      <c r="G100" s="129"/>
+      <c r="F100" s="123"/>
+      <c r="G100" s="123"/>
       <c r="I100" s="21" t="s">
         <v>1403</v>
       </c>
@@ -63540,8 +63540,8 @@
       <c r="D101" s="21">
         <v>2018</v>
       </c>
-      <c r="F101" s="129"/>
-      <c r="G101" s="129"/>
+      <c r="F101" s="123"/>
+      <c r="G101" s="123"/>
       <c r="I101" s="21" t="s">
         <v>1403</v>
       </c>
@@ -64321,7 +64321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C271BA-CB23-45E6-8B41-63042B9AE792}">
   <dimension ref="A1:K111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
@@ -66282,9 +66282,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E323C290-C88C-4E5C-B55A-017ED14783D9}">
   <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A21:C25"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -67446,7 +67446,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f t="shared" si="0"/>
         <v>theatre_osm</v>
@@ -67467,7 +67467,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f t="shared" si="0"/>
         <v>cinema_osm</v>
@@ -67488,7 +67488,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f t="shared" si="0"/>
         <v>art gallery_osm</v>
@@ -67509,7 +67509,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f t="shared" si="0"/>
         <v>art centre_osm</v>
@@ -67530,7 +67530,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f t="shared" si="0"/>
         <v>artwork_osm</v>
@@ -67551,7 +67551,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f t="shared" si="0"/>
         <v>fountain_osm</v>
@@ -67572,7 +67572,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
         <f t="shared" si="0"/>
         <v>viewpoint_osm</v>
@@ -67593,7 +67593,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f t="shared" si="0"/>
         <v>picnic site_osm</v>
@@ -67614,7 +67614,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f t="shared" si="0"/>
         <v>pharmacy_osm</v>
@@ -67635,7 +67635,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f t="shared" si="0"/>
         <v>restaurant_osm</v>
@@ -67651,8 +67651,11 @@
         <f>INDEX(osm_dest_definitions!G:G,MATCH(destinations!$B74,osm_dest_definitions!$A:$A,0))</f>
         <v>Food; Community, Culture and Leisure</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E74">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f t="shared" si="0"/>
         <v>cafe_osm</v>
@@ -67668,8 +67671,11 @@
         <f>INDEX(osm_dest_definitions!G:G,MATCH(destinations!$B75,osm_dest_definitions!$A:$A,0))</f>
         <v>Food; Community, Culture and Leisure</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E75">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f t="shared" si="0"/>
         <v>eatery_osm</v>
@@ -67685,8 +67691,11 @@
         <f>INDEX(osm_dest_definitions!G:G,MATCH(destinations!$B76,osm_dest_definitions!$A:$A,0))</f>
         <v>Food; Community, Culture and Leisure</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f t="shared" si="0"/>
         <v>food_court_osm</v>
@@ -67702,8 +67711,11 @@
         <f>INDEX(osm_dest_definitions!G:G,MATCH(destinations!$B77,osm_dest_definitions!$A:$A,0))</f>
         <v>Food; Community, Culture and Leisure</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
         <f t="shared" si="0"/>
         <v>fast food_osm</v>
@@ -67719,8 +67731,11 @@
         <f>INDEX(osm_dest_definitions!G:G,MATCH(destinations!$B78,osm_dest_definitions!$A:$A,0))</f>
         <v>Food</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E78">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
         <f t="shared" si="0"/>
         <v>pub_osm</v>
@@ -67736,8 +67751,14 @@
         <f>INDEX(osm_dest_definitions!G:G,MATCH(destinations!$B79,osm_dest_definitions!$A:$A,0))</f>
         <v>Food; Community, Culture and Leisure</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E79">
+        <v>3200</v>
+      </c>
+      <c r="F79">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
         <f t="shared" si="0"/>
         <v>bar_osm</v>
@@ -67753,8 +67774,14 @@
         <f>INDEX(osm_dest_definitions!G:G,MATCH(destinations!$B80,osm_dest_definitions!$A:$A,0))</f>
         <v>Alcohol; Community, Culture and Leisure</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <v>3200</v>
+      </c>
+      <c r="F80">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
         <f t="shared" si="0"/>
         <v>nightclub_osm</v>
@@ -67770,8 +67797,14 @@
         <f>INDEX(osm_dest_definitions!G:G,MATCH(destinations!$B81,osm_dest_definitions!$A:$A,0))</f>
         <v>Alcohol; Community, Culture and Leisure</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <v>3200</v>
+      </c>
+      <c r="F81">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
         <f t="shared" si="0"/>
         <v>gambling_osm</v>
@@ -67787,8 +67820,14 @@
         <f>INDEX(osm_dest_definitions!G:G,MATCH(destinations!$B82,osm_dest_definitions!$A:$A,0))</f>
         <v>Gambling</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82">
+        <v>3200</v>
+      </c>
+      <c r="F82">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>1418</v>
       </c>
@@ -67801,8 +67840,11 @@
       <c r="D83" t="s">
         <v>1428</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>1419</v>
       </c>
@@ -67815,8 +67857,11 @@
       <c r="D84" t="s">
         <v>1428</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>1420</v>
       </c>
@@ -67829,8 +67874,11 @@
       <c r="D85" t="s">
         <v>1428</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>1421</v>
       </c>
@@ -67843,8 +67891,11 @@
       <c r="D86" t="s">
         <v>1428</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>1422</v>
       </c>
@@ -67856,6 +67907,9 @@
       </c>
       <c r="D87" t="s">
         <v>1428</v>
+      </c>
+      <c r="E87">
+        <v>1600</v>
       </c>
     </row>
   </sheetData>
@@ -67903,31 +67957,31 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="120" t="s">
+      <c r="G1" s="125" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="121"/>
-      <c r="I1" s="121"/>
-      <c r="J1" s="121"/>
-      <c r="K1" s="121"/>
-      <c r="L1" s="121"/>
-      <c r="M1" s="121"/>
-      <c r="N1" s="121"/>
-      <c r="O1" s="121"/>
-      <c r="P1" s="121"/>
-      <c r="Q1" s="121"/>
-      <c r="R1" s="121"/>
-      <c r="S1" s="121"/>
-      <c r="T1" s="121"/>
-      <c r="U1" s="121"/>
-      <c r="V1" s="121"/>
-      <c r="W1" s="121"/>
-      <c r="X1" s="122"/>
-      <c r="Y1" s="123" t="s">
+      <c r="H1" s="126"/>
+      <c r="I1" s="126"/>
+      <c r="J1" s="126"/>
+      <c r="K1" s="126"/>
+      <c r="L1" s="126"/>
+      <c r="M1" s="126"/>
+      <c r="N1" s="126"/>
+      <c r="O1" s="126"/>
+      <c r="P1" s="126"/>
+      <c r="Q1" s="126"/>
+      <c r="R1" s="126"/>
+      <c r="S1" s="126"/>
+      <c r="T1" s="126"/>
+      <c r="U1" s="126"/>
+      <c r="V1" s="126"/>
+      <c r="W1" s="126"/>
+      <c r="X1" s="127"/>
+      <c r="Y1" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="Z1" s="121"/>
-      <c r="AA1" s="124"/>
+      <c r="Z1" s="126"/>
+      <c r="AA1" s="129"/>
       <c r="AB1" s="2" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
updated the ind study region matrix file with library details
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302F7E9A-802B-491C-B5A7-6FC142AAF8B7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F800517F-9A3B-463D-9AE7-7E167577FB4A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" firstSheet="3" activeTab="4" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3696" uniqueCount="1525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3715" uniqueCount="1540">
   <si>
     <t>Domain</t>
   </si>
@@ -4688,6 +4688,9 @@
     <t xml:space="preserve">	Libraries ACT</t>
   </si>
   <si>
+    <t>Libraries SA</t>
+  </si>
+  <si>
     <t>State Libraries of NSW</t>
   </si>
   <si>
@@ -4719,7 +4722,52 @@
     <t>Z:/RESEARCH/GIS/Projects/ntnl_li_2018_template/data/destinations/libraries/libraries_australia_20181119.gpkg</t>
   </si>
   <si>
-    <t>I compiled a database of libraries around Australia based on official sources for each state using the most recent data which was accessible.  Where data was not publicly available, or recent, contact was made to request the data.</t>
+    <t>Received upon inquiry on 20160301.</t>
+  </si>
+  <si>
+    <t>Libraries Tasmania</t>
+  </si>
+  <si>
+    <t>Libraries Tasmania, Archives &amp; Online Access Centre (OAC) locations by name, address, latitude and longitude</t>
+  </si>
+  <si>
+    <t>CC BY 3.0 AU</t>
+  </si>
+  <si>
+    <t>public listing</t>
+  </si>
+  <si>
+    <t>public listing ("fair use for the purpose of … research")</t>
+  </si>
+  <si>
+    <t>State Library of Queensland</t>
+  </si>
+  <si>
+    <t>Department of Premier and Cabinet</t>
+  </si>
+  <si>
+    <t>State Library of Western Australia</t>
+  </si>
+  <si>
+    <t>not stated</t>
+  </si>
+  <si>
+    <t>"Western Australia public library branch names, locations and phone numbers.  New for 2016: now includes Map references (lat/long and elevation)."</t>
+  </si>
+  <si>
+    <t>Locations of Public Libraries in Victoria (2010, updated 2016)</t>
+  </si>
+  <si>
+    <t>Locations of Public Libraries in Tasmania (updated 2018).  QGIS was used to output the geojson as CSV with added latitude and longitude (YX) coordinates. The geojson specific fields were removed to retain the following fields: library, address, y, x</t>
+  </si>
+  <si>
+    <t>I compiled a database of libraries around Australia based on official sources for each state using the most recent data which was accessible.  Where data was not publicly available, or recent, contact was made to request the data.  The geopackage contains two national feature datasets, one in EPSG 4326 (as per the data source files) and another in EPSG 7845 GDA 2020 GA LCC (as per our project requirements).</t>
+  </si>
+  <si>
+    <t>"Location information about Queensland Public libraries, including addresses and geotags" (March 2018).
+Ifracrombe public library had an error with incorrect coordinate polarity which was cleaned as per the following:
+incorrect: 23.489799	 144.507568
+cleaned:  -23.489799	 144.507568</t>
   </si>
 </sst>
 </file>
@@ -5207,7 +5255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -5578,7 +5626,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -63649,8 +63702,8 @@
   <dimension ref="A1:K110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K104" sqref="K104"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J110" sqref="J110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63658,9 +63711,10 @@
     <col min="1" max="1" width="32.85546875" style="64" customWidth="1"/>
     <col min="2" max="2" width="19" style="21" customWidth="1"/>
     <col min="3" max="3" width="31.28515625" style="21" customWidth="1"/>
-    <col min="4" max="4" width="19" style="21" customWidth="1"/>
+    <col min="4" max="4" width="8" style="21" customWidth="1"/>
     <col min="5" max="5" width="19" style="64" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="21"/>
+    <col min="6" max="6" width="15.140625" style="64" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="21"/>
     <col min="8" max="9" width="19" style="21" customWidth="1"/>
     <col min="10" max="10" width="25" style="64" customWidth="1"/>
     <col min="11" max="11" width="72.85546875" style="64" customWidth="1"/>
@@ -63683,7 +63737,7 @@
       <c r="E1" s="119" t="s">
         <v>1420</v>
       </c>
-      <c r="F1" s="118" t="s">
+      <c r="F1" s="140" t="s">
         <v>1384</v>
       </c>
       <c r="G1" s="118" t="s">
@@ -63718,7 +63772,7 @@
       <c r="E2" s="64" t="s">
         <v>1424</v>
       </c>
-      <c r="F2" s="120" t="s">
+      <c r="F2" s="141" t="s">
         <v>1433</v>
       </c>
       <c r="G2" s="121" t="s">
@@ -63753,7 +63807,7 @@
       <c r="E3" s="64" t="s">
         <v>1424</v>
       </c>
-      <c r="F3" s="120" t="s">
+      <c r="F3" s="141" t="s">
         <v>1433</v>
       </c>
       <c r="G3" s="121" t="s">
@@ -63785,7 +63839,7 @@
       <c r="E4" s="64" t="s">
         <v>1424</v>
       </c>
-      <c r="F4" s="120" t="s">
+      <c r="F4" s="141" t="s">
         <v>1433</v>
       </c>
       <c r="G4" s="121" t="s">
@@ -63817,7 +63871,7 @@
       <c r="D5" s="21">
         <v>2016</v>
       </c>
-      <c r="F5" s="120"/>
+      <c r="F5" s="141"/>
       <c r="G5" s="121"/>
       <c r="K5" s="64" t="s">
         <v>1441</v>
@@ -63836,7 +63890,7 @@
       <c r="D6" s="21">
         <v>2016</v>
       </c>
-      <c r="F6" s="120"/>
+      <c r="F6" s="141"/>
       <c r="G6" s="121"/>
       <c r="K6" s="64" t="s">
         <v>1442</v>
@@ -63855,42 +63909,42 @@
       <c r="E7" s="64" t="s">
         <v>1424</v>
       </c>
-      <c r="F7" s="120"/>
+      <c r="F7" s="141"/>
       <c r="G7" s="120"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="64" t="s">
         <v>1424</v>
       </c>
-      <c r="F8" s="120"/>
+      <c r="F8" s="141"/>
       <c r="G8" s="120"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="64" t="s">
         <v>1424</v>
       </c>
-      <c r="F9" s="120"/>
+      <c r="F9" s="141"/>
       <c r="G9" s="120"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="64" t="s">
         <v>1424</v>
       </c>
-      <c r="F10" s="120"/>
+      <c r="F10" s="141"/>
       <c r="G10" s="120"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="64" t="s">
         <v>1424</v>
       </c>
-      <c r="F11" s="120"/>
+      <c r="F11" s="141"/>
       <c r="G11" s="120"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="64" t="s">
         <v>1424</v>
       </c>
-      <c r="F12" s="120"/>
+      <c r="F12" s="141"/>
       <c r="G12" s="120"/>
     </row>
     <row r="13" spans="1:11" ht="165" x14ac:dyDescent="0.25">
@@ -63903,7 +63957,7 @@
       <c r="E13" s="64" t="s">
         <v>1421</v>
       </c>
-      <c r="F13" s="120" t="s">
+      <c r="F13" s="141" t="s">
         <v>1383</v>
       </c>
       <c r="G13" s="120"/>
@@ -64373,7 +64427,7 @@
       <c r="D69" s="21">
         <v>2018</v>
       </c>
-      <c r="F69" s="120"/>
+      <c r="F69" s="141"/>
       <c r="G69" s="120"/>
       <c r="I69" s="21" t="s">
         <v>1386</v>
@@ -64392,7 +64446,7 @@
       <c r="D70" s="21">
         <v>2018</v>
       </c>
-      <c r="F70" s="120"/>
+      <c r="F70" s="141"/>
       <c r="G70" s="120"/>
       <c r="I70" s="21" t="s">
         <v>1386</v>
@@ -64411,7 +64465,7 @@
       <c r="D71" s="21">
         <v>2018</v>
       </c>
-      <c r="F71" s="120"/>
+      <c r="F71" s="141"/>
       <c r="G71" s="120"/>
       <c r="I71" s="21" t="s">
         <v>1386</v>
@@ -64430,7 +64484,7 @@
       <c r="D72" s="21">
         <v>2018</v>
       </c>
-      <c r="F72" s="120"/>
+      <c r="F72" s="141"/>
       <c r="G72" s="120"/>
       <c r="I72" s="21" t="s">
         <v>1386</v>
@@ -64449,7 +64503,7 @@
       <c r="D73" s="21">
         <v>2018</v>
       </c>
-      <c r="F73" s="120"/>
+      <c r="F73" s="141"/>
       <c r="G73" s="120"/>
       <c r="I73" s="21" t="s">
         <v>1386</v>
@@ -64468,7 +64522,7 @@
       <c r="D74" s="21">
         <v>2018</v>
       </c>
-      <c r="F74" s="120"/>
+      <c r="F74" s="141"/>
       <c r="G74" s="120"/>
       <c r="I74" s="21" t="s">
         <v>1386</v>
@@ -64487,7 +64541,7 @@
       <c r="D75" s="21">
         <v>2018</v>
       </c>
-      <c r="F75" s="120"/>
+      <c r="F75" s="141"/>
       <c r="G75" s="120"/>
       <c r="I75" s="21" t="s">
         <v>1386</v>
@@ -64506,7 +64560,7 @@
       <c r="D76" s="21">
         <v>2018</v>
       </c>
-      <c r="F76" s="120"/>
+      <c r="F76" s="141"/>
       <c r="G76" s="120"/>
       <c r="I76" s="21" t="s">
         <v>1386</v>
@@ -64525,7 +64579,7 @@
       <c r="D77" s="21">
         <v>2018</v>
       </c>
-      <c r="F77" s="120"/>
+      <c r="F77" s="141"/>
       <c r="G77" s="120"/>
       <c r="I77" s="21" t="s">
         <v>1386</v>
@@ -64544,7 +64598,7 @@
       <c r="D78" s="21">
         <v>2018</v>
       </c>
-      <c r="F78" s="120"/>
+      <c r="F78" s="141"/>
       <c r="G78" s="120"/>
       <c r="I78" s="21" t="s">
         <v>1386</v>
@@ -64563,7 +64617,7 @@
       <c r="D79" s="21">
         <v>2018</v>
       </c>
-      <c r="F79" s="120"/>
+      <c r="F79" s="141"/>
       <c r="G79" s="120"/>
       <c r="I79" s="21" t="s">
         <v>1386</v>
@@ -64582,7 +64636,7 @@
       <c r="D80" s="21">
         <v>2018</v>
       </c>
-      <c r="F80" s="120"/>
+      <c r="F80" s="141"/>
       <c r="G80" s="120"/>
       <c r="I80" s="21" t="s">
         <v>1386</v>
@@ -64601,7 +64655,7 @@
       <c r="D81" s="21">
         <v>2018</v>
       </c>
-      <c r="F81" s="120"/>
+      <c r="F81" s="141"/>
       <c r="G81" s="120"/>
       <c r="I81" s="21" t="s">
         <v>1386</v>
@@ -64620,7 +64674,7 @@
       <c r="D82" s="21">
         <v>2018</v>
       </c>
-      <c r="F82" s="120"/>
+      <c r="F82" s="141"/>
       <c r="G82" s="120"/>
       <c r="I82" s="21" t="s">
         <v>1386</v>
@@ -64639,7 +64693,7 @@
       <c r="D83" s="21">
         <v>2018</v>
       </c>
-      <c r="F83" s="120"/>
+      <c r="F83" s="141"/>
       <c r="G83" s="120"/>
       <c r="I83" s="21" t="s">
         <v>1386</v>
@@ -64658,7 +64712,7 @@
       <c r="D84" s="21">
         <v>2018</v>
       </c>
-      <c r="F84" s="120"/>
+      <c r="F84" s="141"/>
       <c r="G84" s="120"/>
       <c r="I84" s="21" t="s">
         <v>1386</v>
@@ -64677,7 +64731,7 @@
       <c r="D85" s="21">
         <v>2018</v>
       </c>
-      <c r="F85" s="120"/>
+      <c r="F85" s="141"/>
       <c r="G85" s="120"/>
       <c r="I85" s="21" t="s">
         <v>1386</v>
@@ -64696,7 +64750,7 @@
       <c r="D86" s="21">
         <v>2018</v>
       </c>
-      <c r="F86" s="120"/>
+      <c r="F86" s="141"/>
       <c r="G86" s="120"/>
       <c r="I86" s="21" t="s">
         <v>1386</v>
@@ -64715,7 +64769,7 @@
       <c r="D87" s="21">
         <v>2018</v>
       </c>
-      <c r="F87" s="120"/>
+      <c r="F87" s="141"/>
       <c r="G87" s="120"/>
       <c r="I87" s="21" t="s">
         <v>1386</v>
@@ -64734,7 +64788,7 @@
       <c r="D88" s="21">
         <v>2018</v>
       </c>
-      <c r="F88" s="120"/>
+      <c r="F88" s="141"/>
       <c r="G88" s="120"/>
       <c r="I88" s="21" t="s">
         <v>1386</v>
@@ -64753,7 +64807,7 @@
       <c r="D89" s="21">
         <v>2018</v>
       </c>
-      <c r="F89" s="120"/>
+      <c r="F89" s="141"/>
       <c r="G89" s="120"/>
       <c r="I89" s="21" t="s">
         <v>1386</v>
@@ -64772,7 +64826,7 @@
       <c r="D90" s="21">
         <v>2018</v>
       </c>
-      <c r="F90" s="120"/>
+      <c r="F90" s="141"/>
       <c r="G90" s="120"/>
       <c r="I90" s="21" t="s">
         <v>1386</v>
@@ -64791,7 +64845,7 @@
       <c r="D91" s="21">
         <v>2018</v>
       </c>
-      <c r="F91" s="120"/>
+      <c r="F91" s="141"/>
       <c r="G91" s="120"/>
       <c r="I91" s="21" t="s">
         <v>1386</v>
@@ -64810,7 +64864,7 @@
       <c r="D92" s="21">
         <v>2018</v>
       </c>
-      <c r="F92" s="120"/>
+      <c r="F92" s="141"/>
       <c r="G92" s="120"/>
       <c r="I92" s="21" t="s">
         <v>1386</v>
@@ -64829,7 +64883,7 @@
       <c r="D93" s="21">
         <v>2018</v>
       </c>
-      <c r="F93" s="120"/>
+      <c r="F93" s="141"/>
       <c r="G93" s="120"/>
       <c r="I93" s="21" t="s">
         <v>1386</v>
@@ -64848,7 +64902,7 @@
       <c r="D94" s="21">
         <v>2018</v>
       </c>
-      <c r="F94" s="120"/>
+      <c r="F94" s="141"/>
       <c r="G94" s="120"/>
       <c r="I94" s="21" t="s">
         <v>1386</v>
@@ -64867,7 +64921,7 @@
       <c r="D95" s="21">
         <v>2018</v>
       </c>
-      <c r="F95" s="120"/>
+      <c r="F95" s="141"/>
       <c r="G95" s="120"/>
       <c r="I95" s="21" t="s">
         <v>1386</v>
@@ -64886,7 +64940,7 @@
       <c r="D96" s="21">
         <v>2018</v>
       </c>
-      <c r="F96" s="120"/>
+      <c r="F96" s="141"/>
       <c r="G96" s="120"/>
       <c r="I96" s="21" t="s">
         <v>1386</v>
@@ -64905,7 +64959,7 @@
       <c r="D97" s="21">
         <v>2018</v>
       </c>
-      <c r="F97" s="120"/>
+      <c r="F97" s="141"/>
       <c r="G97" s="120"/>
       <c r="I97" s="21" t="s">
         <v>1386</v>
@@ -64924,7 +64978,7 @@
       <c r="D98" s="21">
         <v>2018</v>
       </c>
-      <c r="F98" s="120"/>
+      <c r="F98" s="141"/>
       <c r="G98" s="120"/>
       <c r="I98" s="21" t="s">
         <v>1386</v>
@@ -64943,7 +64997,7 @@
       <c r="D99" s="21">
         <v>2018</v>
       </c>
-      <c r="F99" s="120"/>
+      <c r="F99" s="141"/>
       <c r="G99" s="120"/>
       <c r="I99" s="21" t="s">
         <v>1386</v>
@@ -64962,7 +65016,7 @@
       <c r="D100" s="21">
         <v>2018</v>
       </c>
-      <c r="F100" s="120"/>
+      <c r="F100" s="141"/>
       <c r="G100" s="120"/>
       <c r="I100" s="21" t="s">
         <v>1386</v>
@@ -64981,15 +65035,15 @@
       <c r="D101" s="21">
         <v>2018</v>
       </c>
-      <c r="F101" s="120"/>
+      <c r="F101" s="141"/>
       <c r="G101" s="120"/>
       <c r="I101" s="21" t="s">
         <v>1386</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A102" s="64" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="B102" s="21" t="s">
         <v>657</v>
@@ -65000,15 +65054,18 @@
       <c r="D102" s="21">
         <v>2018</v>
       </c>
-      <c r="G102" s="140"/>
+      <c r="G102" s="121"/>
+      <c r="H102" s="21">
+        <v>20181119</v>
+      </c>
       <c r="I102" s="21" t="s">
         <v>1462</v>
       </c>
       <c r="J102" s="64" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="K102" s="64" t="s">
-        <v>1524</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="103" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -65027,7 +65084,10 @@
       <c r="E103" s="64" t="s">
         <v>1516</v>
       </c>
-      <c r="G103" s="140" t="s">
+      <c r="F103" s="64" t="s">
+        <v>1433</v>
+      </c>
+      <c r="G103" s="121" t="s">
         <v>1136</v>
       </c>
       <c r="H103" s="21">
@@ -65040,7 +65100,7 @@
         <v>1135</v>
       </c>
       <c r="K103" s="64" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="104" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -65057,10 +65117,13 @@
         <v>2016</v>
       </c>
       <c r="E104" s="64" t="s">
-        <v>1517</v>
+        <v>1518</v>
+      </c>
+      <c r="F104" s="64" t="s">
+        <v>1534</v>
       </c>
       <c r="G104" s="21" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="H104" s="21">
         <v>20160301</v>
@@ -65070,6 +65133,9 @@
       </c>
       <c r="J104" s="64" t="s">
         <v>1137</v>
+      </c>
+      <c r="K104" s="64" t="s">
+        <v>1525</v>
       </c>
     </row>
     <row r="105" spans="1:11" ht="360" x14ac:dyDescent="0.25">
@@ -65086,11 +65152,17 @@
         <v>2018</v>
       </c>
       <c r="E105" s="64" t="s">
-        <v>1520</v>
+        <v>1521</v>
+      </c>
+      <c r="F105" s="64" t="s">
+        <v>1530</v>
       </c>
       <c r="G105" s="21" t="s">
         <v>1160</v>
       </c>
+      <c r="H105" s="21">
+        <v>20181119</v>
+      </c>
       <c r="I105" s="21" t="s">
         <v>1462</v>
       </c>
@@ -65098,7 +65170,7 @@
         <v>1161</v>
       </c>
       <c r="K105" s="64" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="106" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -65114,14 +65186,26 @@
       <c r="D106" s="21">
         <v>2018</v>
       </c>
-      <c r="G106" s="21" t="s">
+      <c r="E106" s="64" t="s">
+        <v>1526</v>
+      </c>
+      <c r="F106" s="64" t="s">
+        <v>1433</v>
+      </c>
+      <c r="G106" s="121" t="s">
         <v>1156</v>
+      </c>
+      <c r="H106" s="21">
+        <v>20181119</v>
       </c>
       <c r="I106" s="21" t="s">
         <v>1462</v>
       </c>
       <c r="J106" s="64" t="s">
         <v>1157</v>
+      </c>
+      <c r="K106" s="64" t="s">
+        <v>1527</v>
       </c>
     </row>
     <row r="107" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -65137,14 +65221,26 @@
       <c r="D107" s="21">
         <v>2018</v>
       </c>
-      <c r="G107" s="21" t="s">
+      <c r="E107" s="64" t="s">
+        <v>1531</v>
+      </c>
+      <c r="F107" s="64" t="s">
+        <v>1528</v>
+      </c>
+      <c r="G107" s="121" t="s">
         <v>1124</v>
+      </c>
+      <c r="H107" s="21">
+        <v>20181119</v>
       </c>
       <c r="I107" s="21" t="s">
         <v>1462</v>
       </c>
       <c r="J107" s="64" t="s">
         <v>1125</v>
+      </c>
+      <c r="K107" s="64" t="s">
+        <v>1539</v>
       </c>
     </row>
     <row r="108" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -65160,14 +65256,26 @@
       <c r="D108" s="21">
         <v>2017</v>
       </c>
-      <c r="G108" s="21" t="s">
+      <c r="E108" s="64" t="s">
+        <v>1517</v>
+      </c>
+      <c r="F108" s="64" t="s">
+        <v>1529</v>
+      </c>
+      <c r="G108" s="121" t="s">
         <v>1158</v>
+      </c>
+      <c r="H108" s="21">
+        <v>20181119</v>
       </c>
       <c r="I108" s="21" t="s">
         <v>1462</v>
       </c>
       <c r="J108" s="64" t="s">
         <v>1159</v>
+      </c>
+      <c r="K108" s="64" t="s">
+        <v>1537</v>
       </c>
     </row>
     <row r="109" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -65183,14 +65291,26 @@
       <c r="D109" s="21">
         <v>2016</v>
       </c>
-      <c r="G109" s="21" t="s">
+      <c r="E109" s="64" t="s">
+        <v>1532</v>
+      </c>
+      <c r="F109" s="64" t="s">
+        <v>1433</v>
+      </c>
+      <c r="G109" s="121" t="s">
         <v>1133</v>
+      </c>
+      <c r="H109" s="21">
+        <v>20181119</v>
       </c>
       <c r="I109" s="21" t="s">
         <v>1462</v>
       </c>
       <c r="J109" s="64" t="s">
         <v>1134</v>
+      </c>
+      <c r="K109" s="64" t="s">
+        <v>1536</v>
       </c>
     </row>
     <row r="110" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -65206,14 +65326,26 @@
       <c r="D110" s="21">
         <v>2016</v>
       </c>
-      <c r="G110" s="21" t="s">
+      <c r="E110" s="64" t="s">
+        <v>1533</v>
+      </c>
+      <c r="F110" s="64" t="s">
+        <v>1528</v>
+      </c>
+      <c r="G110" s="121" t="s">
         <v>1126</v>
+      </c>
+      <c r="H110" s="21">
+        <v>20181119</v>
       </c>
       <c r="I110" s="21" t="s">
         <v>1462</v>
       </c>
       <c r="J110" s="64" t="s">
         <v>1127</v>
+      </c>
+      <c r="K110" s="64" t="s">
+        <v>1535</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved the housekeeping in recompile destinations script (ie. all destinations imported must be removed following processing; there was a mismatch in case in previous version for some destination names, so the method has been modified to ensure destinations are lower, and the full list is processed to keep our databases cleaner)
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92AAA91-CEB0-4BE6-B536-E156EB4F4D80}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE173F8-6EC3-44C8-8DD7-C5DFCE739FAE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10215" firstSheet="4" activeTab="8" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10215" firstSheet="5" activeTab="12" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -7640,8 +7640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EB87C6-56E0-4FAE-AF8A-78226C6D4F30}">
   <dimension ref="A1:A147"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B156" sqref="B156"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -66070,7 +66070,7 @@
   <dimension ref="A1:F104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
@@ -68115,7 +68115,7 @@
   </sheetPr>
   <dimension ref="A1:Q87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
fixed up bug in parcel exclusion in case of 'None' specified for island exceptions
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C86499-2B8C-4F41-B5AC-6CA79EB3B145}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C0BD4D-33DB-4FD6-8FCA-9BAF525E84DF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10215" firstSheet="2" activeTab="3" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3473" uniqueCount="1584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3478" uniqueCount="1585">
   <si>
     <t>Type</t>
   </si>
@@ -4858,6 +4858,9 @@
   </si>
   <si>
     <t>sa1_maincode IN ('50702116525')</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -59208,7 +59211,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M11" sqref="M11"/>
+      <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59312,7 +59315,7 @@
         <v>753</v>
       </c>
       <c r="M2" s="55" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="N2" s="57"/>
       <c r="O2" s="57">
@@ -59357,7 +59360,9 @@
       <c r="L3" s="55" t="s">
         <v>295</v>
       </c>
-      <c r="M3" s="55"/>
+      <c r="M3" s="55" t="s">
+        <v>1584</v>
+      </c>
       <c r="N3" s="57"/>
       <c r="O3" s="57">
         <v>0</v>
@@ -59749,7 +59754,9 @@
       <c r="L12" s="59" t="s">
         <v>748</v>
       </c>
-      <c r="M12" s="59"/>
+      <c r="M12" s="59" t="s">
+        <v>1584</v>
+      </c>
       <c r="O12" s="12">
         <v>0</v>
       </c>
@@ -59879,7 +59886,9 @@
       <c r="L15" s="62" t="s">
         <v>283</v>
       </c>
-      <c r="M15" s="62"/>
+      <c r="M15" s="62" t="s">
+        <v>1584</v>
+      </c>
       <c r="N15" s="31"/>
       <c r="O15" s="31">
         <v>0</v>
@@ -60010,7 +60019,9 @@
       <c r="L18" s="59" t="s">
         <v>285</v>
       </c>
-      <c r="M18" s="59"/>
+      <c r="M18" s="59" t="s">
+        <v>1584</v>
+      </c>
       <c r="O18" s="12">
         <v>0</v>
       </c>
@@ -60097,7 +60108,9 @@
       <c r="L20" s="59" t="s">
         <v>750</v>
       </c>
-      <c r="M20" s="59"/>
+      <c r="M20" s="59" t="s">
+        <v>1584</v>
+      </c>
       <c r="O20" s="12">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
fix melb no forwrd edges
</commit_message>
<xml_diff>
--- a/ind_study_region_matrix.xlsx
+++ b/ind_study_region_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntnl_li_2018_template\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC927DA7-7CDE-472C-87DE-DA4D3AE8AE4C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA0A6C3-70FE-4EEF-9DAE-04334D4D1C8E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10215" firstSheet="2" activeTab="8" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10215" firstSheet="2" activeTab="3" xr2:uid="{71BC767C-B39D-429D-9856-28668EC837A1}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="5" r:id="rId1"/>
@@ -5528,12 +5528,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -5545,6 +5539,12 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5950,38 +5950,38 @@
       <c r="E1" s="106" t="s">
         <v>1100</v>
       </c>
-      <c r="F1" s="117" t="s">
+      <c r="F1" s="121" t="s">
         <v>1071</v>
       </c>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="O1" s="117" t="s">
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="121"/>
+      <c r="J1" s="121"/>
+      <c r="K1" s="121"/>
+      <c r="L1" s="121"/>
+      <c r="M1" s="121"/>
+      <c r="O1" s="121" t="s">
         <v>1103</v>
       </c>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="117"/>
+      <c r="P1" s="121"/>
+      <c r="Q1" s="121"/>
+      <c r="R1" s="121"/>
       <c r="S1" s="106"/>
-      <c r="T1" s="118" t="s">
+      <c r="T1" s="122" t="s">
         <v>1104</v>
       </c>
-      <c r="U1" s="118"/>
-      <c r="V1" s="118"/>
-      <c r="W1" s="118"/>
-      <c r="X1" s="118"/>
+      <c r="U1" s="122"/>
+      <c r="V1" s="122"/>
+      <c r="W1" s="122"/>
+      <c r="X1" s="122"/>
       <c r="Y1" s="106"/>
-      <c r="Z1" s="117" t="s">
+      <c r="Z1" s="121" t="s">
         <v>1105</v>
       </c>
-      <c r="AA1" s="117"/>
-      <c r="AB1" s="117"/>
-      <c r="AC1" s="117"/>
-      <c r="AD1" s="117"/>
+      <c r="AA1" s="121"/>
+      <c r="AB1" s="121"/>
+      <c r="AC1" s="121"/>
+      <c r="AD1" s="121"/>
     </row>
     <row r="2" spans="1:30" s="102" customFormat="1" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="104"/>
@@ -59334,11 +59334,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317EB008-F691-4F16-B99A-D5845A82BBBD}">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M24" sqref="M24"/>
+      <selection pane="bottomRight" activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59713,7 +59713,7 @@
       </c>
       <c r="M8" s="59"/>
       <c r="O8" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -68074,7 +68074,7 @@
   </sheetPr>
   <dimension ref="A1:T86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -69782,25 +69782,25 @@
       <c r="E38" s="10" t="s">
         <v>1381</v>
       </c>
-      <c r="F38" s="120">
+      <c r="F38" s="118">
         <v>20190103</v>
       </c>
-      <c r="G38" s="121" t="s">
+      <c r="G38" s="119" t="s">
         <v>1460</v>
       </c>
-      <c r="H38" s="121" t="s">
+      <c r="H38" s="119" t="s">
         <v>1461</v>
       </c>
-      <c r="I38" s="121"/>
-      <c r="J38" s="121"/>
-      <c r="K38" s="121"/>
+      <c r="I38" s="119"/>
+      <c r="J38" s="119"/>
+      <c r="K38" s="119"/>
       <c r="L38" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="M38" s="121" t="s">
+      <c r="M38" s="119" t="s">
         <v>1505</v>
       </c>
-      <c r="N38" s="121" t="s">
+      <c r="N38" s="119" t="s">
         <v>1511</v>
       </c>
       <c r="O38" s="76" t="s">
@@ -69836,25 +69836,25 @@
       <c r="E39" s="10" t="s">
         <v>1381</v>
       </c>
-      <c r="F39" s="120">
+      <c r="F39" s="118">
         <v>20190103</v>
       </c>
-      <c r="G39" s="121" t="s">
+      <c r="G39" s="119" t="s">
         <v>1462</v>
       </c>
-      <c r="H39" s="121" t="s">
+      <c r="H39" s="119" t="s">
         <v>1463</v>
       </c>
-      <c r="I39" s="121"/>
-      <c r="J39" s="121"/>
-      <c r="K39" s="121"/>
+      <c r="I39" s="119"/>
+      <c r="J39" s="119"/>
+      <c r="K39" s="119"/>
       <c r="L39" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="M39" s="121" t="s">
+      <c r="M39" s="119" t="s">
         <v>1505</v>
       </c>
-      <c r="N39" s="121" t="s">
+      <c r="N39" s="119" t="s">
         <v>1513</v>
       </c>
       <c r="O39" s="76" t="s">
@@ -69890,25 +69890,25 @@
       <c r="E40" s="10" t="s">
         <v>1381</v>
       </c>
-      <c r="F40" s="120">
+      <c r="F40" s="118">
         <v>20190103</v>
       </c>
-      <c r="G40" s="121" t="s">
+      <c r="G40" s="119" t="s">
         <v>1464</v>
       </c>
-      <c r="H40" s="121" t="s">
+      <c r="H40" s="119" t="s">
         <v>1465</v>
       </c>
-      <c r="I40" s="121"/>
-      <c r="J40" s="121"/>
-      <c r="K40" s="121"/>
+      <c r="I40" s="119"/>
+      <c r="J40" s="119"/>
+      <c r="K40" s="119"/>
       <c r="L40" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="M40" s="121" t="s">
+      <c r="M40" s="119" t="s">
         <v>1505</v>
       </c>
-      <c r="N40" s="121" t="s">
+      <c r="N40" s="119" t="s">
         <v>1515</v>
       </c>
       <c r="O40" s="76" t="s">
@@ -69944,25 +69944,25 @@
       <c r="E41" s="10" t="s">
         <v>1381</v>
       </c>
-      <c r="F41" s="120">
+      <c r="F41" s="118">
         <v>20190103</v>
       </c>
-      <c r="G41" s="121" t="s">
+      <c r="G41" s="119" t="s">
         <v>1466</v>
       </c>
-      <c r="H41" s="121" t="s">
+      <c r="H41" s="119" t="s">
         <v>1467</v>
       </c>
-      <c r="I41" s="121"/>
-      <c r="J41" s="121"/>
-      <c r="K41" s="121"/>
+      <c r="I41" s="119"/>
+      <c r="J41" s="119"/>
+      <c r="K41" s="119"/>
       <c r="L41" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="M41" s="121" t="s">
+      <c r="M41" s="119" t="s">
         <v>1505</v>
       </c>
-      <c r="N41" s="121" t="s">
+      <c r="N41" s="119" t="s">
         <v>1517</v>
       </c>
       <c r="O41" s="76" t="s">
@@ -69998,25 +69998,25 @@
       <c r="E42" s="10" t="s">
         <v>1381</v>
       </c>
-      <c r="F42" s="120">
+      <c r="F42" s="118">
         <v>20190103</v>
       </c>
-      <c r="G42" s="121" t="s">
+      <c r="G42" s="119" t="s">
         <v>1468</v>
       </c>
-      <c r="H42" s="121" t="s">
+      <c r="H42" s="119" t="s">
         <v>1469</v>
       </c>
-      <c r="I42" s="121"/>
-      <c r="J42" s="121"/>
-      <c r="K42" s="121"/>
-      <c r="L42" s="121" t="s">
+      <c r="I42" s="119"/>
+      <c r="J42" s="119"/>
+      <c r="K42" s="119"/>
+      <c r="L42" s="119" t="s">
         <v>119</v>
       </c>
-      <c r="M42" s="121" t="s">
+      <c r="M42" s="119" t="s">
         <v>1505</v>
       </c>
-      <c r="N42" s="121" t="s">
+      <c r="N42" s="119" t="s">
         <v>1519</v>
       </c>
       <c r="O42" s="76" t="s">
@@ -70039,7 +70039,7 @@
       </c>
     </row>
     <row r="43" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="119" t="s">
+      <c r="A43" s="117" t="s">
         <v>66</v>
       </c>
       <c r="B43" s="3"/>
@@ -70052,25 +70052,25 @@
       <c r="E43" s="10" t="s">
         <v>1381</v>
       </c>
-      <c r="F43" s="120">
+      <c r="F43" s="118">
         <v>20190103</v>
       </c>
-      <c r="G43" s="121" t="s">
+      <c r="G43" s="119" t="s">
         <v>1470</v>
       </c>
-      <c r="H43" s="121" t="s">
+      <c r="H43" s="119" t="s">
         <v>1471</v>
       </c>
-      <c r="I43" s="121"/>
-      <c r="J43" s="121"/>
-      <c r="K43" s="121"/>
-      <c r="L43" s="121" t="s">
+      <c r="I43" s="119"/>
+      <c r="J43" s="119"/>
+      <c r="K43" s="119"/>
+      <c r="L43" s="119" t="s">
         <v>119</v>
       </c>
-      <c r="M43" s="121" t="s">
+      <c r="M43" s="119" t="s">
         <v>1505</v>
       </c>
-      <c r="N43" s="121" t="s">
+      <c r="N43" s="119" t="s">
         <v>1521</v>
       </c>
       <c r="O43" s="76" t="s">
@@ -70093,7 +70093,7 @@
       </c>
     </row>
     <row r="44" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="119" t="s">
+      <c r="A44" s="117" t="s">
         <v>67</v>
       </c>
       <c r="B44" s="3"/>
@@ -70432,10 +70432,10 @@
       <c r="M52" s="23" t="s">
         <v>1540</v>
       </c>
-      <c r="N52" s="122" t="s">
+      <c r="N52" s="120" t="s">
         <v>84</v>
       </c>
-      <c r="O52" s="121" t="s">
+      <c r="O52" s="119" t="s">
         <v>89</v>
       </c>
       <c r="P52" s="9" t="s">
@@ -70477,10 +70477,10 @@
       <c r="M53" s="23" t="s">
         <v>1387</v>
       </c>
-      <c r="N53" s="121" t="s">
+      <c r="N53" s="119" t="s">
         <v>1579</v>
       </c>
-      <c r="O53" s="121" t="s">
+      <c r="O53" s="119" t="s">
         <v>90</v>
       </c>
       <c r="P53" s="9" t="s">
@@ -70523,10 +70523,10 @@
       <c r="M54" s="23" t="s">
         <v>1387</v>
       </c>
-      <c r="N54" s="121" t="s">
+      <c r="N54" s="119" t="s">
         <v>1580</v>
       </c>
-      <c r="O54" s="121" t="s">
+      <c r="O54" s="119" t="s">
         <v>90</v>
       </c>
       <c r="P54" s="9" t="s">
@@ -70569,10 +70569,10 @@
       <c r="M55" s="23" t="s">
         <v>1543</v>
       </c>
-      <c r="N55" s="122" t="s">
+      <c r="N55" s="120" t="s">
         <v>1544</v>
       </c>
-      <c r="O55" s="122" t="s">
+      <c r="O55" s="120" t="s">
         <v>1576</v>
       </c>
       <c r="P55" s="9" t="s">
@@ -70618,7 +70618,7 @@
       <c r="N56" s="23" t="s">
         <v>1547</v>
       </c>
-      <c r="O56" s="121" t="s">
+      <c r="O56" s="119" t="s">
         <v>89</v>
       </c>
       <c r="P56" s="9" t="s">
@@ -70661,7 +70661,7 @@
       <c r="N57" s="23" t="s">
         <v>1581</v>
       </c>
-      <c r="O57" s="121" t="s">
+      <c r="O57" s="119" t="s">
         <v>89</v>
       </c>
       <c r="P57" s="9" t="s">

</xml_diff>